<commit_message>
- parsed structural data from `10.1016/j.intermet.2025.108929`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Aug2025.xlsx
+++ b/MiscSmallUploads_Aug2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF716CF7-9C11-8A4D-8813-04B10BE5837C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF32D69-F17B-F847-9797-6DCA8625E766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="94">
   <si>
     <r>
       <rPr>
@@ -319,6 +319,99 @@
   </si>
   <si>
     <t>hardness HV</t>
+  </si>
+  <si>
+    <t>FCC</t>
+  </si>
+  <si>
+    <t>AAM</t>
+  </si>
+  <si>
+    <t>BCC+B2</t>
+  </si>
+  <si>
+    <t>FCC+BCC</t>
+  </si>
+  <si>
+    <t>FCC+B2</t>
+  </si>
+  <si>
+    <t>FeCoNiPdCu0.5</t>
+  </si>
+  <si>
+    <t>FeCoNiPdCu1</t>
+  </si>
+  <si>
+    <t>FeCoNiPdCu1.5</t>
+  </si>
+  <si>
+    <t>FeCoNiPdCu2</t>
+  </si>
+  <si>
+    <t>FeCoNiPdV0.5</t>
+  </si>
+  <si>
+    <t>FeCoNiPdV1</t>
+  </si>
+  <si>
+    <t>FeCoNiPdV1.5</t>
+  </si>
+  <si>
+    <t>FeCoNiPdV2</t>
+  </si>
+  <si>
+    <t>small 4g samples prepared by arc melting</t>
+  </si>
+  <si>
+    <t>FeCoNiPdMn0.5</t>
+  </si>
+  <si>
+    <t>FeCoNiPdMn1</t>
+  </si>
+  <si>
+    <t>FeCoNiPdMn1.5</t>
+  </si>
+  <si>
+    <t>FeCoNiPdAl0.5</t>
+  </si>
+  <si>
+    <t>FeCoNiPdAl1</t>
+  </si>
+  <si>
+    <t>FeCoNiPdAl1.5</t>
+  </si>
+  <si>
+    <t>FeCoNiPdTi0.5</t>
+  </si>
+  <si>
+    <t>FeCoNiPdTi1</t>
+  </si>
+  <si>
+    <t>FeCoNiPdTi1.5</t>
+  </si>
+  <si>
+    <t>FCC+L10</t>
+  </si>
+  <si>
+    <t>FCC+B19</t>
+  </si>
+  <si>
+    <t>FCC+FCC+FCC</t>
+  </si>
+  <si>
+    <t>FCC+C14</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>10.1016/j.intermet.2025.108929</t>
   </si>
 </sst>
 </file>
@@ -2822,7 +2915,7 @@
   <dimension ref="A1:T960"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O305" sqref="O305"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -3179,10 +3272,18 @@
     </row>
     <row r="10" spans="1:20" ht="19.5" customHeight="1">
       <c r="A10" s="30"/>
-      <c r="B10" s="67"/>
-      <c r="C10" s="68"/>
-      <c r="D10" s="68"/>
-      <c r="E10" s="67"/>
+      <c r="B10" s="67" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="67" t="s">
+        <v>76</v>
+      </c>
       <c r="F10" s="69"/>
       <c r="G10" s="69"/>
       <c r="H10" s="70"/>
@@ -3191,7 +3292,9 @@
       <c r="K10" s="90"/>
       <c r="L10" s="69"/>
       <c r="M10" s="69"/>
-      <c r="N10" s="72"/>
+      <c r="N10" s="72" t="s">
+        <v>93</v>
+      </c>
       <c r="O10" s="73"/>
       <c r="P10" s="74"/>
       <c r="Q10" s="74"/>
@@ -3201,10 +3304,18 @@
     </row>
     <row r="11" spans="1:20" ht="18.75" customHeight="1">
       <c r="A11" s="30"/>
-      <c r="B11" s="67"/>
-      <c r="C11" s="68"/>
-      <c r="D11" s="68"/>
-      <c r="E11" s="67"/>
+      <c r="B11" s="67" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="67" t="s">
+        <v>76</v>
+      </c>
       <c r="F11" s="69"/>
       <c r="G11" s="69"/>
       <c r="H11" s="70"/>
@@ -3213,7 +3324,9 @@
       <c r="K11" s="90"/>
       <c r="L11" s="69"/>
       <c r="M11" s="69"/>
-      <c r="N11" s="72"/>
+      <c r="N11" s="72" t="s">
+        <v>93</v>
+      </c>
       <c r="O11" s="37"/>
       <c r="P11" s="38"/>
       <c r="Q11" s="38"/>
@@ -3223,10 +3336,18 @@
     </row>
     <row r="12" spans="1:20" ht="18.75" customHeight="1">
       <c r="A12" s="30"/>
-      <c r="B12" s="67"/>
-      <c r="C12" s="68"/>
-      <c r="D12" s="68"/>
-      <c r="E12" s="67"/>
+      <c r="B12" s="67" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="67" t="s">
+        <v>76</v>
+      </c>
       <c r="F12" s="69"/>
       <c r="G12" s="69"/>
       <c r="H12" s="70"/>
@@ -3235,7 +3356,9 @@
       <c r="K12" s="90"/>
       <c r="L12" s="69"/>
       <c r="M12" s="69"/>
-      <c r="N12" s="72"/>
+      <c r="N12" s="72" t="s">
+        <v>93</v>
+      </c>
       <c r="O12" s="37"/>
       <c r="P12" s="38"/>
       <c r="Q12" s="38"/>
@@ -3245,10 +3368,18 @@
     </row>
     <row r="13" spans="1:20" ht="18.75" customHeight="1">
       <c r="A13" s="30"/>
-      <c r="B13" s="67"/>
-      <c r="C13" s="68"/>
-      <c r="D13" s="68"/>
-      <c r="E13" s="67"/>
+      <c r="B13" s="67" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="67" t="s">
+        <v>76</v>
+      </c>
       <c r="F13" s="69"/>
       <c r="G13" s="69"/>
       <c r="H13" s="33"/>
@@ -3257,7 +3388,9 @@
       <c r="K13" s="90"/>
       <c r="L13" s="69"/>
       <c r="M13" s="69"/>
-      <c r="N13" s="72"/>
+      <c r="N13" s="72" t="s">
+        <v>93</v>
+      </c>
       <c r="O13" s="37"/>
       <c r="P13" s="38"/>
       <c r="Q13" s="38"/>
@@ -3267,10 +3400,18 @@
     </row>
     <row r="14" spans="1:20" ht="18.75" customHeight="1">
       <c r="A14" s="30"/>
-      <c r="B14" s="67"/>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="31"/>
+      <c r="B14" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="67" t="s">
+        <v>76</v>
+      </c>
       <c r="F14" s="69"/>
       <c r="G14" s="69"/>
       <c r="H14" s="33"/>
@@ -3279,7 +3420,9 @@
       <c r="K14" s="90"/>
       <c r="L14" s="69"/>
       <c r="M14" s="32"/>
-      <c r="N14" s="72"/>
+      <c r="N14" s="72" t="s">
+        <v>93</v>
+      </c>
       <c r="O14" s="37"/>
       <c r="P14" s="37"/>
       <c r="Q14" s="37"/>
@@ -3289,10 +3432,18 @@
     </row>
     <row r="15" spans="1:20" ht="18.75" customHeight="1">
       <c r="A15" s="30"/>
-      <c r="B15" s="67"/>
-      <c r="C15" s="68"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="31"/>
+      <c r="B15" s="67" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="67" t="s">
+        <v>76</v>
+      </c>
       <c r="F15" s="69"/>
       <c r="G15" s="69"/>
       <c r="H15" s="33"/>
@@ -3301,7 +3452,9 @@
       <c r="K15" s="90"/>
       <c r="L15" s="69"/>
       <c r="M15" s="32"/>
-      <c r="N15" s="72"/>
+      <c r="N15" s="72" t="s">
+        <v>93</v>
+      </c>
       <c r="O15" s="37"/>
       <c r="P15" s="37"/>
       <c r="Q15" s="37"/>
@@ -3311,10 +3464,18 @@
     </row>
     <row r="16" spans="1:20" ht="18.75" customHeight="1">
       <c r="A16" s="30"/>
-      <c r="B16" s="67"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="68"/>
-      <c r="E16" s="31"/>
+      <c r="B16" s="67" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="67" t="s">
+        <v>76</v>
+      </c>
       <c r="F16" s="69"/>
       <c r="G16" s="69"/>
       <c r="H16" s="33"/>
@@ -3323,7 +3484,9 @@
       <c r="K16" s="90"/>
       <c r="L16" s="69"/>
       <c r="M16" s="32"/>
-      <c r="N16" s="72"/>
+      <c r="N16" s="72" t="s">
+        <v>93</v>
+      </c>
       <c r="O16" s="37"/>
       <c r="P16" s="37"/>
       <c r="Q16" s="37"/>
@@ -3333,10 +3496,18 @@
     </row>
     <row r="17" spans="1:20" ht="18.75" customHeight="1">
       <c r="A17" s="38"/>
-      <c r="B17" s="67"/>
-      <c r="C17" s="68"/>
-      <c r="D17" s="68"/>
-      <c r="E17" s="31"/>
+      <c r="B17" s="67" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="67" t="s">
+        <v>76</v>
+      </c>
       <c r="F17" s="69"/>
       <c r="G17" s="69"/>
       <c r="H17" s="33"/>
@@ -3345,7 +3516,9 @@
       <c r="K17" s="90"/>
       <c r="L17" s="69"/>
       <c r="M17" s="32"/>
-      <c r="N17" s="72"/>
+      <c r="N17" s="72" t="s">
+        <v>93</v>
+      </c>
       <c r="O17" s="37"/>
       <c r="P17" s="37"/>
       <c r="Q17" s="37"/>
@@ -3355,10 +3528,18 @@
     </row>
     <row r="18" spans="1:20" ht="18.75" customHeight="1">
       <c r="A18" s="38"/>
-      <c r="B18" s="67"/>
-      <c r="C18" s="68"/>
-      <c r="D18" s="68"/>
-      <c r="E18" s="31"/>
+      <c r="B18" s="67" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="67" t="s">
+        <v>76</v>
+      </c>
       <c r="F18" s="32"/>
       <c r="G18" s="69"/>
       <c r="H18" s="33"/>
@@ -3366,8 +3547,12 @@
       <c r="J18" s="71"/>
       <c r="K18" s="38"/>
       <c r="L18" s="69"/>
-      <c r="M18" s="32"/>
-      <c r="N18" s="72"/>
+      <c r="M18" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="N18" s="72" t="s">
+        <v>93</v>
+      </c>
       <c r="O18" s="37"/>
       <c r="P18" s="37"/>
       <c r="Q18" s="39"/>
@@ -3377,10 +3562,18 @@
     </row>
     <row r="19" spans="1:20" ht="18.75" customHeight="1">
       <c r="A19" s="38"/>
-      <c r="B19" s="67"/>
-      <c r="C19" s="68"/>
-      <c r="D19" s="68"/>
-      <c r="E19" s="31"/>
+      <c r="B19" s="67" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="67" t="s">
+        <v>76</v>
+      </c>
       <c r="F19" s="32"/>
       <c r="G19" s="69"/>
       <c r="H19" s="33"/>
@@ -3388,8 +3581,12 @@
       <c r="J19" s="71"/>
       <c r="K19" s="38"/>
       <c r="L19" s="69"/>
-      <c r="M19" s="32"/>
-      <c r="N19" s="72"/>
+      <c r="M19" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="N19" s="72" t="s">
+        <v>93</v>
+      </c>
       <c r="O19" s="37"/>
       <c r="P19" s="37"/>
       <c r="Q19" s="39"/>
@@ -3399,10 +3596,18 @@
     </row>
     <row r="20" spans="1:20" ht="18.75" customHeight="1">
       <c r="A20" s="38"/>
-      <c r="B20" s="67"/>
-      <c r="C20" s="68"/>
-      <c r="D20" s="68"/>
-      <c r="E20" s="31"/>
+      <c r="B20" s="67" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="67" t="s">
+        <v>76</v>
+      </c>
       <c r="F20" s="32"/>
       <c r="G20" s="69"/>
       <c r="H20" s="33"/>
@@ -3410,8 +3615,12 @@
       <c r="J20" s="35"/>
       <c r="K20" s="38"/>
       <c r="L20" s="69"/>
-      <c r="M20" s="32"/>
-      <c r="N20" s="72"/>
+      <c r="M20" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="N20" s="72" t="s">
+        <v>93</v>
+      </c>
       <c r="O20" s="37"/>
       <c r="P20" s="37"/>
       <c r="Q20" s="39"/>
@@ -3421,10 +3630,18 @@
     </row>
     <row r="21" spans="1:20" ht="18.75" customHeight="1">
       <c r="A21" s="38"/>
-      <c r="B21" s="67"/>
-      <c r="C21" s="68"/>
-      <c r="D21" s="68"/>
-      <c r="E21" s="31"/>
+      <c r="B21" s="67" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" s="68" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" s="67" t="s">
+        <v>76</v>
+      </c>
       <c r="F21" s="32"/>
       <c r="G21" s="69"/>
       <c r="H21" s="33"/>
@@ -3432,8 +3649,12 @@
       <c r="J21" s="35"/>
       <c r="K21" s="38"/>
       <c r="L21" s="69"/>
-      <c r="M21" s="32"/>
-      <c r="N21" s="72"/>
+      <c r="M21" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="N21" s="72" t="s">
+        <v>93</v>
+      </c>
       <c r="O21" s="37"/>
       <c r="P21" s="37"/>
       <c r="Q21" s="39"/>
@@ -3443,10 +3664,18 @@
     </row>
     <row r="22" spans="1:20" ht="18.75" customHeight="1">
       <c r="A22" s="38"/>
-      <c r="B22" s="67"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="31"/>
+      <c r="B22" s="67" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="68" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" s="67" t="s">
+        <v>76</v>
+      </c>
       <c r="F22" s="32"/>
       <c r="G22" s="69"/>
       <c r="H22" s="33"/>
@@ -3454,8 +3683,12 @@
       <c r="J22" s="35"/>
       <c r="K22" s="35"/>
       <c r="L22" s="69"/>
-      <c r="M22" s="32"/>
-      <c r="N22" s="72"/>
+      <c r="M22" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="N22" s="72" t="s">
+        <v>93</v>
+      </c>
       <c r="O22" s="37"/>
       <c r="P22" s="37"/>
       <c r="Q22" s="39"/>
@@ -3465,10 +3698,18 @@
     </row>
     <row r="23" spans="1:20" ht="18.75" customHeight="1">
       <c r="A23" s="30"/>
-      <c r="B23" s="67"/>
-      <c r="C23" s="68"/>
-      <c r="D23" s="68"/>
-      <c r="E23" s="31"/>
+      <c r="B23" s="67" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="68" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="67" t="s">
+        <v>76</v>
+      </c>
       <c r="F23" s="32"/>
       <c r="G23" s="69"/>
       <c r="H23" s="33"/>
@@ -3476,8 +3717,12 @@
       <c r="J23" s="35"/>
       <c r="K23" s="58"/>
       <c r="L23" s="69"/>
-      <c r="M23" s="32"/>
-      <c r="N23" s="72"/>
+      <c r="M23" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="N23" s="72" t="s">
+        <v>93</v>
+      </c>
       <c r="O23" s="37"/>
       <c r="P23" s="37"/>
       <c r="Q23" s="39"/>
@@ -3487,10 +3732,18 @@
     </row>
     <row r="24" spans="1:20" ht="18.75" customHeight="1">
       <c r="A24" s="30"/>
-      <c r="B24" s="67"/>
-      <c r="C24" s="68"/>
-      <c r="D24" s="68"/>
-      <c r="E24" s="31"/>
+      <c r="B24" s="67" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" s="67" t="s">
+        <v>76</v>
+      </c>
       <c r="F24" s="32"/>
       <c r="G24" s="69"/>
       <c r="H24" s="33"/>
@@ -3498,8 +3751,12 @@
       <c r="J24" s="35"/>
       <c r="K24" s="58"/>
       <c r="L24" s="69"/>
-      <c r="M24" s="32"/>
-      <c r="N24" s="72"/>
+      <c r="M24" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="N24" s="72" t="s">
+        <v>93</v>
+      </c>
       <c r="O24" s="37"/>
       <c r="P24" s="37"/>
       <c r="Q24" s="39"/>
@@ -3509,10 +3766,18 @@
     </row>
     <row r="25" spans="1:20" ht="18.75" customHeight="1">
       <c r="A25" s="88"/>
-      <c r="B25" s="67"/>
-      <c r="C25" s="68"/>
-      <c r="D25" s="68"/>
-      <c r="E25" s="31"/>
+      <c r="B25" s="67" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="68" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" s="67" t="s">
+        <v>76</v>
+      </c>
       <c r="F25" s="32"/>
       <c r="G25" s="69"/>
       <c r="H25" s="33"/>
@@ -3520,8 +3785,12 @@
       <c r="J25" s="35"/>
       <c r="K25" s="58"/>
       <c r="L25" s="69"/>
-      <c r="M25" s="32"/>
-      <c r="N25" s="72"/>
+      <c r="M25" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="N25" s="72" t="s">
+        <v>93</v>
+      </c>
       <c r="O25" s="37"/>
       <c r="P25" s="38"/>
       <c r="Q25" s="39"/>
@@ -3531,10 +3800,18 @@
     </row>
     <row r="26" spans="1:20" ht="18.75" customHeight="1">
       <c r="A26" s="30"/>
-      <c r="B26" s="41"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
+      <c r="B26" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" s="67" t="s">
+        <v>76</v>
+      </c>
       <c r="F26" s="32"/>
       <c r="G26" s="32"/>
       <c r="H26" s="33"/>
@@ -3542,8 +3819,12 @@
       <c r="J26" s="90"/>
       <c r="K26" s="58"/>
       <c r="L26" s="32"/>
-      <c r="M26" s="40"/>
-      <c r="N26" s="36"/>
+      <c r="M26" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="N26" s="72" t="s">
+        <v>93</v>
+      </c>
       <c r="O26" s="37"/>
       <c r="P26" s="42"/>
       <c r="Q26" s="39"/>

</xml_diff>

<commit_message>
- parsed data from `10.1016/j.scriptamat.2022.115016`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Aug2025.xlsx
+++ b/MiscSmallUploads_Aug2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AD453E-F0E8-884D-A153-0EA5A2804F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF20BB8-B402-9A4F-BBE4-3E0E6F4A9341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9680" yWindow="7860" windowWidth="24880" windowHeight="13520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6760" yWindow="7700" windowWidth="24880" windowHeight="13520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="120">
   <si>
     <r>
       <rPr>
@@ -327,6 +327,9 @@
     <t>AAM</t>
   </si>
   <si>
+    <t>FCC+BCC+B2</t>
+  </si>
+  <si>
     <t>BCC+B2</t>
   </si>
   <si>
@@ -469,6 +472,24 @@
   </si>
   <si>
     <t>10.1007/s12598-025-03420-w</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(CoCrNi)29 Al13 </t>
+  </si>
+  <si>
+    <t>L-DED under 600W power with 3.4g/min deposition over 1mm beam and 8mm/s scan depositing around 0.3mm thick layer under argon</t>
+  </si>
+  <si>
+    <t>LDED(DED)</t>
+  </si>
+  <si>
+    <t>L-DED under 600W power with 3.7g/min deposition over 1mm beam and 8mm/s scan depositing around 0.3mm thick layer under argon</t>
+  </si>
+  <si>
+    <t>uniform elongation</t>
+  </si>
+  <si>
+    <t>10.1016/j.scriptamat.2022.115016</t>
   </si>
 </sst>
 </file>
@@ -2961,8 +2982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T960"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N47" sqref="N47"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C33" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N56" sqref="N56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -3320,7 +3341,7 @@
     <row r="10" spans="1:20" ht="19.5" customHeight="1">
       <c r="A10" s="30"/>
       <c r="B10" s="67" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C10" s="68" t="s">
         <v>63</v>
@@ -3329,7 +3350,7 @@
         <v>64</v>
       </c>
       <c r="E10" s="67" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F10" s="69"/>
       <c r="G10" s="69"/>
@@ -3340,7 +3361,7 @@
       <c r="L10" s="69"/>
       <c r="M10" s="69"/>
       <c r="N10" s="72" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O10" s="73"/>
       <c r="P10" s="74"/>
@@ -3352,7 +3373,7 @@
     <row r="11" spans="1:20" ht="18.75" customHeight="1">
       <c r="A11" s="30"/>
       <c r="B11" s="67" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C11" s="68" t="s">
         <v>63</v>
@@ -3361,7 +3382,7 @@
         <v>64</v>
       </c>
       <c r="E11" s="67" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F11" s="69"/>
       <c r="G11" s="69"/>
@@ -3372,7 +3393,7 @@
       <c r="L11" s="69"/>
       <c r="M11" s="69"/>
       <c r="N11" s="72" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O11" s="37"/>
       <c r="P11" s="38"/>
@@ -3384,7 +3405,7 @@
     <row r="12" spans="1:20" ht="18.75" customHeight="1">
       <c r="A12" s="30"/>
       <c r="B12" s="67" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C12" s="68" t="s">
         <v>63</v>
@@ -3393,7 +3414,7 @@
         <v>64</v>
       </c>
       <c r="E12" s="67" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F12" s="69"/>
       <c r="G12" s="69"/>
@@ -3404,7 +3425,7 @@
       <c r="L12" s="69"/>
       <c r="M12" s="69"/>
       <c r="N12" s="72" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O12" s="37"/>
       <c r="P12" s="38"/>
@@ -3416,7 +3437,7 @@
     <row r="13" spans="1:20" ht="18.75" customHeight="1">
       <c r="A13" s="30"/>
       <c r="B13" s="67" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C13" s="68" t="s">
         <v>63</v>
@@ -3425,7 +3446,7 @@
         <v>64</v>
       </c>
       <c r="E13" s="67" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F13" s="69"/>
       <c r="G13" s="69"/>
@@ -3436,7 +3457,7 @@
       <c r="L13" s="69"/>
       <c r="M13" s="69"/>
       <c r="N13" s="72" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O13" s="37"/>
       <c r="P13" s="38"/>
@@ -3448,7 +3469,7 @@
     <row r="14" spans="1:20" ht="18.75" customHeight="1">
       <c r="A14" s="30"/>
       <c r="B14" s="67" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C14" s="68" t="s">
         <v>63</v>
@@ -3457,7 +3478,7 @@
         <v>64</v>
       </c>
       <c r="E14" s="67" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F14" s="69"/>
       <c r="G14" s="69"/>
@@ -3468,7 +3489,7 @@
       <c r="L14" s="69"/>
       <c r="M14" s="32"/>
       <c r="N14" s="72" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O14" s="37"/>
       <c r="P14" s="37"/>
@@ -3480,7 +3501,7 @@
     <row r="15" spans="1:20" ht="18.75" customHeight="1">
       <c r="A15" s="30"/>
       <c r="B15" s="67" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C15" s="68" t="s">
         <v>63</v>
@@ -3489,7 +3510,7 @@
         <v>64</v>
       </c>
       <c r="E15" s="67" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F15" s="69"/>
       <c r="G15" s="69"/>
@@ -3500,7 +3521,7 @@
       <c r="L15" s="69"/>
       <c r="M15" s="32"/>
       <c r="N15" s="72" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O15" s="37"/>
       <c r="P15" s="37"/>
@@ -3512,7 +3533,7 @@
     <row r="16" spans="1:20" ht="18.75" customHeight="1">
       <c r="A16" s="30"/>
       <c r="B16" s="67" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C16" s="68" t="s">
         <v>63</v>
@@ -3521,7 +3542,7 @@
         <v>64</v>
       </c>
       <c r="E16" s="67" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F16" s="69"/>
       <c r="G16" s="69"/>
@@ -3532,7 +3553,7 @@
       <c r="L16" s="69"/>
       <c r="M16" s="32"/>
       <c r="N16" s="72" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O16" s="37"/>
       <c r="P16" s="37"/>
@@ -3544,7 +3565,7 @@
     <row r="17" spans="1:20" ht="18.75" customHeight="1">
       <c r="A17" s="38"/>
       <c r="B17" s="67" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C17" s="68" t="s">
         <v>63</v>
@@ -3553,7 +3574,7 @@
         <v>64</v>
       </c>
       <c r="E17" s="67" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F17" s="69"/>
       <c r="G17" s="69"/>
@@ -3564,7 +3585,7 @@
       <c r="L17" s="69"/>
       <c r="M17" s="32"/>
       <c r="N17" s="72" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O17" s="37"/>
       <c r="P17" s="37"/>
@@ -3576,16 +3597,16 @@
     <row r="18" spans="1:20" ht="18.75" customHeight="1">
       <c r="A18" s="38"/>
       <c r="B18" s="67" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C18" s="68" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D18" s="68" t="s">
         <v>64</v>
       </c>
       <c r="E18" s="67" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F18" s="32"/>
       <c r="G18" s="69"/>
@@ -3595,10 +3616,10 @@
       <c r="K18" s="38"/>
       <c r="L18" s="69"/>
       <c r="M18" s="32" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N18" s="72" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O18" s="37"/>
       <c r="P18" s="37"/>
@@ -3610,16 +3631,16 @@
     <row r="19" spans="1:20" ht="18.75" customHeight="1">
       <c r="A19" s="38"/>
       <c r="B19" s="67" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C19" s="68" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D19" s="68" t="s">
         <v>64</v>
       </c>
       <c r="E19" s="67" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F19" s="32"/>
       <c r="G19" s="69"/>
@@ -3629,10 +3650,10 @@
       <c r="K19" s="38"/>
       <c r="L19" s="69"/>
       <c r="M19" s="32" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N19" s="72" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O19" s="37"/>
       <c r="P19" s="37"/>
@@ -3644,16 +3665,16 @@
     <row r="20" spans="1:20" ht="18.75" customHeight="1">
       <c r="A20" s="38"/>
       <c r="B20" s="67" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C20" s="68" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D20" s="68" t="s">
         <v>64</v>
       </c>
       <c r="E20" s="67" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F20" s="32"/>
       <c r="G20" s="69"/>
@@ -3663,10 +3684,10 @@
       <c r="K20" s="38"/>
       <c r="L20" s="69"/>
       <c r="M20" s="32" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N20" s="72" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O20" s="37"/>
       <c r="P20" s="37"/>
@@ -3678,16 +3699,16 @@
     <row r="21" spans="1:20" ht="18.75" customHeight="1">
       <c r="A21" s="38"/>
       <c r="B21" s="67" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C21" s="68" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D21" s="68" t="s">
         <v>64</v>
       </c>
       <c r="E21" s="67" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F21" s="32"/>
       <c r="G21" s="69"/>
@@ -3697,10 +3718,10 @@
       <c r="K21" s="38"/>
       <c r="L21" s="69"/>
       <c r="M21" s="32" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N21" s="72" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O21" s="37"/>
       <c r="P21" s="37"/>
@@ -3712,16 +3733,16 @@
     <row r="22" spans="1:20" ht="18.75" customHeight="1">
       <c r="A22" s="38"/>
       <c r="B22" s="67" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C22" s="68" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D22" s="68" t="s">
         <v>64</v>
       </c>
       <c r="E22" s="67" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F22" s="32"/>
       <c r="G22" s="69"/>
@@ -3731,10 +3752,10 @@
       <c r="K22" s="35"/>
       <c r="L22" s="69"/>
       <c r="M22" s="32" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N22" s="72" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O22" s="37"/>
       <c r="P22" s="37"/>
@@ -3746,16 +3767,16 @@
     <row r="23" spans="1:20" ht="18.75" customHeight="1">
       <c r="A23" s="30"/>
       <c r="B23" s="67" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C23" s="68" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D23" s="68" t="s">
         <v>64</v>
       </c>
       <c r="E23" s="67" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F23" s="32"/>
       <c r="G23" s="69"/>
@@ -3765,10 +3786,10 @@
       <c r="K23" s="58"/>
       <c r="L23" s="69"/>
       <c r="M23" s="32" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N23" s="72" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O23" s="37"/>
       <c r="P23" s="37"/>
@@ -3780,16 +3801,16 @@
     <row r="24" spans="1:20" ht="18.75" customHeight="1">
       <c r="A24" s="30"/>
       <c r="B24" s="67" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C24" s="68" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D24" s="68" t="s">
         <v>64</v>
       </c>
       <c r="E24" s="67" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F24" s="32"/>
       <c r="G24" s="69"/>
@@ -3799,10 +3820,10 @@
       <c r="K24" s="58"/>
       <c r="L24" s="69"/>
       <c r="M24" s="32" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="N24" s="72" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O24" s="37"/>
       <c r="P24" s="37"/>
@@ -3814,16 +3835,16 @@
     <row r="25" spans="1:20" ht="18.75" customHeight="1">
       <c r="A25" s="88"/>
       <c r="B25" s="67" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C25" s="68" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D25" s="68" t="s">
         <v>64</v>
       </c>
       <c r="E25" s="67" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F25" s="32"/>
       <c r="G25" s="69"/>
@@ -3833,10 +3854,10 @@
       <c r="K25" s="58"/>
       <c r="L25" s="69"/>
       <c r="M25" s="32" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="N25" s="72" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O25" s="37"/>
       <c r="P25" s="38"/>
@@ -3848,16 +3869,16 @@
     <row r="26" spans="1:20" ht="18.75" customHeight="1">
       <c r="A26" s="30"/>
       <c r="B26" s="41" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D26" s="68" t="s">
         <v>64</v>
       </c>
       <c r="E26" s="67" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F26" s="32"/>
       <c r="G26" s="32"/>
@@ -3867,10 +3888,10 @@
       <c r="K26" s="58"/>
       <c r="L26" s="32"/>
       <c r="M26" s="32" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="N26" s="72" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O26" s="37"/>
       <c r="P26" s="42"/>
@@ -3881,22 +3902,22 @@
     </row>
     <row r="27" spans="1:20" ht="18.75" customHeight="1">
       <c r="A27" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B27" s="41" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C27" s="30" t="s">
         <v>63</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F27" s="32" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G27" s="32" t="s">
         <v>29</v>
@@ -3913,10 +3934,10 @@
         <v>33</v>
       </c>
       <c r="M27" s="40" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N27" s="36" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O27" s="37"/>
       <c r="P27" s="42"/>
@@ -3927,22 +3948,22 @@
     </row>
     <row r="28" spans="1:20" ht="18.75" customHeight="1">
       <c r="A28" s="30" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B28" s="41" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C28" s="30" t="s">
         <v>63</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F28" s="32" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G28" s="32" t="s">
         <v>29</v>
@@ -3959,10 +3980,10 @@
         <v>33</v>
       </c>
       <c r="M28" s="40" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N28" s="36" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O28" s="37"/>
       <c r="P28" s="42"/>
@@ -3973,22 +3994,22 @@
     </row>
     <row r="29" spans="1:20" ht="18.75" customHeight="1">
       <c r="A29" s="101" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B29" s="41" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C29" s="30" t="s">
         <v>63</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F29" s="32" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G29" s="32" t="s">
         <v>29</v>
@@ -4005,10 +4026,10 @@
         <v>33</v>
       </c>
       <c r="M29" s="40" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N29" s="36" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O29" s="37"/>
       <c r="P29" s="42"/>
@@ -4019,22 +4040,22 @@
     </row>
     <row r="30" spans="1:20" ht="18.75" customHeight="1">
       <c r="A30" s="30" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B30" s="41" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C30" s="30" t="s">
         <v>63</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F30" s="32" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G30" s="32" t="s">
         <v>29</v>
@@ -4051,10 +4072,10 @@
         <v>33</v>
       </c>
       <c r="M30" s="40" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N30" s="36" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O30" s="37"/>
       <c r="P30" s="42"/>
@@ -4065,22 +4086,22 @@
     </row>
     <row r="31" spans="1:20" ht="18.75" customHeight="1">
       <c r="A31" s="30" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B31" s="41" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C31" s="30" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F31" s="32" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G31" s="32" t="s">
         <v>29</v>
@@ -4097,10 +4118,10 @@
         <v>33</v>
       </c>
       <c r="M31" s="40" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N31" s="36" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O31" s="37"/>
       <c r="P31" s="42"/>
@@ -4111,22 +4132,22 @@
     </row>
     <row r="32" spans="1:20" ht="18.75" customHeight="1">
       <c r="A32" s="30" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B32" s="41" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D32" s="30" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F32" s="32" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G32" s="32" t="s">
         <v>29</v>
@@ -4143,10 +4164,10 @@
         <v>33</v>
       </c>
       <c r="M32" s="40" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N32" s="36" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O32" s="37"/>
       <c r="P32" s="42"/>
@@ -4157,22 +4178,22 @@
     </row>
     <row r="33" spans="1:20" ht="18.75" customHeight="1">
       <c r="A33" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B33" s="41" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C33" s="30" t="s">
         <v>63</v>
       </c>
       <c r="D33" s="30" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F33" s="32" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G33" s="32" t="s">
         <v>29</v>
@@ -4189,10 +4210,10 @@
         <v>33</v>
       </c>
       <c r="M33" s="40" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N33" s="36" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O33" s="37"/>
       <c r="P33" s="42"/>
@@ -4203,22 +4224,22 @@
     </row>
     <row r="34" spans="1:20" ht="18.75" customHeight="1">
       <c r="A34" s="30" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B34" s="41" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C34" s="30" t="s">
         <v>63</v>
       </c>
       <c r="D34" s="30" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F34" s="32" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G34" s="32" t="s">
         <v>29</v>
@@ -4235,10 +4256,10 @@
         <v>33</v>
       </c>
       <c r="M34" s="40" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N34" s="36" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O34" s="37"/>
       <c r="P34" s="38"/>
@@ -4249,22 +4270,22 @@
     </row>
     <row r="35" spans="1:20" ht="18.75" customHeight="1">
       <c r="A35" s="101" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B35" s="41" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C35" s="30" t="s">
         <v>63</v>
       </c>
       <c r="D35" s="30" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F35" s="32" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G35" s="32" t="s">
         <v>29</v>
@@ -4281,10 +4302,10 @@
         <v>33</v>
       </c>
       <c r="M35" s="40" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N35" s="36" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O35" s="37"/>
       <c r="P35" s="38"/>
@@ -4295,22 +4316,22 @@
     </row>
     <row r="36" spans="1:20" ht="18.75" customHeight="1">
       <c r="A36" s="30" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B36" s="41" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C36" s="30" t="s">
         <v>63</v>
       </c>
       <c r="D36" s="30" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F36" s="32" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G36" s="32" t="s">
         <v>29</v>
@@ -4327,10 +4348,10 @@
         <v>33</v>
       </c>
       <c r="M36" s="40" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N36" s="36" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O36" s="37"/>
       <c r="P36" s="38"/>
@@ -4341,22 +4362,22 @@
     </row>
     <row r="37" spans="1:20" ht="18.75" customHeight="1">
       <c r="A37" s="30" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B37" s="41" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C37" s="30" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D37" s="30" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F37" s="32" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G37" s="32" t="s">
         <v>29</v>
@@ -4373,10 +4394,10 @@
         <v>33</v>
       </c>
       <c r="M37" s="40" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N37" s="36" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O37" s="37"/>
       <c r="P37" s="38"/>
@@ -4387,22 +4408,22 @@
     </row>
     <row r="38" spans="1:20" ht="18.75" customHeight="1">
       <c r="A38" s="30" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B38" s="41" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C38" s="30" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D38" s="30" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F38" s="32" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G38" s="32" t="s">
         <v>29</v>
@@ -4419,10 +4440,10 @@
         <v>33</v>
       </c>
       <c r="M38" s="40" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N38" s="36" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O38" s="45"/>
       <c r="P38" s="39"/>
@@ -4433,22 +4454,22 @@
     </row>
     <row r="39" spans="1:20" ht="18.75" customHeight="1">
       <c r="A39" s="147" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B39" s="103" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C39" s="90" t="s">
         <v>63</v>
       </c>
       <c r="D39" s="90" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E39" s="90" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F39" s="32" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G39" s="32" t="s">
         <v>29</v>
@@ -4462,13 +4483,13 @@
       </c>
       <c r="K39" s="35"/>
       <c r="L39" s="32" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M39" s="40" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N39" s="36" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O39" s="45"/>
       <c r="P39" s="39"/>
@@ -4479,22 +4500,22 @@
     </row>
     <row r="40" spans="1:20" ht="18.75" customHeight="1">
       <c r="A40" s="148" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B40" s="105" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C40" s="91" t="s">
         <v>63</v>
       </c>
       <c r="D40" s="91" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E40" s="91" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F40" s="32" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G40" s="32" t="s">
         <v>29</v>
@@ -4508,13 +4529,13 @@
       </c>
       <c r="K40" s="46"/>
       <c r="L40" s="32" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M40" s="40" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N40" s="36" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O40" s="45"/>
       <c r="P40" s="39"/>
@@ -4525,22 +4546,22 @@
     </row>
     <row r="41" spans="1:20" ht="18.75" customHeight="1">
       <c r="A41" s="101" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B41" s="104" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C41" s="91" t="s">
         <v>63</v>
       </c>
       <c r="D41" s="91" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E41" s="91" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F41" s="32" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G41" s="32" t="s">
         <v>29</v>
@@ -4554,13 +4575,13 @@
       </c>
       <c r="K41" s="46"/>
       <c r="L41" s="32" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M41" s="40" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N41" s="36" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O41" s="45"/>
       <c r="P41" s="39"/>
@@ -4571,22 +4592,22 @@
     </row>
     <row r="42" spans="1:20" ht="18.75" customHeight="1">
       <c r="A42" s="147" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B42" s="105" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C42" s="91" t="s">
         <v>63</v>
       </c>
       <c r="D42" s="91" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E42" s="91" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F42" s="32" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G42" s="32" t="s">
         <v>29</v>
@@ -4600,13 +4621,13 @@
       </c>
       <c r="K42" s="46"/>
       <c r="L42" s="32" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M42" s="40" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N42" s="36" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O42" s="45"/>
       <c r="P42" s="46"/>
@@ -4617,22 +4638,22 @@
     </row>
     <row r="43" spans="1:20" ht="18" customHeight="1">
       <c r="A43" s="148" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B43" s="105" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C43" s="91" t="s">
+        <v>72</v>
+      </c>
+      <c r="D43" s="91" t="s">
+        <v>110</v>
+      </c>
+      <c r="E43" s="91" t="s">
+        <v>112</v>
+      </c>
+      <c r="F43" s="32" t="s">
         <v>71</v>
-      </c>
-      <c r="D43" s="91" t="s">
-        <v>109</v>
-      </c>
-      <c r="E43" s="91" t="s">
-        <v>111</v>
-      </c>
-      <c r="F43" s="32" t="s">
-        <v>70</v>
       </c>
       <c r="G43" s="32" t="s">
         <v>29</v>
@@ -4646,13 +4667,13 @@
       </c>
       <c r="K43" s="46"/>
       <c r="L43" s="32" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M43" s="40" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N43" s="36" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O43" s="45"/>
       <c r="P43" s="46"/>
@@ -4663,22 +4684,22 @@
     </row>
     <row r="44" spans="1:20" ht="18" customHeight="1">
       <c r="A44" s="148" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B44" s="105" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C44" s="91" t="s">
+        <v>72</v>
+      </c>
+      <c r="D44" s="91" t="s">
+        <v>110</v>
+      </c>
+      <c r="E44" s="91" t="s">
+        <v>112</v>
+      </c>
+      <c r="F44" s="32" t="s">
         <v>71</v>
-      </c>
-      <c r="D44" s="91" t="s">
-        <v>109</v>
-      </c>
-      <c r="E44" s="91" t="s">
-        <v>111</v>
-      </c>
-      <c r="F44" s="32" t="s">
-        <v>70</v>
       </c>
       <c r="G44" s="32" t="s">
         <v>29</v>
@@ -4692,13 +4713,13 @@
       </c>
       <c r="K44" s="48"/>
       <c r="L44" s="32" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M44" s="40" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N44" s="36" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O44" s="45"/>
       <c r="P44" s="45"/>
@@ -4709,19 +4730,39 @@
     </row>
     <row r="45" spans="1:20" ht="18" customHeight="1">
       <c r="A45" s="30"/>
-      <c r="B45" s="41"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="30"/>
-      <c r="E45" s="30"/>
-      <c r="F45" s="32"/>
-      <c r="G45" s="32"/>
+      <c r="B45" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="C45" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D45" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="E45" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F45" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="G45" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H45" s="33"/>
-      <c r="I45" s="34"/>
-      <c r="J45" s="89"/>
+      <c r="I45" s="34">
+        <v>298</v>
+      </c>
+      <c r="J45" s="89">
+        <v>346000000</v>
+      </c>
       <c r="K45" s="48"/>
-      <c r="L45" s="32"/>
+      <c r="L45" s="32" t="s">
+        <v>33</v>
+      </c>
       <c r="M45" s="40"/>
-      <c r="N45" s="36"/>
+      <c r="N45" s="36" t="s">
+        <v>119</v>
+      </c>
       <c r="O45" s="45"/>
       <c r="P45" s="45"/>
       <c r="Q45" s="39"/>
@@ -4731,19 +4772,39 @@
     </row>
     <row r="46" spans="1:20" ht="18" customHeight="1">
       <c r="A46" s="30"/>
-      <c r="B46" s="41"/>
-      <c r="C46" s="30"/>
-      <c r="D46" s="30"/>
-      <c r="E46" s="30"/>
-      <c r="F46" s="32"/>
-      <c r="G46" s="32"/>
+      <c r="B46" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="C46" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="D46" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="E46" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="F46" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="G46" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H46" s="33"/>
-      <c r="I46" s="34"/>
-      <c r="J46" s="89"/>
+      <c r="I46" s="34">
+        <v>298</v>
+      </c>
+      <c r="J46" s="89">
+        <v>578000000</v>
+      </c>
       <c r="K46" s="35"/>
-      <c r="L46" s="32"/>
+      <c r="L46" s="32" t="s">
+        <v>33</v>
+      </c>
       <c r="M46" s="40"/>
-      <c r="N46" s="36"/>
+      <c r="N46" s="36" t="s">
+        <v>119</v>
+      </c>
       <c r="O46" s="45"/>
       <c r="P46" s="45"/>
       <c r="Q46" s="39"/>
@@ -4753,19 +4814,39 @@
     </row>
     <row r="47" spans="1:20" ht="18" customHeight="1">
       <c r="A47" s="30"/>
-      <c r="B47" s="41"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="32"/>
-      <c r="G47" s="32"/>
+      <c r="B47" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="C47" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D47" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="E47" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F47" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G47" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H47" s="33"/>
-      <c r="I47" s="34"/>
-      <c r="J47" s="89"/>
+      <c r="I47" s="34">
+        <v>298</v>
+      </c>
+      <c r="J47" s="89">
+        <v>605000000</v>
+      </c>
       <c r="K47" s="46"/>
-      <c r="L47" s="32"/>
+      <c r="L47" s="32" t="s">
+        <v>33</v>
+      </c>
       <c r="M47" s="40"/>
-      <c r="N47" s="36"/>
+      <c r="N47" s="36" t="s">
+        <v>119</v>
+      </c>
       <c r="O47" s="45"/>
       <c r="P47" s="45"/>
       <c r="Q47" s="39"/>
@@ -4775,19 +4856,39 @@
     </row>
     <row r="48" spans="1:20" ht="18" customHeight="1">
       <c r="A48" s="30"/>
-      <c r="B48" s="41"/>
-      <c r="C48" s="30"/>
-      <c r="D48" s="30"/>
-      <c r="E48" s="30"/>
-      <c r="F48" s="32"/>
-      <c r="G48" s="32"/>
+      <c r="B48" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="C48" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="D48" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="E48" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="F48" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G48" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H48" s="33"/>
-      <c r="I48" s="34"/>
-      <c r="J48" s="89"/>
+      <c r="I48" s="34">
+        <v>298</v>
+      </c>
+      <c r="J48" s="89">
+        <v>960000000</v>
+      </c>
       <c r="K48" s="46"/>
-      <c r="L48" s="32"/>
+      <c r="L48" s="32" t="s">
+        <v>33</v>
+      </c>
       <c r="M48" s="40"/>
-      <c r="N48" s="36"/>
+      <c r="N48" s="36" t="s">
+        <v>119</v>
+      </c>
       <c r="O48" s="45"/>
       <c r="P48" s="45"/>
       <c r="Q48" s="39"/>
@@ -4797,19 +4898,39 @@
     </row>
     <row r="49" spans="1:20" ht="18" customHeight="1">
       <c r="A49" s="30"/>
-      <c r="B49" s="41"/>
-      <c r="C49" s="30"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="30"/>
-      <c r="F49" s="32"/>
-      <c r="G49" s="32"/>
+      <c r="B49" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="C49" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D49" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="E49" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F49" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="G49" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H49" s="33"/>
-      <c r="I49" s="34"/>
-      <c r="J49" s="89"/>
+      <c r="I49" s="34">
+        <v>298</v>
+      </c>
+      <c r="J49" s="89">
+        <v>31.7</v>
+      </c>
       <c r="K49" s="46"/>
-      <c r="L49" s="32"/>
+      <c r="L49" s="32" t="s">
+        <v>68</v>
+      </c>
       <c r="M49" s="40"/>
-      <c r="N49" s="36"/>
+      <c r="N49" s="36" t="s">
+        <v>119</v>
+      </c>
       <c r="O49" s="45"/>
       <c r="P49" s="45"/>
       <c r="Q49" s="39"/>
@@ -4819,19 +4940,39 @@
     </row>
     <row r="50" spans="1:20" ht="18" customHeight="1">
       <c r="A50" s="30"/>
-      <c r="B50" s="41"/>
-      <c r="C50" s="30"/>
-      <c r="D50" s="30"/>
-      <c r="E50" s="30"/>
-      <c r="F50" s="32"/>
-      <c r="G50" s="32"/>
+      <c r="B50" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="C50" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="D50" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="E50" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="F50" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="G50" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H50" s="33"/>
-      <c r="I50" s="34"/>
-      <c r="J50" s="89"/>
+      <c r="I50" s="34">
+        <v>298</v>
+      </c>
+      <c r="J50" s="89">
+        <v>21.7</v>
+      </c>
       <c r="K50" s="46"/>
-      <c r="L50" s="32"/>
+      <c r="L50" s="32" t="s">
+        <v>68</v>
+      </c>
       <c r="M50" s="40"/>
-      <c r="N50" s="36"/>
+      <c r="N50" s="36" t="s">
+        <v>119</v>
+      </c>
       <c r="O50" s="45"/>
       <c r="P50" s="45"/>
       <c r="Q50" s="39"/>
@@ -4841,19 +4982,39 @@
     </row>
     <row r="51" spans="1:20" ht="18" customHeight="1">
       <c r="A51" s="30"/>
-      <c r="B51" s="41"/>
-      <c r="C51" s="30"/>
-      <c r="D51" s="30"/>
-      <c r="E51" s="30"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="32"/>
+      <c r="B51" s="102" t="s">
+        <v>99</v>
+      </c>
+      <c r="C51" s="90" t="s">
+        <v>63</v>
+      </c>
+      <c r="D51" s="90" t="s">
+        <v>116</v>
+      </c>
+      <c r="E51" s="90" t="s">
+        <v>115</v>
+      </c>
+      <c r="F51" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="G51" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H51" s="33"/>
-      <c r="I51" s="34"/>
-      <c r="J51" s="89"/>
+      <c r="I51" s="34">
+        <v>298</v>
+      </c>
+      <c r="J51" s="89">
+        <v>39.5</v>
+      </c>
       <c r="K51" s="48"/>
-      <c r="L51" s="32"/>
+      <c r="L51" s="32" t="s">
+        <v>68</v>
+      </c>
       <c r="M51" s="40"/>
-      <c r="N51" s="36"/>
+      <c r="N51" s="36" t="s">
+        <v>119</v>
+      </c>
       <c r="O51" s="45"/>
       <c r="P51" s="45"/>
       <c r="Q51" s="39"/>
@@ -4863,19 +5024,39 @@
     </row>
     <row r="52" spans="1:20" ht="18" customHeight="1">
       <c r="A52" s="30"/>
-      <c r="B52" s="41"/>
-      <c r="C52" s="30"/>
-      <c r="D52" s="30"/>
-      <c r="E52" s="30"/>
-      <c r="F52" s="32"/>
-      <c r="G52" s="32"/>
+      <c r="B52" s="104" t="s">
+        <v>114</v>
+      </c>
+      <c r="C52" s="91" t="s">
+        <v>65</v>
+      </c>
+      <c r="D52" s="91" t="s">
+        <v>116</v>
+      </c>
+      <c r="E52" s="91" t="s">
+        <v>117</v>
+      </c>
+      <c r="F52" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="G52" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H52" s="33"/>
-      <c r="I52" s="34"/>
-      <c r="J52" s="89"/>
+      <c r="I52" s="34">
+        <v>298</v>
+      </c>
+      <c r="J52" s="89">
+        <v>23.5</v>
+      </c>
       <c r="K52" s="48"/>
-      <c r="L52" s="32"/>
+      <c r="L52" s="32" t="s">
+        <v>68</v>
+      </c>
       <c r="M52" s="40"/>
-      <c r="N52" s="36"/>
+      <c r="N52" s="36" t="s">
+        <v>119</v>
+      </c>
       <c r="O52" s="45"/>
       <c r="P52" s="46"/>
       <c r="Q52" s="39"/>

</xml_diff>

<commit_message>
- parsed data from `10.1016/j.mssp.2024.108498`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Aug2025.xlsx
+++ b/MiscSmallUploads_Aug2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF20BB8-B402-9A4F-BBE4-3E0E6F4A9341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC1945B-A6D4-2F49-B272-7D0409B990DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6760" yWindow="7700" windowWidth="24880" windowHeight="13520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4100" yWindow="4780" windowWidth="24880" windowHeight="13520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="130">
   <si>
     <r>
       <rPr>
@@ -490,6 +490,36 @@
   </si>
   <si>
     <t>10.1016/j.scriptamat.2022.115016</t>
+  </si>
+  <si>
+    <t>GaInSnBiZn</t>
+  </si>
+  <si>
+    <t>VAM</t>
+  </si>
+  <si>
+    <t>melting temperature</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>BCT+B10</t>
+  </si>
+  <si>
+    <t>BCT or A5 is beta-Sn phase and B10 is InBi intermetallic; ? is a minor Ga and Zn rich phase possibly A11 Ga that couldn't be easily identified and was not reported in XRD later on in the paper; 1g of powders melted into 4mm bead in vacuum</t>
+  </si>
+  <si>
+    <t>degrees</t>
+  </si>
+  <si>
+    <t>contact angle on copper</t>
+  </si>
+  <si>
+    <t>10.1016/j.mssp.2024.108498</t>
+  </si>
+  <si>
+    <t>F3</t>
   </si>
 </sst>
 </file>
@@ -1707,57 +1737,8 @@
     <xf numFmtId="0" fontId="15" fillId="10" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="10" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1818,8 +1799,57 @@
     <xf numFmtId="164" fontId="5" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2982,8 +3012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T960"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C33" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N56" sqref="N56"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M64" sqref="M64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -3040,19 +3070,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" s="127" t="s">
+      <c r="D2" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="128"/>
-      <c r="F2" s="131"/>
-      <c r="G2" s="132"/>
-      <c r="H2" s="132"/>
-      <c r="I2" s="133"/>
-      <c r="J2" s="134"/>
-      <c r="K2" s="134"/>
-      <c r="L2" s="132"/>
-      <c r="M2" s="132"/>
-      <c r="N2" s="135"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="119"/>
+      <c r="K2" s="119"/>
+      <c r="L2" s="117"/>
+      <c r="M2" s="117"/>
+      <c r="N2" s="120"/>
       <c r="O2" s="13"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -3068,17 +3098,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="129"/>
-      <c r="E3" s="130"/>
-      <c r="F3" s="136"/>
-      <c r="G3" s="136"/>
-      <c r="H3" s="136"/>
-      <c r="I3" s="137"/>
-      <c r="J3" s="138"/>
-      <c r="K3" s="138"/>
-      <c r="L3" s="136"/>
-      <c r="M3" s="136"/>
-      <c r="N3" s="139"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="121"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="121"/>
+      <c r="I3" s="122"/>
+      <c r="J3" s="123"/>
+      <c r="K3" s="123"/>
+      <c r="L3" s="121"/>
+      <c r="M3" s="121"/>
+      <c r="N3" s="124"/>
       <c r="O3" s="13"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -3119,43 +3149,43 @@
       <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="140" t="s">
+      <c r="C5" s="125" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="142" t="s">
+      <c r="D5" s="127" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="142" t="s">
+      <c r="E5" s="127" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="142" t="s">
+      <c r="F5" s="127" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="142" t="s">
+      <c r="G5" s="127" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="143" t="s">
+      <c r="H5" s="128" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="142" t="s">
+      <c r="I5" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="142" t="s">
+      <c r="J5" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="142" t="s">
+      <c r="K5" s="127" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="142" t="s">
+      <c r="L5" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="142" t="s">
+      <c r="M5" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="142" t="s">
+      <c r="N5" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="110" t="s">
+      <c r="O5" s="132" t="s">
         <v>20</v>
       </c>
       <c r="P5" s="25"/>
@@ -3171,19 +3201,19 @@
       <c r="B6" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="141"/>
-      <c r="D6" s="141"/>
-      <c r="E6" s="141"/>
-      <c r="F6" s="141"/>
-      <c r="G6" s="141"/>
-      <c r="H6" s="144"/>
-      <c r="I6" s="145"/>
-      <c r="J6" s="146"/>
-      <c r="K6" s="146"/>
-      <c r="L6" s="141"/>
-      <c r="M6" s="141"/>
-      <c r="N6" s="141"/>
-      <c r="O6" s="111"/>
+      <c r="C6" s="126"/>
+      <c r="D6" s="126"/>
+      <c r="E6" s="126"/>
+      <c r="F6" s="126"/>
+      <c r="G6" s="126"/>
+      <c r="H6" s="129"/>
+      <c r="I6" s="130"/>
+      <c r="J6" s="131"/>
+      <c r="K6" s="131"/>
+      <c r="L6" s="126"/>
+      <c r="M6" s="126"/>
+      <c r="N6" s="126"/>
+      <c r="O6" s="133"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="9"/>
@@ -3233,7 +3263,7 @@
       <c r="N7" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="112"/>
+      <c r="O7" s="134"/>
       <c r="P7" s="64" t="s">
         <v>62</v>
       </c>
@@ -3248,35 +3278,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" thickBot="1">
       <c r="A8" s="59"/>
-      <c r="B8" s="113" t="s">
+      <c r="B8" s="135" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="114"/>
-      <c r="D8" s="114"/>
-      <c r="E8" s="115"/>
-      <c r="F8" s="116" t="s">
+      <c r="C8" s="136"/>
+      <c r="D8" s="136"/>
+      <c r="E8" s="137"/>
+      <c r="F8" s="138" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="117"/>
-      <c r="H8" s="117"/>
-      <c r="I8" s="118"/>
-      <c r="J8" s="119"/>
-      <c r="K8" s="119"/>
-      <c r="L8" s="120"/>
-      <c r="M8" s="121" t="s">
+      <c r="G8" s="139"/>
+      <c r="H8" s="139"/>
+      <c r="I8" s="140"/>
+      <c r="J8" s="141"/>
+      <c r="K8" s="141"/>
+      <c r="L8" s="142"/>
+      <c r="M8" s="143" t="s">
         <v>40</v>
       </c>
-      <c r="N8" s="122"/>
+      <c r="N8" s="144"/>
       <c r="O8" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="P8" s="123" t="s">
+      <c r="P8" s="145" t="s">
         <v>42</v>
       </c>
-      <c r="Q8" s="124"/>
-      <c r="R8" s="125"/>
-      <c r="S8" s="125"/>
-      <c r="T8" s="126"/>
+      <c r="Q8" s="146"/>
+      <c r="R8" s="147"/>
+      <c r="S8" s="147"/>
+      <c r="T8" s="148"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1">
       <c r="A9" s="60" t="s">
@@ -4453,7 +4483,7 @@
       <c r="T38" s="37"/>
     </row>
     <row r="39" spans="1:20" ht="18.75" customHeight="1">
-      <c r="A39" s="147" t="s">
+      <c r="A39" s="110" t="s">
         <v>99</v>
       </c>
       <c r="B39" s="103" t="s">
@@ -4499,7 +4529,7 @@
       <c r="T39" s="37"/>
     </row>
     <row r="40" spans="1:20" ht="18.75" customHeight="1">
-      <c r="A40" s="148" t="s">
+      <c r="A40" s="111" t="s">
         <v>105</v>
       </c>
       <c r="B40" s="105" t="s">
@@ -4591,7 +4621,7 @@
       <c r="T41" s="37"/>
     </row>
     <row r="42" spans="1:20" ht="18.75" customHeight="1">
-      <c r="A42" s="147" t="s">
+      <c r="A42" s="110" t="s">
         <v>107</v>
       </c>
       <c r="B42" s="105" t="s">
@@ -4637,7 +4667,7 @@
       <c r="T42" s="37"/>
     </row>
     <row r="43" spans="1:20" ht="18" customHeight="1">
-      <c r="A43" s="148" t="s">
+      <c r="A43" s="111" t="s">
         <v>108</v>
       </c>
       <c r="B43" s="105" t="s">
@@ -4683,7 +4713,7 @@
       <c r="T43" s="37"/>
     </row>
     <row r="44" spans="1:20" ht="18" customHeight="1">
-      <c r="A44" s="148" t="s">
+      <c r="A44" s="111" t="s">
         <v>109</v>
       </c>
       <c r="B44" s="105" t="s">
@@ -5066,154 +5096,353 @@
     </row>
     <row r="53" spans="1:20" ht="18" customHeight="1">
       <c r="A53" s="30"/>
-      <c r="B53" s="31"/>
-      <c r="C53" s="30"/>
-      <c r="D53" s="30"/>
-      <c r="E53" s="30"/>
-      <c r="F53" s="32"/>
-      <c r="G53" s="32"/>
+      <c r="B53" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="C53" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="D53" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="E53" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="F53" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="G53" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H53" s="33"/>
       <c r="I53" s="34"/>
-      <c r="J53" s="89"/>
+      <c r="J53" s="89">
+        <f>273+62</f>
+        <v>335</v>
+      </c>
       <c r="K53" s="48"/>
-      <c r="L53" s="32"/>
+      <c r="L53" s="32" t="s">
+        <v>123</v>
+      </c>
       <c r="M53" s="40"/>
-      <c r="N53" s="36"/>
+      <c r="N53" s="36" t="s">
+        <v>128</v>
+      </c>
       <c r="O53" s="45"/>
-      <c r="P53" s="46"/>
-      <c r="Q53" s="39"/>
+      <c r="P53" s="45"/>
+      <c r="Q53" s="45"/>
       <c r="R53" s="45"/>
       <c r="S53" s="37"/>
       <c r="T53" s="37"/>
     </row>
     <row r="54" spans="1:20" ht="18" customHeight="1">
       <c r="A54" s="30"/>
-      <c r="B54" s="31"/>
-      <c r="C54" s="30"/>
-      <c r="D54" s="30"/>
-      <c r="E54" s="30"/>
-      <c r="F54" s="32"/>
-      <c r="G54" s="32"/>
+      <c r="B54" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="C54" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="D54" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="E54" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="F54" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="G54" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H54" s="33"/>
-      <c r="I54" s="34"/>
-      <c r="J54" s="89"/>
-      <c r="K54" s="48"/>
-      <c r="L54" s="32"/>
-      <c r="M54" s="40"/>
-      <c r="N54" s="36"/>
+      <c r="I54" s="34">
+        <v>373</v>
+      </c>
+      <c r="J54" s="89">
+        <f>P54</f>
+        <v>30.848068669527802</v>
+      </c>
+      <c r="K54" s="48">
+        <f>Q54-P54</f>
+        <v>1.1896995708154954</v>
+      </c>
+      <c r="L54" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="M54" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="N54" s="36" t="s">
+        <v>128</v>
+      </c>
       <c r="O54" s="45"/>
-      <c r="P54" s="46"/>
-      <c r="Q54" s="39"/>
+      <c r="P54" s="45">
+        <v>30.848068669527802</v>
+      </c>
+      <c r="Q54" s="45">
+        <v>32.037768240343297</v>
+      </c>
       <c r="R54" s="45"/>
       <c r="S54" s="37"/>
       <c r="T54" s="37"/>
     </row>
     <row r="55" spans="1:20" ht="18" customHeight="1">
       <c r="A55" s="30"/>
-      <c r="B55" s="31"/>
-      <c r="C55" s="30"/>
-      <c r="D55" s="30"/>
-      <c r="E55" s="30"/>
-      <c r="F55" s="32"/>
-      <c r="G55" s="32"/>
+      <c r="B55" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="C55" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="D55" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="E55" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="F55" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="G55" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H55" s="33"/>
-      <c r="I55" s="34"/>
-      <c r="J55" s="89"/>
-      <c r="K55" s="48"/>
-      <c r="L55" s="32"/>
-      <c r="M55" s="40"/>
-      <c r="N55" s="36"/>
+      <c r="I55" s="34">
+        <v>423</v>
+      </c>
+      <c r="J55" s="89">
+        <f t="shared" ref="J55:J58" si="0">P55</f>
+        <v>28.515021459227398</v>
+      </c>
+      <c r="K55" s="48">
+        <f t="shared" ref="K55:K59" si="1">Q55-P55</f>
+        <v>1.6686695278970021</v>
+      </c>
+      <c r="L55" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="M55" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="N55" s="36" t="s">
+        <v>128</v>
+      </c>
       <c r="O55" s="45"/>
-      <c r="P55" s="46"/>
-      <c r="Q55" s="39"/>
+      <c r="P55" s="45">
+        <v>28.515021459227398</v>
+      </c>
+      <c r="Q55" s="45">
+        <v>30.1836909871244</v>
+      </c>
       <c r="R55" s="45"/>
       <c r="S55" s="37"/>
       <c r="T55" s="37"/>
     </row>
     <row r="56" spans="1:20" ht="18" customHeight="1">
       <c r="A56" s="30"/>
-      <c r="B56" s="31"/>
-      <c r="C56" s="30"/>
-      <c r="D56" s="30"/>
-      <c r="E56" s="30"/>
-      <c r="F56" s="32"/>
-      <c r="G56" s="32"/>
+      <c r="B56" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="C56" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="D56" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="E56" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="F56" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="G56" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H56" s="33"/>
-      <c r="I56" s="34"/>
-      <c r="J56" s="89"/>
-      <c r="K56" s="48"/>
-      <c r="L56" s="32"/>
-      <c r="M56" s="40"/>
-      <c r="N56" s="36"/>
+      <c r="I56" s="34">
+        <v>473</v>
+      </c>
+      <c r="J56" s="89">
+        <f t="shared" si="0"/>
+        <v>26.614592274678099</v>
+      </c>
+      <c r="K56" s="48">
+        <f t="shared" si="1"/>
+        <v>1.3287553648068027</v>
+      </c>
+      <c r="L56" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="M56" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="N56" s="36" t="s">
+        <v>128</v>
+      </c>
       <c r="O56" s="45"/>
-      <c r="P56" s="45"/>
-      <c r="Q56" s="45"/>
+      <c r="P56" s="45">
+        <v>26.614592274678099</v>
+      </c>
+      <c r="Q56" s="45">
+        <v>27.943347639484902</v>
+      </c>
       <c r="R56" s="45"/>
       <c r="S56" s="37"/>
       <c r="T56" s="37"/>
     </row>
     <row r="57" spans="1:20" ht="18" customHeight="1">
       <c r="A57" s="30"/>
-      <c r="B57" s="31"/>
-      <c r="C57" s="30"/>
-      <c r="D57" s="30"/>
-      <c r="E57" s="30"/>
-      <c r="F57" s="32"/>
-      <c r="G57" s="32"/>
+      <c r="B57" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="C57" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="D57" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="E57" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="F57" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="G57" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H57" s="33"/>
-      <c r="I57" s="34"/>
-      <c r="J57" s="89"/>
-      <c r="K57" s="48"/>
-      <c r="L57" s="32"/>
-      <c r="M57" s="40"/>
-      <c r="N57" s="36"/>
+      <c r="I57" s="34">
+        <v>523</v>
+      </c>
+      <c r="J57" s="89">
+        <f t="shared" si="0"/>
+        <v>24.837768240343301</v>
+      </c>
+      <c r="K57" s="48">
+        <f t="shared" si="1"/>
+        <v>1.1896995708154989</v>
+      </c>
+      <c r="L57" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="M57" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="N57" s="36" t="s">
+        <v>128</v>
+      </c>
       <c r="O57" s="45"/>
-      <c r="P57" s="45"/>
-      <c r="Q57" s="45"/>
+      <c r="P57" s="45">
+        <v>24.837768240343301</v>
+      </c>
+      <c r="Q57" s="45">
+        <v>26.0274678111588</v>
+      </c>
       <c r="R57" s="45"/>
       <c r="S57" s="37"/>
       <c r="T57" s="37"/>
     </row>
     <row r="58" spans="1:20" ht="18" customHeight="1">
       <c r="A58" s="30"/>
-      <c r="B58" s="31"/>
-      <c r="C58" s="30"/>
-      <c r="D58" s="30"/>
-      <c r="E58" s="30"/>
-      <c r="F58" s="32"/>
-      <c r="G58" s="32"/>
+      <c r="B58" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="C58" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="D58" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="E58" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="F58" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="G58" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H58" s="33"/>
-      <c r="I58" s="34"/>
-      <c r="J58" s="89"/>
-      <c r="K58" s="48"/>
-      <c r="L58" s="32"/>
-      <c r="M58" s="40"/>
-      <c r="N58" s="36"/>
+      <c r="I58" s="34">
+        <v>573</v>
+      </c>
+      <c r="J58" s="89">
+        <f t="shared" si="0"/>
+        <v>20.619742489270301</v>
+      </c>
+      <c r="K58" s="48">
+        <f t="shared" si="1"/>
+        <v>0.86523605150219751</v>
+      </c>
+      <c r="L58" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="M58" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="N58" s="36" t="s">
+        <v>128</v>
+      </c>
       <c r="O58" s="45"/>
-      <c r="P58" s="45"/>
-      <c r="Q58" s="45"/>
+      <c r="P58" s="45">
+        <v>20.619742489270301</v>
+      </c>
+      <c r="Q58" s="45">
+        <v>21.484978540772499</v>
+      </c>
       <c r="R58" s="45"/>
       <c r="S58" s="37"/>
       <c r="T58" s="37"/>
     </row>
     <row r="59" spans="1:20" ht="18" customHeight="1">
       <c r="A59" s="30"/>
-      <c r="B59" s="31"/>
-      <c r="C59" s="30"/>
-      <c r="D59" s="30"/>
-      <c r="E59" s="30"/>
-      <c r="F59" s="32"/>
-      <c r="G59" s="32"/>
+      <c r="B59" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="C59" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="D59" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="E59" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="F59" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="G59" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H59" s="33"/>
-      <c r="I59" s="34"/>
-      <c r="J59" s="89"/>
-      <c r="K59" s="48"/>
-      <c r="L59" s="32"/>
-      <c r="M59" s="40"/>
-      <c r="N59" s="36"/>
+      <c r="I59" s="34">
+        <v>623</v>
+      </c>
+      <c r="J59" s="89">
+        <f>P59</f>
+        <v>15.6137339055793</v>
+      </c>
+      <c r="K59" s="48">
+        <f t="shared" si="1"/>
+        <v>0.77253218884129815</v>
+      </c>
+      <c r="L59" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="M59" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="N59" s="36" t="s">
+        <v>128</v>
+      </c>
       <c r="O59" s="45"/>
-      <c r="P59" s="45"/>
-      <c r="Q59" s="45"/>
+      <c r="P59" s="45">
+        <v>15.6137339055793</v>
+      </c>
+      <c r="Q59" s="45">
+        <v>16.386266094420598</v>
+      </c>
       <c r="R59" s="45"/>
       <c r="S59" s="37"/>
       <c r="T59" s="37"/>
@@ -24899,6 +25128,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -24913,11 +25147,6 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
- parsed data from `10.1016/j.matlet.2022.132901`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Aug2025.xlsx
+++ b/MiscSmallUploads_Aug2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC1945B-A6D4-2F49-B272-7D0409B990DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD17245-C9FA-6949-85EE-BA9A452F1B3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4100" yWindow="4780" windowWidth="24880" windowHeight="13520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1740" yWindow="8760" windowWidth="24880" windowHeight="13520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="139">
   <si>
     <r>
       <rPr>
@@ -520,6 +520,33 @@
   </si>
   <si>
     <t>F3</t>
+  </si>
+  <si>
+    <t>SnPbInBiSb</t>
+  </si>
+  <si>
+    <t>AIM</t>
+  </si>
+  <si>
+    <t>BCT+B3+eta</t>
+  </si>
+  <si>
+    <t>molten at 953K for 20min with mechanical agitator inside resistance furnace under argon flow similar to induction melting process; BCT or A5 is beta-Sn and B3 is InSb ordered FCC intermetallic and eta is SnPbBi mixture occupying Pb7Bi3 complex superconducting eta phase</t>
+  </si>
+  <si>
+    <t>solidus temperature</t>
+  </si>
+  <si>
+    <t>liquidus temperature</t>
+  </si>
+  <si>
+    <t>F1a</t>
+  </si>
+  <si>
+    <t>F1c</t>
+  </si>
+  <si>
+    <t>10.1016/j.matlet.2022.132901</t>
   </si>
 </sst>
 </file>
@@ -3012,8 +3039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T960"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M64" sqref="M64"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D47" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N68" sqref="N68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -5449,19 +5476,40 @@
     </row>
     <row r="60" spans="1:20" ht="18" customHeight="1">
       <c r="A60" s="30"/>
-      <c r="B60" s="31"/>
-      <c r="C60" s="30"/>
-      <c r="D60" s="30"/>
-      <c r="E60" s="30"/>
-      <c r="F60" s="32"/>
-      <c r="G60" s="32"/>
+      <c r="B60" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="C60" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="D60" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="E60" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="F60" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="G60" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H60" s="33"/>
       <c r="I60" s="34"/>
-      <c r="J60" s="89"/>
+      <c r="J60" s="89">
+        <f>273+80.1</f>
+        <v>353.1</v>
+      </c>
       <c r="K60" s="48"/>
-      <c r="L60" s="32"/>
-      <c r="M60" s="40"/>
-      <c r="N60" s="36"/>
+      <c r="L60" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="M60" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="N60" s="36" t="s">
+        <v>138</v>
+      </c>
       <c r="O60" s="45"/>
       <c r="P60" s="45"/>
       <c r="Q60" s="45"/>
@@ -5471,19 +5519,40 @@
     </row>
     <row r="61" spans="1:20" ht="18" customHeight="1">
       <c r="A61" s="30"/>
-      <c r="B61" s="31"/>
-      <c r="C61" s="30"/>
-      <c r="D61" s="30"/>
-      <c r="E61" s="30"/>
-      <c r="F61" s="32"/>
-      <c r="G61" s="32"/>
+      <c r="B61" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="C61" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="D61" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="E61" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="F61" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="G61" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H61" s="33"/>
       <c r="I61" s="34"/>
-      <c r="J61" s="89"/>
+      <c r="J61" s="89">
+        <f>273+112.8</f>
+        <v>385.8</v>
+      </c>
       <c r="K61" s="48"/>
-      <c r="L61" s="32"/>
-      <c r="M61" s="40"/>
-      <c r="N61" s="36"/>
+      <c r="L61" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="M61" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="N61" s="36" t="s">
+        <v>138</v>
+      </c>
       <c r="O61" s="45"/>
       <c r="P61" s="45"/>
       <c r="Q61" s="45"/>
@@ -5493,19 +5562,42 @@
     </row>
     <row r="62" spans="1:20" ht="18" customHeight="1">
       <c r="A62" s="30"/>
-      <c r="B62" s="31"/>
-      <c r="C62" s="30"/>
-      <c r="D62" s="30"/>
-      <c r="E62" s="30"/>
-      <c r="F62" s="32"/>
-      <c r="G62" s="32"/>
+      <c r="B62" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="C62" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="D62" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="E62" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="F62" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="G62" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H62" s="33"/>
-      <c r="I62" s="34"/>
-      <c r="J62" s="89"/>
+      <c r="I62" s="34">
+        <f>273+180</f>
+        <v>453</v>
+      </c>
+      <c r="J62" s="89">
+        <v>39.799999999999997</v>
+      </c>
       <c r="K62" s="48"/>
-      <c r="L62" s="32"/>
-      <c r="M62" s="40"/>
-      <c r="N62" s="36"/>
+      <c r="L62" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="M62" s="40" t="s">
+        <v>137</v>
+      </c>
+      <c r="N62" s="36" t="s">
+        <v>138</v>
+      </c>
       <c r="O62" s="45"/>
       <c r="P62" s="45"/>
       <c r="Q62" s="45"/>

</xml_diff>

<commit_message>
- parsed data from `10.1007/s11661-015-3091-1`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Aug2025.xlsx
+++ b/MiscSmallUploads_Aug2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD17245-C9FA-6949-85EE-BA9A452F1B3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70343ED4-7B49-6243-9CE8-6A31529FD03D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="8760" windowWidth="24880" windowHeight="13520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1740" yWindow="7260" windowWidth="24880" windowHeight="13520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="151">
   <si>
     <r>
       <rPr>
@@ -547,6 +547,42 @@
   </si>
   <si>
     <t>10.1016/j.matlet.2022.132901</t>
+  </si>
+  <si>
+    <t>DyGdLuTbY</t>
+  </si>
+  <si>
+    <t>CoOsReRu</t>
+  </si>
+  <si>
+    <t>MoPdRhRu</t>
+  </si>
+  <si>
+    <t>HCP</t>
+  </si>
+  <si>
+    <t>AIMD simulations</t>
+  </si>
+  <si>
+    <t>DFT</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>CoFeReRu</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>CoReRuV</t>
+  </si>
+  <si>
+    <t>HCP+?+?</t>
+  </si>
+  <si>
+    <t>10.1007/s11661-015-3091-1</t>
   </si>
 </sst>
 </file>
@@ -1766,6 +1802,57 @@
     <xf numFmtId="0" fontId="15" fillId="10" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1825,57 +1912,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3039,8 +3075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T960"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D47" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N68" sqref="N68"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A47" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N70" sqref="N70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -3097,19 +3133,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" s="112" t="s">
+      <c r="D2" s="129" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="113"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="117"/>
-      <c r="H2" s="117"/>
-      <c r="I2" s="118"/>
-      <c r="J2" s="119"/>
-      <c r="K2" s="119"/>
-      <c r="L2" s="117"/>
-      <c r="M2" s="117"/>
-      <c r="N2" s="120"/>
+      <c r="E2" s="130"/>
+      <c r="F2" s="133"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="135"/>
+      <c r="J2" s="136"/>
+      <c r="K2" s="136"/>
+      <c r="L2" s="134"/>
+      <c r="M2" s="134"/>
+      <c r="N2" s="137"/>
       <c r="O2" s="13"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -3125,17 +3161,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="114"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="121"/>
-      <c r="G3" s="121"/>
-      <c r="H3" s="121"/>
-      <c r="I3" s="122"/>
-      <c r="J3" s="123"/>
-      <c r="K3" s="123"/>
-      <c r="L3" s="121"/>
-      <c r="M3" s="121"/>
-      <c r="N3" s="124"/>
+      <c r="D3" s="131"/>
+      <c r="E3" s="132"/>
+      <c r="F3" s="138"/>
+      <c r="G3" s="138"/>
+      <c r="H3" s="138"/>
+      <c r="I3" s="139"/>
+      <c r="J3" s="140"/>
+      <c r="K3" s="140"/>
+      <c r="L3" s="138"/>
+      <c r="M3" s="138"/>
+      <c r="N3" s="141"/>
       <c r="O3" s="13"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -3176,43 +3212,43 @@
       <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="125" t="s">
+      <c r="C5" s="142" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="127" t="s">
+      <c r="D5" s="144" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="127" t="s">
+      <c r="E5" s="144" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="127" t="s">
+      <c r="F5" s="144" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="127" t="s">
+      <c r="G5" s="144" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="128" t="s">
+      <c r="H5" s="145" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="127" t="s">
+      <c r="I5" s="144" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="127" t="s">
+      <c r="J5" s="144" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="127" t="s">
+      <c r="K5" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="127" t="s">
+      <c r="L5" s="144" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="127" t="s">
+      <c r="M5" s="144" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="127" t="s">
+      <c r="N5" s="144" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="132" t="s">
+      <c r="O5" s="112" t="s">
         <v>20</v>
       </c>
       <c r="P5" s="25"/>
@@ -3228,19 +3264,19 @@
       <c r="B6" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="126"/>
-      <c r="D6" s="126"/>
-      <c r="E6" s="126"/>
-      <c r="F6" s="126"/>
-      <c r="G6" s="126"/>
-      <c r="H6" s="129"/>
-      <c r="I6" s="130"/>
-      <c r="J6" s="131"/>
-      <c r="K6" s="131"/>
-      <c r="L6" s="126"/>
-      <c r="M6" s="126"/>
-      <c r="N6" s="126"/>
-      <c r="O6" s="133"/>
+      <c r="C6" s="143"/>
+      <c r="D6" s="143"/>
+      <c r="E6" s="143"/>
+      <c r="F6" s="143"/>
+      <c r="G6" s="143"/>
+      <c r="H6" s="146"/>
+      <c r="I6" s="147"/>
+      <c r="J6" s="148"/>
+      <c r="K6" s="148"/>
+      <c r="L6" s="143"/>
+      <c r="M6" s="143"/>
+      <c r="N6" s="143"/>
+      <c r="O6" s="113"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="9"/>
@@ -3290,7 +3326,7 @@
       <c r="N7" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="134"/>
+      <c r="O7" s="114"/>
       <c r="P7" s="64" t="s">
         <v>62</v>
       </c>
@@ -3305,35 +3341,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" thickBot="1">
       <c r="A8" s="59"/>
-      <c r="B8" s="135" t="s">
+      <c r="B8" s="115" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="136"/>
-      <c r="D8" s="136"/>
-      <c r="E8" s="137"/>
-      <c r="F8" s="138" t="s">
+      <c r="C8" s="116"/>
+      <c r="D8" s="116"/>
+      <c r="E8" s="117"/>
+      <c r="F8" s="118" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="139"/>
-      <c r="H8" s="139"/>
-      <c r="I8" s="140"/>
-      <c r="J8" s="141"/>
-      <c r="K8" s="141"/>
-      <c r="L8" s="142"/>
-      <c r="M8" s="143" t="s">
+      <c r="G8" s="119"/>
+      <c r="H8" s="119"/>
+      <c r="I8" s="120"/>
+      <c r="J8" s="121"/>
+      <c r="K8" s="121"/>
+      <c r="L8" s="122"/>
+      <c r="M8" s="123" t="s">
         <v>40</v>
       </c>
-      <c r="N8" s="144"/>
+      <c r="N8" s="124"/>
       <c r="O8" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="P8" s="145" t="s">
+      <c r="P8" s="125" t="s">
         <v>42</v>
       </c>
-      <c r="Q8" s="146"/>
-      <c r="R8" s="147"/>
-      <c r="S8" s="147"/>
-      <c r="T8" s="148"/>
+      <c r="Q8" s="126"/>
+      <c r="R8" s="127"/>
+      <c r="S8" s="127"/>
+      <c r="T8" s="128"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1">
       <c r="A9" s="60" t="s">
@@ -5607,19 +5643,37 @@
     </row>
     <row r="63" spans="1:20" ht="18" customHeight="1">
       <c r="A63" s="30"/>
-      <c r="B63" s="31"/>
-      <c r="C63" s="30"/>
+      <c r="B63" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="C63" s="30" t="s">
+        <v>142</v>
+      </c>
       <c r="D63" s="30"/>
-      <c r="E63" s="30"/>
-      <c r="F63" s="32"/>
-      <c r="G63" s="32"/>
+      <c r="E63" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="F63" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="G63" s="32" t="s">
+        <v>144</v>
+      </c>
       <c r="H63" s="33"/>
       <c r="I63" s="34"/>
-      <c r="J63" s="89"/>
+      <c r="J63" s="89">
+        <v>1724</v>
+      </c>
       <c r="K63" s="48"/>
-      <c r="L63" s="32"/>
-      <c r="M63" s="40"/>
-      <c r="N63" s="36"/>
+      <c r="L63" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="M63" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="N63" s="36" t="s">
+        <v>150</v>
+      </c>
       <c r="O63" s="45"/>
       <c r="P63" s="45"/>
       <c r="Q63" s="45"/>
@@ -5629,19 +5683,37 @@
     </row>
     <row r="64" spans="1:20" ht="18" customHeight="1">
       <c r="A64" s="30"/>
-      <c r="B64" s="31"/>
-      <c r="C64" s="30"/>
+      <c r="B64" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="C64" s="30" t="s">
+        <v>142</v>
+      </c>
       <c r="D64" s="30"/>
-      <c r="E64" s="30"/>
-      <c r="F64" s="32"/>
-      <c r="G64" s="32"/>
+      <c r="E64" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="F64" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="G64" s="32" t="s">
+        <v>144</v>
+      </c>
       <c r="H64" s="33"/>
       <c r="I64" s="34"/>
-      <c r="J64" s="89"/>
+      <c r="J64" s="89">
+        <v>2901</v>
+      </c>
       <c r="K64" s="48"/>
-      <c r="L64" s="32"/>
-      <c r="M64" s="40"/>
-      <c r="N64" s="36"/>
+      <c r="L64" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="M64" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="N64" s="36" t="s">
+        <v>150</v>
+      </c>
       <c r="O64" s="45"/>
       <c r="P64" s="45"/>
       <c r="Q64" s="45"/>
@@ -5651,19 +5723,37 @@
     </row>
     <row r="65" spans="1:20" ht="18" customHeight="1">
       <c r="A65" s="30"/>
-      <c r="B65" s="31"/>
-      <c r="C65" s="30"/>
+      <c r="B65" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="C65" s="30" t="s">
+        <v>142</v>
+      </c>
       <c r="D65" s="30"/>
-      <c r="E65" s="30"/>
-      <c r="F65" s="32"/>
-      <c r="G65" s="32"/>
+      <c r="E65" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="F65" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="G65" s="32" t="s">
+        <v>144</v>
+      </c>
       <c r="H65" s="33"/>
       <c r="I65" s="34"/>
-      <c r="J65" s="89"/>
+      <c r="J65" s="89">
+        <v>2168</v>
+      </c>
       <c r="K65" s="48"/>
-      <c r="L65" s="32"/>
-      <c r="M65" s="40"/>
-      <c r="N65" s="36"/>
+      <c r="L65" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="M65" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="N65" s="36" t="s">
+        <v>150</v>
+      </c>
       <c r="O65" s="45"/>
       <c r="P65" s="45"/>
       <c r="Q65" s="45"/>
@@ -5673,9 +5763,15 @@
     </row>
     <row r="66" spans="1:20" ht="18" customHeight="1">
       <c r="A66" s="30"/>
-      <c r="B66" s="31"/>
-      <c r="C66" s="30"/>
-      <c r="D66" s="30"/>
+      <c r="B66" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="C66" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D66" s="30" t="s">
+        <v>147</v>
+      </c>
       <c r="E66" s="30"/>
       <c r="F66" s="32"/>
       <c r="G66" s="32"/>
@@ -5685,7 +5781,9 @@
       <c r="K66" s="46"/>
       <c r="L66" s="32"/>
       <c r="M66" s="40"/>
-      <c r="N66" s="36"/>
+      <c r="N66" s="36" t="s">
+        <v>150</v>
+      </c>
       <c r="O66" s="45"/>
       <c r="P66" s="45"/>
       <c r="Q66" s="45"/>
@@ -5695,9 +5793,15 @@
     </row>
     <row r="67" spans="1:20" ht="18" customHeight="1">
       <c r="A67" s="30"/>
-      <c r="B67" s="31"/>
-      <c r="C67" s="30"/>
-      <c r="D67" s="30"/>
+      <c r="B67" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="C67" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="D67" s="30" t="s">
+        <v>147</v>
+      </c>
       <c r="E67" s="30"/>
       <c r="F67" s="32"/>
       <c r="G67" s="32"/>
@@ -5707,7 +5811,9 @@
       <c r="K67" s="46"/>
       <c r="L67" s="32"/>
       <c r="M67" s="40"/>
-      <c r="N67" s="36"/>
+      <c r="N67" s="36" t="s">
+        <v>150</v>
+      </c>
       <c r="O67" s="45"/>
       <c r="P67" s="45"/>
       <c r="Q67" s="45"/>
@@ -25220,11 +25326,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -25239,6 +25340,11 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
- parsed data from `10.2320/matertrans.M2012370`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Aug2025.xlsx
+++ b/MiscSmallUploads_Aug2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70343ED4-7B49-6243-9CE8-6A31529FD03D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BBA8A7E-85D4-474A-BC23-A7047F4DF6A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="7260" windowWidth="24880" windowHeight="13520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4220" yWindow="8700" windowWidth="24880" windowHeight="13520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="172">
   <si>
     <r>
       <rPr>
@@ -583,6 +583,69 @@
   </si>
   <si>
     <t>10.1007/s11661-015-3091-1</t>
+  </si>
+  <si>
+    <t>Ti20Zr20Pd20Cu20Ni20</t>
+  </si>
+  <si>
+    <t>Ti20Zr20Hf20Cu20Ni20</t>
+  </si>
+  <si>
+    <t>Al0.5TiZrPdCuNi</t>
+  </si>
+  <si>
+    <t>Al0.5TiZrHfCuNi</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>melt spun 20um by 1.2mm ribbons</t>
+  </si>
+  <si>
+    <t>amorphous</t>
+  </si>
+  <si>
+    <t>FCC+HCP+laves+?</t>
+  </si>
+  <si>
+    <t>BCC</t>
+  </si>
+  <si>
+    <t>FCC+laves</t>
+  </si>
+  <si>
+    <t>Ti20Zr20Pd20Cu30Ni10</t>
+  </si>
+  <si>
+    <t>HCP+laves+laves+FCC+BCT+?</t>
+  </si>
+  <si>
+    <t>1.5mm diameter rod cast sample</t>
+  </si>
+  <si>
+    <t>TiZrHfPdCuNi</t>
+  </si>
+  <si>
+    <t>amorphous+HCP+laves</t>
+  </si>
+  <si>
+    <t>10.2320/matertrans.M2012370</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>glass transition temperature</t>
   </si>
 </sst>
 </file>
@@ -3075,8 +3138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T960"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A47" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N70" sqref="N70"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A55" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J86" sqref="J86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -5823,10 +5886,18 @@
     </row>
     <row r="68" spans="1:20" ht="18" customHeight="1">
       <c r="A68" s="30"/>
-      <c r="B68" s="31"/>
-      <c r="C68" s="30"/>
-      <c r="D68" s="30"/>
-      <c r="E68" s="30"/>
+      <c r="B68" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="C68" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="D68" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="E68" s="30" t="s">
+        <v>157</v>
+      </c>
       <c r="F68" s="32"/>
       <c r="G68" s="32"/>
       <c r="H68" s="33"/>
@@ -5834,8 +5905,12 @@
       <c r="J68" s="89"/>
       <c r="K68" s="46"/>
       <c r="L68" s="32"/>
-      <c r="M68" s="40"/>
-      <c r="N68" s="36"/>
+      <c r="M68" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="N68" s="36" t="s">
+        <v>167</v>
+      </c>
       <c r="O68" s="45"/>
       <c r="P68" s="45"/>
       <c r="Q68" s="45"/>
@@ -5845,10 +5920,18 @@
     </row>
     <row r="69" spans="1:20" ht="18" customHeight="1">
       <c r="A69" s="30"/>
-      <c r="B69" s="31"/>
-      <c r="C69" s="30"/>
-      <c r="D69" s="30"/>
-      <c r="E69" s="30"/>
+      <c r="B69" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="C69" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="D69" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="E69" s="30" t="s">
+        <v>157</v>
+      </c>
       <c r="F69" s="32"/>
       <c r="G69" s="32"/>
       <c r="H69" s="33"/>
@@ -5856,8 +5939,12 @@
       <c r="J69" s="89"/>
       <c r="K69" s="89"/>
       <c r="L69" s="32"/>
-      <c r="M69" s="40"/>
-      <c r="N69" s="36"/>
+      <c r="M69" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="N69" s="36" t="s">
+        <v>167</v>
+      </c>
       <c r="O69" s="45"/>
       <c r="P69" s="45"/>
       <c r="Q69" s="48"/>
@@ -5867,10 +5954,18 @@
     </row>
     <row r="70" spans="1:20" ht="18" customHeight="1">
       <c r="A70" s="30"/>
-      <c r="B70" s="31"/>
-      <c r="C70" s="30"/>
-      <c r="D70" s="30"/>
-      <c r="E70" s="30"/>
+      <c r="B70" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="C70" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="D70" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="E70" s="30" t="s">
+        <v>157</v>
+      </c>
       <c r="F70" s="32"/>
       <c r="G70" s="32"/>
       <c r="H70" s="33"/>
@@ -5878,8 +5973,12 @@
       <c r="J70" s="89"/>
       <c r="K70" s="89"/>
       <c r="L70" s="32"/>
-      <c r="M70" s="40"/>
-      <c r="N70" s="36"/>
+      <c r="M70" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="N70" s="36" t="s">
+        <v>167</v>
+      </c>
       <c r="O70" s="45"/>
       <c r="P70" s="45"/>
       <c r="Q70" s="48"/>
@@ -5889,10 +5988,18 @@
     </row>
     <row r="71" spans="1:20" ht="18" customHeight="1">
       <c r="A71" s="30"/>
-      <c r="B71" s="31"/>
-      <c r="C71" s="30"/>
-      <c r="D71" s="30"/>
-      <c r="E71" s="30"/>
+      <c r="B71" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="C71" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="D71" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="E71" s="30" t="s">
+        <v>157</v>
+      </c>
       <c r="F71" s="32"/>
       <c r="G71" s="32"/>
       <c r="H71" s="33"/>
@@ -5900,8 +6007,12 @@
       <c r="J71" s="89"/>
       <c r="K71" s="89"/>
       <c r="L71" s="32"/>
-      <c r="M71" s="40"/>
-      <c r="N71" s="36"/>
+      <c r="M71" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="N71" s="36" t="s">
+        <v>167</v>
+      </c>
       <c r="O71" s="45"/>
       <c r="Q71" s="48"/>
       <c r="R71" s="45"/>
@@ -5910,10 +6021,18 @@
     </row>
     <row r="72" spans="1:20" ht="18" customHeight="1">
       <c r="A72" s="30"/>
-      <c r="B72" s="31"/>
-      <c r="C72" s="30"/>
-      <c r="D72" s="30"/>
-      <c r="E72" s="30"/>
+      <c r="B72" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="C72" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="D72" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="E72" s="30" t="s">
+        <v>164</v>
+      </c>
       <c r="F72" s="32"/>
       <c r="G72" s="32"/>
       <c r="H72" s="33"/>
@@ -5921,8 +6040,12 @@
       <c r="J72" s="89"/>
       <c r="K72" s="89"/>
       <c r="L72" s="32"/>
-      <c r="M72" s="40"/>
-      <c r="N72" s="36"/>
+      <c r="M72" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="N72" s="36" t="s">
+        <v>167</v>
+      </c>
       <c r="O72" s="45"/>
       <c r="P72" s="46"/>
       <c r="Q72" s="48"/>
@@ -5932,10 +6055,18 @@
     </row>
     <row r="73" spans="1:20" ht="18" customHeight="1">
       <c r="A73" s="30"/>
-      <c r="B73" s="31"/>
-      <c r="C73" s="30"/>
-      <c r="D73" s="30"/>
-      <c r="E73" s="30"/>
+      <c r="B73" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="C73" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="D73" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="E73" s="30" t="s">
+        <v>164</v>
+      </c>
       <c r="F73" s="32"/>
       <c r="G73" s="32"/>
       <c r="H73" s="33"/>
@@ -5943,8 +6074,12 @@
       <c r="J73" s="89"/>
       <c r="K73" s="89"/>
       <c r="L73" s="32"/>
-      <c r="M73" s="40"/>
-      <c r="N73" s="36"/>
+      <c r="M73" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="N73" s="36" t="s">
+        <v>167</v>
+      </c>
       <c r="O73" s="45"/>
       <c r="P73" s="45"/>
       <c r="Q73" s="45"/>
@@ -5954,10 +6089,18 @@
     </row>
     <row r="74" spans="1:20" ht="18" customHeight="1">
       <c r="A74" s="30"/>
-      <c r="B74" s="31"/>
-      <c r="C74" s="30"/>
-      <c r="D74" s="30"/>
-      <c r="E74" s="30"/>
+      <c r="B74" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="C74" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="D74" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="E74" s="30" t="s">
+        <v>164</v>
+      </c>
       <c r="F74" s="32"/>
       <c r="G74" s="32"/>
       <c r="H74" s="33"/>
@@ -5965,8 +6108,12 @@
       <c r="J74" s="89"/>
       <c r="K74" s="89"/>
       <c r="L74" s="32"/>
-      <c r="M74" s="40"/>
-      <c r="N74" s="36"/>
+      <c r="M74" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="N74" s="36" t="s">
+        <v>167</v>
+      </c>
       <c r="O74" s="45"/>
       <c r="P74" s="45"/>
       <c r="Q74" s="45"/>
@@ -5976,10 +6123,18 @@
     </row>
     <row r="75" spans="1:20" ht="18" customHeight="1">
       <c r="A75" s="30"/>
-      <c r="B75" s="31"/>
-      <c r="C75" s="30"/>
-      <c r="D75" s="30"/>
-      <c r="E75" s="30"/>
+      <c r="B75" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="C75" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="D75" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="E75" s="30" t="s">
+        <v>164</v>
+      </c>
       <c r="F75" s="32"/>
       <c r="G75" s="32"/>
       <c r="H75" s="33"/>
@@ -5987,8 +6142,12 @@
       <c r="J75" s="89"/>
       <c r="K75" s="89"/>
       <c r="L75" s="32"/>
-      <c r="M75" s="40"/>
-      <c r="N75" s="36"/>
+      <c r="M75" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="N75" s="36" t="s">
+        <v>167</v>
+      </c>
       <c r="O75" s="45"/>
       <c r="P75" s="45"/>
       <c r="Q75" s="45"/>
@@ -5998,10 +6157,18 @@
     </row>
     <row r="76" spans="1:20" ht="18" customHeight="1">
       <c r="A76" s="30"/>
-      <c r="B76" s="31"/>
-      <c r="C76" s="30"/>
-      <c r="D76" s="30"/>
-      <c r="E76" s="30"/>
+      <c r="B76" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="C76" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="D76" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="E76" s="30" t="s">
+        <v>164</v>
+      </c>
       <c r="F76" s="32"/>
       <c r="G76" s="32"/>
       <c r="H76" s="33"/>
@@ -6009,8 +6176,12 @@
       <c r="J76" s="89"/>
       <c r="K76" s="89"/>
       <c r="L76" s="32"/>
-      <c r="M76" s="40"/>
-      <c r="N76" s="36"/>
+      <c r="M76" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="N76" s="36" t="s">
+        <v>167</v>
+      </c>
       <c r="O76" s="45"/>
       <c r="P76" s="45"/>
       <c r="Q76" s="45"/>
@@ -6020,10 +6191,18 @@
     </row>
     <row r="77" spans="1:20" ht="18" customHeight="1">
       <c r="A77" s="30"/>
-      <c r="B77" s="31"/>
-      <c r="C77" s="30"/>
-      <c r="D77" s="30"/>
-      <c r="E77" s="30"/>
+      <c r="B77" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="C77" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="D77" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="E77" s="30" t="s">
+        <v>157</v>
+      </c>
       <c r="F77" s="32"/>
       <c r="G77" s="32"/>
       <c r="H77" s="33"/>
@@ -6031,8 +6210,12 @@
       <c r="J77" s="89"/>
       <c r="K77" s="46"/>
       <c r="L77" s="32"/>
-      <c r="M77" s="40"/>
-      <c r="N77" s="36"/>
+      <c r="M77" s="40" t="s">
+        <v>169</v>
+      </c>
+      <c r="N77" s="36" t="s">
+        <v>167</v>
+      </c>
       <c r="O77" s="45"/>
       <c r="P77" s="48"/>
       <c r="Q77" s="39"/>
@@ -6042,19 +6225,39 @@
     </row>
     <row r="78" spans="1:20" ht="18" customHeight="1">
       <c r="A78" s="30"/>
-      <c r="B78" s="31"/>
-      <c r="C78" s="30"/>
-      <c r="D78" s="30"/>
-      <c r="E78" s="30"/>
-      <c r="F78" s="32"/>
-      <c r="G78" s="32"/>
+      <c r="B78" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="C78" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="D78" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="E78" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="F78" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="G78" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H78" s="33"/>
       <c r="I78" s="34"/>
-      <c r="J78" s="89"/>
+      <c r="J78" s="89">
+        <v>755</v>
+      </c>
       <c r="K78" s="46"/>
-      <c r="L78" s="32"/>
-      <c r="M78" s="40"/>
-      <c r="N78" s="36"/>
+      <c r="L78" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="M78" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="N78" s="36" t="s">
+        <v>167</v>
+      </c>
       <c r="O78" s="45"/>
       <c r="P78" s="48"/>
       <c r="Q78" s="39"/>

</xml_diff>

<commit_message>
- parsed data from `10.1016/j.matchemphys.2007.01.003`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Aug2025.xlsx
+++ b/MiscSmallUploads_Aug2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BBA8A7E-85D4-474A-BC23-A7047F4DF6A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1607ED2B-3F40-8446-86B6-F35FB63896B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4220" yWindow="8700" windowWidth="24880" windowHeight="13520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="8040" windowWidth="34560" windowHeight="12760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="182">
   <si>
     <r>
       <rPr>
@@ -646,6 +646,36 @@
   </si>
   <si>
     <t>glass transition temperature</t>
+  </si>
+  <si>
+    <t>Cu</t>
+  </si>
+  <si>
+    <t>CuNi</t>
+  </si>
+  <si>
+    <t>CuNiAl</t>
+  </si>
+  <si>
+    <t>CuNiAlCo</t>
+  </si>
+  <si>
+    <t>CuNiAlCoCr</t>
+  </si>
+  <si>
+    <t>CuNiAlCoCrFe</t>
+  </si>
+  <si>
+    <t>CuNiAlCoCrFeSi</t>
+  </si>
+  <si>
+    <t>hardness</t>
+  </si>
+  <si>
+    <t>10.1016/j.matchemphys.2007.01.003</t>
+  </si>
+  <si>
+    <t>F6a</t>
   </si>
 </sst>
 </file>
@@ -3138,8 +3168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T960"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A55" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J86" sqref="J86"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A67" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N90" sqref="N90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -6267,21 +6297,44 @@
     </row>
     <row r="79" spans="1:20" ht="18" customHeight="1">
       <c r="A79" s="30"/>
-      <c r="B79" s="31"/>
-      <c r="C79" s="30"/>
-      <c r="D79" s="30"/>
+      <c r="B79" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="C79" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D79" s="30" t="s">
+        <v>121</v>
+      </c>
       <c r="E79" s="30"/>
-      <c r="F79" s="32"/>
-      <c r="G79" s="32"/>
+      <c r="F79" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="G79" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H79" s="33"/>
-      <c r="I79" s="34"/>
-      <c r="J79" s="89"/>
+      <c r="I79" s="34">
+        <v>298</v>
+      </c>
+      <c r="J79" s="35">
+        <f t="shared" ref="J79:J85" si="2">P79*9807000</f>
+        <v>410764397.90575814</v>
+      </c>
       <c r="K79" s="48"/>
-      <c r="L79" s="32"/>
-      <c r="M79" s="40"/>
-      <c r="N79" s="36"/>
+      <c r="L79" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M79" s="40" t="s">
+        <v>181</v>
+      </c>
+      <c r="N79" s="36" t="s">
+        <v>180</v>
+      </c>
       <c r="O79" s="45"/>
-      <c r="P79" s="45"/>
+      <c r="P79" s="45">
+        <v>41.8848167539266</v>
+      </c>
       <c r="Q79" s="39"/>
       <c r="R79" s="45"/>
       <c r="S79" s="37"/>
@@ -6289,21 +6342,44 @@
     </row>
     <row r="80" spans="1:20" ht="18" customHeight="1">
       <c r="A80" s="30"/>
-      <c r="B80" s="31"/>
-      <c r="C80" s="30"/>
-      <c r="D80" s="30"/>
+      <c r="B80" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="C80" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D80" s="30" t="s">
+        <v>121</v>
+      </c>
       <c r="E80" s="30"/>
-      <c r="F80" s="32"/>
-      <c r="G80" s="32"/>
+      <c r="F80" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="G80" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H80" s="33"/>
-      <c r="I80" s="34"/>
-      <c r="J80" s="89"/>
+      <c r="I80" s="34">
+        <v>298</v>
+      </c>
+      <c r="J80" s="35">
+        <f t="shared" si="2"/>
+        <v>770183246.07329774</v>
+      </c>
       <c r="K80" s="35"/>
-      <c r="L80" s="32"/>
-      <c r="M80" s="40"/>
-      <c r="N80" s="36"/>
+      <c r="L80" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M80" s="40" t="s">
+        <v>181</v>
+      </c>
+      <c r="N80" s="36" t="s">
+        <v>180</v>
+      </c>
       <c r="O80" s="45"/>
-      <c r="P80" s="39"/>
+      <c r="P80" s="39">
+        <v>78.534031413612496</v>
+      </c>
       <c r="Q80" s="39"/>
       <c r="R80" s="45"/>
       <c r="S80" s="37"/>
@@ -6311,21 +6387,44 @@
     </row>
     <row r="81" spans="1:20" ht="18" customHeight="1">
       <c r="A81" s="30"/>
-      <c r="B81" s="31"/>
-      <c r="C81" s="30"/>
-      <c r="D81" s="30"/>
+      <c r="B81" s="31" t="s">
+        <v>174</v>
+      </c>
+      <c r="C81" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="D81" s="30" t="s">
+        <v>121</v>
+      </c>
       <c r="E81" s="30"/>
-      <c r="F81" s="32"/>
-      <c r="G81" s="32"/>
+      <c r="F81" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="G81" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H81" s="33"/>
-      <c r="I81" s="34"/>
-      <c r="J81" s="89"/>
+      <c r="I81" s="34">
+        <v>298</v>
+      </c>
+      <c r="J81" s="35">
+        <f t="shared" si="2"/>
+        <v>3737956020.9424081</v>
+      </c>
       <c r="K81" s="35"/>
-      <c r="L81" s="32"/>
-      <c r="M81" s="40"/>
-      <c r="N81" s="36"/>
+      <c r="L81" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M81" s="40" t="s">
+        <v>181</v>
+      </c>
+      <c r="N81" s="36" t="s">
+        <v>180</v>
+      </c>
       <c r="O81" s="45"/>
-      <c r="P81" s="39"/>
+      <c r="P81" s="39">
+        <v>381.15183246073298</v>
+      </c>
       <c r="Q81" s="39"/>
       <c r="R81" s="45"/>
       <c r="S81" s="37"/>
@@ -6333,21 +6432,44 @@
     </row>
     <row r="82" spans="1:20" ht="18" customHeight="1">
       <c r="A82" s="30"/>
-      <c r="B82" s="31"/>
-      <c r="C82" s="30"/>
-      <c r="D82" s="30"/>
+      <c r="B82" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="C82" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="D82" s="30" t="s">
+        <v>121</v>
+      </c>
       <c r="E82" s="30"/>
-      <c r="F82" s="32"/>
-      <c r="G82" s="32"/>
+      <c r="F82" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="G82" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H82" s="33"/>
-      <c r="I82" s="34"/>
-      <c r="J82" s="89"/>
+      <c r="I82" s="34">
+        <v>298</v>
+      </c>
+      <c r="J82" s="35">
+        <f t="shared" si="2"/>
+        <v>3429882722.5130796</v>
+      </c>
       <c r="K82" s="35"/>
-      <c r="L82" s="32"/>
-      <c r="M82" s="40"/>
-      <c r="N82" s="36"/>
+      <c r="L82" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M82" s="40" t="s">
+        <v>181</v>
+      </c>
+      <c r="N82" s="36" t="s">
+        <v>180</v>
+      </c>
       <c r="O82" s="45"/>
-      <c r="P82" s="39"/>
+      <c r="P82" s="39">
+        <v>349.73821989528699</v>
+      </c>
       <c r="Q82" s="39"/>
       <c r="R82" s="45"/>
       <c r="S82" s="37"/>
@@ -6355,21 +6477,44 @@
     </row>
     <row r="83" spans="1:20" ht="18" customHeight="1">
       <c r="A83" s="30"/>
-      <c r="B83" s="31"/>
-      <c r="C83" s="30"/>
-      <c r="D83" s="30"/>
+      <c r="B83" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="C83" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="D83" s="30" t="s">
+        <v>121</v>
+      </c>
       <c r="E83" s="30"/>
-      <c r="F83" s="32"/>
-      <c r="G83" s="32"/>
+      <c r="F83" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="G83" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H83" s="33"/>
-      <c r="I83" s="34"/>
-      <c r="J83" s="89"/>
+      <c r="I83" s="34">
+        <v>298</v>
+      </c>
+      <c r="J83" s="35">
+        <f t="shared" si="2"/>
+        <v>4107643979.0575919</v>
+      </c>
       <c r="K83" s="35"/>
-      <c r="L83" s="32"/>
-      <c r="M83" s="40"/>
-      <c r="N83" s="36"/>
+      <c r="L83" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M83" s="40" t="s">
+        <v>181</v>
+      </c>
+      <c r="N83" s="36" t="s">
+        <v>180</v>
+      </c>
       <c r="O83" s="45"/>
-      <c r="P83" s="39"/>
+      <c r="P83" s="39">
+        <v>418.84816753926702</v>
+      </c>
       <c r="Q83" s="39"/>
       <c r="R83" s="45"/>
       <c r="S83" s="37"/>
@@ -6377,21 +6522,44 @@
     </row>
     <row r="84" spans="1:20" ht="18" customHeight="1">
       <c r="A84" s="30"/>
-      <c r="B84" s="31"/>
-      <c r="C84" s="30"/>
-      <c r="D84" s="30"/>
+      <c r="B84" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="C84" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="D84" s="30" t="s">
+        <v>121</v>
+      </c>
       <c r="E84" s="30"/>
-      <c r="F84" s="32"/>
-      <c r="G84" s="32"/>
+      <c r="F84" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="G84" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H84" s="33"/>
-      <c r="I84" s="34"/>
-      <c r="J84" s="89"/>
+      <c r="I84" s="34">
+        <v>298</v>
+      </c>
+      <c r="J84" s="35">
+        <f t="shared" si="2"/>
+        <v>4087105759.1622968</v>
+      </c>
       <c r="K84" s="35"/>
-      <c r="L84" s="32"/>
-      <c r="M84" s="40"/>
-      <c r="N84" s="36"/>
+      <c r="L84" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M84" s="40" t="s">
+        <v>181</v>
+      </c>
+      <c r="N84" s="36" t="s">
+        <v>180</v>
+      </c>
       <c r="O84" s="45"/>
-      <c r="P84" s="39"/>
+      <c r="P84" s="39">
+        <v>416.75392670156998</v>
+      </c>
       <c r="Q84" s="39"/>
       <c r="R84" s="45"/>
       <c r="S84" s="37"/>
@@ -6399,21 +6567,44 @@
     </row>
     <row r="85" spans="1:20" ht="18" customHeight="1">
       <c r="A85" s="30"/>
-      <c r="B85" s="31"/>
-      <c r="C85" s="30"/>
-      <c r="D85" s="30"/>
+      <c r="B85" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="C85" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="D85" s="30" t="s">
+        <v>121</v>
+      </c>
       <c r="E85" s="30"/>
-      <c r="F85" s="32"/>
-      <c r="G85" s="32"/>
+      <c r="F85" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="G85" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H85" s="33"/>
-      <c r="I85" s="34"/>
-      <c r="J85" s="89"/>
+      <c r="I85" s="34">
+        <v>298</v>
+      </c>
+      <c r="J85" s="35">
+        <f t="shared" si="2"/>
+        <v>5565857591.6230278</v>
+      </c>
       <c r="K85" s="35"/>
-      <c r="L85" s="32"/>
-      <c r="M85" s="40"/>
-      <c r="N85" s="36"/>
+      <c r="L85" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M85" s="40" t="s">
+        <v>181</v>
+      </c>
+      <c r="N85" s="36" t="s">
+        <v>180</v>
+      </c>
       <c r="O85" s="45"/>
-      <c r="P85" s="39"/>
+      <c r="P85" s="39">
+        <v>567.53926701570595</v>
+      </c>
       <c r="Q85" s="39"/>
       <c r="R85" s="45"/>
       <c r="S85" s="37"/>

</xml_diff>

<commit_message>
- parsed data from `10.1007/s11661-004-0254-x`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Aug2025.xlsx
+++ b/MiscSmallUploads_Aug2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1607ED2B-3F40-8446-86B6-F35FB63896B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111C7040-33CB-0840-9AE2-1D2E779854AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="8040" windowWidth="34560" windowHeight="12760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="197">
   <si>
     <r>
       <rPr>
@@ -676,6 +676,51 @@
   </si>
   <si>
     <t>F6a</t>
+  </si>
+  <si>
+    <t>10.1007/s11661-004-0254-x</t>
+  </si>
+  <si>
+    <t>CuCoNiCrAl0.5Fe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CuCoNiCrAl0.5FeB0.2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CuCoNiCrAl0.5FeB0.6 </t>
+  </si>
+  <si>
+    <t>CuCoNiCrAl0.5FeB</t>
+  </si>
+  <si>
+    <t>B-0</t>
+  </si>
+  <si>
+    <t>B-0.2</t>
+  </si>
+  <si>
+    <t>B-0.6</t>
+  </si>
+  <si>
+    <t>B-1.0</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t>FCC+boride</t>
+  </si>
+  <si>
+    <t>L12+boride</t>
+  </si>
+  <si>
+    <t>compressive yield stress</t>
+  </si>
+  <si>
+    <t>1e-3 strain rate</t>
+  </si>
+  <si>
+    <t>F7</t>
   </si>
 </sst>
 </file>
@@ -3168,8 +3213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T960"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A67" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N90" sqref="N90"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A92" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O98" sqref="O98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -6318,7 +6363,7 @@
         <v>298</v>
       </c>
       <c r="J79" s="35">
-        <f t="shared" ref="J79:J85" si="2">P79*9807000</f>
+        <f t="shared" ref="J79:J89" si="2">P79*9807000</f>
         <v>410764397.90575814</v>
       </c>
       <c r="K79" s="48"/>
@@ -6611,130 +6656,278 @@
       <c r="T85" s="37"/>
     </row>
     <row r="86" spans="1:20" ht="18" customHeight="1">
-      <c r="A86" s="30"/>
-      <c r="B86" s="31"/>
-      <c r="C86" s="30"/>
-      <c r="D86" s="30"/>
+      <c r="A86" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="B86" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="C86" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D86" s="30" t="s">
+        <v>121</v>
+      </c>
       <c r="E86" s="30"/>
-      <c r="F86" s="32"/>
-      <c r="G86" s="32"/>
+      <c r="F86" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="G86" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H86" s="33"/>
-      <c r="I86" s="34"/>
-      <c r="J86" s="89"/>
+      <c r="I86" s="34">
+        <v>298</v>
+      </c>
+      <c r="J86" s="35">
+        <f t="shared" si="2"/>
+        <v>2903550471.698112</v>
+      </c>
       <c r="K86" s="48"/>
-      <c r="L86" s="32"/>
-      <c r="M86" s="40"/>
-      <c r="N86" s="36"/>
+      <c r="L86" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M86" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="N86" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O86" s="45"/>
-      <c r="P86" s="39"/>
+      <c r="P86" s="39">
+        <v>296.069182389937</v>
+      </c>
       <c r="Q86" s="39"/>
       <c r="R86" s="45"/>
       <c r="S86" s="37"/>
       <c r="T86" s="37"/>
     </row>
     <row r="87" spans="1:20" ht="18" customHeight="1">
-      <c r="A87" s="30"/>
-      <c r="B87" s="31"/>
-      <c r="C87" s="30"/>
-      <c r="D87" s="30"/>
+      <c r="A87" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="B87" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="C87" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="D87" s="30" t="s">
+        <v>121</v>
+      </c>
       <c r="E87" s="30"/>
-      <c r="F87" s="32"/>
-      <c r="G87" s="32"/>
+      <c r="F87" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="G87" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H87" s="33"/>
-      <c r="I87" s="34"/>
-      <c r="J87" s="89"/>
+      <c r="I87" s="34">
+        <v>298</v>
+      </c>
+      <c r="J87" s="35">
+        <f t="shared" si="2"/>
+        <v>4144845283.0188656</v>
+      </c>
       <c r="K87" s="48"/>
-      <c r="L87" s="32"/>
-      <c r="M87" s="40"/>
-      <c r="N87" s="36"/>
+      <c r="L87" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M87" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="N87" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O87" s="45"/>
-      <c r="P87" s="39"/>
+      <c r="P87" s="39">
+        <v>422.64150943396203</v>
+      </c>
       <c r="Q87" s="39"/>
       <c r="R87" s="45"/>
       <c r="S87" s="37"/>
       <c r="T87" s="37"/>
     </row>
     <row r="88" spans="1:20" ht="18" customHeight="1">
-      <c r="A88" s="30"/>
-      <c r="B88" s="31"/>
-      <c r="C88" s="30"/>
-      <c r="D88" s="30"/>
+      <c r="A88" s="30" t="s">
+        <v>189</v>
+      </c>
+      <c r="B88" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="C88" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="D88" s="30" t="s">
+        <v>121</v>
+      </c>
       <c r="E88" s="30"/>
-      <c r="F88" s="32"/>
-      <c r="G88" s="32"/>
+      <c r="F88" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="G88" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H88" s="33"/>
-      <c r="I88" s="34"/>
-      <c r="J88" s="89"/>
+      <c r="I88" s="34">
+        <v>298</v>
+      </c>
+      <c r="J88" s="35">
+        <f t="shared" si="2"/>
+        <v>4938965566.0377274</v>
+      </c>
       <c r="K88" s="48"/>
-      <c r="L88" s="32"/>
-      <c r="M88" s="40"/>
-      <c r="N88" s="36"/>
+      <c r="L88" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M88" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="N88" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O88" s="45"/>
-      <c r="P88" s="39"/>
+      <c r="P88" s="39">
+        <v>503.61635220125697</v>
+      </c>
       <c r="Q88" s="39"/>
       <c r="R88" s="45"/>
       <c r="S88" s="37"/>
       <c r="T88" s="37"/>
     </row>
     <row r="89" spans="1:20" ht="18" customHeight="1">
-      <c r="A89" s="30"/>
-      <c r="B89" s="31"/>
-      <c r="C89" s="30"/>
-      <c r="D89" s="30"/>
+      <c r="A89" s="30" t="s">
+        <v>190</v>
+      </c>
+      <c r="B89" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="C89" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="D89" s="30" t="s">
+        <v>121</v>
+      </c>
       <c r="E89" s="30"/>
-      <c r="F89" s="32"/>
-      <c r="G89" s="32"/>
+      <c r="F89" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="G89" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H89" s="33"/>
-      <c r="I89" s="34"/>
-      <c r="J89" s="89"/>
+      <c r="I89" s="34">
+        <v>298</v>
+      </c>
+      <c r="J89" s="35">
+        <f t="shared" si="2"/>
+        <v>7221097641.5094328</v>
+      </c>
       <c r="K89" s="48"/>
-      <c r="L89" s="32"/>
-      <c r="M89" s="40"/>
-      <c r="N89" s="36"/>
+      <c r="L89" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M89" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="N89" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O89" s="45"/>
-      <c r="P89" s="39"/>
+      <c r="P89" s="39">
+        <v>736.32075471698101</v>
+      </c>
       <c r="Q89" s="39"/>
       <c r="R89" s="45"/>
       <c r="S89" s="37"/>
       <c r="T89" s="37"/>
     </row>
     <row r="90" spans="1:20" ht="18" customHeight="1">
-      <c r="A90" s="30"/>
-      <c r="B90" s="31"/>
-      <c r="C90" s="30"/>
-      <c r="D90" s="30"/>
+      <c r="A90" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="B90" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="C90" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D90" s="30" t="s">
+        <v>121</v>
+      </c>
       <c r="E90" s="30"/>
-      <c r="F90" s="32"/>
-      <c r="G90" s="32"/>
-      <c r="H90" s="33"/>
-      <c r="I90" s="34"/>
-      <c r="J90" s="89"/>
+      <c r="F90" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="G90" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H90" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I90" s="34">
+        <v>300</v>
+      </c>
+      <c r="J90" s="45">
+        <v>422421524.66367698</v>
+      </c>
       <c r="K90" s="48"/>
-      <c r="L90" s="32"/>
-      <c r="M90" s="40"/>
-      <c r="N90" s="36"/>
+      <c r="L90" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M90" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="N90" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O90" s="45"/>
-      <c r="P90" s="39"/>
+      <c r="P90" s="46"/>
       <c r="Q90" s="39"/>
       <c r="R90" s="45"/>
       <c r="S90" s="37"/>
       <c r="T90" s="37"/>
     </row>
     <row r="91" spans="1:20" ht="18" customHeight="1">
-      <c r="A91" s="30"/>
-      <c r="B91" s="31"/>
-      <c r="C91" s="30"/>
-      <c r="D91" s="30"/>
+      <c r="A91" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="B91" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="C91" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="D91" s="30" t="s">
+        <v>121</v>
+      </c>
       <c r="E91" s="30"/>
-      <c r="F91" s="32"/>
-      <c r="G91" s="32"/>
-      <c r="H91" s="33"/>
-      <c r="I91" s="34"/>
-      <c r="J91" s="89"/>
+      <c r="F91" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="G91" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H91" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I91" s="34">
+        <v>300</v>
+      </c>
+      <c r="J91" s="45">
+        <v>630493273.54260004</v>
+      </c>
       <c r="K91" s="48"/>
-      <c r="L91" s="32"/>
-      <c r="M91" s="40"/>
-      <c r="N91" s="36"/>
+      <c r="L91" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M91" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="N91" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O91" s="45"/>
       <c r="P91" s="46"/>
       <c r="Q91" s="39"/>
@@ -6743,20 +6936,44 @@
       <c r="T91" s="37"/>
     </row>
     <row r="92" spans="1:20" ht="18" customHeight="1">
-      <c r="A92" s="30"/>
-      <c r="B92" s="31"/>
-      <c r="C92" s="30"/>
-      <c r="D92" s="30"/>
+      <c r="A92" s="30" t="s">
+        <v>189</v>
+      </c>
+      <c r="B92" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="C92" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="D92" s="30" t="s">
+        <v>121</v>
+      </c>
       <c r="E92" s="30"/>
-      <c r="F92" s="32"/>
-      <c r="G92" s="32"/>
-      <c r="H92" s="33"/>
-      <c r="I92" s="34"/>
-      <c r="J92" s="89"/>
+      <c r="F92" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="G92" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H92" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I92" s="34">
+        <v>300</v>
+      </c>
+      <c r="J92" s="45">
+        <v>831390134.52914798</v>
+      </c>
       <c r="K92" s="48"/>
-      <c r="L92" s="32"/>
-      <c r="M92" s="40"/>
-      <c r="N92" s="36"/>
+      <c r="L92" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M92" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="N92" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O92" s="45"/>
       <c r="P92" s="46"/>
       <c r="Q92" s="39"/>
@@ -6765,20 +6982,44 @@
       <c r="T92" s="37"/>
     </row>
     <row r="93" spans="1:20" ht="18" customHeight="1">
-      <c r="A93" s="30"/>
-      <c r="B93" s="31"/>
-      <c r="C93" s="30"/>
-      <c r="D93" s="30"/>
+      <c r="A93" s="30" t="s">
+        <v>190</v>
+      </c>
+      <c r="B93" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="C93" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="D93" s="30" t="s">
+        <v>121</v>
+      </c>
       <c r="E93" s="30"/>
-      <c r="F93" s="32"/>
-      <c r="G93" s="32"/>
-      <c r="H93" s="33"/>
-      <c r="I93" s="34"/>
-      <c r="J93" s="89"/>
+      <c r="F93" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="G93" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H93" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I93" s="34">
+        <v>300</v>
+      </c>
+      <c r="J93" s="45">
+        <v>1168609865.47085</v>
+      </c>
       <c r="K93" s="48"/>
-      <c r="L93" s="32"/>
-      <c r="M93" s="40"/>
-      <c r="N93" s="36"/>
+      <c r="L93" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M93" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="N93" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O93" s="45"/>
       <c r="P93" s="46"/>
       <c r="Q93" s="39"/>
@@ -6787,20 +7028,44 @@
       <c r="T93" s="37"/>
     </row>
     <row r="94" spans="1:20" ht="18" customHeight="1">
-      <c r="A94" s="30"/>
-      <c r="B94" s="31"/>
-      <c r="C94" s="30"/>
-      <c r="D94" s="30"/>
+      <c r="A94" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="B94" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="C94" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D94" s="30" t="s">
+        <v>121</v>
+      </c>
       <c r="E94" s="30"/>
-      <c r="F94" s="32"/>
-      <c r="G94" s="32"/>
-      <c r="H94" s="33"/>
-      <c r="I94" s="34"/>
-      <c r="J94" s="89"/>
+      <c r="F94" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="G94" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H94" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I94" s="34">
+        <v>573</v>
+      </c>
+      <c r="J94" s="45">
+        <v>413452914.79820597</v>
+      </c>
       <c r="K94" s="48"/>
-      <c r="L94" s="32"/>
-      <c r="M94" s="40"/>
-      <c r="N94" s="36"/>
+      <c r="L94" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M94" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="N94" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O94" s="45"/>
       <c r="P94" s="46"/>
       <c r="Q94" s="39"/>
@@ -6809,42 +7074,90 @@
       <c r="T94" s="37"/>
     </row>
     <row r="95" spans="1:20" ht="18" customHeight="1">
-      <c r="A95" s="30"/>
-      <c r="B95" s="31"/>
-      <c r="C95" s="30"/>
-      <c r="D95" s="30"/>
+      <c r="A95" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="B95" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="C95" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="D95" s="30" t="s">
+        <v>121</v>
+      </c>
       <c r="E95" s="30"/>
-      <c r="F95" s="32"/>
-      <c r="G95" s="32"/>
-      <c r="H95" s="33"/>
-      <c r="I95" s="34"/>
-      <c r="J95" s="89"/>
+      <c r="F95" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="G95" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H95" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I95" s="34">
+        <v>573</v>
+      </c>
+      <c r="J95" s="45">
+        <v>664573991.03138995</v>
+      </c>
       <c r="K95" s="48"/>
-      <c r="L95" s="32"/>
-      <c r="M95" s="40"/>
-      <c r="N95" s="36"/>
+      <c r="L95" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M95" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="N95" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O95" s="45"/>
-      <c r="P95" s="46"/>
+      <c r="P95" s="45"/>
       <c r="Q95" s="39"/>
       <c r="R95" s="45"/>
       <c r="S95" s="37"/>
       <c r="T95" s="37"/>
     </row>
     <row r="96" spans="1:20" ht="18" customHeight="1">
-      <c r="A96" s="30"/>
-      <c r="B96" s="31"/>
-      <c r="C96" s="30"/>
-      <c r="D96" s="30"/>
+      <c r="A96" s="30" t="s">
+        <v>189</v>
+      </c>
+      <c r="B96" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="C96" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="D96" s="30" t="s">
+        <v>121</v>
+      </c>
       <c r="E96" s="30"/>
-      <c r="F96" s="32"/>
-      <c r="G96" s="32"/>
-      <c r="H96" s="33"/>
-      <c r="I96" s="34"/>
-      <c r="J96" s="89"/>
+      <c r="F96" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="G96" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H96" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I96" s="34">
+        <v>573</v>
+      </c>
+      <c r="J96" s="45">
+        <v>1168609865.47085</v>
+      </c>
       <c r="K96" s="48"/>
-      <c r="L96" s="32"/>
-      <c r="M96" s="40"/>
-      <c r="N96" s="36"/>
+      <c r="L96" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M96" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="N96" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O96" s="45"/>
       <c r="P96" s="45"/>
       <c r="Q96" s="45"/>
@@ -6853,20 +7166,44 @@
       <c r="T96" s="37"/>
     </row>
     <row r="97" spans="1:20" ht="18" customHeight="1">
-      <c r="A97" s="30"/>
-      <c r="B97" s="31"/>
-      <c r="C97" s="30"/>
-      <c r="D97" s="30"/>
+      <c r="A97" s="30" t="s">
+        <v>190</v>
+      </c>
+      <c r="B97" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="C97" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="D97" s="30" t="s">
+        <v>121</v>
+      </c>
       <c r="E97" s="30"/>
-      <c r="F97" s="32"/>
-      <c r="G97" s="32"/>
-      <c r="H97" s="33"/>
-      <c r="I97" s="34"/>
-      <c r="J97" s="89"/>
+      <c r="F97" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="G97" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H97" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I97" s="34">
+        <v>573</v>
+      </c>
+      <c r="J97" s="45">
+        <v>1376681614.3497701</v>
+      </c>
       <c r="K97" s="48"/>
-      <c r="L97" s="32"/>
-      <c r="M97" s="40"/>
-      <c r="N97" s="36"/>
+      <c r="L97" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M97" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="N97" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O97" s="45"/>
       <c r="P97" s="45"/>
       <c r="Q97" s="45"/>
@@ -6875,20 +7212,44 @@
       <c r="T97" s="37"/>
     </row>
     <row r="98" spans="1:20" ht="18" customHeight="1">
-      <c r="A98" s="30"/>
-      <c r="B98" s="31"/>
-      <c r="C98" s="30"/>
-      <c r="D98" s="30"/>
-      <c r="E98" s="30"/>
-      <c r="F98" s="32"/>
-      <c r="G98" s="32"/>
-      <c r="H98" s="33"/>
-      <c r="I98" s="34"/>
-      <c r="J98" s="89"/>
+      <c r="A98" s="110" t="s">
+        <v>187</v>
+      </c>
+      <c r="B98" s="103" t="s">
+        <v>183</v>
+      </c>
+      <c r="C98" s="90" t="s">
+        <v>63</v>
+      </c>
+      <c r="D98" s="90" t="s">
+        <v>121</v>
+      </c>
+      <c r="E98" s="90"/>
+      <c r="F98" s="97" t="s">
+        <v>194</v>
+      </c>
+      <c r="G98" s="97" t="s">
+        <v>29</v>
+      </c>
+      <c r="H98" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I98" s="34">
+        <v>773</v>
+      </c>
+      <c r="J98" s="45">
+        <v>424215246.63677102</v>
+      </c>
       <c r="K98" s="48"/>
-      <c r="L98" s="32"/>
-      <c r="M98" s="40"/>
-      <c r="N98" s="36"/>
+      <c r="L98" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M98" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="N98" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O98" s="45"/>
       <c r="P98" s="45"/>
       <c r="Q98" s="45"/>
@@ -6897,20 +7258,44 @@
       <c r="T98" s="37"/>
     </row>
     <row r="99" spans="1:20" ht="18" customHeight="1">
-      <c r="A99" s="30"/>
-      <c r="B99" s="31"/>
-      <c r="C99" s="30"/>
-      <c r="D99" s="30"/>
-      <c r="E99" s="30"/>
-      <c r="F99" s="32"/>
-      <c r="G99" s="32"/>
-      <c r="H99" s="33"/>
-      <c r="I99" s="34"/>
-      <c r="J99" s="89"/>
+      <c r="A99" s="111" t="s">
+        <v>188</v>
+      </c>
+      <c r="B99" s="105" t="s">
+        <v>184</v>
+      </c>
+      <c r="C99" s="91" t="s">
+        <v>192</v>
+      </c>
+      <c r="D99" s="91" t="s">
+        <v>121</v>
+      </c>
+      <c r="E99" s="91"/>
+      <c r="F99" s="98" t="s">
+        <v>194</v>
+      </c>
+      <c r="G99" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="H99" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I99" s="34">
+        <v>773</v>
+      </c>
+      <c r="J99" s="45">
+        <v>716591928.25112104</v>
+      </c>
       <c r="K99" s="48"/>
-      <c r="L99" s="32"/>
-      <c r="M99" s="40"/>
-      <c r="N99" s="36"/>
+      <c r="L99" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M99" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="N99" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O99" s="45"/>
       <c r="P99" s="45"/>
       <c r="Q99" s="45"/>
@@ -6919,20 +7304,44 @@
       <c r="T99" s="37"/>
     </row>
     <row r="100" spans="1:20" ht="18" customHeight="1">
-      <c r="A100" s="30"/>
-      <c r="B100" s="31"/>
-      <c r="C100" s="30"/>
-      <c r="D100" s="30"/>
-      <c r="E100" s="30"/>
-      <c r="F100" s="32"/>
-      <c r="G100" s="32"/>
-      <c r="H100" s="33"/>
-      <c r="I100" s="34"/>
-      <c r="J100" s="89"/>
+      <c r="A100" s="111" t="s">
+        <v>189</v>
+      </c>
+      <c r="B100" s="105" t="s">
+        <v>185</v>
+      </c>
+      <c r="C100" s="91" t="s">
+        <v>192</v>
+      </c>
+      <c r="D100" s="91" t="s">
+        <v>121</v>
+      </c>
+      <c r="E100" s="91"/>
+      <c r="F100" s="98" t="s">
+        <v>194</v>
+      </c>
+      <c r="G100" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="H100" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I100" s="34">
+        <v>773</v>
+      </c>
+      <c r="J100" s="45">
+        <v>1091479820.6278</v>
+      </c>
       <c r="K100" s="48"/>
-      <c r="L100" s="32"/>
-      <c r="M100" s="40"/>
-      <c r="N100" s="36"/>
+      <c r="L100" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M100" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="N100" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O100" s="45"/>
       <c r="P100" s="45"/>
       <c r="Q100" s="45"/>
@@ -6941,20 +7350,44 @@
       <c r="T100" s="37"/>
     </row>
     <row r="101" spans="1:20" ht="18" customHeight="1">
-      <c r="A101" s="30"/>
-      <c r="B101" s="31"/>
-      <c r="C101" s="30"/>
-      <c r="D101" s="30"/>
-      <c r="E101" s="30"/>
-      <c r="F101" s="32"/>
-      <c r="G101" s="32"/>
-      <c r="H101" s="33"/>
-      <c r="I101" s="34"/>
-      <c r="J101" s="89"/>
+      <c r="A101" s="111" t="s">
+        <v>190</v>
+      </c>
+      <c r="B101" s="105" t="s">
+        <v>186</v>
+      </c>
+      <c r="C101" s="91" t="s">
+        <v>193</v>
+      </c>
+      <c r="D101" s="91" t="s">
+        <v>121</v>
+      </c>
+      <c r="E101" s="91"/>
+      <c r="F101" s="98" t="s">
+        <v>194</v>
+      </c>
+      <c r="G101" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="H101" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I101" s="34">
+        <v>773</v>
+      </c>
+      <c r="J101" s="45">
+        <v>1342600896.86098</v>
+      </c>
       <c r="K101" s="48"/>
-      <c r="L101" s="32"/>
-      <c r="M101" s="40"/>
-      <c r="N101" s="36"/>
+      <c r="L101" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M101" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="N101" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O101" s="45"/>
       <c r="P101" s="45"/>
       <c r="Q101" s="45"/>
@@ -6963,42 +7396,90 @@
       <c r="T101" s="37"/>
     </row>
     <row r="102" spans="1:20" ht="18" customHeight="1">
-      <c r="A102" s="30"/>
-      <c r="B102" s="31"/>
-      <c r="C102" s="30"/>
-      <c r="D102" s="30"/>
-      <c r="E102" s="30"/>
-      <c r="F102" s="32"/>
-      <c r="G102" s="32"/>
-      <c r="H102" s="33"/>
-      <c r="I102" s="34"/>
-      <c r="J102" s="89"/>
+      <c r="A102" s="110" t="s">
+        <v>187</v>
+      </c>
+      <c r="B102" s="103" t="s">
+        <v>183</v>
+      </c>
+      <c r="C102" s="90" t="s">
+        <v>63</v>
+      </c>
+      <c r="D102" s="90" t="s">
+        <v>121</v>
+      </c>
+      <c r="E102" s="90"/>
+      <c r="F102" s="97" t="s">
+        <v>194</v>
+      </c>
+      <c r="G102" s="97" t="s">
+        <v>29</v>
+      </c>
+      <c r="H102" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I102" s="34">
+        <v>973</v>
+      </c>
+      <c r="J102" s="45">
+        <v>449327354.26008898</v>
+      </c>
       <c r="K102" s="48"/>
-      <c r="L102" s="32"/>
-      <c r="M102" s="40"/>
-      <c r="N102" s="36"/>
+      <c r="L102" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M102" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="N102" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O102" s="45"/>
-      <c r="P102" s="45"/>
+      <c r="P102" s="39"/>
       <c r="Q102" s="37"/>
       <c r="R102" s="45"/>
       <c r="S102" s="37"/>
       <c r="T102" s="37"/>
     </row>
     <row r="103" spans="1:20" ht="18" customHeight="1">
-      <c r="A103" s="50"/>
-      <c r="B103" s="31"/>
-      <c r="C103" s="30"/>
-      <c r="D103" s="30"/>
-      <c r="E103" s="30"/>
-      <c r="F103" s="32"/>
-      <c r="G103" s="32"/>
-      <c r="H103" s="33"/>
-      <c r="I103" s="34"/>
-      <c r="J103" s="89"/>
+      <c r="A103" s="111" t="s">
+        <v>188</v>
+      </c>
+      <c r="B103" s="105" t="s">
+        <v>184</v>
+      </c>
+      <c r="C103" s="91" t="s">
+        <v>192</v>
+      </c>
+      <c r="D103" s="91" t="s">
+        <v>121</v>
+      </c>
+      <c r="E103" s="91"/>
+      <c r="F103" s="98" t="s">
+        <v>194</v>
+      </c>
+      <c r="G103" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="H103" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I103" s="34">
+        <v>973</v>
+      </c>
+      <c r="J103" s="45">
+        <v>580269058.295964</v>
+      </c>
       <c r="K103" s="48"/>
-      <c r="L103" s="32"/>
-      <c r="M103" s="40"/>
-      <c r="N103" s="36"/>
+      <c r="L103" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M103" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="N103" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O103" s="45"/>
       <c r="P103" s="39"/>
       <c r="Q103" s="39"/>
@@ -7007,20 +7488,44 @@
       <c r="T103" s="37"/>
     </row>
     <row r="104" spans="1:20" ht="18" customHeight="1">
-      <c r="A104" s="50"/>
-      <c r="B104" s="31"/>
-      <c r="C104" s="30"/>
-      <c r="D104" s="30"/>
-      <c r="E104" s="30"/>
-      <c r="F104" s="32"/>
-      <c r="G104" s="32"/>
-      <c r="H104" s="33"/>
-      <c r="I104" s="34"/>
-      <c r="J104" s="89"/>
+      <c r="A104" s="111" t="s">
+        <v>189</v>
+      </c>
+      <c r="B104" s="105" t="s">
+        <v>185</v>
+      </c>
+      <c r="C104" s="91" t="s">
+        <v>192</v>
+      </c>
+      <c r="D104" s="91" t="s">
+        <v>121</v>
+      </c>
+      <c r="E104" s="91"/>
+      <c r="F104" s="98" t="s">
+        <v>194</v>
+      </c>
+      <c r="G104" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="H104" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I104" s="34">
+        <v>973</v>
+      </c>
+      <c r="J104" s="45">
+        <v>817040358.74439394</v>
+      </c>
       <c r="K104" s="48"/>
-      <c r="L104" s="32"/>
-      <c r="M104" s="40"/>
-      <c r="N104" s="36"/>
+      <c r="L104" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M104" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="N104" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O104" s="45"/>
       <c r="P104" s="39"/>
       <c r="Q104" s="39"/>
@@ -7029,20 +7534,44 @@
       <c r="T104" s="37"/>
     </row>
     <row r="105" spans="1:20" ht="18" customHeight="1">
-      <c r="A105" s="50"/>
-      <c r="B105" s="31"/>
-      <c r="C105" s="30"/>
-      <c r="D105" s="30"/>
-      <c r="E105" s="30"/>
-      <c r="F105" s="32"/>
-      <c r="G105" s="32"/>
-      <c r="H105" s="33"/>
-      <c r="I105" s="34"/>
-      <c r="J105" s="89"/>
+      <c r="A105" s="111" t="s">
+        <v>190</v>
+      </c>
+      <c r="B105" s="105" t="s">
+        <v>186</v>
+      </c>
+      <c r="C105" s="91" t="s">
+        <v>193</v>
+      </c>
+      <c r="D105" s="91" t="s">
+        <v>121</v>
+      </c>
+      <c r="E105" s="91"/>
+      <c r="F105" s="98" t="s">
+        <v>194</v>
+      </c>
+      <c r="G105" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="H105" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I105" s="34">
+        <v>973</v>
+      </c>
+      <c r="J105" s="45">
+        <v>1095067264.5739901</v>
+      </c>
       <c r="K105" s="48"/>
-      <c r="L105" s="32"/>
-      <c r="M105" s="40"/>
-      <c r="N105" s="36"/>
+      <c r="L105" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M105" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="N105" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O105" s="45"/>
       <c r="P105" s="39"/>
       <c r="Q105" s="39"/>
@@ -7051,20 +7580,44 @@
       <c r="T105" s="37"/>
     </row>
     <row r="106" spans="1:20" ht="18" customHeight="1">
-      <c r="A106" s="50"/>
-      <c r="B106" s="31"/>
-      <c r="C106" s="30"/>
-      <c r="D106" s="30"/>
-      <c r="E106" s="30"/>
-      <c r="F106" s="32"/>
-      <c r="G106" s="32"/>
-      <c r="H106" s="33"/>
-      <c r="I106" s="34"/>
-      <c r="J106" s="89"/>
+      <c r="A106" s="110" t="s">
+        <v>187</v>
+      </c>
+      <c r="B106" s="103" t="s">
+        <v>183</v>
+      </c>
+      <c r="C106" s="90" t="s">
+        <v>63</v>
+      </c>
+      <c r="D106" s="90" t="s">
+        <v>121</v>
+      </c>
+      <c r="E106" s="90"/>
+      <c r="F106" s="97" t="s">
+        <v>194</v>
+      </c>
+      <c r="G106" s="97" t="s">
+        <v>29</v>
+      </c>
+      <c r="H106" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I106" s="34">
+        <v>1173</v>
+      </c>
+      <c r="J106" s="45">
+        <v>233482805.60275301</v>
+      </c>
       <c r="K106" s="51"/>
-      <c r="L106" s="32"/>
-      <c r="M106" s="40"/>
-      <c r="N106" s="36"/>
+      <c r="L106" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M106" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="N106" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O106" s="45"/>
       <c r="P106" s="39"/>
       <c r="Q106" s="39"/>
@@ -7073,20 +7626,44 @@
       <c r="T106" s="37"/>
     </row>
     <row r="107" spans="1:20" ht="18" customHeight="1">
-      <c r="A107" s="50"/>
-      <c r="B107" s="31"/>
-      <c r="C107" s="30"/>
-      <c r="D107" s="30"/>
-      <c r="E107" s="30"/>
-      <c r="F107" s="32"/>
-      <c r="G107" s="32"/>
-      <c r="H107" s="33"/>
-      <c r="I107" s="34"/>
-      <c r="J107" s="89"/>
+      <c r="A107" s="111" t="s">
+        <v>188</v>
+      </c>
+      <c r="B107" s="105" t="s">
+        <v>184</v>
+      </c>
+      <c r="C107" s="91" t="s">
+        <v>192</v>
+      </c>
+      <c r="D107" s="91" t="s">
+        <v>121</v>
+      </c>
+      <c r="E107" s="91"/>
+      <c r="F107" s="98" t="s">
+        <v>194</v>
+      </c>
+      <c r="G107" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="H107" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I107" s="34">
+        <v>1173</v>
+      </c>
+      <c r="J107" s="45">
+        <v>267563523.09154201</v>
+      </c>
       <c r="K107" s="51"/>
-      <c r="L107" s="32"/>
-      <c r="M107" s="40"/>
-      <c r="N107" s="36"/>
+      <c r="L107" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M107" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="N107" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O107" s="45"/>
       <c r="P107" s="39"/>
       <c r="Q107" s="39"/>
@@ -7095,20 +7672,44 @@
       <c r="T107" s="37"/>
     </row>
     <row r="108" spans="1:20" ht="18" customHeight="1">
-      <c r="A108" s="50"/>
-      <c r="B108" s="31"/>
-      <c r="C108" s="30"/>
-      <c r="D108" s="30"/>
-      <c r="E108" s="30"/>
-      <c r="F108" s="32"/>
-      <c r="G108" s="32"/>
-      <c r="H108" s="33"/>
-      <c r="I108" s="34"/>
-      <c r="J108" s="89"/>
+      <c r="A108" s="111" t="s">
+        <v>189</v>
+      </c>
+      <c r="B108" s="105" t="s">
+        <v>185</v>
+      </c>
+      <c r="C108" s="91" t="s">
+        <v>192</v>
+      </c>
+      <c r="D108" s="91" t="s">
+        <v>121</v>
+      </c>
+      <c r="E108" s="91"/>
+      <c r="F108" s="98" t="s">
+        <v>194</v>
+      </c>
+      <c r="G108" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="H108" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I108" s="34">
+        <v>1173</v>
+      </c>
+      <c r="J108" s="45">
+        <v>235276527.575847</v>
+      </c>
       <c r="K108" s="48"/>
-      <c r="L108" s="32"/>
-      <c r="M108" s="40"/>
-      <c r="N108" s="36"/>
+      <c r="L108" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M108" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="N108" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O108" s="45"/>
       <c r="P108" s="39"/>
       <c r="Q108" s="39"/>
@@ -7117,20 +7718,44 @@
       <c r="T108" s="37"/>
     </row>
     <row r="109" spans="1:20" ht="18" customHeight="1">
-      <c r="A109" s="50"/>
-      <c r="B109" s="31"/>
-      <c r="C109" s="30"/>
-      <c r="D109" s="30"/>
-      <c r="E109" s="30"/>
-      <c r="F109" s="32"/>
-      <c r="G109" s="32"/>
-      <c r="H109" s="33"/>
-      <c r="I109" s="34"/>
-      <c r="J109" s="89"/>
+      <c r="A109" s="111" t="s">
+        <v>190</v>
+      </c>
+      <c r="B109" s="105" t="s">
+        <v>186</v>
+      </c>
+      <c r="C109" s="91" t="s">
+        <v>193</v>
+      </c>
+      <c r="D109" s="91" t="s">
+        <v>121</v>
+      </c>
+      <c r="E109" s="91"/>
+      <c r="F109" s="98" t="s">
+        <v>194</v>
+      </c>
+      <c r="G109" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="H109" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I109" s="34">
+        <v>1173</v>
+      </c>
+      <c r="J109" s="37">
+        <v>276532132.95701301</v>
+      </c>
       <c r="K109" s="48"/>
-      <c r="L109" s="32"/>
-      <c r="M109" s="40"/>
-      <c r="N109" s="36"/>
+      <c r="L109" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M109" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="N109" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O109" s="37"/>
       <c r="P109" s="39"/>
       <c r="Q109" s="39"/>
@@ -7139,42 +7764,90 @@
       <c r="T109" s="37"/>
     </row>
     <row r="110" spans="1:20" ht="18" customHeight="1">
-      <c r="A110" s="50"/>
-      <c r="B110" s="31"/>
-      <c r="C110" s="30"/>
-      <c r="D110" s="30"/>
-      <c r="E110" s="30"/>
-      <c r="F110" s="32"/>
-      <c r="G110" s="32"/>
-      <c r="H110" s="33"/>
-      <c r="I110" s="34"/>
-      <c r="J110" s="89"/>
+      <c r="A110" s="110" t="s">
+        <v>187</v>
+      </c>
+      <c r="B110" s="103" t="s">
+        <v>183</v>
+      </c>
+      <c r="C110" s="90" t="s">
+        <v>63</v>
+      </c>
+      <c r="D110" s="90" t="s">
+        <v>121</v>
+      </c>
+      <c r="E110" s="90"/>
+      <c r="F110" s="97" t="s">
+        <v>194</v>
+      </c>
+      <c r="G110" s="97" t="s">
+        <v>29</v>
+      </c>
+      <c r="H110" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I110" s="34">
+        <v>1373</v>
+      </c>
+      <c r="J110" s="37">
+        <v>73841549.997372299</v>
+      </c>
       <c r="K110" s="48"/>
-      <c r="L110" s="32"/>
-      <c r="M110" s="40"/>
-      <c r="N110" s="36"/>
+      <c r="L110" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M110" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="N110" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O110" s="37"/>
-      <c r="P110" s="39"/>
+      <c r="P110" s="46"/>
       <c r="Q110" s="39"/>
       <c r="R110" s="45"/>
       <c r="S110" s="37"/>
       <c r="T110" s="37"/>
     </row>
     <row r="111" spans="1:20" ht="18" customHeight="1">
-      <c r="A111" s="50"/>
-      <c r="B111" s="31"/>
-      <c r="C111" s="30"/>
-      <c r="D111" s="30"/>
-      <c r="E111" s="31"/>
-      <c r="F111" s="32"/>
-      <c r="G111" s="32"/>
-      <c r="H111" s="33"/>
-      <c r="I111" s="34"/>
-      <c r="J111" s="35"/>
+      <c r="A111" s="111" t="s">
+        <v>188</v>
+      </c>
+      <c r="B111" s="105" t="s">
+        <v>184</v>
+      </c>
+      <c r="C111" s="91" t="s">
+        <v>192</v>
+      </c>
+      <c r="D111" s="91" t="s">
+        <v>121</v>
+      </c>
+      <c r="E111" s="91"/>
+      <c r="F111" s="98" t="s">
+        <v>194</v>
+      </c>
+      <c r="G111" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="H111" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I111" s="34">
+        <v>1373</v>
+      </c>
+      <c r="J111" s="45">
+        <v>37967110.535489</v>
+      </c>
       <c r="K111" s="35"/>
-      <c r="L111" s="49"/>
-      <c r="M111" s="32"/>
-      <c r="N111" s="30"/>
+      <c r="L111" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M111" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="N111" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O111" s="45"/>
       <c r="P111" s="46"/>
       <c r="Q111" s="39"/>
@@ -7183,20 +7856,44 @@
       <c r="T111" s="37"/>
     </row>
     <row r="112" spans="1:20" ht="18" customHeight="1">
-      <c r="A112" s="50"/>
-      <c r="B112" s="31"/>
-      <c r="C112" s="30"/>
-      <c r="D112" s="30"/>
-      <c r="E112" s="31"/>
-      <c r="F112" s="32"/>
-      <c r="G112" s="32"/>
-      <c r="H112" s="33"/>
-      <c r="I112" s="34"/>
-      <c r="J112" s="35"/>
+      <c r="A112" s="111" t="s">
+        <v>189</v>
+      </c>
+      <c r="B112" s="105" t="s">
+        <v>185</v>
+      </c>
+      <c r="C112" s="91" t="s">
+        <v>192</v>
+      </c>
+      <c r="D112" s="91" t="s">
+        <v>121</v>
+      </c>
+      <c r="E112" s="91"/>
+      <c r="F112" s="98" t="s">
+        <v>194</v>
+      </c>
+      <c r="G112" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="H112" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I112" s="34">
+        <v>1373</v>
+      </c>
+      <c r="J112" s="45">
+        <v>68460384.078089893</v>
+      </c>
       <c r="K112" s="35"/>
-      <c r="L112" s="49"/>
-      <c r="M112" s="32"/>
-      <c r="N112" s="30"/>
+      <c r="L112" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M112" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="N112" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O112" s="45"/>
       <c r="P112" s="46"/>
       <c r="Q112" s="39"/>
@@ -7205,20 +7902,44 @@
       <c r="T112" s="37"/>
     </row>
     <row r="113" spans="1:20" ht="18" customHeight="1">
-      <c r="A113" s="50"/>
-      <c r="B113" s="31"/>
-      <c r="C113" s="30"/>
-      <c r="D113" s="30"/>
-      <c r="E113" s="31"/>
-      <c r="F113" s="32"/>
-      <c r="G113" s="32"/>
-      <c r="H113" s="33"/>
-      <c r="I113" s="34"/>
-      <c r="J113" s="35"/>
+      <c r="A113" s="111" t="s">
+        <v>190</v>
+      </c>
+      <c r="B113" s="105" t="s">
+        <v>186</v>
+      </c>
+      <c r="C113" s="91" t="s">
+        <v>193</v>
+      </c>
+      <c r="D113" s="91" t="s">
+        <v>121</v>
+      </c>
+      <c r="E113" s="91"/>
+      <c r="F113" s="98" t="s">
+        <v>194</v>
+      </c>
+      <c r="G113" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="H113" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I113" s="34">
+        <v>1373</v>
+      </c>
+      <c r="J113" s="45">
+        <v>27204778.6969239</v>
+      </c>
       <c r="K113" s="35"/>
-      <c r="L113" s="49"/>
-      <c r="M113" s="32"/>
-      <c r="N113" s="30"/>
+      <c r="L113" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M113" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="N113" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O113" s="45"/>
       <c r="P113" s="46"/>
       <c r="Q113" s="38"/>
@@ -7227,42 +7948,90 @@
       <c r="T113" s="37"/>
     </row>
     <row r="114" spans="1:20" ht="18" customHeight="1">
-      <c r="A114" s="50"/>
-      <c r="B114" s="31"/>
-      <c r="C114" s="30"/>
-      <c r="D114" s="30"/>
-      <c r="E114" s="31"/>
-      <c r="F114" s="32"/>
-      <c r="G114" s="32"/>
-      <c r="H114" s="33"/>
-      <c r="I114" s="34"/>
-      <c r="J114" s="35"/>
+      <c r="A114" s="111" t="s">
+        <v>188</v>
+      </c>
+      <c r="B114" s="105" t="s">
+        <v>184</v>
+      </c>
+      <c r="C114" s="91" t="s">
+        <v>192</v>
+      </c>
+      <c r="D114" s="91" t="s">
+        <v>121</v>
+      </c>
+      <c r="E114" s="91"/>
+      <c r="F114" s="98" t="s">
+        <v>194</v>
+      </c>
+      <c r="G114" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="H114" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I114" s="34">
+        <v>1073</v>
+      </c>
+      <c r="J114" s="45">
+        <v>441554554.481677</v>
+      </c>
       <c r="K114" s="35"/>
-      <c r="L114" s="49"/>
-      <c r="M114" s="32"/>
-      <c r="N114" s="30"/>
+      <c r="L114" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M114" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="N114" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O114" s="45"/>
-      <c r="P114" s="46"/>
+      <c r="P114" s="39"/>
       <c r="Q114" s="38"/>
       <c r="R114" s="45"/>
       <c r="S114" s="37"/>
       <c r="T114" s="37"/>
     </row>
     <row r="115" spans="1:20" ht="18" customHeight="1">
-      <c r="A115" s="50"/>
-      <c r="B115" s="31"/>
-      <c r="C115" s="30"/>
-      <c r="D115" s="30"/>
-      <c r="E115" s="31"/>
-      <c r="F115" s="32"/>
-      <c r="G115" s="32"/>
-      <c r="H115" s="33"/>
-      <c r="I115" s="34"/>
-      <c r="J115" s="35"/>
+      <c r="A115" s="111" t="s">
+        <v>189</v>
+      </c>
+      <c r="B115" s="105" t="s">
+        <v>185</v>
+      </c>
+      <c r="C115" s="91" t="s">
+        <v>192</v>
+      </c>
+      <c r="D115" s="91" t="s">
+        <v>121</v>
+      </c>
+      <c r="E115" s="91"/>
+      <c r="F115" s="98" t="s">
+        <v>194</v>
+      </c>
+      <c r="G115" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="H115" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I115" s="34">
+        <v>1073</v>
+      </c>
+      <c r="J115" s="45">
+        <v>504334823.53997302</v>
+      </c>
       <c r="K115" s="35"/>
-      <c r="L115" s="49"/>
-      <c r="M115" s="32"/>
-      <c r="N115" s="30"/>
+      <c r="L115" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M115" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="N115" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O115" s="45"/>
       <c r="P115" s="39"/>
       <c r="Q115" s="38"/>
@@ -7271,20 +8040,44 @@
       <c r="T115" s="37"/>
     </row>
     <row r="116" spans="1:20" ht="18" customHeight="1">
-      <c r="A116" s="50"/>
-      <c r="B116" s="31"/>
-      <c r="C116" s="30"/>
-      <c r="D116" s="30"/>
-      <c r="E116" s="31"/>
-      <c r="F116" s="32"/>
-      <c r="G116" s="32"/>
-      <c r="H116" s="33"/>
-      <c r="I116" s="34"/>
-      <c r="J116" s="35"/>
+      <c r="A116" s="111" t="s">
+        <v>190</v>
+      </c>
+      <c r="B116" s="105" t="s">
+        <v>186</v>
+      </c>
+      <c r="C116" s="91" t="s">
+        <v>193</v>
+      </c>
+      <c r="D116" s="91" t="s">
+        <v>121</v>
+      </c>
+      <c r="E116" s="91"/>
+      <c r="F116" s="98" t="s">
+        <v>194</v>
+      </c>
+      <c r="G116" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="H116" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I116" s="34">
+        <v>1073</v>
+      </c>
+      <c r="J116" s="45">
+        <v>707025406.499614</v>
+      </c>
       <c r="K116" s="35"/>
-      <c r="L116" s="49"/>
-      <c r="M116" s="32"/>
-      <c r="N116" s="30"/>
+      <c r="L116" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M116" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="N116" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O116" s="45"/>
       <c r="P116" s="39"/>
       <c r="Q116" s="38"/>
@@ -7308,7 +8101,7 @@
       <c r="M117" s="32"/>
       <c r="N117" s="30"/>
       <c r="O117" s="45"/>
-      <c r="P117" s="39"/>
+      <c r="P117" s="38"/>
       <c r="Q117" s="38"/>
       <c r="R117" s="45"/>
       <c r="S117" s="37"/>
@@ -7352,7 +8145,7 @@
       <c r="M119" s="32"/>
       <c r="N119" s="30"/>
       <c r="O119" s="45"/>
-      <c r="P119" s="38"/>
+      <c r="P119" s="39"/>
       <c r="Q119" s="38"/>
       <c r="R119" s="37"/>
       <c r="S119" s="37"/>
@@ -7638,7 +8431,7 @@
       <c r="M132" s="32"/>
       <c r="N132" s="30"/>
       <c r="O132" s="37"/>
-      <c r="P132" s="39"/>
+      <c r="P132" s="38"/>
       <c r="Q132" s="38"/>
       <c r="R132" s="45"/>
       <c r="S132" s="37"/>
@@ -8188,7 +8981,7 @@
       <c r="M157" s="49"/>
       <c r="N157" s="30"/>
       <c r="O157" s="37"/>
-      <c r="P157" s="38"/>
+      <c r="P157" s="39"/>
       <c r="Q157" s="38"/>
       <c r="R157" s="37"/>
       <c r="S157" s="37"/>
@@ -8210,7 +9003,7 @@
       <c r="M158" s="49"/>
       <c r="N158" s="30"/>
       <c r="O158" s="37"/>
-      <c r="P158" s="39"/>
+      <c r="P158" s="46"/>
       <c r="Q158" s="38"/>
       <c r="R158" s="37"/>
       <c r="S158" s="37"/>
@@ -8408,7 +9201,7 @@
       <c r="M167" s="49"/>
       <c r="N167" s="30"/>
       <c r="O167" s="37"/>
-      <c r="P167" s="46"/>
+      <c r="P167" s="38"/>
       <c r="Q167" s="38"/>
       <c r="R167" s="37"/>
       <c r="S167" s="37"/>
@@ -8694,7 +9487,7 @@
       <c r="M180" s="49"/>
       <c r="N180" s="30"/>
       <c r="O180" s="37"/>
-      <c r="P180" s="38"/>
+      <c r="P180" s="37"/>
       <c r="Q180" s="38"/>
       <c r="R180" s="37"/>
       <c r="S180" s="37"/>
@@ -9090,7 +9883,7 @@
       <c r="M198" s="40"/>
       <c r="N198" s="30"/>
       <c r="O198" s="37"/>
-      <c r="P198" s="37"/>
+      <c r="P198" s="38"/>
       <c r="Q198" s="38"/>
       <c r="R198" s="37"/>
       <c r="S198" s="37"/>
@@ -9420,7 +10213,7 @@
       <c r="M213" s="40"/>
       <c r="N213" s="30"/>
       <c r="O213" s="37"/>
-      <c r="P213" s="38"/>
+      <c r="P213" s="37"/>
       <c r="Q213" s="38"/>
       <c r="R213" s="37"/>
       <c r="S213" s="37"/>
@@ -9442,7 +10235,7 @@
       <c r="M214" s="40"/>
       <c r="N214" s="30"/>
       <c r="O214" s="37"/>
-      <c r="P214" s="37"/>
+      <c r="P214" s="44"/>
       <c r="Q214" s="38"/>
       <c r="R214" s="37"/>
       <c r="S214" s="37"/>
@@ -16460,7 +17253,6 @@
       <c r="M533" s="57"/>
       <c r="N533" s="57"/>
       <c r="O533" s="44"/>
-      <c r="P533" s="44"/>
       <c r="Q533" s="44"/>
       <c r="R533" s="44"/>
       <c r="S533" s="37"/>
@@ -16482,6 +17274,7 @@
       <c r="M534" s="57"/>
       <c r="N534" s="57"/>
       <c r="O534" s="44"/>
+      <c r="P534" s="44"/>
       <c r="Q534" s="44"/>
       <c r="R534" s="44"/>
       <c r="S534" s="37"/>
@@ -25662,7 +26455,6 @@
       <c r="M954" s="44"/>
       <c r="N954" s="44"/>
       <c r="O954" s="44"/>
-      <c r="P954" s="44"/>
       <c r="Q954" s="44"/>
       <c r="R954" s="44"/>
       <c r="S954" s="44"/>

</xml_diff>

<commit_message>
- parsed data from `10.1007/s10948-022-06253-1`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Aug2025.xlsx
+++ b/MiscSmallUploads_Aug2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111C7040-33CB-0840-9AE2-1D2E779854AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA19D588-E82F-114C-B1EA-695A19A40E2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="8040" windowWidth="34560" windowHeight="12760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="204">
   <si>
     <r>
       <rPr>
@@ -721,6 +721,27 @@
   </si>
   <si>
     <t>F7</t>
+  </si>
+  <si>
+    <t>10.1007/s10948-022-06253-1</t>
+  </si>
+  <si>
+    <t>arc melting under flowing helium</t>
+  </si>
+  <si>
+    <t>ScGdHo</t>
+  </si>
+  <si>
+    <t>neel temperature</t>
+  </si>
+  <si>
+    <t>peak magnetic entropy change</t>
+  </si>
+  <si>
+    <t>J/kgK</t>
+  </si>
+  <si>
+    <t>5T</t>
   </si>
 </sst>
 </file>
@@ -1940,57 +1961,6 @@
     <xf numFmtId="0" fontId="15" fillId="10" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2050,6 +2020,57 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3213,8 +3234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T960"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A92" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O98" sqref="O98"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A101" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J126" sqref="J126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -3271,19 +3292,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" s="129" t="s">
+      <c r="D2" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="130"/>
-      <c r="F2" s="133"/>
-      <c r="G2" s="134"/>
-      <c r="H2" s="134"/>
-      <c r="I2" s="135"/>
-      <c r="J2" s="136"/>
-      <c r="K2" s="136"/>
-      <c r="L2" s="134"/>
-      <c r="M2" s="134"/>
-      <c r="N2" s="137"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="119"/>
+      <c r="K2" s="119"/>
+      <c r="L2" s="117"/>
+      <c r="M2" s="117"/>
+      <c r="N2" s="120"/>
       <c r="O2" s="13"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -3299,17 +3320,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="131"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="138"/>
-      <c r="G3" s="138"/>
-      <c r="H3" s="138"/>
-      <c r="I3" s="139"/>
-      <c r="J3" s="140"/>
-      <c r="K3" s="140"/>
-      <c r="L3" s="138"/>
-      <c r="M3" s="138"/>
-      <c r="N3" s="141"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="121"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="121"/>
+      <c r="I3" s="122"/>
+      <c r="J3" s="123"/>
+      <c r="K3" s="123"/>
+      <c r="L3" s="121"/>
+      <c r="M3" s="121"/>
+      <c r="N3" s="124"/>
       <c r="O3" s="13"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -3350,43 +3371,43 @@
       <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="142" t="s">
+      <c r="C5" s="125" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="144" t="s">
+      <c r="D5" s="127" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="144" t="s">
+      <c r="E5" s="127" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="144" t="s">
+      <c r="F5" s="127" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="144" t="s">
+      <c r="G5" s="127" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="145" t="s">
+      <c r="H5" s="128" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="144" t="s">
+      <c r="I5" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="144" t="s">
+      <c r="J5" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="144" t="s">
+      <c r="K5" s="127" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="144" t="s">
+      <c r="L5" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="144" t="s">
+      <c r="M5" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="144" t="s">
+      <c r="N5" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="112" t="s">
+      <c r="O5" s="132" t="s">
         <v>20</v>
       </c>
       <c r="P5" s="25"/>
@@ -3402,19 +3423,19 @@
       <c r="B6" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="143"/>
-      <c r="D6" s="143"/>
-      <c r="E6" s="143"/>
-      <c r="F6" s="143"/>
-      <c r="G6" s="143"/>
-      <c r="H6" s="146"/>
-      <c r="I6" s="147"/>
-      <c r="J6" s="148"/>
-      <c r="K6" s="148"/>
-      <c r="L6" s="143"/>
-      <c r="M6" s="143"/>
-      <c r="N6" s="143"/>
-      <c r="O6" s="113"/>
+      <c r="C6" s="126"/>
+      <c r="D6" s="126"/>
+      <c r="E6" s="126"/>
+      <c r="F6" s="126"/>
+      <c r="G6" s="126"/>
+      <c r="H6" s="129"/>
+      <c r="I6" s="130"/>
+      <c r="J6" s="131"/>
+      <c r="K6" s="131"/>
+      <c r="L6" s="126"/>
+      <c r="M6" s="126"/>
+      <c r="N6" s="126"/>
+      <c r="O6" s="133"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="9"/>
@@ -3464,7 +3485,7 @@
       <c r="N7" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="114"/>
+      <c r="O7" s="134"/>
       <c r="P7" s="64" t="s">
         <v>62</v>
       </c>
@@ -3479,35 +3500,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" thickBot="1">
       <c r="A8" s="59"/>
-      <c r="B8" s="115" t="s">
+      <c r="B8" s="135" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="116"/>
-      <c r="D8" s="116"/>
-      <c r="E8" s="117"/>
-      <c r="F8" s="118" t="s">
+      <c r="C8" s="136"/>
+      <c r="D8" s="136"/>
+      <c r="E8" s="137"/>
+      <c r="F8" s="138" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="119"/>
-      <c r="H8" s="119"/>
-      <c r="I8" s="120"/>
-      <c r="J8" s="121"/>
-      <c r="K8" s="121"/>
-      <c r="L8" s="122"/>
-      <c r="M8" s="123" t="s">
+      <c r="G8" s="139"/>
+      <c r="H8" s="139"/>
+      <c r="I8" s="140"/>
+      <c r="J8" s="141"/>
+      <c r="K8" s="141"/>
+      <c r="L8" s="142"/>
+      <c r="M8" s="143" t="s">
         <v>40</v>
       </c>
-      <c r="N8" s="124"/>
+      <c r="N8" s="144"/>
       <c r="O8" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="P8" s="125" t="s">
+      <c r="P8" s="145" t="s">
         <v>42</v>
       </c>
-      <c r="Q8" s="126"/>
-      <c r="R8" s="127"/>
-      <c r="S8" s="127"/>
-      <c r="T8" s="128"/>
+      <c r="Q8" s="146"/>
+      <c r="R8" s="147"/>
+      <c r="S8" s="147"/>
+      <c r="T8" s="148"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1">
       <c r="A9" s="60" t="s">
@@ -8087,19 +8108,39 @@
     </row>
     <row r="117" spans="1:20" ht="18" customHeight="1">
       <c r="A117" s="50"/>
-      <c r="B117" s="31"/>
-      <c r="C117" s="30"/>
-      <c r="D117" s="30"/>
-      <c r="E117" s="31"/>
-      <c r="F117" s="32"/>
-      <c r="G117" s="32"/>
+      <c r="B117" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="C117" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D117" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E117" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="F117" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="G117" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H117" s="33"/>
       <c r="I117" s="34"/>
-      <c r="J117" s="35"/>
+      <c r="J117" s="35">
+        <v>109</v>
+      </c>
       <c r="K117" s="35"/>
-      <c r="L117" s="49"/>
-      <c r="M117" s="32"/>
-      <c r="N117" s="30"/>
+      <c r="L117" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="M117" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="N117" s="30" t="s">
+        <v>197</v>
+      </c>
       <c r="O117" s="45"/>
       <c r="P117" s="38"/>
       <c r="Q117" s="38"/>
@@ -8109,19 +8150,41 @@
     </row>
     <row r="118" spans="1:20" ht="18" customHeight="1">
       <c r="A118" s="50"/>
-      <c r="B118" s="31"/>
-      <c r="C118" s="30"/>
-      <c r="D118" s="30"/>
-      <c r="E118" s="31"/>
-      <c r="F118" s="32"/>
-      <c r="G118" s="32"/>
-      <c r="H118" s="33"/>
+      <c r="B118" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="C118" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D118" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E118" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="F118" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="G118" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H118" s="33" t="s">
+        <v>203</v>
+      </c>
       <c r="I118" s="34"/>
-      <c r="J118" s="35"/>
+      <c r="J118" s="35">
+        <v>8.93</v>
+      </c>
       <c r="K118" s="35"/>
-      <c r="L118" s="49"/>
-      <c r="M118" s="32"/>
-      <c r="N118" s="30"/>
+      <c r="L118" s="49" t="s">
+        <v>202</v>
+      </c>
+      <c r="M118" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="N118" s="30" t="s">
+        <v>197</v>
+      </c>
       <c r="O118" s="45"/>
       <c r="P118" s="38"/>
       <c r="Q118" s="38"/>
@@ -8136,7 +8199,6 @@
       <c r="D119" s="30"/>
       <c r="E119" s="31"/>
       <c r="F119" s="32"/>
-      <c r="G119" s="32"/>
       <c r="H119" s="33"/>
       <c r="I119" s="34"/>
       <c r="J119" s="35"/>
@@ -26512,6 +26574,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -26526,11 +26593,6 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
- parsed data from `10.1007/s10854-021-05749-1`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Aug2025.xlsx
+++ b/MiscSmallUploads_Aug2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA19D588-E82F-114C-B1EA-695A19A40E2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFD311F-A4B5-0D47-8602-8C85AB4F886D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="8040" windowWidth="34560" windowHeight="12760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="207">
   <si>
     <r>
       <rPr>
@@ -742,6 +742,15 @@
   </si>
   <si>
     <t>5T</t>
+  </si>
+  <si>
+    <t>GdTbErHoY</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>10.1007/s10854-021-05749-1</t>
   </si>
 </sst>
 </file>
@@ -3235,7 +3244,7 @@
   <dimension ref="A1:T960"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A101" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J126" sqref="J126"/>
+      <selection activeCell="N123" sqref="N123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -8194,18 +8203,37 @@
     </row>
     <row r="119" spans="1:20" ht="18" customHeight="1">
       <c r="A119" s="50"/>
-      <c r="B119" s="31"/>
-      <c r="C119" s="30"/>
-      <c r="D119" s="30"/>
+      <c r="B119" s="31" t="s">
+        <v>204</v>
+      </c>
+      <c r="C119" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D119" s="30" t="s">
+        <v>64</v>
+      </c>
       <c r="E119" s="31"/>
-      <c r="F119" s="32"/>
+      <c r="F119" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="G119" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H119" s="33"/>
       <c r="I119" s="34"/>
-      <c r="J119" s="35"/>
+      <c r="J119" s="35">
+        <v>163</v>
+      </c>
       <c r="K119" s="35"/>
-      <c r="L119" s="49"/>
-      <c r="M119" s="32"/>
-      <c r="N119" s="30"/>
+      <c r="L119" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="M119" s="32" t="s">
+        <v>205</v>
+      </c>
+      <c r="N119" s="30" t="s">
+        <v>206</v>
+      </c>
       <c r="O119" s="45"/>
       <c r="P119" s="39"/>
       <c r="Q119" s="38"/>
@@ -8215,19 +8243,39 @@
     </row>
     <row r="120" spans="1:20" ht="18" customHeight="1">
       <c r="A120" s="50"/>
-      <c r="B120" s="31"/>
-      <c r="C120" s="30"/>
-      <c r="D120" s="30"/>
+      <c r="B120" s="31" t="s">
+        <v>204</v>
+      </c>
+      <c r="C120" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D120" s="30" t="s">
+        <v>64</v>
+      </c>
       <c r="E120" s="31"/>
-      <c r="F120" s="32"/>
-      <c r="G120" s="32"/>
-      <c r="H120" s="33"/>
+      <c r="F120" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="G120" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H120" s="33" t="s">
+        <v>203</v>
+      </c>
       <c r="I120" s="34"/>
-      <c r="J120" s="35"/>
+      <c r="J120" s="35">
+        <v>5.4</v>
+      </c>
       <c r="K120" s="35"/>
-      <c r="L120" s="49"/>
-      <c r="M120" s="32"/>
-      <c r="N120" s="30"/>
+      <c r="L120" s="49" t="s">
+        <v>202</v>
+      </c>
+      <c r="M120" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="N120" s="30" t="s">
+        <v>206</v>
+      </c>
       <c r="O120" s="45"/>
       <c r="P120" s="39"/>
       <c r="Q120" s="38"/>

</xml_diff>

<commit_message>
- parsed data from `10.1016/j.intermet.2022.107678`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Aug2025.xlsx
+++ b/MiscSmallUploads_Aug2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFD311F-A4B5-0D47-8602-8C85AB4F886D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DBB1FE-BBE0-F14D-854F-E34754DBDA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="8040" windowWidth="34560" windowHeight="12760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="222">
   <si>
     <r>
       <rPr>
@@ -751,6 +751,51 @@
   </si>
   <si>
     <t>10.1007/s10854-021-05749-1</t>
+  </si>
+  <si>
+    <t>10.1016/j.intermet.2022.107678</t>
+  </si>
+  <si>
+    <t>ScGdTbDyHo</t>
+  </si>
+  <si>
+    <t>arc melting under flowing helium and then suction cast for rapid solidification</t>
+  </si>
+  <si>
+    <t>AAM+RS</t>
+  </si>
+  <si>
+    <t>AAM+A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arc melting under flowing helium and then severely cold-deformed </t>
+  </si>
+  <si>
+    <t>AAM+SPD</t>
+  </si>
+  <si>
+    <t>arc melting under flowing helium; very minor FCC phase in HCP</t>
+  </si>
+  <si>
+    <t>HCP+FCC</t>
+  </si>
+  <si>
+    <t>arc melting under flowing helium and then annealed at 1173K for 2h; very minor FCC phase in HCP</t>
+  </si>
+  <si>
+    <t>as cast</t>
+  </si>
+  <si>
+    <t>quenched</t>
+  </si>
+  <si>
+    <t>annealed</t>
+  </si>
+  <si>
+    <t>deformed</t>
+  </si>
+  <si>
+    <t>T4</t>
   </si>
 </sst>
 </file>
@@ -3243,8 +3288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T960"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A101" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N123" sqref="N123"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A106" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H131" sqref="H131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -8284,20 +8329,42 @@
       <c r="T120" s="37"/>
     </row>
     <row r="121" spans="1:20" ht="18" customHeight="1">
-      <c r="A121" s="50"/>
-      <c r="B121" s="31"/>
-      <c r="C121" s="30"/>
-      <c r="D121" s="30"/>
-      <c r="E121" s="31"/>
-      <c r="F121" s="32"/>
-      <c r="G121" s="32"/>
+      <c r="A121" s="50" t="s">
+        <v>217</v>
+      </c>
+      <c r="B121" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="C121" s="30" t="s">
+        <v>215</v>
+      </c>
+      <c r="D121" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E121" s="31" t="s">
+        <v>214</v>
+      </c>
+      <c r="F121" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="G121" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H121" s="33"/>
       <c r="I121" s="34"/>
-      <c r="J121" s="35"/>
+      <c r="J121" s="35">
+        <v>144</v>
+      </c>
       <c r="K121" s="35"/>
-      <c r="L121" s="49"/>
-      <c r="M121" s="32"/>
-      <c r="N121" s="30"/>
+      <c r="L121" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="M121" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="N121" s="30" t="s">
+        <v>207</v>
+      </c>
       <c r="O121" s="45"/>
       <c r="P121" s="39"/>
       <c r="Q121" s="38"/>
@@ -8306,20 +8373,42 @@
       <c r="T121" s="37"/>
     </row>
     <row r="122" spans="1:20" ht="18" customHeight="1">
-      <c r="A122" s="50"/>
-      <c r="B122" s="31"/>
-      <c r="C122" s="30"/>
-      <c r="D122" s="30"/>
-      <c r="E122" s="31"/>
-      <c r="F122" s="32"/>
-      <c r="G122" s="32"/>
+      <c r="A122" s="50" t="s">
+        <v>218</v>
+      </c>
+      <c r="B122" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="C122" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D122" s="30" t="s">
+        <v>210</v>
+      </c>
+      <c r="E122" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="F122" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="G122" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H122" s="33"/>
       <c r="I122" s="34"/>
-      <c r="J122" s="35"/>
+      <c r="J122" s="35">
+        <v>143</v>
+      </c>
       <c r="K122" s="35"/>
-      <c r="L122" s="49"/>
-      <c r="M122" s="32"/>
-      <c r="N122" s="30"/>
+      <c r="L122" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="M122" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="N122" s="30" t="s">
+        <v>207</v>
+      </c>
       <c r="O122" s="45"/>
       <c r="P122" s="39"/>
       <c r="Q122" s="38"/>
@@ -8328,20 +8417,42 @@
       <c r="T122" s="37"/>
     </row>
     <row r="123" spans="1:20" ht="18" customHeight="1">
-      <c r="A123" s="50"/>
-      <c r="B123" s="31"/>
-      <c r="C123" s="30"/>
-      <c r="D123" s="30"/>
-      <c r="E123" s="31"/>
-      <c r="F123" s="32"/>
-      <c r="G123" s="32"/>
+      <c r="A123" s="50" t="s">
+        <v>219</v>
+      </c>
+      <c r="B123" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="C123" s="30" t="s">
+        <v>215</v>
+      </c>
+      <c r="D123" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="E123" s="31" t="s">
+        <v>216</v>
+      </c>
+      <c r="F123" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="G123" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H123" s="33"/>
       <c r="I123" s="34"/>
-      <c r="J123" s="35"/>
+      <c r="J123" s="35">
+        <v>146</v>
+      </c>
       <c r="K123" s="35"/>
-      <c r="L123" s="49"/>
-      <c r="M123" s="32"/>
-      <c r="N123" s="30"/>
+      <c r="L123" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="M123" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="N123" s="30" t="s">
+        <v>207</v>
+      </c>
       <c r="O123" s="45"/>
       <c r="P123" s="39"/>
       <c r="Q123" s="38"/>
@@ -8350,20 +8461,42 @@
       <c r="T123" s="37"/>
     </row>
     <row r="124" spans="1:20" ht="18" customHeight="1">
-      <c r="A124" s="50"/>
-      <c r="B124" s="31"/>
-      <c r="C124" s="30"/>
-      <c r="D124" s="30"/>
-      <c r="E124" s="31"/>
-      <c r="F124" s="32"/>
-      <c r="G124" s="32"/>
+      <c r="A124" s="50" t="s">
+        <v>220</v>
+      </c>
+      <c r="B124" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="C124" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D124" s="30" t="s">
+        <v>213</v>
+      </c>
+      <c r="E124" s="102" t="s">
+        <v>212</v>
+      </c>
+      <c r="F124" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="G124" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H124" s="33"/>
       <c r="I124" s="34"/>
-      <c r="J124" s="35"/>
+      <c r="J124" s="35">
+        <v>139</v>
+      </c>
       <c r="K124" s="35"/>
-      <c r="L124" s="49"/>
-      <c r="M124" s="32"/>
-      <c r="N124" s="30"/>
+      <c r="L124" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="M124" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="N124" s="30" t="s">
+        <v>207</v>
+      </c>
       <c r="O124" s="37"/>
       <c r="P124" s="39"/>
       <c r="Q124" s="38"/>
@@ -8372,20 +8505,44 @@
       <c r="T124" s="37"/>
     </row>
     <row r="125" spans="1:20" ht="18" customHeight="1">
-      <c r="A125" s="50"/>
-      <c r="B125" s="31"/>
-      <c r="C125" s="30"/>
-      <c r="D125" s="30"/>
-      <c r="E125" s="31"/>
-      <c r="F125" s="32"/>
-      <c r="G125" s="32"/>
-      <c r="H125" s="33"/>
+      <c r="A125" s="50" t="s">
+        <v>217</v>
+      </c>
+      <c r="B125" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="C125" s="30" t="s">
+        <v>215</v>
+      </c>
+      <c r="D125" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E125" s="31" t="s">
+        <v>214</v>
+      </c>
+      <c r="F125" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="G125" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H125" s="33" t="s">
+        <v>203</v>
+      </c>
       <c r="I125" s="34"/>
-      <c r="J125" s="35"/>
+      <c r="J125" s="35">
+        <v>9.0299999999999994</v>
+      </c>
       <c r="K125" s="35"/>
-      <c r="L125" s="49"/>
-      <c r="M125" s="32"/>
-      <c r="N125" s="30"/>
+      <c r="L125" s="49" t="s">
+        <v>202</v>
+      </c>
+      <c r="M125" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="N125" s="30" t="s">
+        <v>207</v>
+      </c>
       <c r="O125" s="37"/>
       <c r="P125" s="39"/>
       <c r="Q125" s="38"/>
@@ -8394,20 +8551,44 @@
       <c r="T125" s="37"/>
     </row>
     <row r="126" spans="1:20" ht="18" customHeight="1">
-      <c r="A126" s="50"/>
-      <c r="B126" s="31"/>
-      <c r="C126" s="30"/>
-      <c r="D126" s="30"/>
-      <c r="E126" s="31"/>
-      <c r="F126" s="32"/>
-      <c r="G126" s="32"/>
-      <c r="H126" s="33"/>
+      <c r="A126" s="50" t="s">
+        <v>218</v>
+      </c>
+      <c r="B126" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="C126" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D126" s="30" t="s">
+        <v>210</v>
+      </c>
+      <c r="E126" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="F126" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="G126" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H126" s="33" t="s">
+        <v>203</v>
+      </c>
       <c r="I126" s="34"/>
-      <c r="J126" s="35"/>
+      <c r="J126" s="35">
+        <v>9.23</v>
+      </c>
       <c r="K126" s="35"/>
-      <c r="L126" s="49"/>
-      <c r="M126" s="32"/>
-      <c r="N126" s="30"/>
+      <c r="L126" s="49" t="s">
+        <v>202</v>
+      </c>
+      <c r="M126" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="N126" s="30" t="s">
+        <v>207</v>
+      </c>
       <c r="O126" s="37"/>
       <c r="P126" s="39"/>
       <c r="Q126" s="38"/>
@@ -8416,20 +8597,44 @@
       <c r="T126" s="37"/>
     </row>
     <row r="127" spans="1:20" ht="18" customHeight="1">
-      <c r="A127" s="50"/>
-      <c r="B127" s="31"/>
-      <c r="C127" s="90"/>
-      <c r="D127" s="30"/>
-      <c r="E127" s="31"/>
-      <c r="F127" s="32"/>
-      <c r="G127" s="32"/>
-      <c r="H127" s="33"/>
+      <c r="A127" s="50" t="s">
+        <v>219</v>
+      </c>
+      <c r="B127" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="C127" s="30" t="s">
+        <v>215</v>
+      </c>
+      <c r="D127" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="E127" s="31" t="s">
+        <v>216</v>
+      </c>
+      <c r="F127" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="G127" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H127" s="33" t="s">
+        <v>203</v>
+      </c>
       <c r="I127" s="34"/>
-      <c r="J127" s="35"/>
+      <c r="J127" s="35">
+        <v>7.86</v>
+      </c>
       <c r="K127" s="35"/>
-      <c r="L127" s="49"/>
-      <c r="M127" s="32"/>
-      <c r="N127" s="30"/>
+      <c r="L127" s="49" t="s">
+        <v>202</v>
+      </c>
+      <c r="M127" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="N127" s="30" t="s">
+        <v>207</v>
+      </c>
       <c r="O127" s="37"/>
       <c r="P127" s="39"/>
       <c r="Q127" s="38"/>
@@ -8438,20 +8643,44 @@
       <c r="T127" s="37"/>
     </row>
     <row r="128" spans="1:20" ht="18" customHeight="1">
-      <c r="A128" s="50"/>
-      <c r="B128" s="31"/>
-      <c r="C128" s="90"/>
-      <c r="D128" s="30"/>
-      <c r="E128" s="31"/>
-      <c r="F128" s="32"/>
-      <c r="G128" s="32"/>
-      <c r="H128" s="33"/>
+      <c r="A128" s="50" t="s">
+        <v>220</v>
+      </c>
+      <c r="B128" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="C128" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D128" s="30" t="s">
+        <v>213</v>
+      </c>
+      <c r="E128" s="102" t="s">
+        <v>212</v>
+      </c>
+      <c r="F128" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="G128" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H128" s="33" t="s">
+        <v>203</v>
+      </c>
       <c r="I128" s="34"/>
-      <c r="J128" s="35"/>
+      <c r="J128" s="35">
+        <v>8.56</v>
+      </c>
       <c r="K128" s="35"/>
-      <c r="L128" s="49"/>
-      <c r="M128" s="32"/>
-      <c r="N128" s="30"/>
+      <c r="L128" s="49" t="s">
+        <v>202</v>
+      </c>
+      <c r="M128" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="N128" s="30" t="s">
+        <v>207</v>
+      </c>
       <c r="O128" s="37"/>
       <c r="P128" s="39"/>
       <c r="Q128" s="38"/>

</xml_diff>

<commit_message>
- parsed data from `10.1016/j.jmst.2021.08.076`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Aug2025.xlsx
+++ b/MiscSmallUploads_Aug2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DBB1FE-BBE0-F14D-854F-E34754DBDA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B20CC73-4079-FC4D-ADE9-B41B1220D214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8040" windowWidth="34560" windowHeight="12760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="10900" windowWidth="34560" windowHeight="12760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1263" uniqueCount="244">
   <si>
     <r>
       <rPr>
@@ -796,6 +796,72 @@
   </si>
   <si>
     <t>T4</t>
+  </si>
+  <si>
+    <t>Gd20 (Tb0.25 Dy0.25 Ho0.25 Er0.25)80</t>
+  </si>
+  <si>
+    <t>Gd40 (Tb0.25 Dy0.25 Ho0.25 Er0.25)60</t>
+  </si>
+  <si>
+    <t>Gd60 (Tb0.25 Dy0.25 Ho0.25 Er0.25)40</t>
+  </si>
+  <si>
+    <t>Gd80 (Tb0.25 Dy0.25 Ho0.25 Er0.25)20</t>
+  </si>
+  <si>
+    <t>Gd90 (Tb0.25 Dy0.25 Ho0.25 Er0.25)10</t>
+  </si>
+  <si>
+    <t>AAM+DC</t>
+  </si>
+  <si>
+    <t>drop cast into 10x30mm cylinders</t>
+  </si>
+  <si>
+    <t>curie temperature</t>
+  </si>
+  <si>
+    <t>Gd</t>
+  </si>
+  <si>
+    <t>10.1016/j.jallcom.2023.170901</t>
+  </si>
+  <si>
+    <t>Gd20Tb18Dy18Co20Al24</t>
+  </si>
+  <si>
+    <t>AAM+BM</t>
+  </si>
+  <si>
+    <t>(Gd0.2Tb0.18Dy0.18Co0.2Al0.24)43H57</t>
+  </si>
+  <si>
+    <t>amorphous+Al3Dy+TbAl3+Al2Gd3+CoGd3</t>
+  </si>
+  <si>
+    <t>AAM+BM+A</t>
+  </si>
+  <si>
+    <t>first fabricated as BMG in copper molds and then ball milled 50 aroud 50um</t>
+  </si>
+  <si>
+    <t>first fabricated as BMG in copper molds and then ball milled 50 aroud 50um and annealed at 538K for 42h in vacuum; critically the annealing was below Tg; many nanoprecipitates in amorphous phase</t>
+  </si>
+  <si>
+    <t>amorphous+hydride</t>
+  </si>
+  <si>
+    <t>first fabricated as BMG in copper molds and then ball milled 50 aroud 50um and annealed at 538K for 42h in hydrogen atmosphere of 5MPa initially to result in 1.2wt% hydrogenation; critically the annealing was below Tg; many nanoprecipitates in amorphous phase</t>
+  </si>
+  <si>
+    <t>nanohardness</t>
+  </si>
+  <si>
+    <t>reduced elastic modulus</t>
+  </si>
+  <si>
+    <t>10.1016/j.jmst.2021.08.076</t>
   </si>
 </sst>
 </file>
@@ -3288,8 +3354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T960"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A106" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H131" sqref="H131"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A134" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I154" sqref="I154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -8690,19 +8756,39 @@
     </row>
     <row r="129" spans="1:20" ht="18" customHeight="1">
       <c r="A129" s="50"/>
-      <c r="B129" s="31"/>
-      <c r="C129" s="91"/>
-      <c r="D129" s="30"/>
-      <c r="E129" s="31"/>
-      <c r="F129" s="32"/>
-      <c r="G129" s="32"/>
+      <c r="B129" s="31" t="s">
+        <v>222</v>
+      </c>
+      <c r="C129" s="91" t="s">
+        <v>142</v>
+      </c>
+      <c r="D129" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="E129" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="F129" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="G129" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H129" s="33"/>
       <c r="I129" s="34"/>
-      <c r="J129" s="35"/>
+      <c r="J129" s="35">
+        <v>198</v>
+      </c>
       <c r="K129" s="35"/>
-      <c r="L129" s="49"/>
-      <c r="M129" s="32"/>
-      <c r="N129" s="30"/>
+      <c r="L129" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="M129" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="N129" s="30" t="s">
+        <v>231</v>
+      </c>
       <c r="O129" s="37"/>
       <c r="P129" s="39"/>
       <c r="Q129" s="38"/>
@@ -8712,19 +8798,39 @@
     </row>
     <row r="130" spans="1:20" ht="18" customHeight="1">
       <c r="A130" s="50"/>
-      <c r="B130" s="31"/>
-      <c r="C130" s="91"/>
-      <c r="D130" s="30"/>
-      <c r="E130" s="31"/>
-      <c r="F130" s="32"/>
-      <c r="G130" s="32"/>
+      <c r="B130" s="31" t="s">
+        <v>223</v>
+      </c>
+      <c r="C130" s="91" t="s">
+        <v>142</v>
+      </c>
+      <c r="D130" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="E130" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="F130" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="G130" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H130" s="33"/>
       <c r="I130" s="34"/>
-      <c r="J130" s="35"/>
+      <c r="J130" s="35">
+        <v>221</v>
+      </c>
       <c r="K130" s="35"/>
-      <c r="L130" s="49"/>
-      <c r="M130" s="32"/>
-      <c r="N130" s="30"/>
+      <c r="L130" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="M130" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="N130" s="30" t="s">
+        <v>231</v>
+      </c>
       <c r="O130" s="37"/>
       <c r="P130" s="39"/>
       <c r="Q130" s="38"/>
@@ -8734,19 +8840,39 @@
     </row>
     <row r="131" spans="1:20" ht="18" customHeight="1">
       <c r="A131" s="50"/>
-      <c r="B131" s="31"/>
-      <c r="C131" s="91"/>
-      <c r="D131" s="30"/>
-      <c r="E131" s="31"/>
-      <c r="F131" s="32"/>
-      <c r="G131" s="32"/>
+      <c r="B131" s="31" t="s">
+        <v>224</v>
+      </c>
+      <c r="C131" s="91" t="s">
+        <v>142</v>
+      </c>
+      <c r="D131" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="E131" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="F131" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="G131" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H131" s="33"/>
       <c r="I131" s="34"/>
-      <c r="J131" s="35"/>
+      <c r="J131" s="35">
+        <v>244</v>
+      </c>
       <c r="K131" s="35"/>
-      <c r="L131" s="49"/>
-      <c r="M131" s="32"/>
-      <c r="N131" s="30"/>
+      <c r="L131" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="M131" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="N131" s="30" t="s">
+        <v>231</v>
+      </c>
       <c r="O131" s="37"/>
       <c r="P131" s="39"/>
       <c r="Q131" s="38"/>
@@ -8756,19 +8882,39 @@
     </row>
     <row r="132" spans="1:20" ht="18" customHeight="1">
       <c r="A132" s="50"/>
-      <c r="B132" s="31"/>
-      <c r="C132" s="91"/>
-      <c r="D132" s="30"/>
-      <c r="E132" s="31"/>
-      <c r="F132" s="32"/>
-      <c r="G132" s="32"/>
+      <c r="B132" s="31" t="s">
+        <v>225</v>
+      </c>
+      <c r="C132" s="91" t="s">
+        <v>142</v>
+      </c>
+      <c r="D132" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="E132" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="F132" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="G132" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H132" s="33"/>
       <c r="I132" s="34"/>
-      <c r="J132" s="35"/>
+      <c r="J132" s="35">
+        <v>268</v>
+      </c>
       <c r="K132" s="35"/>
-      <c r="L132" s="49"/>
-      <c r="M132" s="32"/>
-      <c r="N132" s="30"/>
+      <c r="L132" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="M132" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="N132" s="30" t="s">
+        <v>231</v>
+      </c>
       <c r="O132" s="37"/>
       <c r="P132" s="38"/>
       <c r="Q132" s="38"/>
@@ -8778,19 +8924,39 @@
     </row>
     <row r="133" spans="1:20" ht="18" customHeight="1">
       <c r="A133" s="50"/>
-      <c r="B133" s="31"/>
-      <c r="C133" s="91"/>
-      <c r="D133" s="30"/>
-      <c r="E133" s="31"/>
-      <c r="F133" s="32"/>
-      <c r="G133" s="32"/>
+      <c r="B133" s="31" t="s">
+        <v>226</v>
+      </c>
+      <c r="C133" s="91" t="s">
+        <v>142</v>
+      </c>
+      <c r="D133" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="E133" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="F133" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="G133" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H133" s="33"/>
       <c r="I133" s="34"/>
-      <c r="J133" s="35"/>
+      <c r="J133" s="35">
+        <v>279</v>
+      </c>
       <c r="K133" s="35"/>
-      <c r="L133" s="49"/>
-      <c r="M133" s="32"/>
-      <c r="N133" s="30"/>
+      <c r="L133" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="M133" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="N133" s="30" t="s">
+        <v>231</v>
+      </c>
       <c r="O133" s="37"/>
       <c r="P133" s="38"/>
       <c r="Q133" s="38"/>
@@ -8800,19 +8966,39 @@
     </row>
     <row r="134" spans="1:20" ht="18" customHeight="1">
       <c r="A134" s="50"/>
-      <c r="B134" s="31"/>
-      <c r="C134" s="91"/>
-      <c r="D134" s="30"/>
-      <c r="E134" s="31"/>
-      <c r="F134" s="32"/>
-      <c r="G134" s="32"/>
+      <c r="B134" s="31" t="s">
+        <v>230</v>
+      </c>
+      <c r="C134" s="91" t="s">
+        <v>142</v>
+      </c>
+      <c r="D134" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="E134" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="F134" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="G134" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H134" s="33"/>
       <c r="I134" s="34"/>
-      <c r="J134" s="35"/>
+      <c r="J134" s="35">
+        <v>296</v>
+      </c>
       <c r="K134" s="35"/>
-      <c r="L134" s="49"/>
-      <c r="M134" s="32"/>
-      <c r="N134" s="30"/>
+      <c r="L134" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="M134" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="N134" s="30" t="s">
+        <v>231</v>
+      </c>
       <c r="O134" s="37"/>
       <c r="P134" s="38"/>
       <c r="Q134" s="38"/>
@@ -8822,19 +9008,41 @@
     </row>
     <row r="135" spans="1:20" ht="18" customHeight="1">
       <c r="A135" s="50"/>
-      <c r="B135" s="31"/>
-      <c r="C135" s="91"/>
-      <c r="D135" s="30"/>
-      <c r="E135" s="31"/>
-      <c r="F135" s="32"/>
-      <c r="G135" s="32"/>
-      <c r="H135" s="33"/>
+      <c r="B135" s="31" t="s">
+        <v>222</v>
+      </c>
+      <c r="C135" s="91" t="s">
+        <v>142</v>
+      </c>
+      <c r="D135" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="E135" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="F135" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="G135" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H135" s="33" t="s">
+        <v>203</v>
+      </c>
       <c r="I135" s="34"/>
-      <c r="J135" s="35"/>
+      <c r="J135" s="35">
+        <v>11.01</v>
+      </c>
       <c r="K135" s="35"/>
-      <c r="L135" s="49"/>
-      <c r="M135" s="32"/>
-      <c r="N135" s="30"/>
+      <c r="L135" s="49" t="s">
+        <v>202</v>
+      </c>
+      <c r="M135" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="N135" s="30" t="s">
+        <v>231</v>
+      </c>
       <c r="O135" s="37"/>
       <c r="P135" s="38"/>
       <c r="Q135" s="38"/>
@@ -8844,19 +9052,41 @@
     </row>
     <row r="136" spans="1:20" ht="18" customHeight="1">
       <c r="A136" s="50"/>
-      <c r="B136" s="31"/>
-      <c r="C136" s="91"/>
-      <c r="D136" s="30"/>
-      <c r="E136" s="31"/>
-      <c r="F136" s="32"/>
-      <c r="G136" s="32"/>
-      <c r="H136" s="33"/>
+      <c r="B136" s="31" t="s">
+        <v>223</v>
+      </c>
+      <c r="C136" s="91" t="s">
+        <v>142</v>
+      </c>
+      <c r="D136" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="E136" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="F136" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="G136" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H136" s="33" t="s">
+        <v>203</v>
+      </c>
       <c r="I136" s="34"/>
-      <c r="J136" s="35"/>
+      <c r="J136" s="35">
+        <v>10.86</v>
+      </c>
       <c r="K136" s="35"/>
-      <c r="L136" s="49"/>
-      <c r="M136" s="32"/>
-      <c r="N136" s="30"/>
+      <c r="L136" s="49" t="s">
+        <v>202</v>
+      </c>
+      <c r="M136" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="N136" s="30" t="s">
+        <v>231</v>
+      </c>
       <c r="O136" s="37"/>
       <c r="P136" s="38"/>
       <c r="Q136" s="38"/>
@@ -8866,19 +9096,41 @@
     </row>
     <row r="137" spans="1:20" ht="18" customHeight="1">
       <c r="A137" s="50"/>
-      <c r="B137" s="31"/>
-      <c r="C137" s="90"/>
-      <c r="D137" s="30"/>
-      <c r="E137" s="31"/>
-      <c r="F137" s="32"/>
-      <c r="G137" s="32"/>
-      <c r="H137" s="33"/>
+      <c r="B137" s="31" t="s">
+        <v>224</v>
+      </c>
+      <c r="C137" s="91" t="s">
+        <v>142</v>
+      </c>
+      <c r="D137" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="E137" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="F137" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="G137" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H137" s="33" t="s">
+        <v>203</v>
+      </c>
       <c r="I137" s="34"/>
-      <c r="J137" s="35"/>
+      <c r="J137" s="35">
+        <v>10.57</v>
+      </c>
       <c r="K137" s="35"/>
-      <c r="L137" s="49"/>
-      <c r="M137" s="32"/>
-      <c r="N137" s="30"/>
+      <c r="L137" s="49" t="s">
+        <v>202</v>
+      </c>
+      <c r="M137" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="N137" s="30" t="s">
+        <v>231</v>
+      </c>
       <c r="O137" s="37"/>
       <c r="P137" s="38"/>
       <c r="Q137" s="38"/>
@@ -8888,19 +9140,41 @@
     </row>
     <row r="138" spans="1:20" ht="18" customHeight="1">
       <c r="A138" s="50"/>
-      <c r="B138" s="31"/>
-      <c r="C138" s="91"/>
-      <c r="D138" s="30"/>
-      <c r="E138" s="31"/>
-      <c r="F138" s="32"/>
-      <c r="G138" s="32"/>
-      <c r="H138" s="33"/>
+      <c r="B138" s="31" t="s">
+        <v>225</v>
+      </c>
+      <c r="C138" s="91" t="s">
+        <v>142</v>
+      </c>
+      <c r="D138" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="E138" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="F138" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="G138" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H138" s="33" t="s">
+        <v>203</v>
+      </c>
       <c r="I138" s="34"/>
-      <c r="J138" s="35"/>
+      <c r="J138" s="35">
+        <v>10.53</v>
+      </c>
       <c r="K138" s="35"/>
-      <c r="L138" s="49"/>
-      <c r="M138" s="32"/>
-      <c r="N138" s="30"/>
+      <c r="L138" s="49" t="s">
+        <v>202</v>
+      </c>
+      <c r="M138" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="N138" s="30" t="s">
+        <v>231</v>
+      </c>
       <c r="O138" s="37"/>
       <c r="P138" s="38"/>
       <c r="Q138" s="38"/>
@@ -8910,19 +9184,41 @@
     </row>
     <row r="139" spans="1:20" ht="18" customHeight="1">
       <c r="A139" s="50"/>
-      <c r="B139" s="31"/>
-      <c r="C139" s="91"/>
-      <c r="D139" s="30"/>
-      <c r="E139" s="31"/>
-      <c r="F139" s="32"/>
-      <c r="G139" s="32"/>
-      <c r="H139" s="33"/>
+      <c r="B139" s="31" t="s">
+        <v>226</v>
+      </c>
+      <c r="C139" s="91" t="s">
+        <v>142</v>
+      </c>
+      <c r="D139" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="E139" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="F139" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="G139" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H139" s="33" t="s">
+        <v>203</v>
+      </c>
       <c r="I139" s="34"/>
-      <c r="J139" s="35"/>
+      <c r="J139" s="35">
+        <v>9.67</v>
+      </c>
       <c r="K139" s="35"/>
-      <c r="L139" s="49"/>
-      <c r="M139" s="32"/>
-      <c r="N139" s="30"/>
+      <c r="L139" s="49" t="s">
+        <v>202</v>
+      </c>
+      <c r="M139" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="N139" s="30" t="s">
+        <v>231</v>
+      </c>
       <c r="O139" s="37"/>
       <c r="P139" s="38"/>
       <c r="Q139" s="38"/>
@@ -8932,19 +9228,41 @@
     </row>
     <row r="140" spans="1:20" ht="18" customHeight="1">
       <c r="A140" s="50"/>
-      <c r="B140" s="31"/>
-      <c r="C140" s="91"/>
-      <c r="D140" s="30"/>
-      <c r="E140" s="31"/>
-      <c r="F140" s="32"/>
-      <c r="G140" s="32"/>
-      <c r="H140" s="33"/>
+      <c r="B140" s="31" t="s">
+        <v>230</v>
+      </c>
+      <c r="C140" s="91" t="s">
+        <v>142</v>
+      </c>
+      <c r="D140" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="E140" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="F140" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="G140" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H140" s="33" t="s">
+        <v>203</v>
+      </c>
       <c r="I140" s="34"/>
-      <c r="J140" s="35"/>
+      <c r="J140" s="35">
+        <v>9.44</v>
+      </c>
       <c r="K140" s="35"/>
-      <c r="L140" s="49"/>
-      <c r="M140" s="32"/>
-      <c r="N140" s="30"/>
+      <c r="L140" s="49" t="s">
+        <v>202</v>
+      </c>
+      <c r="M140" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="N140" s="30" t="s">
+        <v>231</v>
+      </c>
       <c r="O140" s="37"/>
       <c r="P140" s="38"/>
       <c r="Q140" s="38"/>
@@ -8954,19 +9272,37 @@
     </row>
     <row r="141" spans="1:20" ht="18" customHeight="1">
       <c r="A141" s="50"/>
-      <c r="B141" s="31"/>
-      <c r="C141" s="91"/>
-      <c r="D141" s="30"/>
-      <c r="E141" s="31"/>
-      <c r="F141" s="32"/>
-      <c r="G141" s="32"/>
+      <c r="B141" s="31" t="s">
+        <v>232</v>
+      </c>
+      <c r="C141" s="91" t="s">
+        <v>158</v>
+      </c>
+      <c r="D141" s="30" t="s">
+        <v>233</v>
+      </c>
+      <c r="E141" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="F141" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="G141" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H141" s="33"/>
       <c r="I141" s="34"/>
-      <c r="J141" s="35"/>
+      <c r="J141" s="35">
+        <v>606</v>
+      </c>
       <c r="K141" s="35"/>
-      <c r="L141" s="49"/>
+      <c r="L141" s="49" t="s">
+        <v>123</v>
+      </c>
       <c r="M141" s="32"/>
-      <c r="N141" s="30"/>
+      <c r="N141" s="30" t="s">
+        <v>243</v>
+      </c>
       <c r="O141" s="37"/>
       <c r="P141" s="38"/>
       <c r="Q141" s="38"/>
@@ -8976,19 +9312,37 @@
     </row>
     <row r="142" spans="1:20" ht="18" customHeight="1">
       <c r="A142" s="50"/>
-      <c r="B142" s="31"/>
-      <c r="C142" s="91"/>
-      <c r="D142" s="30"/>
-      <c r="E142" s="31"/>
-      <c r="F142" s="32"/>
-      <c r="G142" s="32"/>
+      <c r="B142" s="31" t="s">
+        <v>232</v>
+      </c>
+      <c r="C142" s="91" t="s">
+        <v>235</v>
+      </c>
+      <c r="D142" s="30" t="s">
+        <v>236</v>
+      </c>
+      <c r="E142" s="31" t="s">
+        <v>238</v>
+      </c>
+      <c r="F142" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="G142" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H142" s="33"/>
       <c r="I142" s="34"/>
-      <c r="J142" s="35"/>
+      <c r="J142" s="35">
+        <v>59</v>
+      </c>
       <c r="K142" s="35"/>
-      <c r="L142" s="49"/>
+      <c r="L142" s="49" t="s">
+        <v>123</v>
+      </c>
       <c r="M142" s="32"/>
-      <c r="N142" s="30"/>
+      <c r="N142" s="30" t="s">
+        <v>243</v>
+      </c>
       <c r="O142" s="37"/>
       <c r="P142" s="38"/>
       <c r="Q142" s="38"/>
@@ -8998,19 +9352,37 @@
     </row>
     <row r="143" spans="1:20" ht="18" customHeight="1">
       <c r="A143" s="50"/>
-      <c r="B143" s="31"/>
-      <c r="C143" s="30"/>
-      <c r="D143" s="30"/>
-      <c r="E143" s="31"/>
-      <c r="F143" s="32"/>
-      <c r="G143" s="32"/>
+      <c r="B143" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="C143" s="30" t="s">
+        <v>239</v>
+      </c>
+      <c r="D143" s="30" t="s">
+        <v>236</v>
+      </c>
+      <c r="E143" s="31" t="s">
+        <v>240</v>
+      </c>
+      <c r="F143" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="G143" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H143" s="33"/>
       <c r="I143" s="34"/>
-      <c r="J143" s="35"/>
+      <c r="J143" s="35">
+        <v>8</v>
+      </c>
       <c r="K143" s="35"/>
-      <c r="L143" s="49"/>
+      <c r="L143" s="49" t="s">
+        <v>123</v>
+      </c>
       <c r="M143" s="32"/>
-      <c r="N143" s="30"/>
+      <c r="N143" s="30" t="s">
+        <v>243</v>
+      </c>
       <c r="O143" s="37"/>
       <c r="P143" s="38"/>
       <c r="Q143" s="38"/>
@@ -9020,19 +9392,39 @@
     </row>
     <row r="144" spans="1:20" ht="18" customHeight="1">
       <c r="A144" s="50"/>
-      <c r="B144" s="31"/>
-      <c r="C144" s="30"/>
-      <c r="D144" s="30"/>
-      <c r="E144" s="31"/>
-      <c r="F144" s="32"/>
-      <c r="G144" s="32"/>
-      <c r="H144" s="33"/>
+      <c r="B144" s="31" t="s">
+        <v>232</v>
+      </c>
+      <c r="C144" s="91" t="s">
+        <v>235</v>
+      </c>
+      <c r="D144" s="30" t="s">
+        <v>236</v>
+      </c>
+      <c r="E144" s="31" t="s">
+        <v>238</v>
+      </c>
+      <c r="F144" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="G144" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H144" s="33" t="s">
+        <v>203</v>
+      </c>
       <c r="I144" s="34"/>
-      <c r="J144" s="35"/>
+      <c r="J144" s="35">
+        <v>8.8000000000000007</v>
+      </c>
       <c r="K144" s="35"/>
-      <c r="L144" s="49"/>
+      <c r="L144" s="49" t="s">
+        <v>202</v>
+      </c>
       <c r="M144" s="32"/>
-      <c r="N144" s="30"/>
+      <c r="N144" s="30" t="s">
+        <v>243</v>
+      </c>
       <c r="O144" s="37"/>
       <c r="P144" s="38"/>
       <c r="Q144" s="38"/>
@@ -9042,19 +9434,39 @@
     </row>
     <row r="145" spans="1:20" ht="18" customHeight="1">
       <c r="A145" s="50"/>
-      <c r="B145" s="31"/>
-      <c r="C145" s="30"/>
-      <c r="D145" s="30"/>
-      <c r="E145" s="31"/>
-      <c r="F145" s="32"/>
-      <c r="G145" s="32"/>
-      <c r="H145" s="33"/>
+      <c r="B145" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="C145" s="30" t="s">
+        <v>239</v>
+      </c>
+      <c r="D145" s="30" t="s">
+        <v>236</v>
+      </c>
+      <c r="E145" s="31" t="s">
+        <v>240</v>
+      </c>
+      <c r="F145" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="G145" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H145" s="33" t="s">
+        <v>203</v>
+      </c>
       <c r="I145" s="34"/>
-      <c r="J145" s="35"/>
+      <c r="J145" s="35">
+        <v>13.6</v>
+      </c>
       <c r="K145" s="35"/>
-      <c r="L145" s="49"/>
+      <c r="L145" s="49" t="s">
+        <v>202</v>
+      </c>
       <c r="M145" s="32"/>
-      <c r="N145" s="30"/>
+      <c r="N145" s="30" t="s">
+        <v>243</v>
+      </c>
       <c r="O145" s="37"/>
       <c r="P145" s="38"/>
       <c r="Q145" s="38"/>
@@ -9064,19 +9476,41 @@
     </row>
     <row r="146" spans="1:20" ht="18" customHeight="1">
       <c r="A146" s="50"/>
-      <c r="B146" s="31"/>
-      <c r="C146" s="30"/>
-      <c r="D146" s="30"/>
-      <c r="E146" s="31"/>
-      <c r="F146" s="32"/>
-      <c r="G146" s="32"/>
+      <c r="B146" s="31" t="s">
+        <v>232</v>
+      </c>
+      <c r="C146" s="91" t="s">
+        <v>235</v>
+      </c>
+      <c r="D146" s="30" t="s">
+        <v>236</v>
+      </c>
+      <c r="E146" s="31" t="s">
+        <v>238</v>
+      </c>
+      <c r="F146" s="32" t="s">
+        <v>241</v>
+      </c>
+      <c r="G146" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H146" s="33"/>
-      <c r="I146" s="34"/>
-      <c r="J146" s="35"/>
-      <c r="K146" s="35"/>
-      <c r="L146" s="49"/>
+      <c r="I146" s="34">
+        <v>298</v>
+      </c>
+      <c r="J146" s="35">
+        <v>4460000000</v>
+      </c>
+      <c r="K146" s="35">
+        <v>90000000</v>
+      </c>
+      <c r="L146" s="49" t="s">
+        <v>33</v>
+      </c>
       <c r="M146" s="32"/>
-      <c r="N146" s="30"/>
+      <c r="N146" s="30" t="s">
+        <v>243</v>
+      </c>
       <c r="O146" s="37"/>
       <c r="P146" s="38"/>
       <c r="Q146" s="38"/>
@@ -9086,19 +9520,41 @@
     </row>
     <row r="147" spans="1:20" ht="18" customHeight="1">
       <c r="A147" s="50"/>
-      <c r="B147" s="31"/>
-      <c r="C147" s="30"/>
-      <c r="D147" s="30"/>
-      <c r="E147" s="31"/>
-      <c r="F147" s="32"/>
-      <c r="G147" s="32"/>
+      <c r="B147" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="C147" s="30" t="s">
+        <v>239</v>
+      </c>
+      <c r="D147" s="30" t="s">
+        <v>236</v>
+      </c>
+      <c r="E147" s="31" t="s">
+        <v>240</v>
+      </c>
+      <c r="F147" s="32" t="s">
+        <v>241</v>
+      </c>
+      <c r="G147" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H147" s="33"/>
-      <c r="I147" s="34"/>
-      <c r="J147" s="35"/>
-      <c r="K147" s="35"/>
-      <c r="L147" s="49"/>
+      <c r="I147" s="34">
+        <v>298</v>
+      </c>
+      <c r="J147" s="35">
+        <v>4360000000</v>
+      </c>
+      <c r="K147" s="35">
+        <v>360000000</v>
+      </c>
+      <c r="L147" s="49" t="s">
+        <v>33</v>
+      </c>
       <c r="M147" s="32"/>
-      <c r="N147" s="30"/>
+      <c r="N147" s="30" t="s">
+        <v>243</v>
+      </c>
       <c r="O147" s="37"/>
       <c r="P147" s="38"/>
       <c r="Q147" s="38"/>
@@ -9108,19 +9564,41 @@
     </row>
     <row r="148" spans="1:20" ht="18" customHeight="1">
       <c r="A148" s="50"/>
-      <c r="B148" s="31"/>
-      <c r="C148" s="30"/>
-      <c r="D148" s="30"/>
-      <c r="E148" s="31"/>
-      <c r="F148" s="52"/>
-      <c r="G148" s="32"/>
+      <c r="B148" s="31" t="s">
+        <v>232</v>
+      </c>
+      <c r="C148" s="91" t="s">
+        <v>235</v>
+      </c>
+      <c r="D148" s="30" t="s">
+        <v>236</v>
+      </c>
+      <c r="E148" s="31" t="s">
+        <v>238</v>
+      </c>
+      <c r="F148" s="52" t="s">
+        <v>242</v>
+      </c>
+      <c r="G148" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H148" s="33"/>
-      <c r="I148" s="34"/>
-      <c r="J148" s="37"/>
-      <c r="K148" s="51"/>
-      <c r="L148" s="49"/>
+      <c r="I148" s="34">
+        <v>298</v>
+      </c>
+      <c r="J148" s="58">
+        <v>68150000000</v>
+      </c>
+      <c r="K148" s="51">
+        <v>1160000000</v>
+      </c>
+      <c r="L148" s="49" t="s">
+        <v>33</v>
+      </c>
       <c r="M148" s="49"/>
-      <c r="N148" s="30"/>
+      <c r="N148" s="30" t="s">
+        <v>243</v>
+      </c>
       <c r="O148" s="37"/>
       <c r="P148" s="38"/>
       <c r="Q148" s="38"/>
@@ -9130,19 +9608,41 @@
     </row>
     <row r="149" spans="1:20" ht="18" customHeight="1">
       <c r="A149" s="50"/>
-      <c r="B149" s="31"/>
-      <c r="C149" s="30"/>
-      <c r="D149" s="30"/>
-      <c r="E149" s="31"/>
-      <c r="F149" s="52"/>
-      <c r="G149" s="32"/>
+      <c r="B149" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="C149" s="30" t="s">
+        <v>239</v>
+      </c>
+      <c r="D149" s="30" t="s">
+        <v>236</v>
+      </c>
+      <c r="E149" s="31" t="s">
+        <v>240</v>
+      </c>
+      <c r="F149" s="52" t="s">
+        <v>242</v>
+      </c>
+      <c r="G149" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H149" s="33"/>
-      <c r="I149" s="34"/>
-      <c r="J149" s="37"/>
-      <c r="K149" s="51"/>
-      <c r="L149" s="49"/>
+      <c r="I149" s="34">
+        <v>298</v>
+      </c>
+      <c r="J149" s="58">
+        <v>51250000000</v>
+      </c>
+      <c r="K149" s="51">
+        <v>4740000000</v>
+      </c>
+      <c r="L149" s="49" t="s">
+        <v>33</v>
+      </c>
       <c r="M149" s="49"/>
-      <c r="N149" s="30"/>
+      <c r="N149" s="30" t="s">
+        <v>243</v>
+      </c>
       <c r="O149" s="37"/>
       <c r="P149" s="38"/>
       <c r="Q149" s="38"/>

</xml_diff>

<commit_message>
- parsed data from `10.1016/j.jmst.2025.06.055`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Aug2025.xlsx
+++ b/MiscSmallUploads_Aug2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B20CC73-4079-FC4D-ADE9-B41B1220D214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F525816F-C067-CD44-9B20-474F1DA3C2E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="10900" windowWidth="34560" windowHeight="12760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="8020" windowWidth="34560" windowHeight="12760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1263" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1298" uniqueCount="251">
   <si>
     <r>
       <rPr>
@@ -862,6 +862,27 @@
   </si>
   <si>
     <t>10.1016/j.jmst.2021.08.076</t>
+  </si>
+  <si>
+    <t>10.1016/j.jmst.2025.06.055</t>
+  </si>
+  <si>
+    <t>Al11.94 Cr17.76 Fe18.71 Ni47.67 V3.87</t>
+  </si>
+  <si>
+    <t>LPBF</t>
+  </si>
+  <si>
+    <t>1e-4 strain rate</t>
+  </si>
+  <si>
+    <t>LPBF with 140W laser in Ar atmosphere with 1m/s scanning speed hatch distance of 50um and 20um layers; 99.8% density reported; HCF in temperature control at 293+/-2K</t>
+  </si>
+  <si>
+    <t>FCC+L12+B2</t>
+  </si>
+  <si>
+    <t>fatigue limit</t>
   </si>
 </sst>
 </file>
@@ -2081,6 +2102,57 @@
     <xf numFmtId="0" fontId="15" fillId="10" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2140,57 +2212,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3354,8 +3375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T960"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A134" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I154" sqref="I154"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A135" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L159" sqref="L159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -3412,19 +3433,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" s="112" t="s">
+      <c r="D2" s="129" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="113"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="117"/>
-      <c r="H2" s="117"/>
-      <c r="I2" s="118"/>
-      <c r="J2" s="119"/>
-      <c r="K2" s="119"/>
-      <c r="L2" s="117"/>
-      <c r="M2" s="117"/>
-      <c r="N2" s="120"/>
+      <c r="E2" s="130"/>
+      <c r="F2" s="133"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="135"/>
+      <c r="J2" s="136"/>
+      <c r="K2" s="136"/>
+      <c r="L2" s="134"/>
+      <c r="M2" s="134"/>
+      <c r="N2" s="137"/>
       <c r="O2" s="13"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -3440,17 +3461,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="114"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="121"/>
-      <c r="G3" s="121"/>
-      <c r="H3" s="121"/>
-      <c r="I3" s="122"/>
-      <c r="J3" s="123"/>
-      <c r="K3" s="123"/>
-      <c r="L3" s="121"/>
-      <c r="M3" s="121"/>
-      <c r="N3" s="124"/>
+      <c r="D3" s="131"/>
+      <c r="E3" s="132"/>
+      <c r="F3" s="138"/>
+      <c r="G3" s="138"/>
+      <c r="H3" s="138"/>
+      <c r="I3" s="139"/>
+      <c r="J3" s="140"/>
+      <c r="K3" s="140"/>
+      <c r="L3" s="138"/>
+      <c r="M3" s="138"/>
+      <c r="N3" s="141"/>
       <c r="O3" s="13"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -3491,43 +3512,43 @@
       <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="125" t="s">
+      <c r="C5" s="142" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="127" t="s">
+      <c r="D5" s="144" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="127" t="s">
+      <c r="E5" s="144" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="127" t="s">
+      <c r="F5" s="144" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="127" t="s">
+      <c r="G5" s="144" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="128" t="s">
+      <c r="H5" s="145" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="127" t="s">
+      <c r="I5" s="144" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="127" t="s">
+      <c r="J5" s="144" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="127" t="s">
+      <c r="K5" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="127" t="s">
+      <c r="L5" s="144" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="127" t="s">
+      <c r="M5" s="144" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="127" t="s">
+      <c r="N5" s="144" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="132" t="s">
+      <c r="O5" s="112" t="s">
         <v>20</v>
       </c>
       <c r="P5" s="25"/>
@@ -3543,19 +3564,19 @@
       <c r="B6" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="126"/>
-      <c r="D6" s="126"/>
-      <c r="E6" s="126"/>
-      <c r="F6" s="126"/>
-      <c r="G6" s="126"/>
-      <c r="H6" s="129"/>
-      <c r="I6" s="130"/>
-      <c r="J6" s="131"/>
-      <c r="K6" s="131"/>
-      <c r="L6" s="126"/>
-      <c r="M6" s="126"/>
-      <c r="N6" s="126"/>
-      <c r="O6" s="133"/>
+      <c r="C6" s="143"/>
+      <c r="D6" s="143"/>
+      <c r="E6" s="143"/>
+      <c r="F6" s="143"/>
+      <c r="G6" s="143"/>
+      <c r="H6" s="146"/>
+      <c r="I6" s="147"/>
+      <c r="J6" s="148"/>
+      <c r="K6" s="148"/>
+      <c r="L6" s="143"/>
+      <c r="M6" s="143"/>
+      <c r="N6" s="143"/>
+      <c r="O6" s="113"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="9"/>
@@ -3605,7 +3626,7 @@
       <c r="N7" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="134"/>
+      <c r="O7" s="114"/>
       <c r="P7" s="64" t="s">
         <v>62</v>
       </c>
@@ -3620,35 +3641,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" thickBot="1">
       <c r="A8" s="59"/>
-      <c r="B8" s="135" t="s">
+      <c r="B8" s="115" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="136"/>
-      <c r="D8" s="136"/>
-      <c r="E8" s="137"/>
-      <c r="F8" s="138" t="s">
+      <c r="C8" s="116"/>
+      <c r="D8" s="116"/>
+      <c r="E8" s="117"/>
+      <c r="F8" s="118" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="139"/>
-      <c r="H8" s="139"/>
-      <c r="I8" s="140"/>
-      <c r="J8" s="141"/>
-      <c r="K8" s="141"/>
-      <c r="L8" s="142"/>
-      <c r="M8" s="143" t="s">
+      <c r="G8" s="119"/>
+      <c r="H8" s="119"/>
+      <c r="I8" s="120"/>
+      <c r="J8" s="121"/>
+      <c r="K8" s="121"/>
+      <c r="L8" s="122"/>
+      <c r="M8" s="123" t="s">
         <v>40</v>
       </c>
-      <c r="N8" s="144"/>
+      <c r="N8" s="124"/>
       <c r="O8" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="P8" s="145" t="s">
+      <c r="P8" s="125" t="s">
         <v>42</v>
       </c>
-      <c r="Q8" s="146"/>
-      <c r="R8" s="147"/>
-      <c r="S8" s="147"/>
-      <c r="T8" s="148"/>
+      <c r="Q8" s="126"/>
+      <c r="R8" s="127"/>
+      <c r="S8" s="127"/>
+      <c r="T8" s="128"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1">
       <c r="A9" s="60" t="s">
@@ -9652,19 +9673,41 @@
     </row>
     <row r="150" spans="1:20" ht="18" customHeight="1">
       <c r="A150" s="50"/>
-      <c r="B150" s="31"/>
-      <c r="C150" s="30"/>
-      <c r="D150" s="30"/>
-      <c r="E150" s="31"/>
-      <c r="F150" s="52"/>
-      <c r="G150" s="32"/>
-      <c r="H150" s="33"/>
-      <c r="I150" s="34"/>
-      <c r="J150" s="37"/>
+      <c r="B150" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="C150" s="30" t="s">
+        <v>249</v>
+      </c>
+      <c r="D150" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="E150" s="31" t="s">
+        <v>248</v>
+      </c>
+      <c r="F150" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="G150" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H150" s="33" t="s">
+        <v>247</v>
+      </c>
+      <c r="I150" s="34">
+        <v>293</v>
+      </c>
+      <c r="J150" s="58">
+        <v>587000000</v>
+      </c>
       <c r="K150" s="48"/>
-      <c r="L150" s="49"/>
+      <c r="L150" s="49" t="s">
+        <v>33</v>
+      </c>
       <c r="M150" s="49"/>
-      <c r="N150" s="30"/>
+      <c r="N150" s="30" t="s">
+        <v>244</v>
+      </c>
       <c r="O150" s="37"/>
       <c r="P150" s="38"/>
       <c r="Q150" s="38"/>
@@ -9674,19 +9717,41 @@
     </row>
     <row r="151" spans="1:20" ht="18" customHeight="1">
       <c r="A151" s="50"/>
-      <c r="B151" s="31"/>
-      <c r="C151" s="30"/>
-      <c r="D151" s="30"/>
-      <c r="E151" s="31"/>
-      <c r="F151" s="52"/>
-      <c r="G151" s="32"/>
-      <c r="H151" s="33"/>
-      <c r="I151" s="34"/>
-      <c r="J151" s="37"/>
+      <c r="B151" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="C151" s="30" t="s">
+        <v>249</v>
+      </c>
+      <c r="D151" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="E151" s="31" t="s">
+        <v>248</v>
+      </c>
+      <c r="F151" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="G151" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H151" s="33" t="s">
+        <v>247</v>
+      </c>
+      <c r="I151" s="34">
+        <v>293</v>
+      </c>
+      <c r="J151" s="58">
+        <v>993000000</v>
+      </c>
       <c r="K151" s="48"/>
-      <c r="L151" s="49"/>
+      <c r="L151" s="49" t="s">
+        <v>33</v>
+      </c>
       <c r="M151" s="49"/>
-      <c r="N151" s="30"/>
+      <c r="N151" s="30" t="s">
+        <v>244</v>
+      </c>
       <c r="O151" s="37"/>
       <c r="P151" s="38"/>
       <c r="Q151" s="38"/>
@@ -9696,19 +9761,41 @@
     </row>
     <row r="152" spans="1:20" ht="18" customHeight="1">
       <c r="A152" s="50"/>
-      <c r="B152" s="31"/>
-      <c r="C152" s="30"/>
-      <c r="D152" s="30"/>
-      <c r="E152" s="31"/>
-      <c r="F152" s="52"/>
-      <c r="G152" s="32"/>
-      <c r="H152" s="33"/>
-      <c r="I152" s="34"/>
-      <c r="J152" s="48"/>
+      <c r="B152" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="C152" s="30" t="s">
+        <v>249</v>
+      </c>
+      <c r="D152" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="E152" s="31" t="s">
+        <v>248</v>
+      </c>
+      <c r="F152" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="G152" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H152" s="33" t="s">
+        <v>247</v>
+      </c>
+      <c r="I152" s="34">
+        <v>293</v>
+      </c>
+      <c r="J152" s="48">
+        <v>24.4</v>
+      </c>
       <c r="K152" s="48"/>
-      <c r="L152" s="49"/>
+      <c r="L152" s="49" t="s">
+        <v>68</v>
+      </c>
       <c r="M152" s="49"/>
-      <c r="N152" s="30"/>
+      <c r="N152" s="30" t="s">
+        <v>244</v>
+      </c>
       <c r="O152" s="37"/>
       <c r="P152" s="38"/>
       <c r="Q152" s="38"/>
@@ -9718,19 +9805,39 @@
     </row>
     <row r="153" spans="1:20" ht="18" customHeight="1">
       <c r="A153" s="50"/>
-      <c r="B153" s="31"/>
-      <c r="C153" s="30"/>
-      <c r="D153" s="30"/>
-      <c r="E153" s="31"/>
-      <c r="F153" s="52"/>
-      <c r="G153" s="32"/>
+      <c r="B153" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="C153" s="30" t="s">
+        <v>249</v>
+      </c>
+      <c r="D153" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="E153" s="31" t="s">
+        <v>248</v>
+      </c>
+      <c r="F153" s="52" t="s">
+        <v>250</v>
+      </c>
+      <c r="G153" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H153" s="33"/>
-      <c r="I153" s="34"/>
-      <c r="J153" s="48"/>
+      <c r="I153" s="34">
+        <v>293</v>
+      </c>
+      <c r="J153" s="48">
+        <v>310000000</v>
+      </c>
       <c r="K153" s="48"/>
-      <c r="L153" s="49"/>
+      <c r="L153" s="49" t="s">
+        <v>33</v>
+      </c>
       <c r="M153" s="49"/>
-      <c r="N153" s="30"/>
+      <c r="N153" s="30" t="s">
+        <v>244</v>
+      </c>
       <c r="O153" s="37"/>
       <c r="P153" s="38"/>
       <c r="Q153" s="38"/>
@@ -27351,11 +27458,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -27370,6 +27472,11 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
- parsed data from `10.1016/j.addma.2020.101832` and `10.1016/j.intermet.2019.106486`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Aug2025.xlsx
+++ b/MiscSmallUploads_Aug2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F525816F-C067-CD44-9B20-474F1DA3C2E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE67F77D-FF9E-DB40-BE87-6BDACCAD9CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="8020" windowWidth="34560" windowHeight="12760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1298" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1403" uniqueCount="262">
   <si>
     <r>
       <rPr>
@@ -883,6 +883,39 @@
   </si>
   <si>
     <t>fatigue limit</t>
+  </si>
+  <si>
+    <t>CoCrFeMnNi</t>
+  </si>
+  <si>
+    <t>SLM with 90W laser in Ar atmosphere with 0.6m/s scanning speed hatch distance of 80um and 25um layers for VED of 75 J/mm^3</t>
+  </si>
+  <si>
+    <t>SLM</t>
+  </si>
+  <si>
+    <t>10.1016/j.intermet.2019.106486</t>
+  </si>
+  <si>
+    <t>VIM+HR+H</t>
+  </si>
+  <si>
+    <t>hot rolled into a slab and homogenized at 1273K for 24h in Ar</t>
+  </si>
+  <si>
+    <t>hot rolled into a slab then homogenized at 1273K for 24h in Ar and underwent high cycle fatigue cold work of 10000 cycles under 300MPa stress</t>
+  </si>
+  <si>
+    <t>VIM+HR+H+CW</t>
+  </si>
+  <si>
+    <t>10.1016/j.addma.2020.101832</t>
+  </si>
+  <si>
+    <t>density</t>
+  </si>
+  <si>
+    <t>kg/m^3</t>
   </si>
 </sst>
 </file>
@@ -3375,8 +3408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T960"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A135" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L159" sqref="L159"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A145" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H169" sqref="H169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -9847,19 +9880,41 @@
     </row>
     <row r="154" spans="1:20" ht="18" customHeight="1">
       <c r="A154" s="50"/>
-      <c r="B154" s="31"/>
-      <c r="C154" s="30"/>
-      <c r="D154" s="30"/>
-      <c r="E154" s="31"/>
-      <c r="F154" s="52"/>
-      <c r="G154" s="32"/>
-      <c r="H154" s="33"/>
-      <c r="I154" s="34"/>
-      <c r="J154" s="48"/>
+      <c r="B154" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="C154" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D154" s="30" t="s">
+        <v>253</v>
+      </c>
+      <c r="E154" s="31" t="s">
+        <v>252</v>
+      </c>
+      <c r="F154" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="G154" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H154" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I154" s="34">
+        <v>298</v>
+      </c>
+      <c r="J154" s="48">
+        <v>774800000</v>
+      </c>
       <c r="K154" s="48"/>
-      <c r="L154" s="49"/>
+      <c r="L154" s="49" t="s">
+        <v>33</v>
+      </c>
       <c r="M154" s="49"/>
-      <c r="N154" s="30"/>
+      <c r="N154" s="30" t="s">
+        <v>259</v>
+      </c>
       <c r="O154" s="37"/>
       <c r="P154" s="38"/>
       <c r="Q154" s="38"/>
@@ -9869,19 +9924,41 @@
     </row>
     <row r="155" spans="1:20" ht="18" customHeight="1">
       <c r="A155" s="50"/>
-      <c r="B155" s="31"/>
-      <c r="C155" s="30"/>
-      <c r="D155" s="30"/>
-      <c r="E155" s="31"/>
-      <c r="F155" s="52"/>
-      <c r="G155" s="32"/>
-      <c r="H155" s="33"/>
-      <c r="I155" s="34"/>
-      <c r="J155" s="48"/>
+      <c r="B155" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="C155" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D155" s="30" t="s">
+        <v>255</v>
+      </c>
+      <c r="E155" s="31" t="s">
+        <v>256</v>
+      </c>
+      <c r="F155" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="G155" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H155" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I155" s="34">
+        <v>298</v>
+      </c>
+      <c r="J155" s="48">
+        <v>293100000</v>
+      </c>
       <c r="K155" s="48"/>
-      <c r="L155" s="49"/>
+      <c r="L155" s="49" t="s">
+        <v>33</v>
+      </c>
       <c r="M155" s="49"/>
-      <c r="N155" s="30"/>
+      <c r="N155" s="30" t="s">
+        <v>254</v>
+      </c>
       <c r="O155" s="37"/>
       <c r="P155" s="38"/>
       <c r="Q155" s="38"/>
@@ -9891,19 +9968,41 @@
     </row>
     <row r="156" spans="1:20" ht="18" customHeight="1">
       <c r="A156" s="50"/>
-      <c r="B156" s="31"/>
-      <c r="C156" s="30"/>
-      <c r="D156" s="30"/>
-      <c r="E156" s="31"/>
-      <c r="F156" s="52"/>
-      <c r="G156" s="32"/>
-      <c r="H156" s="33"/>
-      <c r="I156" s="34"/>
-      <c r="J156" s="48"/>
+      <c r="B156" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="C156" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D156" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="E156" s="31" t="s">
+        <v>257</v>
+      </c>
+      <c r="F156" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="G156" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H156" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I156" s="34">
+        <v>298</v>
+      </c>
+      <c r="J156" s="48">
+        <v>572300000</v>
+      </c>
       <c r="K156" s="38"/>
-      <c r="L156" s="49"/>
+      <c r="L156" s="49" t="s">
+        <v>33</v>
+      </c>
       <c r="M156" s="49"/>
-      <c r="N156" s="30"/>
+      <c r="N156" s="30" t="s">
+        <v>254</v>
+      </c>
       <c r="O156" s="37"/>
       <c r="P156" s="38"/>
       <c r="Q156" s="38"/>
@@ -9913,19 +10012,41 @@
     </row>
     <row r="157" spans="1:20" ht="18" customHeight="1">
       <c r="A157" s="50"/>
-      <c r="B157" s="31"/>
-      <c r="C157" s="30"/>
-      <c r="D157" s="30"/>
-      <c r="E157" s="31"/>
-      <c r="F157" s="52"/>
-      <c r="G157" s="32"/>
-      <c r="H157" s="33"/>
-      <c r="I157" s="34"/>
-      <c r="J157" s="48"/>
+      <c r="B157" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="C157" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D157" s="30" t="s">
+        <v>253</v>
+      </c>
+      <c r="E157" s="31" t="s">
+        <v>252</v>
+      </c>
+      <c r="F157" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="G157" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H157" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I157" s="34">
+        <v>298</v>
+      </c>
+      <c r="J157" s="48">
+        <v>923300000</v>
+      </c>
       <c r="K157" s="38"/>
-      <c r="L157" s="49"/>
+      <c r="L157" s="49" t="s">
+        <v>33</v>
+      </c>
       <c r="M157" s="49"/>
-      <c r="N157" s="30"/>
+      <c r="N157" s="30" t="s">
+        <v>259</v>
+      </c>
       <c r="O157" s="37"/>
       <c r="P157" s="39"/>
       <c r="Q157" s="38"/>
@@ -9935,19 +10056,41 @@
     </row>
     <row r="158" spans="1:20" ht="18" customHeight="1">
       <c r="A158" s="50"/>
-      <c r="B158" s="31"/>
-      <c r="C158" s="30"/>
-      <c r="D158" s="30"/>
-      <c r="E158" s="31"/>
-      <c r="F158" s="52"/>
-      <c r="G158" s="32"/>
-      <c r="H158" s="33"/>
-      <c r="I158" s="34"/>
-      <c r="J158" s="48"/>
+      <c r="B158" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="C158" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D158" s="30" t="s">
+        <v>255</v>
+      </c>
+      <c r="E158" s="31" t="s">
+        <v>256</v>
+      </c>
+      <c r="F158" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="G158" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H158" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I158" s="34">
+        <v>298</v>
+      </c>
+      <c r="J158" s="48">
+        <v>625000000</v>
+      </c>
       <c r="K158" s="38"/>
-      <c r="L158" s="49"/>
+      <c r="L158" s="49" t="s">
+        <v>33</v>
+      </c>
       <c r="M158" s="49"/>
-      <c r="N158" s="30"/>
+      <c r="N158" s="30" t="s">
+        <v>254</v>
+      </c>
       <c r="O158" s="37"/>
       <c r="P158" s="46"/>
       <c r="Q158" s="38"/>
@@ -9957,19 +10100,41 @@
     </row>
     <row r="159" spans="1:20" ht="18" customHeight="1">
       <c r="A159" s="50"/>
-      <c r="B159" s="31"/>
-      <c r="C159" s="30"/>
-      <c r="D159" s="30"/>
-      <c r="E159" s="31"/>
-      <c r="F159" s="52"/>
-      <c r="G159" s="32"/>
-      <c r="H159" s="33"/>
-      <c r="I159" s="34"/>
-      <c r="J159" s="48"/>
+      <c r="B159" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="C159" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D159" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="E159" s="31" t="s">
+        <v>257</v>
+      </c>
+      <c r="F159" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="G159" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H159" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I159" s="34">
+        <v>298</v>
+      </c>
+      <c r="J159" s="48">
+        <v>732800000</v>
+      </c>
       <c r="K159" s="38"/>
-      <c r="L159" s="49"/>
+      <c r="L159" s="49" t="s">
+        <v>33</v>
+      </c>
       <c r="M159" s="49"/>
-      <c r="N159" s="30"/>
+      <c r="N159" s="30" t="s">
+        <v>254</v>
+      </c>
       <c r="O159" s="37"/>
       <c r="P159" s="46"/>
       <c r="Q159" s="38"/>
@@ -9979,19 +10144,41 @@
     </row>
     <row r="160" spans="1:20" ht="18" customHeight="1">
       <c r="A160" s="50"/>
-      <c r="B160" s="31"/>
-      <c r="C160" s="30"/>
-      <c r="D160" s="30"/>
-      <c r="E160" s="31"/>
-      <c r="F160" s="52"/>
-      <c r="G160" s="32"/>
-      <c r="H160" s="33"/>
-      <c r="I160" s="34"/>
-      <c r="J160" s="48"/>
+      <c r="B160" s="102" t="s">
+        <v>251</v>
+      </c>
+      <c r="C160" s="90" t="s">
+        <v>63</v>
+      </c>
+      <c r="D160" s="90" t="s">
+        <v>253</v>
+      </c>
+      <c r="E160" s="103" t="s">
+        <v>252</v>
+      </c>
+      <c r="F160" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="G160" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H160" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I160" s="34">
+        <v>298</v>
+      </c>
+      <c r="J160" s="48">
+        <v>30.8</v>
+      </c>
       <c r="K160" s="38"/>
-      <c r="L160" s="49"/>
+      <c r="L160" s="49" t="s">
+        <v>68</v>
+      </c>
       <c r="M160" s="49"/>
-      <c r="N160" s="30"/>
+      <c r="N160" s="30" t="s">
+        <v>259</v>
+      </c>
       <c r="O160" s="37"/>
       <c r="P160" s="46"/>
       <c r="Q160" s="38"/>
@@ -10001,19 +10188,41 @@
     </row>
     <row r="161" spans="1:20" ht="18" customHeight="1">
       <c r="A161" s="50"/>
-      <c r="B161" s="31"/>
-      <c r="C161" s="30"/>
-      <c r="D161" s="30"/>
-      <c r="E161" s="31"/>
-      <c r="F161" s="52"/>
-      <c r="G161" s="32"/>
-      <c r="H161" s="33"/>
-      <c r="I161" s="34"/>
-      <c r="J161" s="48"/>
+      <c r="B161" s="104" t="s">
+        <v>251</v>
+      </c>
+      <c r="C161" s="91" t="s">
+        <v>63</v>
+      </c>
+      <c r="D161" s="91" t="s">
+        <v>255</v>
+      </c>
+      <c r="E161" s="105" t="s">
+        <v>256</v>
+      </c>
+      <c r="F161" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="G161" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H161" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I161" s="34">
+        <v>298</v>
+      </c>
+      <c r="J161" s="48">
+        <v>63.1</v>
+      </c>
       <c r="K161" s="51"/>
-      <c r="L161" s="49"/>
+      <c r="L161" s="49" t="s">
+        <v>68</v>
+      </c>
       <c r="M161" s="49"/>
-      <c r="N161" s="30"/>
+      <c r="N161" s="30" t="s">
+        <v>254</v>
+      </c>
       <c r="O161" s="37"/>
       <c r="P161" s="46"/>
       <c r="Q161" s="38"/>
@@ -10023,19 +10232,41 @@
     </row>
     <row r="162" spans="1:20" ht="18" customHeight="1">
       <c r="A162" s="50"/>
-      <c r="B162" s="31"/>
-      <c r="C162" s="30"/>
-      <c r="D162" s="30"/>
-      <c r="E162" s="31"/>
-      <c r="F162" s="52"/>
-      <c r="G162" s="32"/>
-      <c r="H162" s="33"/>
-      <c r="I162" s="34"/>
-      <c r="J162" s="48"/>
+      <c r="B162" s="104" t="s">
+        <v>251</v>
+      </c>
+      <c r="C162" s="91" t="s">
+        <v>63</v>
+      </c>
+      <c r="D162" s="91" t="s">
+        <v>258</v>
+      </c>
+      <c r="E162" s="105" t="s">
+        <v>257</v>
+      </c>
+      <c r="F162" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="G162" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H162" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I162" s="34">
+        <v>298</v>
+      </c>
+      <c r="J162" s="48">
+        <v>55</v>
+      </c>
       <c r="K162" s="51"/>
-      <c r="L162" s="49"/>
+      <c r="L162" s="49" t="s">
+        <v>68</v>
+      </c>
       <c r="M162" s="49"/>
-      <c r="N162" s="30"/>
+      <c r="N162" s="30" t="s">
+        <v>254</v>
+      </c>
       <c r="O162" s="37"/>
       <c r="P162" s="46"/>
       <c r="Q162" s="38"/>
@@ -10045,19 +10276,39 @@
     </row>
     <row r="163" spans="1:20" ht="18" customHeight="1">
       <c r="A163" s="50"/>
-      <c r="B163" s="31"/>
-      <c r="C163" s="30"/>
-      <c r="D163" s="30"/>
-      <c r="E163" s="31"/>
-      <c r="F163" s="52"/>
-      <c r="G163" s="32"/>
+      <c r="B163" s="102" t="s">
+        <v>251</v>
+      </c>
+      <c r="C163" s="90" t="s">
+        <v>63</v>
+      </c>
+      <c r="D163" s="90" t="s">
+        <v>253</v>
+      </c>
+      <c r="E163" s="103" t="s">
+        <v>252</v>
+      </c>
+      <c r="F163" s="52" t="s">
+        <v>250</v>
+      </c>
+      <c r="G163" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H163" s="33"/>
-      <c r="I163" s="34"/>
-      <c r="J163" s="48"/>
+      <c r="I163" s="34">
+        <v>298</v>
+      </c>
+      <c r="J163" s="48">
+        <v>570000000</v>
+      </c>
       <c r="K163" s="51"/>
-      <c r="L163" s="49"/>
+      <c r="L163" s="49" t="s">
+        <v>33</v>
+      </c>
       <c r="M163" s="49"/>
-      <c r="N163" s="30"/>
+      <c r="N163" s="30" t="s">
+        <v>259</v>
+      </c>
       <c r="O163" s="37"/>
       <c r="P163" s="46"/>
       <c r="Q163" s="38"/>
@@ -10067,19 +10318,39 @@
     </row>
     <row r="164" spans="1:20" ht="18" customHeight="1">
       <c r="A164" s="50"/>
-      <c r="B164" s="31"/>
-      <c r="C164" s="30"/>
-      <c r="D164" s="30"/>
-      <c r="E164" s="31"/>
-      <c r="F164" s="52"/>
-      <c r="G164" s="32"/>
+      <c r="B164" s="104" t="s">
+        <v>251</v>
+      </c>
+      <c r="C164" s="91" t="s">
+        <v>63</v>
+      </c>
+      <c r="D164" s="91" t="s">
+        <v>255</v>
+      </c>
+      <c r="E164" s="105" t="s">
+        <v>256</v>
+      </c>
+      <c r="F164" s="52" t="s">
+        <v>250</v>
+      </c>
+      <c r="G164" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H164" s="33"/>
-      <c r="I164" s="34"/>
-      <c r="J164" s="48"/>
+      <c r="I164" s="34">
+        <v>298</v>
+      </c>
+      <c r="J164" s="48">
+        <v>280000000</v>
+      </c>
       <c r="K164" s="51"/>
-      <c r="L164" s="49"/>
+      <c r="L164" s="49" t="s">
+        <v>33</v>
+      </c>
       <c r="M164" s="49"/>
-      <c r="N164" s="30"/>
+      <c r="N164" s="30" t="s">
+        <v>254</v>
+      </c>
       <c r="O164" s="37"/>
       <c r="P164" s="46"/>
       <c r="Q164" s="38"/>
@@ -10089,19 +10360,39 @@
     </row>
     <row r="165" spans="1:20" ht="18" customHeight="1">
       <c r="A165" s="50"/>
-      <c r="B165" s="31"/>
-      <c r="C165" s="30"/>
-      <c r="D165" s="30"/>
-      <c r="E165" s="31"/>
-      <c r="F165" s="52"/>
-      <c r="G165" s="32"/>
+      <c r="B165" s="104" t="s">
+        <v>251</v>
+      </c>
+      <c r="C165" s="91" t="s">
+        <v>63</v>
+      </c>
+      <c r="D165" s="91" t="s">
+        <v>255</v>
+      </c>
+      <c r="E165" s="105" t="s">
+        <v>256</v>
+      </c>
+      <c r="F165" s="52" t="s">
+        <v>260</v>
+      </c>
+      <c r="G165" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H165" s="33"/>
-      <c r="I165" s="34"/>
-      <c r="J165" s="48"/>
+      <c r="I165" s="34">
+        <v>298</v>
+      </c>
+      <c r="J165" s="48">
+        <v>7753</v>
+      </c>
       <c r="K165" s="38"/>
-      <c r="L165" s="49"/>
+      <c r="L165" s="49" t="s">
+        <v>261</v>
+      </c>
       <c r="M165" s="49"/>
-      <c r="N165" s="30"/>
+      <c r="N165" s="30" t="s">
+        <v>254</v>
+      </c>
       <c r="O165" s="37"/>
       <c r="P165" s="46"/>
       <c r="Q165" s="38"/>

</xml_diff>

<commit_message>
- parsed data from `10.1016/j.ijrmhm.2025.107379`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Aug2025.xlsx
+++ b/MiscSmallUploads_Aug2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE67F77D-FF9E-DB40-BE87-6BDACCAD9CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C69DC30-6A10-0947-BF3F-0DD07090A0F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="8020" windowWidth="34560" windowHeight="12760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1403" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1695" uniqueCount="276">
   <si>
     <r>
       <rPr>
@@ -916,6 +916,48 @@
   </si>
   <si>
     <t>kg/m^3</t>
+  </si>
+  <si>
+    <t>(Ti0.25Zr0.25Hf0.25Nb0.25)95 Al5</t>
+  </si>
+  <si>
+    <t>(Ti0.25Zr0.25Hf0.25Nb0.25)90 Al10</t>
+  </si>
+  <si>
+    <t>(Ti0.25Zr0.25Hf0.25Nb0.25)85 Al15</t>
+  </si>
+  <si>
+    <t>(Ti0.25Zr0.25Hf0.25Nb0.25)80 Al20</t>
+  </si>
+  <si>
+    <t>Al5</t>
+  </si>
+  <si>
+    <t>Al10</t>
+  </si>
+  <si>
+    <t>Al15</t>
+  </si>
+  <si>
+    <t>Al20</t>
+  </si>
+  <si>
+    <t>large arc melted 100g buttons remelted 10 times</t>
+  </si>
+  <si>
+    <t>compressive ductility</t>
+  </si>
+  <si>
+    <t>minimum compressive ductility</t>
+  </si>
+  <si>
+    <t>minimum UCS</t>
+  </si>
+  <si>
+    <t>UCS</t>
+  </si>
+  <si>
+    <t>10.1016/j.ijrmhm.2025.107379</t>
   </si>
 </sst>
 </file>
@@ -1938,7 +1980,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2135,57 +2177,6 @@
     <xf numFmtId="0" fontId="15" fillId="10" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2246,6 +2237,65 @@
     <xf numFmtId="164" fontId="5" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="10" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="10" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="14" fillId="10" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="10" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3408,8 +3458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T960"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A145" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H169" sqref="H169"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A172" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O183" sqref="O183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -3466,19 +3516,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" s="129" t="s">
+      <c r="D2" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="130"/>
-      <c r="F2" s="133"/>
-      <c r="G2" s="134"/>
-      <c r="H2" s="134"/>
-      <c r="I2" s="135"/>
-      <c r="J2" s="136"/>
-      <c r="K2" s="136"/>
-      <c r="L2" s="134"/>
-      <c r="M2" s="134"/>
-      <c r="N2" s="137"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="119"/>
+      <c r="K2" s="119"/>
+      <c r="L2" s="117"/>
+      <c r="M2" s="117"/>
+      <c r="N2" s="120"/>
       <c r="O2" s="13"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -3494,17 +3544,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="131"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="138"/>
-      <c r="G3" s="138"/>
-      <c r="H3" s="138"/>
-      <c r="I3" s="139"/>
-      <c r="J3" s="140"/>
-      <c r="K3" s="140"/>
-      <c r="L3" s="138"/>
-      <c r="M3" s="138"/>
-      <c r="N3" s="141"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="121"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="121"/>
+      <c r="I3" s="122"/>
+      <c r="J3" s="123"/>
+      <c r="K3" s="123"/>
+      <c r="L3" s="121"/>
+      <c r="M3" s="121"/>
+      <c r="N3" s="124"/>
       <c r="O3" s="13"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -3545,43 +3595,43 @@
       <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="142" t="s">
+      <c r="C5" s="125" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="144" t="s">
+      <c r="D5" s="127" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="144" t="s">
+      <c r="E5" s="127" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="144" t="s">
+      <c r="F5" s="127" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="144" t="s">
+      <c r="G5" s="127" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="145" t="s">
+      <c r="H5" s="128" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="144" t="s">
+      <c r="I5" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="144" t="s">
+      <c r="J5" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="144" t="s">
+      <c r="K5" s="127" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="144" t="s">
+      <c r="L5" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="144" t="s">
+      <c r="M5" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="144" t="s">
+      <c r="N5" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="112" t="s">
+      <c r="O5" s="132" t="s">
         <v>20</v>
       </c>
       <c r="P5" s="25"/>
@@ -3597,19 +3647,19 @@
       <c r="B6" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="143"/>
-      <c r="D6" s="143"/>
-      <c r="E6" s="143"/>
-      <c r="F6" s="143"/>
-      <c r="G6" s="143"/>
-      <c r="H6" s="146"/>
-      <c r="I6" s="147"/>
-      <c r="J6" s="148"/>
-      <c r="K6" s="148"/>
-      <c r="L6" s="143"/>
-      <c r="M6" s="143"/>
-      <c r="N6" s="143"/>
-      <c r="O6" s="113"/>
+      <c r="C6" s="126"/>
+      <c r="D6" s="126"/>
+      <c r="E6" s="126"/>
+      <c r="F6" s="126"/>
+      <c r="G6" s="126"/>
+      <c r="H6" s="129"/>
+      <c r="I6" s="130"/>
+      <c r="J6" s="131"/>
+      <c r="K6" s="131"/>
+      <c r="L6" s="126"/>
+      <c r="M6" s="126"/>
+      <c r="N6" s="126"/>
+      <c r="O6" s="133"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="9"/>
@@ -3659,7 +3709,7 @@
       <c r="N7" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="114"/>
+      <c r="O7" s="134"/>
       <c r="P7" s="64" t="s">
         <v>62</v>
       </c>
@@ -3674,35 +3724,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" thickBot="1">
       <c r="A8" s="59"/>
-      <c r="B8" s="115" t="s">
+      <c r="B8" s="135" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="116"/>
-      <c r="D8" s="116"/>
-      <c r="E8" s="117"/>
-      <c r="F8" s="118" t="s">
+      <c r="C8" s="136"/>
+      <c r="D8" s="136"/>
+      <c r="E8" s="137"/>
+      <c r="F8" s="138" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="119"/>
-      <c r="H8" s="119"/>
-      <c r="I8" s="120"/>
-      <c r="J8" s="121"/>
-      <c r="K8" s="121"/>
-      <c r="L8" s="122"/>
-      <c r="M8" s="123" t="s">
+      <c r="G8" s="139"/>
+      <c r="H8" s="139"/>
+      <c r="I8" s="140"/>
+      <c r="J8" s="141"/>
+      <c r="K8" s="141"/>
+      <c r="L8" s="142"/>
+      <c r="M8" s="143" t="s">
         <v>40</v>
       </c>
-      <c r="N8" s="124"/>
+      <c r="N8" s="144"/>
       <c r="O8" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="P8" s="125" t="s">
+      <c r="P8" s="145" t="s">
         <v>42</v>
       </c>
-      <c r="Q8" s="126"/>
-      <c r="R8" s="127"/>
-      <c r="S8" s="127"/>
-      <c r="T8" s="128"/>
+      <c r="Q8" s="146"/>
+      <c r="R8" s="147"/>
+      <c r="S8" s="147"/>
+      <c r="T8" s="148"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1">
       <c r="A9" s="60" t="s">
@@ -10401,108 +10451,242 @@
       <c r="T165" s="37"/>
     </row>
     <row r="166" spans="1:20" ht="18" customHeight="1">
-      <c r="A166" s="50"/>
-      <c r="B166" s="31"/>
-      <c r="C166" s="30"/>
-      <c r="D166" s="30"/>
-      <c r="E166" s="31"/>
-      <c r="F166" s="52"/>
-      <c r="G166" s="32"/>
+      <c r="A166" s="50" t="s">
+        <v>266</v>
+      </c>
+      <c r="B166" s="31" t="s">
+        <v>262</v>
+      </c>
+      <c r="C166" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="D166" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E166" s="31" t="s">
+        <v>270</v>
+      </c>
+      <c r="F166" s="52" t="s">
+        <v>179</v>
+      </c>
+      <c r="G166" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H166" s="33"/>
-      <c r="I166" s="34"/>
-      <c r="J166" s="48"/>
+      <c r="I166" s="34">
+        <v>298</v>
+      </c>
+      <c r="J166" s="35">
+        <f t="shared" ref="J166:J169" si="3">P166*9807000</f>
+        <v>2844030000</v>
+      </c>
       <c r="K166" s="38"/>
-      <c r="L166" s="49"/>
-      <c r="M166" s="49"/>
-      <c r="N166" s="30"/>
+      <c r="L166" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="M166" s="49" t="s">
+        <v>170</v>
+      </c>
+      <c r="N166" s="30" t="s">
+        <v>275</v>
+      </c>
       <c r="O166" s="37"/>
-      <c r="P166" s="46"/>
+      <c r="P166" s="46">
+        <v>290</v>
+      </c>
       <c r="Q166" s="38"/>
       <c r="R166" s="37"/>
       <c r="S166" s="37"/>
       <c r="T166" s="37"/>
     </row>
     <row r="167" spans="1:20" ht="18" customHeight="1">
-      <c r="A167" s="50"/>
-      <c r="B167" s="31"/>
-      <c r="C167" s="30"/>
-      <c r="D167" s="30"/>
-      <c r="E167" s="31"/>
-      <c r="F167" s="52"/>
-      <c r="G167" s="32"/>
+      <c r="A167" s="50" t="s">
+        <v>267</v>
+      </c>
+      <c r="B167" s="31" t="s">
+        <v>263</v>
+      </c>
+      <c r="C167" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="D167" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E167" s="31" t="s">
+        <v>270</v>
+      </c>
+      <c r="F167" s="52" t="s">
+        <v>179</v>
+      </c>
+      <c r="G167" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H167" s="33"/>
-      <c r="I167" s="34"/>
-      <c r="J167" s="48"/>
+      <c r="I167" s="34">
+        <v>298</v>
+      </c>
+      <c r="J167" s="35">
+        <f t="shared" si="3"/>
+        <v>3275538000</v>
+      </c>
       <c r="K167" s="38"/>
-      <c r="L167" s="49"/>
-      <c r="M167" s="49"/>
-      <c r="N167" s="30"/>
+      <c r="L167" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="M167" s="49" t="s">
+        <v>170</v>
+      </c>
+      <c r="N167" s="30" t="s">
+        <v>275</v>
+      </c>
       <c r="O167" s="37"/>
-      <c r="P167" s="38"/>
+      <c r="P167" s="38">
+        <v>334</v>
+      </c>
       <c r="Q167" s="38"/>
       <c r="R167" s="37"/>
       <c r="S167" s="37"/>
       <c r="T167" s="37"/>
     </row>
     <row r="168" spans="1:20" ht="18" customHeight="1">
-      <c r="A168" s="50"/>
-      <c r="B168" s="31"/>
-      <c r="C168" s="30"/>
-      <c r="D168" s="30"/>
-      <c r="E168" s="31"/>
-      <c r="F168" s="52"/>
-      <c r="G168" s="32"/>
+      <c r="A168" s="50" t="s">
+        <v>268</v>
+      </c>
+      <c r="B168" s="31" t="s">
+        <v>264</v>
+      </c>
+      <c r="C168" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="D168" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E168" s="31" t="s">
+        <v>270</v>
+      </c>
+      <c r="F168" s="52" t="s">
+        <v>179</v>
+      </c>
+      <c r="G168" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H168" s="33"/>
-      <c r="I168" s="34"/>
-      <c r="J168" s="48"/>
+      <c r="I168" s="34">
+        <v>298</v>
+      </c>
+      <c r="J168" s="35">
+        <f t="shared" si="3"/>
+        <v>3863958000</v>
+      </c>
       <c r="K168" s="38"/>
-      <c r="L168" s="49"/>
-      <c r="M168" s="49"/>
-      <c r="N168" s="30"/>
+      <c r="L168" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="M168" s="49" t="s">
+        <v>170</v>
+      </c>
+      <c r="N168" s="30" t="s">
+        <v>275</v>
+      </c>
       <c r="O168" s="37"/>
-      <c r="P168" s="38"/>
+      <c r="P168" s="38">
+        <v>394</v>
+      </c>
       <c r="Q168" s="38"/>
       <c r="R168" s="37"/>
       <c r="S168" s="37"/>
       <c r="T168" s="37"/>
     </row>
     <row r="169" spans="1:20" ht="18" customHeight="1">
-      <c r="A169" s="50"/>
-      <c r="B169" s="31"/>
-      <c r="C169" s="30"/>
-      <c r="D169" s="30"/>
-      <c r="E169" s="31"/>
-      <c r="F169" s="52"/>
-      <c r="G169" s="32"/>
+      <c r="A169" s="50" t="s">
+        <v>269</v>
+      </c>
+      <c r="B169" s="31" t="s">
+        <v>265</v>
+      </c>
+      <c r="C169" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="D169" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E169" s="31" t="s">
+        <v>270</v>
+      </c>
+      <c r="F169" s="52" t="s">
+        <v>179</v>
+      </c>
+      <c r="G169" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H169" s="33"/>
-      <c r="I169" s="34"/>
-      <c r="J169" s="48"/>
+      <c r="I169" s="34">
+        <v>298</v>
+      </c>
+      <c r="J169" s="35">
+        <f t="shared" si="3"/>
+        <v>4256238000</v>
+      </c>
       <c r="K169" s="38"/>
-      <c r="L169" s="49"/>
-      <c r="M169" s="49"/>
-      <c r="N169" s="30"/>
+      <c r="L169" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="M169" s="49" t="s">
+        <v>170</v>
+      </c>
+      <c r="N169" s="30" t="s">
+        <v>275</v>
+      </c>
       <c r="O169" s="37"/>
-      <c r="P169" s="38"/>
+      <c r="P169" s="38">
+        <v>434</v>
+      </c>
       <c r="Q169" s="38"/>
       <c r="R169" s="37"/>
       <c r="S169" s="37"/>
       <c r="T169" s="37"/>
     </row>
     <row r="170" spans="1:20" ht="18" customHeight="1">
-      <c r="A170" s="50"/>
-      <c r="B170" s="31"/>
-      <c r="C170" s="30"/>
-      <c r="D170" s="30"/>
-      <c r="E170" s="31"/>
-      <c r="F170" s="52"/>
-      <c r="G170" s="32"/>
-      <c r="H170" s="33"/>
-      <c r="I170" s="34"/>
-      <c r="J170" s="48"/>
+      <c r="A170" s="50" t="s">
+        <v>266</v>
+      </c>
+      <c r="B170" s="31" t="s">
+        <v>262</v>
+      </c>
+      <c r="C170" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="D170" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E170" s="31" t="s">
+        <v>270</v>
+      </c>
+      <c r="F170" s="52" t="s">
+        <v>194</v>
+      </c>
+      <c r="G170" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H170" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I170" s="34">
+        <v>298</v>
+      </c>
+      <c r="J170" s="48">
+        <v>1073000000</v>
+      </c>
       <c r="K170" s="38"/>
-      <c r="L170" s="49"/>
-      <c r="M170" s="49"/>
-      <c r="N170" s="30"/>
+      <c r="L170" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="M170" s="49" t="s">
+        <v>170</v>
+      </c>
+      <c r="N170" s="30" t="s">
+        <v>275</v>
+      </c>
       <c r="O170" s="37"/>
       <c r="P170" s="38"/>
       <c r="Q170" s="38"/>
@@ -10511,20 +10695,46 @@
       <c r="T170" s="37"/>
     </row>
     <row r="171" spans="1:20" ht="18" customHeight="1">
-      <c r="A171" s="50"/>
-      <c r="B171" s="31"/>
-      <c r="C171" s="30"/>
-      <c r="D171" s="30"/>
-      <c r="E171" s="31"/>
-      <c r="F171" s="52"/>
-      <c r="G171" s="32"/>
-      <c r="H171" s="33"/>
-      <c r="I171" s="34"/>
-      <c r="J171" s="48"/>
+      <c r="A171" s="50" t="s">
+        <v>267</v>
+      </c>
+      <c r="B171" s="31" t="s">
+        <v>263</v>
+      </c>
+      <c r="C171" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="D171" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E171" s="31" t="s">
+        <v>270</v>
+      </c>
+      <c r="F171" s="52" t="s">
+        <v>194</v>
+      </c>
+      <c r="G171" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H171" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I171" s="34">
+        <v>298</v>
+      </c>
+      <c r="J171" s="48">
+        <v>1198000000</v>
+      </c>
       <c r="K171" s="38"/>
-      <c r="L171" s="49"/>
-      <c r="M171" s="49"/>
-      <c r="N171" s="30"/>
+      <c r="L171" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="M171" s="49" t="s">
+        <v>170</v>
+      </c>
+      <c r="N171" s="30" t="s">
+        <v>275</v>
+      </c>
       <c r="O171" s="37"/>
       <c r="P171" s="38"/>
       <c r="Q171" s="38"/>
@@ -10533,20 +10743,46 @@
       <c r="T171" s="37"/>
     </row>
     <row r="172" spans="1:20" ht="18" customHeight="1">
-      <c r="A172" s="50"/>
-      <c r="B172" s="31"/>
-      <c r="C172" s="30"/>
-      <c r="D172" s="30"/>
-      <c r="E172" s="31"/>
-      <c r="F172" s="52"/>
-      <c r="G172" s="32"/>
-      <c r="H172" s="33"/>
-      <c r="I172" s="34"/>
-      <c r="J172" s="48"/>
+      <c r="A172" s="50" t="s">
+        <v>268</v>
+      </c>
+      <c r="B172" s="31" t="s">
+        <v>264</v>
+      </c>
+      <c r="C172" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="D172" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E172" s="31" t="s">
+        <v>270</v>
+      </c>
+      <c r="F172" s="52" t="s">
+        <v>194</v>
+      </c>
+      <c r="G172" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H172" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I172" s="34">
+        <v>298</v>
+      </c>
+      <c r="J172" s="48">
+        <v>1424000000</v>
+      </c>
       <c r="K172" s="38"/>
-      <c r="L172" s="49"/>
-      <c r="M172" s="49"/>
-      <c r="N172" s="30"/>
+      <c r="L172" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="M172" s="49" t="s">
+        <v>170</v>
+      </c>
+      <c r="N172" s="30" t="s">
+        <v>275</v>
+      </c>
       <c r="O172" s="37"/>
       <c r="P172" s="38"/>
       <c r="Q172" s="38"/>
@@ -10555,20 +10791,46 @@
       <c r="T172" s="37"/>
     </row>
     <row r="173" spans="1:20" ht="18" customHeight="1">
-      <c r="A173" s="50"/>
-      <c r="B173" s="31"/>
-      <c r="C173" s="30"/>
-      <c r="D173" s="30"/>
-      <c r="E173" s="31"/>
-      <c r="F173" s="52"/>
-      <c r="G173" s="32"/>
-      <c r="H173" s="33"/>
-      <c r="I173" s="34"/>
-      <c r="J173" s="48"/>
+      <c r="A173" s="50" t="s">
+        <v>269</v>
+      </c>
+      <c r="B173" s="31" t="s">
+        <v>265</v>
+      </c>
+      <c r="C173" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="D173" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E173" s="31" t="s">
+        <v>270</v>
+      </c>
+      <c r="F173" s="52" t="s">
+        <v>194</v>
+      </c>
+      <c r="G173" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H173" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I173" s="34">
+        <v>298</v>
+      </c>
+      <c r="J173" s="48">
+        <v>1773000000</v>
+      </c>
       <c r="K173" s="38"/>
-      <c r="L173" s="49"/>
-      <c r="M173" s="49"/>
-      <c r="N173" s="30"/>
+      <c r="L173" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="M173" s="49" t="s">
+        <v>170</v>
+      </c>
+      <c r="N173" s="30" t="s">
+        <v>275</v>
+      </c>
       <c r="O173" s="37"/>
       <c r="P173" s="38"/>
       <c r="Q173" s="38"/>
@@ -10577,20 +10839,46 @@
       <c r="T173" s="37"/>
     </row>
     <row r="174" spans="1:20" ht="18" customHeight="1">
-      <c r="A174" s="50"/>
-      <c r="B174" s="31"/>
-      <c r="C174" s="30"/>
-      <c r="D174" s="30"/>
-      <c r="E174" s="31"/>
-      <c r="F174" s="52"/>
-      <c r="G174" s="32"/>
-      <c r="H174" s="33"/>
-      <c r="I174" s="34"/>
-      <c r="J174" s="48"/>
+      <c r="A174" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="B174" s="103" t="s">
+        <v>262</v>
+      </c>
+      <c r="C174" s="90" t="s">
+        <v>160</v>
+      </c>
+      <c r="D174" s="90" t="s">
+        <v>64</v>
+      </c>
+      <c r="E174" s="103" t="s">
+        <v>270</v>
+      </c>
+      <c r="F174" s="97" t="s">
+        <v>272</v>
+      </c>
+      <c r="G174" s="97" t="s">
+        <v>29</v>
+      </c>
+      <c r="H174" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I174" s="150">
+        <v>298</v>
+      </c>
+      <c r="J174" s="48">
+        <v>50</v>
+      </c>
       <c r="K174" s="38"/>
-      <c r="L174" s="49"/>
-      <c r="M174" s="49"/>
-      <c r="N174" s="30"/>
+      <c r="L174" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="M174" s="49" t="s">
+        <v>170</v>
+      </c>
+      <c r="N174" s="30" t="s">
+        <v>275</v>
+      </c>
       <c r="O174" s="37"/>
       <c r="P174" s="38"/>
       <c r="Q174" s="38"/>
@@ -10599,20 +10887,46 @@
       <c r="T174" s="37"/>
     </row>
     <row r="175" spans="1:20" ht="18" customHeight="1">
-      <c r="A175" s="50"/>
-      <c r="B175" s="31"/>
-      <c r="C175" s="30"/>
-      <c r="D175" s="30"/>
-      <c r="E175" s="31"/>
-      <c r="F175" s="52"/>
-      <c r="G175" s="32"/>
-      <c r="H175" s="33"/>
-      <c r="I175" s="34"/>
-      <c r="J175" s="48"/>
+      <c r="A175" s="151" t="s">
+        <v>267</v>
+      </c>
+      <c r="B175" s="105" t="s">
+        <v>263</v>
+      </c>
+      <c r="C175" s="91" t="s">
+        <v>160</v>
+      </c>
+      <c r="D175" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="E175" s="105" t="s">
+        <v>270</v>
+      </c>
+      <c r="F175" s="97" t="s">
+        <v>272</v>
+      </c>
+      <c r="G175" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="H175" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I175" s="152">
+        <v>298</v>
+      </c>
+      <c r="J175" s="48">
+        <v>50</v>
+      </c>
       <c r="K175" s="38"/>
-      <c r="L175" s="49"/>
-      <c r="M175" s="49"/>
-      <c r="N175" s="30"/>
+      <c r="L175" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="M175" s="49" t="s">
+        <v>170</v>
+      </c>
+      <c r="N175" s="30" t="s">
+        <v>275</v>
+      </c>
       <c r="O175" s="37"/>
       <c r="P175" s="38"/>
       <c r="Q175" s="38"/>
@@ -10621,20 +10935,46 @@
       <c r="T175" s="37"/>
     </row>
     <row r="176" spans="1:20" ht="18" customHeight="1">
-      <c r="A176" s="50"/>
-      <c r="B176" s="31"/>
-      <c r="C176" s="30"/>
-      <c r="D176" s="30"/>
-      <c r="E176" s="31"/>
-      <c r="F176" s="52"/>
-      <c r="G176" s="32"/>
-      <c r="H176" s="33"/>
-      <c r="I176" s="34"/>
-      <c r="J176" s="48"/>
+      <c r="A176" s="151" t="s">
+        <v>268</v>
+      </c>
+      <c r="B176" s="105" t="s">
+        <v>264</v>
+      </c>
+      <c r="C176" s="91" t="s">
+        <v>160</v>
+      </c>
+      <c r="D176" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="E176" s="105" t="s">
+        <v>270</v>
+      </c>
+      <c r="F176" s="97" t="s">
+        <v>272</v>
+      </c>
+      <c r="G176" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="H176" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I176" s="152">
+        <v>298</v>
+      </c>
+      <c r="J176" s="48">
+        <v>50</v>
+      </c>
       <c r="K176" s="38"/>
-      <c r="L176" s="49"/>
-      <c r="M176" s="49"/>
-      <c r="N176" s="30"/>
+      <c r="L176" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="M176" s="49" t="s">
+        <v>170</v>
+      </c>
+      <c r="N176" s="30" t="s">
+        <v>275</v>
+      </c>
       <c r="O176" s="37"/>
       <c r="P176" s="38"/>
       <c r="Q176" s="38"/>
@@ -10643,20 +10983,46 @@
       <c r="T176" s="37"/>
     </row>
     <row r="177" spans="1:20" ht="18" customHeight="1">
-      <c r="A177" s="50"/>
-      <c r="B177" s="31"/>
-      <c r="C177" s="30"/>
-      <c r="D177" s="30"/>
-      <c r="E177" s="31"/>
-      <c r="F177" s="52"/>
-      <c r="G177" s="32"/>
-      <c r="H177" s="56"/>
-      <c r="I177" s="54"/>
-      <c r="J177" s="35"/>
+      <c r="A177" s="151" t="s">
+        <v>269</v>
+      </c>
+      <c r="B177" s="105" t="s">
+        <v>265</v>
+      </c>
+      <c r="C177" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="D177" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="E177" s="105" t="s">
+        <v>270</v>
+      </c>
+      <c r="F177" s="97" t="s">
+        <v>271</v>
+      </c>
+      <c r="G177" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="H177" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I177" s="152">
+        <v>298</v>
+      </c>
+      <c r="J177" s="35">
+        <v>28</v>
+      </c>
       <c r="K177" s="38"/>
-      <c r="L177" s="49"/>
-      <c r="M177" s="49"/>
-      <c r="N177" s="30"/>
+      <c r="L177" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="M177" s="49" t="s">
+        <v>170</v>
+      </c>
+      <c r="N177" s="30" t="s">
+        <v>275</v>
+      </c>
       <c r="O177" s="37"/>
       <c r="P177" s="38"/>
       <c r="Q177" s="38"/>
@@ -10665,20 +11031,46 @@
       <c r="T177" s="37"/>
     </row>
     <row r="178" spans="1:20" ht="18" customHeight="1">
-      <c r="A178" s="50"/>
-      <c r="B178" s="31"/>
-      <c r="C178" s="30"/>
-      <c r="D178" s="30"/>
-      <c r="E178" s="31"/>
-      <c r="F178" s="52"/>
-      <c r="G178" s="32"/>
-      <c r="H178" s="56"/>
-      <c r="I178" s="54"/>
-      <c r="J178" s="35"/>
+      <c r="A178" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="B178" s="103" t="s">
+        <v>262</v>
+      </c>
+      <c r="C178" s="90" t="s">
+        <v>160</v>
+      </c>
+      <c r="D178" s="90" t="s">
+        <v>64</v>
+      </c>
+      <c r="E178" s="103" t="s">
+        <v>270</v>
+      </c>
+      <c r="F178" s="97" t="s">
+        <v>273</v>
+      </c>
+      <c r="G178" s="97" t="s">
+        <v>29</v>
+      </c>
+      <c r="H178" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I178" s="150">
+        <v>298</v>
+      </c>
+      <c r="J178" s="35">
+        <v>5900000000</v>
+      </c>
       <c r="K178" s="38"/>
-      <c r="L178" s="49"/>
-      <c r="M178" s="49"/>
-      <c r="N178" s="30"/>
+      <c r="L178" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="M178" s="49" t="s">
+        <v>170</v>
+      </c>
+      <c r="N178" s="30" t="s">
+        <v>275</v>
+      </c>
       <c r="O178" s="37"/>
       <c r="P178" s="38"/>
       <c r="Q178" s="38"/>
@@ -10687,20 +11079,46 @@
       <c r="T178" s="37"/>
     </row>
     <row r="179" spans="1:20" ht="18" customHeight="1">
-      <c r="A179" s="50"/>
-      <c r="B179" s="31"/>
-      <c r="C179" s="30"/>
-      <c r="D179" s="30"/>
-      <c r="E179" s="31"/>
-      <c r="F179" s="52"/>
-      <c r="G179" s="32"/>
-      <c r="H179" s="47"/>
-      <c r="I179" s="54"/>
-      <c r="J179" s="35"/>
+      <c r="A179" s="151" t="s">
+        <v>267</v>
+      </c>
+      <c r="B179" s="105" t="s">
+        <v>263</v>
+      </c>
+      <c r="C179" s="91" t="s">
+        <v>160</v>
+      </c>
+      <c r="D179" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="E179" s="105" t="s">
+        <v>270</v>
+      </c>
+      <c r="F179" s="97" t="s">
+        <v>273</v>
+      </c>
+      <c r="G179" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="H179" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I179" s="152">
+        <v>298</v>
+      </c>
+      <c r="J179" s="35">
+        <v>6100000000</v>
+      </c>
       <c r="K179" s="38"/>
-      <c r="L179" s="49"/>
-      <c r="M179" s="49"/>
-      <c r="N179" s="30"/>
+      <c r="L179" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="M179" s="49" t="s">
+        <v>170</v>
+      </c>
+      <c r="N179" s="30" t="s">
+        <v>275</v>
+      </c>
       <c r="O179" s="37"/>
       <c r="P179" s="38"/>
       <c r="Q179" s="38"/>
@@ -10709,20 +11127,46 @@
       <c r="T179" s="37"/>
     </row>
     <row r="180" spans="1:20" ht="18" customHeight="1">
-      <c r="A180" s="50"/>
-      <c r="B180" s="31"/>
-      <c r="C180" s="30"/>
-      <c r="D180" s="30"/>
-      <c r="E180" s="31"/>
-      <c r="F180" s="52"/>
-      <c r="G180" s="32"/>
-      <c r="H180" s="47"/>
-      <c r="I180" s="54"/>
-      <c r="J180" s="35"/>
+      <c r="A180" s="151" t="s">
+        <v>268</v>
+      </c>
+      <c r="B180" s="105" t="s">
+        <v>264</v>
+      </c>
+      <c r="C180" s="91" t="s">
+        <v>160</v>
+      </c>
+      <c r="D180" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="E180" s="105" t="s">
+        <v>270</v>
+      </c>
+      <c r="F180" s="97" t="s">
+        <v>273</v>
+      </c>
+      <c r="G180" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="H180" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I180" s="152">
+        <v>298</v>
+      </c>
+      <c r="J180" s="35">
+        <v>6600000000</v>
+      </c>
       <c r="K180" s="38"/>
-      <c r="L180" s="49"/>
-      <c r="M180" s="49"/>
-      <c r="N180" s="30"/>
+      <c r="L180" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="M180" s="49" t="s">
+        <v>170</v>
+      </c>
+      <c r="N180" s="30" t="s">
+        <v>275</v>
+      </c>
       <c r="O180" s="37"/>
       <c r="P180" s="37"/>
       <c r="Q180" s="38"/>
@@ -10731,20 +11175,46 @@
       <c r="T180" s="37"/>
     </row>
     <row r="181" spans="1:20" ht="18" customHeight="1">
-      <c r="A181" s="40"/>
-      <c r="B181" s="31"/>
-      <c r="C181" s="30"/>
-      <c r="D181" s="30"/>
-      <c r="E181" s="31"/>
-      <c r="F181" s="52"/>
-      <c r="G181" s="32"/>
-      <c r="H181" s="56"/>
-      <c r="I181" s="54"/>
-      <c r="J181" s="48"/>
+      <c r="A181" s="151" t="s">
+        <v>269</v>
+      </c>
+      <c r="B181" s="105" t="s">
+        <v>265</v>
+      </c>
+      <c r="C181" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="D181" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="E181" s="105" t="s">
+        <v>270</v>
+      </c>
+      <c r="F181" s="97" t="s">
+        <v>274</v>
+      </c>
+      <c r="G181" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="H181" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="I181" s="152">
+        <v>298</v>
+      </c>
+      <c r="J181" s="35">
+        <v>1881000000</v>
+      </c>
       <c r="K181" s="38"/>
-      <c r="L181" s="49"/>
-      <c r="M181" s="49"/>
-      <c r="N181" s="30"/>
+      <c r="L181" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="M181" s="49" t="s">
+        <v>170</v>
+      </c>
+      <c r="N181" s="30" t="s">
+        <v>275</v>
+      </c>
       <c r="O181" s="37"/>
       <c r="P181" s="37"/>
       <c r="Q181" s="38"/>
@@ -10753,20 +11223,44 @@
       <c r="T181" s="37"/>
     </row>
     <row r="182" spans="1:20" ht="18" customHeight="1">
-      <c r="A182" s="40"/>
-      <c r="B182" s="31"/>
-      <c r="C182" s="30"/>
-      <c r="D182" s="30"/>
-      <c r="E182" s="31"/>
-      <c r="F182" s="52"/>
-      <c r="G182" s="32"/>
+      <c r="A182" s="50" t="s">
+        <v>266</v>
+      </c>
+      <c r="B182" s="31" t="s">
+        <v>262</v>
+      </c>
+      <c r="C182" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="D182" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E182" s="31" t="s">
+        <v>270</v>
+      </c>
+      <c r="F182" s="52" t="s">
+        <v>194</v>
+      </c>
+      <c r="G182" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H182" s="56"/>
-      <c r="I182" s="54"/>
-      <c r="J182" s="51"/>
+      <c r="I182" s="54">
+        <v>1273</v>
+      </c>
+      <c r="J182" s="51">
+        <v>55000000</v>
+      </c>
       <c r="K182" s="38"/>
-      <c r="L182" s="49"/>
-      <c r="M182" s="49"/>
-      <c r="N182" s="30"/>
+      <c r="L182" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="M182" s="49" t="s">
+        <v>196</v>
+      </c>
+      <c r="N182" s="30" t="s">
+        <v>275</v>
+      </c>
       <c r="O182" s="37"/>
       <c r="P182" s="37"/>
       <c r="Q182" s="38"/>
@@ -10775,20 +11269,44 @@
       <c r="T182" s="37"/>
     </row>
     <row r="183" spans="1:20" ht="18" customHeight="1">
-      <c r="A183" s="40"/>
-      <c r="B183" s="31"/>
-      <c r="C183" s="30"/>
-      <c r="D183" s="30"/>
-      <c r="E183" s="31"/>
-      <c r="F183" s="52"/>
-      <c r="G183" s="32"/>
+      <c r="A183" s="50" t="s">
+        <v>267</v>
+      </c>
+      <c r="B183" s="31" t="s">
+        <v>263</v>
+      </c>
+      <c r="C183" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="D183" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E183" s="31" t="s">
+        <v>270</v>
+      </c>
+      <c r="F183" s="52" t="s">
+        <v>194</v>
+      </c>
+      <c r="G183" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H183" s="56"/>
-      <c r="I183" s="54"/>
-      <c r="J183" s="51"/>
+      <c r="I183" s="54">
+        <v>1273</v>
+      </c>
+      <c r="J183" s="51">
+        <v>48000000</v>
+      </c>
       <c r="K183" s="38"/>
-      <c r="L183" s="49"/>
-      <c r="M183" s="49"/>
-      <c r="N183" s="30"/>
+      <c r="L183" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="M183" s="49" t="s">
+        <v>196</v>
+      </c>
+      <c r="N183" s="30" t="s">
+        <v>275</v>
+      </c>
       <c r="O183" s="37"/>
       <c r="P183" s="37"/>
       <c r="Q183" s="38"/>
@@ -10797,20 +11315,44 @@
       <c r="T183" s="37"/>
     </row>
     <row r="184" spans="1:20" ht="18" customHeight="1">
-      <c r="A184" s="40"/>
-      <c r="B184" s="31"/>
-      <c r="C184" s="30"/>
-      <c r="D184" s="30"/>
-      <c r="E184" s="31"/>
-      <c r="F184" s="52"/>
-      <c r="G184" s="32"/>
+      <c r="A184" s="50" t="s">
+        <v>268</v>
+      </c>
+      <c r="B184" s="31" t="s">
+        <v>264</v>
+      </c>
+      <c r="C184" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="D184" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E184" s="31" t="s">
+        <v>270</v>
+      </c>
+      <c r="F184" s="52" t="s">
+        <v>194</v>
+      </c>
+      <c r="G184" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H184" s="56"/>
-      <c r="I184" s="54"/>
-      <c r="J184" s="51"/>
+      <c r="I184" s="54">
+        <v>1273</v>
+      </c>
+      <c r="J184" s="51">
+        <v>44000000</v>
+      </c>
       <c r="K184" s="38"/>
-      <c r="L184" s="49"/>
-      <c r="M184" s="49"/>
-      <c r="N184" s="30"/>
+      <c r="L184" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="M184" s="49" t="s">
+        <v>196</v>
+      </c>
+      <c r="N184" s="30" t="s">
+        <v>275</v>
+      </c>
       <c r="O184" s="37"/>
       <c r="P184" s="37"/>
       <c r="Q184" s="38"/>
@@ -10819,20 +11361,44 @@
       <c r="T184" s="37"/>
     </row>
     <row r="185" spans="1:20" ht="18" customHeight="1">
-      <c r="A185" s="40"/>
-      <c r="B185" s="31"/>
-      <c r="C185" s="30"/>
-      <c r="D185" s="30"/>
-      <c r="E185" s="31"/>
-      <c r="F185" s="52"/>
-      <c r="G185" s="32"/>
+      <c r="A185" s="50" t="s">
+        <v>269</v>
+      </c>
+      <c r="B185" s="31" t="s">
+        <v>265</v>
+      </c>
+      <c r="C185" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="D185" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E185" s="31" t="s">
+        <v>270</v>
+      </c>
+      <c r="F185" s="52" t="s">
+        <v>194</v>
+      </c>
+      <c r="G185" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H185" s="56"/>
-      <c r="I185" s="54"/>
-      <c r="J185" s="51"/>
+      <c r="I185" s="54">
+        <v>1273</v>
+      </c>
+      <c r="J185" s="51">
+        <v>77000000</v>
+      </c>
       <c r="K185" s="38"/>
-      <c r="L185" s="49"/>
-      <c r="M185" s="49"/>
-      <c r="N185" s="30"/>
+      <c r="L185" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="M185" s="49" t="s">
+        <v>196</v>
+      </c>
+      <c r="N185" s="30" t="s">
+        <v>275</v>
+      </c>
       <c r="O185" s="37"/>
       <c r="P185" s="37"/>
       <c r="Q185" s="38"/>
@@ -10841,20 +11407,44 @@
       <c r="T185" s="37"/>
     </row>
     <row r="186" spans="1:20" ht="18" customHeight="1">
-      <c r="A186" s="40"/>
-      <c r="B186" s="31"/>
-      <c r="C186" s="30"/>
-      <c r="D186" s="30"/>
-      <c r="E186" s="31"/>
-      <c r="F186" s="52"/>
-      <c r="G186" s="32"/>
+      <c r="A186" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="B186" s="103" t="s">
+        <v>262</v>
+      </c>
+      <c r="C186" s="90" t="s">
+        <v>160</v>
+      </c>
+      <c r="D186" s="90" t="s">
+        <v>64</v>
+      </c>
+      <c r="E186" s="103" t="s">
+        <v>270</v>
+      </c>
+      <c r="F186" s="97" t="s">
+        <v>272</v>
+      </c>
+      <c r="G186" s="97" t="s">
+        <v>29</v>
+      </c>
       <c r="H186" s="56"/>
-      <c r="I186" s="54"/>
-      <c r="J186" s="51"/>
+      <c r="I186" s="54">
+        <v>1273</v>
+      </c>
+      <c r="J186" s="51">
+        <v>70</v>
+      </c>
       <c r="K186" s="38"/>
-      <c r="L186" s="49"/>
-      <c r="M186" s="49"/>
-      <c r="N186" s="30"/>
+      <c r="L186" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="M186" s="49" t="s">
+        <v>196</v>
+      </c>
+      <c r="N186" s="30" t="s">
+        <v>275</v>
+      </c>
       <c r="O186" s="37"/>
       <c r="P186" s="37"/>
       <c r="Q186" s="38"/>
@@ -10863,20 +11453,44 @@
       <c r="T186" s="37"/>
     </row>
     <row r="187" spans="1:20" ht="18" customHeight="1">
-      <c r="A187" s="40"/>
-      <c r="B187" s="31"/>
-      <c r="C187" s="30"/>
-      <c r="D187" s="30"/>
-      <c r="E187" s="31"/>
-      <c r="F187" s="52"/>
-      <c r="G187" s="32"/>
+      <c r="A187" s="151" t="s">
+        <v>267</v>
+      </c>
+      <c r="B187" s="105" t="s">
+        <v>263</v>
+      </c>
+      <c r="C187" s="91" t="s">
+        <v>160</v>
+      </c>
+      <c r="D187" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="E187" s="105" t="s">
+        <v>270</v>
+      </c>
+      <c r="F187" s="97" t="s">
+        <v>272</v>
+      </c>
+      <c r="G187" s="98" t="s">
+        <v>29</v>
+      </c>
       <c r="H187" s="56"/>
-      <c r="I187" s="54"/>
-      <c r="J187" s="51"/>
+      <c r="I187" s="54">
+        <v>1273</v>
+      </c>
+      <c r="J187" s="51">
+        <v>70</v>
+      </c>
       <c r="K187" s="38"/>
-      <c r="L187" s="49"/>
-      <c r="M187" s="49"/>
-      <c r="N187" s="30"/>
+      <c r="L187" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="M187" s="49" t="s">
+        <v>196</v>
+      </c>
+      <c r="N187" s="30" t="s">
+        <v>275</v>
+      </c>
       <c r="O187" s="37"/>
       <c r="P187" s="37"/>
       <c r="Q187" s="38"/>
@@ -10885,20 +11499,44 @@
       <c r="T187" s="37"/>
     </row>
     <row r="188" spans="1:20" ht="18" customHeight="1">
-      <c r="A188" s="40"/>
-      <c r="B188" s="31"/>
-      <c r="C188" s="30"/>
-      <c r="D188" s="30"/>
-      <c r="E188" s="31"/>
-      <c r="F188" s="52"/>
-      <c r="G188" s="32"/>
+      <c r="A188" s="151" t="s">
+        <v>268</v>
+      </c>
+      <c r="B188" s="105" t="s">
+        <v>264</v>
+      </c>
+      <c r="C188" s="91" t="s">
+        <v>160</v>
+      </c>
+      <c r="D188" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="E188" s="105" t="s">
+        <v>270</v>
+      </c>
+      <c r="F188" s="97" t="s">
+        <v>272</v>
+      </c>
+      <c r="G188" s="98" t="s">
+        <v>29</v>
+      </c>
       <c r="H188" s="56"/>
-      <c r="I188" s="54"/>
-      <c r="J188" s="51"/>
+      <c r="I188" s="54">
+        <v>1273</v>
+      </c>
+      <c r="J188" s="51">
+        <v>70</v>
+      </c>
       <c r="K188" s="38"/>
-      <c r="L188" s="49"/>
-      <c r="M188" s="49"/>
-      <c r="N188" s="30"/>
+      <c r="L188" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="M188" s="49" t="s">
+        <v>196</v>
+      </c>
+      <c r="N188" s="30" t="s">
+        <v>275</v>
+      </c>
       <c r="O188" s="37"/>
       <c r="P188" s="37"/>
       <c r="Q188" s="38"/>
@@ -10907,20 +11545,44 @@
       <c r="T188" s="37"/>
     </row>
     <row r="189" spans="1:20" ht="18" customHeight="1">
-      <c r="A189" s="40"/>
-      <c r="B189" s="31"/>
-      <c r="C189" s="30"/>
-      <c r="D189" s="30"/>
-      <c r="E189" s="31"/>
-      <c r="F189" s="52"/>
-      <c r="G189" s="32"/>
+      <c r="A189" s="151" t="s">
+        <v>269</v>
+      </c>
+      <c r="B189" s="105" t="s">
+        <v>265</v>
+      </c>
+      <c r="C189" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="D189" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="E189" s="105" t="s">
+        <v>270</v>
+      </c>
+      <c r="F189" s="97" t="s">
+        <v>272</v>
+      </c>
+      <c r="G189" s="98" t="s">
+        <v>29</v>
+      </c>
       <c r="H189" s="56"/>
-      <c r="I189" s="54"/>
-      <c r="J189" s="38"/>
+      <c r="I189" s="54">
+        <v>1273</v>
+      </c>
+      <c r="J189" s="51">
+        <v>70</v>
+      </c>
       <c r="K189" s="38"/>
-      <c r="L189" s="40"/>
-      <c r="M189" s="49"/>
-      <c r="N189" s="30"/>
+      <c r="L189" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="M189" s="49" t="s">
+        <v>196</v>
+      </c>
+      <c r="N189" s="30" t="s">
+        <v>275</v>
+      </c>
       <c r="O189" s="37"/>
       <c r="P189" s="37"/>
       <c r="Q189" s="38"/>
@@ -10929,20 +11591,44 @@
       <c r="T189" s="37"/>
     </row>
     <row r="190" spans="1:20" ht="18" customHeight="1">
-      <c r="A190" s="40"/>
-      <c r="B190" s="31"/>
-      <c r="C190" s="30"/>
-      <c r="D190" s="30"/>
-      <c r="E190" s="31"/>
-      <c r="F190" s="52"/>
-      <c r="G190" s="32"/>
+      <c r="A190" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="B190" s="103" t="s">
+        <v>262</v>
+      </c>
+      <c r="C190" s="90" t="s">
+        <v>160</v>
+      </c>
+      <c r="D190" s="90" t="s">
+        <v>64</v>
+      </c>
+      <c r="E190" s="103" t="s">
+        <v>270</v>
+      </c>
+      <c r="F190" s="97" t="s">
+        <v>274</v>
+      </c>
+      <c r="G190" s="97" t="s">
+        <v>29</v>
+      </c>
       <c r="H190" s="56"/>
-      <c r="I190" s="54"/>
-      <c r="J190" s="38"/>
+      <c r="I190" s="54">
+        <v>1273</v>
+      </c>
+      <c r="J190" s="51">
+        <v>58000000</v>
+      </c>
       <c r="K190" s="38"/>
-      <c r="L190" s="40"/>
-      <c r="M190" s="49"/>
-      <c r="N190" s="30"/>
+      <c r="L190" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="M190" s="49" t="s">
+        <v>221</v>
+      </c>
+      <c r="N190" s="30" t="s">
+        <v>275</v>
+      </c>
       <c r="O190" s="37"/>
       <c r="P190" s="37"/>
       <c r="Q190" s="38"/>
@@ -10951,20 +11637,44 @@
       <c r="T190" s="37"/>
     </row>
     <row r="191" spans="1:20" ht="18" customHeight="1">
-      <c r="A191" s="40"/>
-      <c r="B191" s="31"/>
-      <c r="C191" s="30"/>
-      <c r="D191" s="30"/>
-      <c r="E191" s="31"/>
-      <c r="F191" s="52"/>
-      <c r="G191" s="32"/>
+      <c r="A191" s="151" t="s">
+        <v>267</v>
+      </c>
+      <c r="B191" s="105" t="s">
+        <v>263</v>
+      </c>
+      <c r="C191" s="91" t="s">
+        <v>160</v>
+      </c>
+      <c r="D191" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="E191" s="105" t="s">
+        <v>270</v>
+      </c>
+      <c r="F191" s="97" t="s">
+        <v>274</v>
+      </c>
+      <c r="G191" s="98" t="s">
+        <v>29</v>
+      </c>
       <c r="H191" s="56"/>
-      <c r="I191" s="54"/>
-      <c r="J191" s="38"/>
+      <c r="I191" s="54">
+        <v>1273</v>
+      </c>
+      <c r="J191" s="51">
+        <v>50000000</v>
+      </c>
       <c r="K191" s="38"/>
-      <c r="L191" s="40"/>
-      <c r="M191" s="49"/>
-      <c r="N191" s="30"/>
+      <c r="L191" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="M191" s="49" t="s">
+        <v>221</v>
+      </c>
+      <c r="N191" s="30" t="s">
+        <v>275</v>
+      </c>
       <c r="O191" s="37"/>
       <c r="P191" s="37"/>
       <c r="Q191" s="38"/>
@@ -10973,20 +11683,44 @@
       <c r="T191" s="37"/>
     </row>
     <row r="192" spans="1:20" ht="18" customHeight="1">
-      <c r="A192" s="40"/>
-      <c r="B192" s="31"/>
-      <c r="C192" s="30"/>
-      <c r="D192" s="30"/>
-      <c r="E192" s="31"/>
-      <c r="F192" s="52"/>
-      <c r="G192" s="32"/>
+      <c r="A192" s="151" t="s">
+        <v>268</v>
+      </c>
+      <c r="B192" s="105" t="s">
+        <v>264</v>
+      </c>
+      <c r="C192" s="91" t="s">
+        <v>160</v>
+      </c>
+      <c r="D192" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="E192" s="105" t="s">
+        <v>270</v>
+      </c>
+      <c r="F192" s="97" t="s">
+        <v>274</v>
+      </c>
+      <c r="G192" s="98" t="s">
+        <v>29</v>
+      </c>
       <c r="H192" s="56"/>
-      <c r="I192" s="54"/>
-      <c r="J192" s="38"/>
+      <c r="I192" s="54">
+        <v>1273</v>
+      </c>
+      <c r="J192" s="51">
+        <v>46000000</v>
+      </c>
       <c r="K192" s="38"/>
-      <c r="L192" s="40"/>
-      <c r="M192" s="49"/>
-      <c r="N192" s="30"/>
+      <c r="L192" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="M192" s="49" t="s">
+        <v>221</v>
+      </c>
+      <c r="N192" s="30" t="s">
+        <v>275</v>
+      </c>
       <c r="O192" s="37"/>
       <c r="P192" s="37"/>
       <c r="Q192" s="38"/>
@@ -10995,20 +11729,44 @@
       <c r="T192" s="37"/>
     </row>
     <row r="193" spans="1:20" ht="18" customHeight="1">
-      <c r="A193" s="40"/>
-      <c r="B193" s="31"/>
-      <c r="C193" s="30"/>
-      <c r="D193" s="30"/>
-      <c r="E193" s="31"/>
-      <c r="F193" s="52"/>
-      <c r="G193" s="32"/>
+      <c r="A193" s="151" t="s">
+        <v>269</v>
+      </c>
+      <c r="B193" s="105" t="s">
+        <v>265</v>
+      </c>
+      <c r="C193" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="D193" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="E193" s="105" t="s">
+        <v>270</v>
+      </c>
+      <c r="F193" s="97" t="s">
+        <v>274</v>
+      </c>
+      <c r="G193" s="98" t="s">
+        <v>29</v>
+      </c>
       <c r="H193" s="56"/>
-      <c r="I193" s="34"/>
-      <c r="J193" s="38"/>
+      <c r="I193" s="54">
+        <v>1273</v>
+      </c>
+      <c r="J193" s="51">
+        <v>80000000</v>
+      </c>
       <c r="K193" s="38"/>
-      <c r="L193" s="40"/>
-      <c r="M193" s="40"/>
-      <c r="N193" s="30"/>
+      <c r="L193" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="M193" s="49" t="s">
+        <v>221</v>
+      </c>
+      <c r="N193" s="30" t="s">
+        <v>275</v>
+      </c>
       <c r="O193" s="37"/>
       <c r="P193" s="37"/>
       <c r="Q193" s="38"/>
@@ -27749,6 +28507,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -27763,11 +28526,6 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
- parsed data from `10.1016/j.ijrmhm.2022.105992`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Aug2025.xlsx
+++ b/MiscSmallUploads_Aug2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C69DC30-6A10-0947-BF3F-0DD07090A0F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D140FFC1-EEF5-6449-9805-174F439F344E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8020" windowWidth="34560" windowHeight="12760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-700" yWindow="3880" windowWidth="34560" windowHeight="12760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1695" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1755" uniqueCount="295">
   <si>
     <r>
       <rPr>
@@ -958,6 +958,63 @@
   </si>
   <si>
     <t>10.1016/j.ijrmhm.2025.107379</t>
+  </si>
+  <si>
+    <t>Al0.5CoCrFeNi</t>
+  </si>
+  <si>
+    <t>Al0.5CoCrFeNiNb0.2</t>
+  </si>
+  <si>
+    <t>Al0.5CoCrFeNiNb0.4</t>
+  </si>
+  <si>
+    <t>Al0.5CoCrFeNiNb0.6</t>
+  </si>
+  <si>
+    <t>Al0.5CoCrFeNiNb0.8</t>
+  </si>
+  <si>
+    <t>Al0.5CoCrFeNiNb</t>
+  </si>
+  <si>
+    <t>Nb0</t>
+  </si>
+  <si>
+    <t>Nb0.2</t>
+  </si>
+  <si>
+    <t>Nb0.4</t>
+  </si>
+  <si>
+    <t>Nb0.6</t>
+  </si>
+  <si>
+    <t>Nb0.8</t>
+  </si>
+  <si>
+    <t>Nb1.0</t>
+  </si>
+  <si>
+    <t>BM+LC(DED)</t>
+  </si>
+  <si>
+    <t>ball milled for 5h to mix powders and laser cladded using 1100W laser with 6mm/s scanning speed and 4mm spot diameter feeding 10g/min onto H13 steel preheated to 200*C; hardness average measured over the top 150um of the coating</t>
+  </si>
+  <si>
+    <t>ball milled for 5h to mix powders and laser cladded using 1100W laser with 6mm/s scanning speed and 4mm spot diameter feeding 10g/min onto H13 steel preheated to 200*C; hypoeutectic; hardness average measured over the top 150um of the coating</t>
+  </si>
+  <si>
+    <t>ball milled for 5h to mix powders and laser cladded using 1100W laser with 6mm/s scanning speed and 4mm spot diameter feeding 10g/min onto H13 steel preheated to 200*C; eutectic; hardness average measured over the top 150um of the coating</t>
+  </si>
+  <si>
+    <t>ball milled for 5h to mix powders and laser cladded using 1100W laser with 6mm/s scanning speed and 4mm spot diameter feeding 10g/min onto H13 steel preheated to 200*C; hypereutectic; hardness average measured over the top 150um of the coating</t>
+  </si>
+  <si>
+    <t>F12</t>
+  </si>
+  <si>
+    <t>10.1016/j.ijrmhm.2022.105992</t>
   </si>
 </sst>
 </file>
@@ -2177,6 +2234,65 @@
     <xf numFmtId="0" fontId="15" fillId="10" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="14" fillId="10" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="10" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="14" fillId="10" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="10" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2237,65 +2353,6 @@
     <xf numFmtId="164" fontId="5" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="14" fillId="10" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="10" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="14" fillId="10" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="10" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3458,8 +3515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T960"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A172" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O183" sqref="O183"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A185" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N203" sqref="N203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -3516,19 +3573,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" s="112" t="s">
+      <c r="D2" s="133" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="113"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="117"/>
-      <c r="H2" s="117"/>
-      <c r="I2" s="118"/>
-      <c r="J2" s="119"/>
-      <c r="K2" s="119"/>
-      <c r="L2" s="117"/>
-      <c r="M2" s="117"/>
-      <c r="N2" s="120"/>
+      <c r="E2" s="134"/>
+      <c r="F2" s="137"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="139"/>
+      <c r="J2" s="140"/>
+      <c r="K2" s="140"/>
+      <c r="L2" s="138"/>
+      <c r="M2" s="138"/>
+      <c r="N2" s="141"/>
       <c r="O2" s="13"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -3544,17 +3601,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="114"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="121"/>
-      <c r="G3" s="121"/>
-      <c r="H3" s="121"/>
-      <c r="I3" s="122"/>
-      <c r="J3" s="123"/>
-      <c r="K3" s="123"/>
-      <c r="L3" s="121"/>
-      <c r="M3" s="121"/>
-      <c r="N3" s="124"/>
+      <c r="D3" s="135"/>
+      <c r="E3" s="136"/>
+      <c r="F3" s="142"/>
+      <c r="G3" s="142"/>
+      <c r="H3" s="142"/>
+      <c r="I3" s="143"/>
+      <c r="J3" s="144"/>
+      <c r="K3" s="144"/>
+      <c r="L3" s="142"/>
+      <c r="M3" s="142"/>
+      <c r="N3" s="145"/>
       <c r="O3" s="13"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -3595,43 +3652,43 @@
       <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="125" t="s">
+      <c r="C5" s="146" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="127" t="s">
+      <c r="D5" s="148" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="127" t="s">
+      <c r="E5" s="148" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="127" t="s">
+      <c r="F5" s="148" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="127" t="s">
+      <c r="G5" s="148" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="128" t="s">
+      <c r="H5" s="149" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="127" t="s">
+      <c r="I5" s="148" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="127" t="s">
+      <c r="J5" s="148" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="127" t="s">
+      <c r="K5" s="148" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="127" t="s">
+      <c r="L5" s="148" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="127" t="s">
+      <c r="M5" s="148" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="127" t="s">
+      <c r="N5" s="148" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="132" t="s">
+      <c r="O5" s="116" t="s">
         <v>20</v>
       </c>
       <c r="P5" s="25"/>
@@ -3647,19 +3704,19 @@
       <c r="B6" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="126"/>
-      <c r="D6" s="126"/>
-      <c r="E6" s="126"/>
-      <c r="F6" s="126"/>
-      <c r="G6" s="126"/>
-      <c r="H6" s="129"/>
-      <c r="I6" s="130"/>
-      <c r="J6" s="131"/>
-      <c r="K6" s="131"/>
-      <c r="L6" s="126"/>
-      <c r="M6" s="126"/>
-      <c r="N6" s="126"/>
-      <c r="O6" s="133"/>
+      <c r="C6" s="147"/>
+      <c r="D6" s="147"/>
+      <c r="E6" s="147"/>
+      <c r="F6" s="147"/>
+      <c r="G6" s="147"/>
+      <c r="H6" s="150"/>
+      <c r="I6" s="151"/>
+      <c r="J6" s="152"/>
+      <c r="K6" s="152"/>
+      <c r="L6" s="147"/>
+      <c r="M6" s="147"/>
+      <c r="N6" s="147"/>
+      <c r="O6" s="117"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="9"/>
@@ -3709,7 +3766,7 @@
       <c r="N7" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="134"/>
+      <c r="O7" s="118"/>
       <c r="P7" s="64" t="s">
         <v>62</v>
       </c>
@@ -3724,35 +3781,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" thickBot="1">
       <c r="A8" s="59"/>
-      <c r="B8" s="135" t="s">
+      <c r="B8" s="119" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="136"/>
-      <c r="D8" s="136"/>
-      <c r="E8" s="137"/>
-      <c r="F8" s="138" t="s">
+      <c r="C8" s="120"/>
+      <c r="D8" s="120"/>
+      <c r="E8" s="121"/>
+      <c r="F8" s="122" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="139"/>
-      <c r="H8" s="139"/>
-      <c r="I8" s="140"/>
-      <c r="J8" s="141"/>
-      <c r="K8" s="141"/>
-      <c r="L8" s="142"/>
-      <c r="M8" s="143" t="s">
+      <c r="G8" s="123"/>
+      <c r="H8" s="123"/>
+      <c r="I8" s="124"/>
+      <c r="J8" s="125"/>
+      <c r="K8" s="125"/>
+      <c r="L8" s="126"/>
+      <c r="M8" s="127" t="s">
         <v>40</v>
       </c>
-      <c r="N8" s="144"/>
+      <c r="N8" s="128"/>
       <c r="O8" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="P8" s="145" t="s">
+      <c r="P8" s="129" t="s">
         <v>42</v>
       </c>
-      <c r="Q8" s="146"/>
-      <c r="R8" s="147"/>
-      <c r="S8" s="147"/>
-      <c r="T8" s="148"/>
+      <c r="Q8" s="130"/>
+      <c r="R8" s="131"/>
+      <c r="S8" s="131"/>
+      <c r="T8" s="132"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1">
       <c r="A9" s="60" t="s">
@@ -10575,7 +10632,7 @@
         <v>298</v>
       </c>
       <c r="J168" s="35">
-        <f t="shared" si="3"/>
+        <f>P168*9807000</f>
         <v>3863958000</v>
       </c>
       <c r="K168" s="38"/>
@@ -10839,7 +10896,7 @@
       <c r="T173" s="37"/>
     </row>
     <row r="174" spans="1:20" ht="18" customHeight="1">
-      <c r="A174" s="149" t="s">
+      <c r="A174" s="112" t="s">
         <v>266</v>
       </c>
       <c r="B174" s="103" t="s">
@@ -10863,7 +10920,7 @@
       <c r="H174" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="I174" s="150">
+      <c r="I174" s="113">
         <v>298</v>
       </c>
       <c r="J174" s="48">
@@ -10887,7 +10944,7 @@
       <c r="T174" s="37"/>
     </row>
     <row r="175" spans="1:20" ht="18" customHeight="1">
-      <c r="A175" s="151" t="s">
+      <c r="A175" s="114" t="s">
         <v>267</v>
       </c>
       <c r="B175" s="105" t="s">
@@ -10911,7 +10968,7 @@
       <c r="H175" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="I175" s="152">
+      <c r="I175" s="115">
         <v>298</v>
       </c>
       <c r="J175" s="48">
@@ -10935,7 +10992,7 @@
       <c r="T175" s="37"/>
     </row>
     <row r="176" spans="1:20" ht="18" customHeight="1">
-      <c r="A176" s="151" t="s">
+      <c r="A176" s="114" t="s">
         <v>268</v>
       </c>
       <c r="B176" s="105" t="s">
@@ -10959,7 +11016,7 @@
       <c r="H176" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="I176" s="152">
+      <c r="I176" s="115">
         <v>298</v>
       </c>
       <c r="J176" s="48">
@@ -10983,7 +11040,7 @@
       <c r="T176" s="37"/>
     </row>
     <row r="177" spans="1:20" ht="18" customHeight="1">
-      <c r="A177" s="151" t="s">
+      <c r="A177" s="114" t="s">
         <v>269</v>
       </c>
       <c r="B177" s="105" t="s">
@@ -11007,7 +11064,7 @@
       <c r="H177" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="I177" s="152">
+      <c r="I177" s="115">
         <v>298</v>
       </c>
       <c r="J177" s="35">
@@ -11031,7 +11088,7 @@
       <c r="T177" s="37"/>
     </row>
     <row r="178" spans="1:20" ht="18" customHeight="1">
-      <c r="A178" s="149" t="s">
+      <c r="A178" s="112" t="s">
         <v>266</v>
       </c>
       <c r="B178" s="103" t="s">
@@ -11055,7 +11112,7 @@
       <c r="H178" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="I178" s="150">
+      <c r="I178" s="113">
         <v>298</v>
       </c>
       <c r="J178" s="35">
@@ -11079,7 +11136,7 @@
       <c r="T178" s="37"/>
     </row>
     <row r="179" spans="1:20" ht="18" customHeight="1">
-      <c r="A179" s="151" t="s">
+      <c r="A179" s="114" t="s">
         <v>267</v>
       </c>
       <c r="B179" s="105" t="s">
@@ -11103,7 +11160,7 @@
       <c r="H179" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="I179" s="152">
+      <c r="I179" s="115">
         <v>298</v>
       </c>
       <c r="J179" s="35">
@@ -11127,7 +11184,7 @@
       <c r="T179" s="37"/>
     </row>
     <row r="180" spans="1:20" ht="18" customHeight="1">
-      <c r="A180" s="151" t="s">
+      <c r="A180" s="114" t="s">
         <v>268</v>
       </c>
       <c r="B180" s="105" t="s">
@@ -11151,7 +11208,7 @@
       <c r="H180" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="I180" s="152">
+      <c r="I180" s="115">
         <v>298</v>
       </c>
       <c r="J180" s="35">
@@ -11175,7 +11232,7 @@
       <c r="T180" s="37"/>
     </row>
     <row r="181" spans="1:20" ht="18" customHeight="1">
-      <c r="A181" s="151" t="s">
+      <c r="A181" s="114" t="s">
         <v>269</v>
       </c>
       <c r="B181" s="105" t="s">
@@ -11199,7 +11256,7 @@
       <c r="H181" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="I181" s="152">
+      <c r="I181" s="115">
         <v>298</v>
       </c>
       <c r="J181" s="35">
@@ -11407,7 +11464,7 @@
       <c r="T185" s="37"/>
     </row>
     <row r="186" spans="1:20" ht="18" customHeight="1">
-      <c r="A186" s="149" t="s">
+      <c r="A186" s="112" t="s">
         <v>266</v>
       </c>
       <c r="B186" s="103" t="s">
@@ -11453,7 +11510,7 @@
       <c r="T186" s="37"/>
     </row>
     <row r="187" spans="1:20" ht="18" customHeight="1">
-      <c r="A187" s="151" t="s">
+      <c r="A187" s="114" t="s">
         <v>267</v>
       </c>
       <c r="B187" s="105" t="s">
@@ -11499,7 +11556,7 @@
       <c r="T187" s="37"/>
     </row>
     <row r="188" spans="1:20" ht="18" customHeight="1">
-      <c r="A188" s="151" t="s">
+      <c r="A188" s="114" t="s">
         <v>268</v>
       </c>
       <c r="B188" s="105" t="s">
@@ -11545,7 +11602,7 @@
       <c r="T188" s="37"/>
     </row>
     <row r="189" spans="1:20" ht="18" customHeight="1">
-      <c r="A189" s="151" t="s">
+      <c r="A189" s="114" t="s">
         <v>269</v>
       </c>
       <c r="B189" s="105" t="s">
@@ -11591,7 +11648,7 @@
       <c r="T189" s="37"/>
     </row>
     <row r="190" spans="1:20" ht="18" customHeight="1">
-      <c r="A190" s="149" t="s">
+      <c r="A190" s="112" t="s">
         <v>266</v>
       </c>
       <c r="B190" s="103" t="s">
@@ -11637,7 +11694,7 @@
       <c r="T190" s="37"/>
     </row>
     <row r="191" spans="1:20" ht="18" customHeight="1">
-      <c r="A191" s="151" t="s">
+      <c r="A191" s="114" t="s">
         <v>267</v>
       </c>
       <c r="B191" s="105" t="s">
@@ -11683,7 +11740,7 @@
       <c r="T191" s="37"/>
     </row>
     <row r="192" spans="1:20" ht="18" customHeight="1">
-      <c r="A192" s="151" t="s">
+      <c r="A192" s="114" t="s">
         <v>268</v>
       </c>
       <c r="B192" s="105" t="s">
@@ -11729,7 +11786,7 @@
       <c r="T192" s="37"/>
     </row>
     <row r="193" spans="1:20" ht="18" customHeight="1">
-      <c r="A193" s="151" t="s">
+      <c r="A193" s="114" t="s">
         <v>269</v>
       </c>
       <c r="B193" s="105" t="s">
@@ -11775,134 +11832,338 @@
       <c r="T193" s="37"/>
     </row>
     <row r="194" spans="1:20" ht="18" customHeight="1">
-      <c r="A194" s="40"/>
-      <c r="B194" s="31"/>
-      <c r="C194" s="30"/>
-      <c r="D194" s="30"/>
-      <c r="E194" s="31"/>
-      <c r="F194" s="52"/>
-      <c r="G194" s="32"/>
+      <c r="A194" s="40" t="s">
+        <v>282</v>
+      </c>
+      <c r="B194" s="31" t="s">
+        <v>276</v>
+      </c>
+      <c r="C194" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D194" s="30" t="s">
+        <v>288</v>
+      </c>
+      <c r="E194" s="31" t="s">
+        <v>289</v>
+      </c>
+      <c r="F194" s="52" t="s">
+        <v>179</v>
+      </c>
+      <c r="G194" s="98" t="s">
+        <v>29</v>
+      </c>
       <c r="H194" s="56"/>
-      <c r="I194" s="54"/>
-      <c r="J194" s="38"/>
-      <c r="K194" s="38"/>
-      <c r="L194" s="40"/>
-      <c r="M194" s="40"/>
-      <c r="N194" s="30"/>
+      <c r="I194" s="54">
+        <v>298</v>
+      </c>
+      <c r="J194" s="38">
+        <f>AVERAGE(P194:R194)*9807000</f>
+        <v>5221817899.7613316</v>
+      </c>
+      <c r="K194" s="38">
+        <f>STDEV(P194:R194)*9807000</f>
+        <v>270708265.27492547</v>
+      </c>
+      <c r="L194" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="M194" s="40" t="s">
+        <v>293</v>
+      </c>
+      <c r="N194" s="30" t="s">
+        <v>294</v>
+      </c>
       <c r="O194" s="37"/>
-      <c r="P194" s="37"/>
-      <c r="Q194" s="38"/>
-      <c r="R194" s="37"/>
+      <c r="P194" s="37">
+        <v>504.05727923627597</v>
+      </c>
+      <c r="Q194" s="38">
+        <v>559.18854415274404</v>
+      </c>
+      <c r="R194" s="37">
+        <v>534.12887828162297</v>
+      </c>
       <c r="S194" s="37"/>
       <c r="T194" s="37"/>
     </row>
     <row r="195" spans="1:20" ht="18" customHeight="1">
-      <c r="A195" s="40"/>
-      <c r="B195" s="31"/>
-      <c r="C195" s="30"/>
-      <c r="D195" s="30"/>
-      <c r="E195" s="31"/>
-      <c r="F195" s="52"/>
-      <c r="G195" s="32"/>
+      <c r="A195" s="40" t="s">
+        <v>283</v>
+      </c>
+      <c r="B195" s="31" t="s">
+        <v>277</v>
+      </c>
+      <c r="C195" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="D195" s="30" t="s">
+        <v>288</v>
+      </c>
+      <c r="E195" s="31" t="s">
+        <v>290</v>
+      </c>
+      <c r="F195" s="52" t="s">
+        <v>179</v>
+      </c>
+      <c r="G195" s="98" t="s">
+        <v>29</v>
+      </c>
       <c r="H195" s="56"/>
-      <c r="I195" s="54"/>
-      <c r="J195" s="51"/>
-      <c r="K195" s="38"/>
-      <c r="L195" s="40"/>
-      <c r="M195" s="40"/>
-      <c r="N195" s="30"/>
+      <c r="I195" s="54">
+        <v>298</v>
+      </c>
+      <c r="J195" s="38">
+        <f t="shared" ref="J195:J199" si="4">AVERAGE(P195:R195)*9807000</f>
+        <v>5508538066.8257742</v>
+      </c>
+      <c r="K195" s="38">
+        <f t="shared" ref="K195:K199" si="5">STDEV(P195:R195)*9807000</f>
+        <v>451155651.30960613</v>
+      </c>
+      <c r="L195" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="M195" s="40" t="s">
+        <v>293</v>
+      </c>
+      <c r="N195" s="30" t="s">
+        <v>294</v>
+      </c>
       <c r="O195" s="37"/>
-      <c r="P195" s="37"/>
-      <c r="Q195" s="38"/>
-      <c r="R195" s="37"/>
+      <c r="P195" s="37">
+        <v>509.069212410501</v>
+      </c>
+      <c r="Q195" s="38">
+        <v>594.27207637231504</v>
+      </c>
+      <c r="R195" s="37">
+        <v>581.74224343675405</v>
+      </c>
       <c r="S195" s="37"/>
       <c r="T195" s="37"/>
     </row>
     <row r="196" spans="1:20" ht="18" customHeight="1">
-      <c r="A196" s="40"/>
-      <c r="B196" s="31"/>
-      <c r="C196" s="30"/>
-      <c r="D196" s="30"/>
-      <c r="E196" s="31"/>
-      <c r="F196" s="52"/>
-      <c r="G196" s="32"/>
+      <c r="A196" s="40" t="s">
+        <v>284</v>
+      </c>
+      <c r="B196" s="31" t="s">
+        <v>278</v>
+      </c>
+      <c r="C196" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="D196" s="30" t="s">
+        <v>288</v>
+      </c>
+      <c r="E196" s="31" t="s">
+        <v>291</v>
+      </c>
+      <c r="F196" s="52" t="s">
+        <v>179</v>
+      </c>
+      <c r="G196" s="98" t="s">
+        <v>29</v>
+      </c>
       <c r="H196" s="56"/>
-      <c r="I196" s="54"/>
-      <c r="J196" s="51"/>
-      <c r="K196" s="38"/>
-      <c r="L196" s="40"/>
-      <c r="M196" s="40"/>
-      <c r="N196" s="30"/>
+      <c r="I196" s="54">
+        <v>298</v>
+      </c>
+      <c r="J196" s="38">
+        <f t="shared" si="4"/>
+        <v>6587152028.6396151</v>
+      </c>
+      <c r="K196" s="38">
+        <f t="shared" si="5"/>
+        <v>263336110.21933225</v>
+      </c>
+      <c r="L196" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="M196" s="40" t="s">
+        <v>293</v>
+      </c>
+      <c r="N196" s="30" t="s">
+        <v>294</v>
+      </c>
       <c r="O196" s="37"/>
-      <c r="P196" s="37"/>
-      <c r="Q196" s="38"/>
-      <c r="R196" s="37"/>
+      <c r="P196" s="37">
+        <v>682.81622911694501</v>
+      </c>
+      <c r="Q196" s="38">
+        <v>691.16945107398499</v>
+      </c>
+      <c r="R196" s="37">
+        <v>641.05011933174205</v>
+      </c>
       <c r="S196" s="37"/>
       <c r="T196" s="37"/>
     </row>
     <row r="197" spans="1:20" ht="18" customHeight="1">
-      <c r="A197" s="40"/>
-      <c r="B197" s="31"/>
-      <c r="C197" s="30"/>
-      <c r="D197" s="30"/>
-      <c r="E197" s="31"/>
-      <c r="F197" s="52"/>
-      <c r="G197" s="32"/>
+      <c r="A197" s="40" t="s">
+        <v>285</v>
+      </c>
+      <c r="B197" s="31" t="s">
+        <v>279</v>
+      </c>
+      <c r="C197" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="D197" s="30" t="s">
+        <v>288</v>
+      </c>
+      <c r="E197" s="31" t="s">
+        <v>292</v>
+      </c>
+      <c r="F197" s="52" t="s">
+        <v>179</v>
+      </c>
+      <c r="G197" s="98" t="s">
+        <v>29</v>
+      </c>
       <c r="H197" s="47"/>
-      <c r="I197" s="54"/>
-      <c r="J197" s="38"/>
-      <c r="K197" s="38"/>
-      <c r="L197" s="40"/>
-      <c r="M197" s="40"/>
-      <c r="N197" s="30"/>
+      <c r="I197" s="54">
+        <v>298</v>
+      </c>
+      <c r="J197" s="38">
+        <f t="shared" si="4"/>
+        <v>6734608114.5584688</v>
+      </c>
+      <c r="K197" s="38">
+        <f t="shared" si="5"/>
+        <v>90236088.42497775</v>
+      </c>
+      <c r="L197" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="M197" s="40" t="s">
+        <v>293</v>
+      </c>
+      <c r="N197" s="30" t="s">
+        <v>294</v>
+      </c>
       <c r="O197" s="37"/>
-      <c r="P197" s="37"/>
-      <c r="Q197" s="38"/>
-      <c r="R197" s="37"/>
+      <c r="P197" s="37">
+        <v>696.18138424820995</v>
+      </c>
+      <c r="Q197" s="38">
+        <v>686.15751789976105</v>
+      </c>
+      <c r="R197" s="37">
+        <v>677.80429594272005</v>
+      </c>
       <c r="S197" s="37"/>
       <c r="T197" s="37"/>
     </row>
     <row r="198" spans="1:20" ht="18" customHeight="1">
-      <c r="A198" s="40"/>
-      <c r="B198" s="31"/>
-      <c r="C198" s="30"/>
-      <c r="D198" s="30"/>
-      <c r="E198" s="31"/>
-      <c r="F198" s="52"/>
-      <c r="G198" s="32"/>
+      <c r="A198" s="40" t="s">
+        <v>286</v>
+      </c>
+      <c r="B198" s="31" t="s">
+        <v>280</v>
+      </c>
+      <c r="C198" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="D198" s="30" t="s">
+        <v>288</v>
+      </c>
+      <c r="E198" s="31" t="s">
+        <v>292</v>
+      </c>
+      <c r="F198" s="52" t="s">
+        <v>179</v>
+      </c>
+      <c r="G198" s="98" t="s">
+        <v>29</v>
+      </c>
       <c r="H198" s="47"/>
-      <c r="I198" s="54"/>
-      <c r="J198" s="38"/>
-      <c r="K198" s="38"/>
-      <c r="L198" s="40"/>
-      <c r="M198" s="40"/>
-      <c r="N198" s="30"/>
+      <c r="I198" s="54">
+        <v>298</v>
+      </c>
+      <c r="J198" s="38">
+        <f t="shared" si="4"/>
+        <v>8225552983.2935505</v>
+      </c>
+      <c r="K198" s="38">
+        <f t="shared" si="5"/>
+        <v>94237731.395113662</v>
+      </c>
+      <c r="L198" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="M198" s="40" t="s">
+        <v>293</v>
+      </c>
+      <c r="N198" s="30" t="s">
+        <v>294</v>
+      </c>
       <c r="O198" s="37"/>
-      <c r="P198" s="38"/>
-      <c r="Q198" s="38"/>
-      <c r="R198" s="37"/>
+      <c r="P198" s="38">
+        <v>828.99761336515496</v>
+      </c>
+      <c r="Q198" s="38">
+        <v>848.21002386634802</v>
+      </c>
+      <c r="R198" s="37">
+        <v>839.02147971360296</v>
+      </c>
       <c r="S198" s="37"/>
       <c r="T198" s="37"/>
     </row>
     <row r="199" spans="1:20" ht="18" customHeight="1">
-      <c r="A199" s="40"/>
-      <c r="B199" s="41"/>
-      <c r="C199" s="30"/>
-      <c r="D199" s="30"/>
-      <c r="E199" s="31"/>
-      <c r="F199" s="52"/>
-      <c r="G199" s="32"/>
+      <c r="A199" s="40" t="s">
+        <v>287</v>
+      </c>
+      <c r="B199" s="41" t="s">
+        <v>281</v>
+      </c>
+      <c r="C199" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="D199" s="30" t="s">
+        <v>288</v>
+      </c>
+      <c r="E199" s="31" t="s">
+        <v>289</v>
+      </c>
+      <c r="F199" s="52" t="s">
+        <v>179</v>
+      </c>
+      <c r="G199" s="98" t="s">
+        <v>29</v>
+      </c>
       <c r="H199" s="47"/>
-      <c r="I199" s="54"/>
-      <c r="J199" s="35"/>
-      <c r="K199" s="35"/>
-      <c r="L199" s="40"/>
-      <c r="M199" s="40"/>
-      <c r="N199" s="30"/>
+      <c r="I199" s="54">
+        <v>298</v>
+      </c>
+      <c r="J199" s="38">
+        <f t="shared" si="4"/>
+        <v>8515003818.6157494</v>
+      </c>
+      <c r="K199" s="38">
+        <f t="shared" si="5"/>
+        <v>51159053.411941297</v>
+      </c>
+      <c r="L199" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="M199" s="40" t="s">
+        <v>293</v>
+      </c>
+      <c r="N199" s="30" t="s">
+        <v>294</v>
+      </c>
       <c r="O199" s="37"/>
-      <c r="P199" s="38"/>
-      <c r="Q199" s="38"/>
-      <c r="R199" s="37"/>
+      <c r="P199" s="38">
+        <v>869.92840095465397</v>
+      </c>
+      <c r="Q199" s="38">
+        <v>872.43436754176605</v>
+      </c>
+      <c r="R199" s="37">
+        <v>862.41050119331703</v>
+      </c>
       <c r="S199" s="37"/>
       <c r="T199" s="37"/>
     </row>
@@ -28507,11 +28768,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -28526,6 +28782,11 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
- parsed data from `10.1007/s40195-020-01072-6`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Aug2025.xlsx
+++ b/MiscSmallUploads_Aug2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D140FFC1-EEF5-6449-9805-174F439F344E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6FF4F8-B1F5-1B49-8809-A4927400083F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-700" yWindow="3880" windowWidth="34560" windowHeight="12760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="7580" windowWidth="34560" windowHeight="12760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1755" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2389" uniqueCount="324">
   <si>
     <r>
       <rPr>
@@ -1015,6 +1015,93 @@
   </si>
   <si>
     <t>10.1016/j.ijrmhm.2022.105992</t>
+  </si>
+  <si>
+    <t>(Co0.2128 Fe0.4255 Ni0.2128 V0.1064 Mo0.0426)100</t>
+  </si>
+  <si>
+    <t>(Co0.2128 Fe0.4255 Ni0.2128 V0.1064 Mo0.0426)98 Nb2</t>
+  </si>
+  <si>
+    <t>(Co0.2128 Fe0.4255 Ni0.2128 V0.1064 Mo0.0426)96 Nb4</t>
+  </si>
+  <si>
+    <t>(Co0.2128 Fe0.4255 Ni0.2128 V0.1064 Mo0.0426)94 Nb6</t>
+  </si>
+  <si>
+    <t>(Co0.2128 Fe0.4255 Ni0.2128 V0.1064 Mo0.0426)92 Nb8</t>
+  </si>
+  <si>
+    <t>(Co0.2128 Fe0.4255 Ni0.2128 V0.1064 Mo0.0426)91 Nb9</t>
+  </si>
+  <si>
+    <t>(Co0.2128 Fe0.4255 Ni0.2128 V0.1064 Mo0.0426)90 Nb10</t>
+  </si>
+  <si>
+    <t>(Co0.2128 Fe0.4255 Ni0.2128 V0.1064 Mo0.0426)88 Nb12</t>
+  </si>
+  <si>
+    <t>Nb2</t>
+  </si>
+  <si>
+    <t>Nb4</t>
+  </si>
+  <si>
+    <t>Nb6</t>
+  </si>
+  <si>
+    <t>Nb8</t>
+  </si>
+  <si>
+    <t>Nb10</t>
+  </si>
+  <si>
+    <t>Nb12</t>
+  </si>
+  <si>
+    <t>Nb9</t>
+  </si>
+  <si>
+    <t>hypoeutectic</t>
+  </si>
+  <si>
+    <t>eutectic</t>
+  </si>
+  <si>
+    <t>hypereutectic; interesting flower morphology of laves C14 phase with 6-lobe morhpology</t>
+  </si>
+  <si>
+    <t>compressive plastic strain</t>
+  </si>
+  <si>
+    <t>minimum compressive plastic strain</t>
+  </si>
+  <si>
+    <t>corrosion potential</t>
+  </si>
+  <si>
+    <t>corrosion current density</t>
+  </si>
+  <si>
+    <t>pitting potential</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>A/m^2</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>T6</t>
+  </si>
+  <si>
+    <t>3.5 wt% NaCl</t>
+  </si>
+  <si>
+    <t>10.1007/s40195-020-01072-6</t>
   </si>
 </sst>
 </file>
@@ -1194,7 +1281,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="58">
+  <borders count="59">
     <border>
       <left/>
       <right/>
@@ -2033,11 +2120,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2353,6 +2451,9 @@
     <xf numFmtId="164" fontId="5" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="14" fillId="10" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3515,8 +3616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T960"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A185" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N203" sqref="N203"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A248" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N268" sqref="N268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -12168,20 +12269,42 @@
       <c r="T199" s="37"/>
     </row>
     <row r="200" spans="1:20" ht="18" customHeight="1">
-      <c r="A200" s="40"/>
-      <c r="B200" s="31"/>
-      <c r="C200" s="30"/>
-      <c r="D200" s="30"/>
-      <c r="E200" s="31"/>
-      <c r="F200" s="52"/>
-      <c r="G200" s="32"/>
+      <c r="A200" s="40" t="s">
+        <v>309</v>
+      </c>
+      <c r="B200" s="31" t="s">
+        <v>300</v>
+      </c>
+      <c r="C200" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D200" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="E200" s="31" t="s">
+        <v>311</v>
+      </c>
+      <c r="F200" s="153" t="s">
+        <v>122</v>
+      </c>
+      <c r="G200" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H200" s="56"/>
       <c r="I200" s="54"/>
-      <c r="J200" s="35"/>
+      <c r="J200" s="35">
+        <v>1516</v>
+      </c>
       <c r="K200" s="35"/>
-      <c r="L200" s="40"/>
-      <c r="M200" s="40"/>
-      <c r="N200" s="30"/>
+      <c r="L200" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="M200" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="N200" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O200" s="37"/>
       <c r="P200" s="38"/>
       <c r="Q200" s="38"/>
@@ -12190,20 +12313,42 @@
       <c r="T200" s="37"/>
     </row>
     <row r="201" spans="1:20" ht="18" customHeight="1">
-      <c r="A201" s="40"/>
-      <c r="B201" s="41"/>
-      <c r="C201" s="30"/>
-      <c r="D201" s="30"/>
+      <c r="A201" s="40" t="s">
+        <v>282</v>
+      </c>
+      <c r="B201" s="31" t="s">
+        <v>295</v>
+      </c>
+      <c r="C201" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D201" s="30" t="s">
+        <v>131</v>
+      </c>
       <c r="E201" s="31"/>
-      <c r="F201" s="52"/>
+      <c r="F201" s="52" t="s">
+        <v>194</v>
+      </c>
       <c r="G201" s="32"/>
-      <c r="H201" s="56"/>
-      <c r="I201" s="54"/>
-      <c r="J201" s="35"/>
+      <c r="H201" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I201" s="54">
+        <v>298</v>
+      </c>
+      <c r="J201" s="35">
+        <v>199000000</v>
+      </c>
       <c r="K201" s="35"/>
-      <c r="L201" s="40"/>
-      <c r="M201" s="40"/>
-      <c r="N201" s="30"/>
+      <c r="L201" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M201" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N201" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O201" s="37"/>
       <c r="P201" s="38"/>
       <c r="Q201" s="38"/>
@@ -12212,20 +12357,44 @@
       <c r="T201" s="37"/>
     </row>
     <row r="202" spans="1:20" ht="18" customHeight="1">
-      <c r="A202" s="40"/>
-      <c r="B202" s="41"/>
-      <c r="C202" s="30"/>
-      <c r="D202" s="30"/>
-      <c r="E202" s="31"/>
-      <c r="F202" s="52"/>
+      <c r="A202" s="40" t="s">
+        <v>303</v>
+      </c>
+      <c r="B202" s="31" t="s">
+        <v>296</v>
+      </c>
+      <c r="C202" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D202" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="E202" s="31" t="s">
+        <v>310</v>
+      </c>
+      <c r="F202" s="52" t="s">
+        <v>194</v>
+      </c>
       <c r="G202" s="32"/>
-      <c r="H202" s="56"/>
-      <c r="I202" s="54"/>
-      <c r="J202" s="35"/>
+      <c r="H202" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I202" s="54">
+        <v>298</v>
+      </c>
+      <c r="J202" s="35">
+        <v>261700000</v>
+      </c>
       <c r="K202" s="35"/>
-      <c r="L202" s="40"/>
-      <c r="M202" s="40"/>
-      <c r="N202" s="30"/>
+      <c r="L202" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M202" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N202" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O202" s="37"/>
       <c r="P202" s="38"/>
       <c r="Q202" s="38"/>
@@ -12234,20 +12403,44 @@
       <c r="T202" s="37"/>
     </row>
     <row r="203" spans="1:20" ht="18" customHeight="1">
-      <c r="A203" s="40"/>
-      <c r="B203" s="41"/>
-      <c r="C203" s="30"/>
-      <c r="D203" s="30"/>
-      <c r="E203" s="31"/>
-      <c r="F203" s="52"/>
+      <c r="A203" s="40" t="s">
+        <v>304</v>
+      </c>
+      <c r="B203" s="31" t="s">
+        <v>297</v>
+      </c>
+      <c r="C203" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D203" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="E203" s="31" t="s">
+        <v>310</v>
+      </c>
+      <c r="F203" s="52" t="s">
+        <v>194</v>
+      </c>
       <c r="G203" s="32"/>
-      <c r="H203" s="47"/>
-      <c r="I203" s="54"/>
-      <c r="J203" s="58"/>
+      <c r="H203" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I203" s="54">
+        <v>298</v>
+      </c>
+      <c r="J203" s="58">
+        <v>476400000</v>
+      </c>
       <c r="K203" s="51"/>
-      <c r="L203" s="40"/>
-      <c r="M203" s="40"/>
-      <c r="N203" s="30"/>
+      <c r="L203" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M203" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N203" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O203" s="37"/>
       <c r="P203" s="38"/>
       <c r="Q203" s="38"/>
@@ -12256,20 +12449,44 @@
       <c r="T203" s="37"/>
     </row>
     <row r="204" spans="1:20" ht="18" customHeight="1">
-      <c r="A204" s="40"/>
-      <c r="B204" s="31"/>
-      <c r="C204" s="30"/>
-      <c r="D204" s="30"/>
-      <c r="E204" s="31"/>
-      <c r="F204" s="52"/>
+      <c r="A204" s="40" t="s">
+        <v>305</v>
+      </c>
+      <c r="B204" s="31" t="s">
+        <v>298</v>
+      </c>
+      <c r="C204" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D204" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="E204" s="31" t="s">
+        <v>310</v>
+      </c>
+      <c r="F204" s="52" t="s">
+        <v>194</v>
+      </c>
       <c r="G204" s="32"/>
-      <c r="H204" s="47"/>
-      <c r="I204" s="54"/>
-      <c r="J204" s="58"/>
+      <c r="H204" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I204" s="54">
+        <v>298</v>
+      </c>
+      <c r="J204" s="58">
+        <v>883400000</v>
+      </c>
       <c r="K204" s="51"/>
-      <c r="L204" s="40"/>
-      <c r="M204" s="40"/>
-      <c r="N204" s="30"/>
+      <c r="L204" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M204" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N204" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O204" s="37"/>
       <c r="P204" s="38"/>
       <c r="Q204" s="38"/>
@@ -12278,20 +12495,44 @@
       <c r="T204" s="37"/>
     </row>
     <row r="205" spans="1:20" ht="18" customHeight="1">
-      <c r="A205" s="40"/>
-      <c r="B205" s="41"/>
-      <c r="C205" s="30"/>
-      <c r="D205" s="30"/>
-      <c r="E205" s="31"/>
-      <c r="F205" s="52"/>
+      <c r="A205" s="40" t="s">
+        <v>306</v>
+      </c>
+      <c r="B205" s="31" t="s">
+        <v>299</v>
+      </c>
+      <c r="C205" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D205" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="E205" s="31" t="s">
+        <v>310</v>
+      </c>
+      <c r="F205" s="52" t="s">
+        <v>194</v>
+      </c>
       <c r="G205" s="32"/>
-      <c r="H205" s="47"/>
-      <c r="I205" s="54"/>
-      <c r="J205" s="58"/>
+      <c r="H205" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I205" s="54">
+        <v>298</v>
+      </c>
+      <c r="J205" s="58">
+        <v>1118200000</v>
+      </c>
       <c r="K205" s="51"/>
-      <c r="L205" s="40"/>
-      <c r="M205" s="40"/>
-      <c r="N205" s="30"/>
+      <c r="L205" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M205" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N205" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O205" s="37"/>
       <c r="P205" s="38"/>
       <c r="Q205" s="38"/>
@@ -12300,20 +12541,44 @@
       <c r="T205" s="37"/>
     </row>
     <row r="206" spans="1:20" ht="18" customHeight="1">
-      <c r="A206" s="40"/>
-      <c r="B206" s="41"/>
-      <c r="C206" s="30"/>
-      <c r="D206" s="30"/>
-      <c r="E206" s="31"/>
-      <c r="F206" s="52"/>
+      <c r="A206" s="40" t="s">
+        <v>309</v>
+      </c>
+      <c r="B206" s="31" t="s">
+        <v>300</v>
+      </c>
+      <c r="C206" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D206" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="E206" s="31" t="s">
+        <v>311</v>
+      </c>
+      <c r="F206" s="52" t="s">
+        <v>194</v>
+      </c>
       <c r="G206" s="32"/>
-      <c r="H206" s="47"/>
-      <c r="I206" s="54"/>
-      <c r="J206" s="58"/>
+      <c r="H206" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I206" s="54">
+        <v>298</v>
+      </c>
+      <c r="J206" s="58">
+        <v>1449200000</v>
+      </c>
       <c r="K206" s="51"/>
-      <c r="L206" s="40"/>
-      <c r="M206" s="40"/>
-      <c r="N206" s="30"/>
+      <c r="L206" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M206" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N206" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O206" s="37"/>
       <c r="P206" s="38"/>
       <c r="Q206" s="38"/>
@@ -12322,20 +12587,44 @@
       <c r="T206" s="37"/>
     </row>
     <row r="207" spans="1:20" ht="18" customHeight="1">
-      <c r="A207" s="40"/>
-      <c r="B207" s="102"/>
-      <c r="C207" s="90"/>
-      <c r="D207" s="90"/>
-      <c r="E207" s="103"/>
-      <c r="F207" s="97"/>
+      <c r="A207" s="40" t="s">
+        <v>307</v>
+      </c>
+      <c r="B207" s="31" t="s">
+        <v>301</v>
+      </c>
+      <c r="C207" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D207" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="E207" s="31" t="s">
+        <v>312</v>
+      </c>
+      <c r="F207" s="52" t="s">
+        <v>194</v>
+      </c>
       <c r="G207" s="97"/>
-      <c r="H207" s="47"/>
-      <c r="I207" s="54"/>
-      <c r="J207" s="37"/>
+      <c r="H207" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I207" s="54">
+        <v>298</v>
+      </c>
+      <c r="J207" s="58">
+        <v>1469300000</v>
+      </c>
       <c r="K207" s="38"/>
-      <c r="L207" s="40"/>
-      <c r="M207" s="40"/>
-      <c r="N207" s="30"/>
+      <c r="L207" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M207" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N207" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O207" s="37"/>
       <c r="P207" s="38"/>
       <c r="Q207" s="38"/>
@@ -12344,20 +12633,44 @@
       <c r="T207" s="37"/>
     </row>
     <row r="208" spans="1:20" ht="18" customHeight="1">
-      <c r="A208" s="40"/>
-      <c r="B208" s="104"/>
-      <c r="C208" s="91"/>
-      <c r="D208" s="91"/>
-      <c r="E208" s="105"/>
-      <c r="F208" s="97"/>
+      <c r="A208" s="40" t="s">
+        <v>308</v>
+      </c>
+      <c r="B208" s="31" t="s">
+        <v>302</v>
+      </c>
+      <c r="C208" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D208" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="E208" s="31" t="s">
+        <v>312</v>
+      </c>
+      <c r="F208" s="52" t="s">
+        <v>194</v>
+      </c>
       <c r="G208" s="98"/>
-      <c r="H208" s="47"/>
-      <c r="I208" s="54"/>
-      <c r="J208" s="37"/>
+      <c r="H208" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I208" s="54">
+        <v>298</v>
+      </c>
+      <c r="J208" s="58">
+        <v>1310500000</v>
+      </c>
       <c r="K208" s="38"/>
-      <c r="L208" s="40"/>
-      <c r="M208" s="40"/>
-      <c r="N208" s="30"/>
+      <c r="L208" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M208" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N208" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O208" s="37"/>
       <c r="P208" s="38"/>
       <c r="Q208" s="38"/>
@@ -12366,20 +12679,42 @@
       <c r="T208" s="37"/>
     </row>
     <row r="209" spans="1:20" ht="18" customHeight="1">
-      <c r="A209" s="40"/>
-      <c r="B209" s="104"/>
-      <c r="C209" s="91"/>
-      <c r="D209" s="91"/>
-      <c r="E209" s="105"/>
-      <c r="F209" s="97"/>
+      <c r="A209" s="40" t="s">
+        <v>282</v>
+      </c>
+      <c r="B209" s="31" t="s">
+        <v>295</v>
+      </c>
+      <c r="C209" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D209" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="E209" s="31"/>
+      <c r="F209" s="97" t="s">
+        <v>273</v>
+      </c>
       <c r="G209" s="98"/>
-      <c r="H209" s="47"/>
-      <c r="I209" s="54"/>
-      <c r="J209" s="37"/>
+      <c r="H209" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I209" s="54">
+        <v>298</v>
+      </c>
+      <c r="J209" s="58">
+        <v>2250000000</v>
+      </c>
       <c r="K209" s="38"/>
-      <c r="L209" s="40"/>
-      <c r="M209" s="40"/>
-      <c r="N209" s="30"/>
+      <c r="L209" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M209" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N209" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O209" s="37"/>
       <c r="P209" s="38"/>
       <c r="Q209" s="38"/>
@@ -12388,20 +12723,44 @@
       <c r="T209" s="37"/>
     </row>
     <row r="210" spans="1:20" ht="18" customHeight="1">
-      <c r="A210" s="40"/>
-      <c r="B210" s="104"/>
-      <c r="C210" s="91"/>
-      <c r="D210" s="91"/>
-      <c r="E210" s="105"/>
-      <c r="F210" s="97"/>
+      <c r="A210" s="40" t="s">
+        <v>303</v>
+      </c>
+      <c r="B210" s="31" t="s">
+        <v>296</v>
+      </c>
+      <c r="C210" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D210" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="E210" s="31" t="s">
+        <v>310</v>
+      </c>
+      <c r="F210" s="97" t="s">
+        <v>273</v>
+      </c>
       <c r="G210" s="98"/>
-      <c r="H210" s="47"/>
-      <c r="I210" s="54"/>
-      <c r="J210" s="37"/>
+      <c r="H210" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I210" s="54">
+        <v>298</v>
+      </c>
+      <c r="J210" s="58">
+        <v>2500000000</v>
+      </c>
       <c r="K210" s="38"/>
-      <c r="L210" s="40"/>
-      <c r="M210" s="40"/>
-      <c r="N210" s="30"/>
+      <c r="L210" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M210" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N210" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O210" s="37"/>
       <c r="P210" s="38"/>
       <c r="Q210" s="38"/>
@@ -12410,20 +12769,44 @@
       <c r="T210" s="37"/>
     </row>
     <row r="211" spans="1:20" ht="18" customHeight="1">
-      <c r="A211" s="40"/>
-      <c r="B211" s="102"/>
-      <c r="C211" s="90"/>
-      <c r="D211" s="90"/>
-      <c r="E211" s="103"/>
-      <c r="F211" s="97"/>
+      <c r="A211" s="40" t="s">
+        <v>304</v>
+      </c>
+      <c r="B211" s="31" t="s">
+        <v>297</v>
+      </c>
+      <c r="C211" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D211" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="E211" s="31" t="s">
+        <v>310</v>
+      </c>
+      <c r="F211" s="97" t="s">
+        <v>274</v>
+      </c>
       <c r="G211" s="97"/>
-      <c r="H211" s="47"/>
-      <c r="I211" s="54"/>
-      <c r="J211" s="58"/>
+      <c r="H211" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I211" s="54">
+        <v>298</v>
+      </c>
+      <c r="J211" s="58">
+        <v>2120100000</v>
+      </c>
       <c r="K211" s="38"/>
-      <c r="L211" s="40"/>
-      <c r="M211" s="40"/>
-      <c r="N211" s="30"/>
+      <c r="L211" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M211" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N211" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O211" s="37"/>
       <c r="P211" s="38"/>
       <c r="Q211" s="38"/>
@@ -12432,20 +12815,44 @@
       <c r="T211" s="37"/>
     </row>
     <row r="212" spans="1:20" ht="18" customHeight="1">
-      <c r="A212" s="40"/>
-      <c r="B212" s="104"/>
-      <c r="C212" s="91"/>
-      <c r="D212" s="91"/>
-      <c r="E212" s="105"/>
-      <c r="F212" s="97"/>
+      <c r="A212" s="40" t="s">
+        <v>305</v>
+      </c>
+      <c r="B212" s="31" t="s">
+        <v>298</v>
+      </c>
+      <c r="C212" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D212" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="E212" s="31" t="s">
+        <v>310</v>
+      </c>
+      <c r="F212" s="97" t="s">
+        <v>274</v>
+      </c>
       <c r="G212" s="98"/>
-      <c r="H212" s="47"/>
-      <c r="I212" s="54"/>
-      <c r="J212" s="58"/>
+      <c r="H212" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I212" s="54">
+        <v>298</v>
+      </c>
+      <c r="J212" s="58">
+        <v>2049700000</v>
+      </c>
       <c r="K212" s="38"/>
-      <c r="L212" s="40"/>
-      <c r="M212" s="40"/>
-      <c r="N212" s="30"/>
+      <c r="L212" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M212" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N212" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O212" s="37"/>
       <c r="P212" s="38"/>
       <c r="Q212" s="38"/>
@@ -12454,20 +12861,44 @@
       <c r="T212" s="37"/>
     </row>
     <row r="213" spans="1:20" ht="18" customHeight="1">
-      <c r="A213" s="40"/>
-      <c r="B213" s="104"/>
-      <c r="C213" s="91"/>
-      <c r="D213" s="91"/>
-      <c r="E213" s="105"/>
-      <c r="F213" s="97"/>
+      <c r="A213" s="40" t="s">
+        <v>306</v>
+      </c>
+      <c r="B213" s="31" t="s">
+        <v>299</v>
+      </c>
+      <c r="C213" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D213" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="E213" s="31" t="s">
+        <v>310</v>
+      </c>
+      <c r="F213" s="97" t="s">
+        <v>274</v>
+      </c>
       <c r="G213" s="98"/>
-      <c r="H213" s="47"/>
-      <c r="I213" s="54"/>
-      <c r="J213" s="58"/>
+      <c r="H213" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I213" s="54">
+        <v>298</v>
+      </c>
+      <c r="J213" s="58">
+        <v>2050800000</v>
+      </c>
       <c r="K213" s="38"/>
-      <c r="L213" s="40"/>
-      <c r="M213" s="40"/>
-      <c r="N213" s="30"/>
+      <c r="L213" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M213" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N213" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O213" s="37"/>
       <c r="P213" s="37"/>
       <c r="Q213" s="38"/>
@@ -12476,20 +12907,44 @@
       <c r="T213" s="37"/>
     </row>
     <row r="214" spans="1:20" ht="18" customHeight="1">
-      <c r="A214" s="40"/>
-      <c r="B214" s="104"/>
-      <c r="C214" s="91"/>
-      <c r="D214" s="91"/>
-      <c r="E214" s="105"/>
-      <c r="F214" s="97"/>
+      <c r="A214" s="40" t="s">
+        <v>309</v>
+      </c>
+      <c r="B214" s="31" t="s">
+        <v>300</v>
+      </c>
+      <c r="C214" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D214" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="E214" s="31" t="s">
+        <v>311</v>
+      </c>
+      <c r="F214" s="97" t="s">
+        <v>274</v>
+      </c>
       <c r="G214" s="98"/>
-      <c r="H214" s="47"/>
-      <c r="I214" s="54"/>
-      <c r="J214" s="58"/>
+      <c r="H214" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I214" s="54">
+        <v>298</v>
+      </c>
+      <c r="J214" s="58">
+        <v>2191700000</v>
+      </c>
       <c r="K214" s="38"/>
-      <c r="L214" s="40"/>
-      <c r="M214" s="40"/>
-      <c r="N214" s="30"/>
+      <c r="L214" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M214" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N214" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O214" s="37"/>
       <c r="P214" s="44"/>
       <c r="Q214" s="38"/>
@@ -12498,20 +12953,44 @@
       <c r="T214" s="37"/>
     </row>
     <row r="215" spans="1:20" ht="18" customHeight="1">
-      <c r="A215" s="40"/>
-      <c r="B215" s="31"/>
-      <c r="C215" s="30"/>
-      <c r="D215" s="30"/>
-      <c r="E215" s="31"/>
-      <c r="F215" s="53"/>
+      <c r="A215" s="40" t="s">
+        <v>307</v>
+      </c>
+      <c r="B215" s="31" t="s">
+        <v>301</v>
+      </c>
+      <c r="C215" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D215" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="E215" s="31" t="s">
+        <v>312</v>
+      </c>
+      <c r="F215" s="97" t="s">
+        <v>274</v>
+      </c>
       <c r="G215" s="98"/>
-      <c r="H215" s="47"/>
-      <c r="I215" s="54"/>
-      <c r="J215" s="89"/>
+      <c r="H215" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I215" s="54">
+        <v>298</v>
+      </c>
+      <c r="J215" s="89">
+        <v>2433200000</v>
+      </c>
       <c r="K215" s="51"/>
-      <c r="L215" s="40"/>
-      <c r="M215" s="40"/>
-      <c r="N215" s="40"/>
+      <c r="L215" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M215" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N215" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O215" s="37"/>
       <c r="P215" s="44"/>
       <c r="Q215" s="38"/>
@@ -12520,20 +12999,44 @@
       <c r="T215" s="37"/>
     </row>
     <row r="216" spans="1:20" ht="18" customHeight="1">
-      <c r="A216" s="40"/>
-      <c r="B216" s="31"/>
-      <c r="C216" s="30"/>
-      <c r="D216" s="30"/>
-      <c r="E216" s="31"/>
-      <c r="F216" s="53"/>
+      <c r="A216" s="40" t="s">
+        <v>308</v>
+      </c>
+      <c r="B216" s="31" t="s">
+        <v>302</v>
+      </c>
+      <c r="C216" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D216" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="E216" s="31" t="s">
+        <v>312</v>
+      </c>
+      <c r="F216" s="97" t="s">
+        <v>274</v>
+      </c>
       <c r="G216" s="98"/>
-      <c r="H216" s="47"/>
-      <c r="I216" s="54"/>
-      <c r="J216" s="89"/>
+      <c r="H216" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I216" s="54">
+        <v>298</v>
+      </c>
+      <c r="J216" s="89">
+        <v>1704200000</v>
+      </c>
       <c r="K216" s="51"/>
-      <c r="L216" s="40"/>
-      <c r="M216" s="40"/>
-      <c r="N216" s="40"/>
+      <c r="L216" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M216" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N216" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O216" s="44"/>
       <c r="P216" s="44"/>
       <c r="Q216" s="44"/>
@@ -12542,20 +13045,42 @@
       <c r="T216" s="37"/>
     </row>
     <row r="217" spans="1:20" ht="18" customHeight="1">
-      <c r="A217" s="40"/>
-      <c r="B217" s="31"/>
-      <c r="C217" s="30"/>
-      <c r="D217" s="30"/>
-      <c r="E217" s="31"/>
-      <c r="F217" s="53"/>
+      <c r="A217" s="154" t="s">
+        <v>282</v>
+      </c>
+      <c r="B217" s="103" t="s">
+        <v>295</v>
+      </c>
+      <c r="C217" s="90" t="s">
+        <v>63</v>
+      </c>
+      <c r="D217" s="90" t="s">
+        <v>131</v>
+      </c>
+      <c r="E217" s="103"/>
+      <c r="F217" s="53" t="s">
+        <v>314</v>
+      </c>
       <c r="G217" s="98"/>
-      <c r="H217" s="47"/>
-      <c r="I217" s="54"/>
-      <c r="J217" s="89"/>
+      <c r="H217" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I217" s="54">
+        <v>298</v>
+      </c>
+      <c r="J217" s="89">
+        <v>60</v>
+      </c>
       <c r="K217" s="51"/>
-      <c r="L217" s="40"/>
-      <c r="M217" s="40"/>
-      <c r="N217" s="40"/>
+      <c r="L217" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="M217" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N217" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O217" s="44"/>
       <c r="P217" s="44"/>
       <c r="Q217" s="44"/>
@@ -12564,20 +13089,44 @@
       <c r="T217" s="37"/>
     </row>
     <row r="218" spans="1:20" ht="18" customHeight="1">
-      <c r="A218" s="40"/>
-      <c r="B218" s="31"/>
-      <c r="C218" s="30"/>
-      <c r="D218" s="30"/>
-      <c r="E218" s="31"/>
-      <c r="F218" s="53"/>
+      <c r="A218" s="155" t="s">
+        <v>303</v>
+      </c>
+      <c r="B218" s="105" t="s">
+        <v>296</v>
+      </c>
+      <c r="C218" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D218" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E218" s="105" t="s">
+        <v>310</v>
+      </c>
+      <c r="F218" s="53" t="s">
+        <v>314</v>
+      </c>
       <c r="G218" s="98"/>
-      <c r="H218" s="47"/>
-      <c r="I218" s="54"/>
-      <c r="J218" s="89"/>
+      <c r="H218" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I218" s="54">
+        <v>298</v>
+      </c>
+      <c r="J218" s="89">
+        <v>60</v>
+      </c>
       <c r="K218" s="51"/>
-      <c r="L218" s="40"/>
-      <c r="M218" s="40"/>
-      <c r="N218" s="40"/>
+      <c r="L218" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="M218" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N218" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O218" s="44"/>
       <c r="P218" s="44"/>
       <c r="Q218" s="44"/>
@@ -12586,20 +13135,44 @@
       <c r="T218" s="37"/>
     </row>
     <row r="219" spans="1:20" ht="18" customHeight="1">
-      <c r="A219" s="40"/>
-      <c r="B219" s="31"/>
-      <c r="C219" s="30"/>
-      <c r="D219" s="30"/>
-      <c r="E219" s="31"/>
-      <c r="F219" s="53"/>
+      <c r="A219" s="155" t="s">
+        <v>304</v>
+      </c>
+      <c r="B219" s="105" t="s">
+        <v>297</v>
+      </c>
+      <c r="C219" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D219" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E219" s="105" t="s">
+        <v>310</v>
+      </c>
+      <c r="F219" s="53" t="s">
+        <v>313</v>
+      </c>
       <c r="G219" s="98"/>
-      <c r="H219" s="47"/>
-      <c r="I219" s="54"/>
-      <c r="J219" s="89"/>
+      <c r="H219" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I219" s="54">
+        <v>298</v>
+      </c>
+      <c r="J219" s="89">
+        <v>35.299999999999997</v>
+      </c>
       <c r="K219" s="38"/>
-      <c r="L219" s="40"/>
-      <c r="M219" s="40"/>
-      <c r="N219" s="40"/>
+      <c r="L219" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="M219" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N219" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O219" s="44"/>
       <c r="P219" s="44"/>
       <c r="Q219" s="44"/>
@@ -12608,20 +13181,44 @@
       <c r="T219" s="37"/>
     </row>
     <row r="220" spans="1:20" ht="18" customHeight="1">
-      <c r="A220" s="40"/>
-      <c r="B220" s="31"/>
-      <c r="C220" s="30"/>
-      <c r="D220" s="30"/>
-      <c r="E220" s="31"/>
-      <c r="F220" s="53"/>
+      <c r="A220" s="155" t="s">
+        <v>305</v>
+      </c>
+      <c r="B220" s="105" t="s">
+        <v>298</v>
+      </c>
+      <c r="C220" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D220" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E220" s="105" t="s">
+        <v>310</v>
+      </c>
+      <c r="F220" s="53" t="s">
+        <v>313</v>
+      </c>
       <c r="G220" s="98"/>
-      <c r="H220" s="47"/>
-      <c r="I220" s="54"/>
-      <c r="J220" s="89"/>
+      <c r="H220" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I220" s="54">
+        <v>298</v>
+      </c>
+      <c r="J220" s="89">
+        <v>23.1</v>
+      </c>
       <c r="K220" s="38"/>
-      <c r="L220" s="40"/>
-      <c r="M220" s="40"/>
-      <c r="N220" s="40"/>
+      <c r="L220" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="M220" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N220" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O220" s="44"/>
       <c r="P220" s="44"/>
       <c r="Q220" s="44"/>
@@ -12630,20 +13227,44 @@
       <c r="T220" s="37"/>
     </row>
     <row r="221" spans="1:20" ht="18" customHeight="1">
-      <c r="A221" s="40"/>
-      <c r="B221" s="41"/>
-      <c r="C221" s="30"/>
-      <c r="D221" s="30"/>
-      <c r="E221" s="31"/>
-      <c r="F221" s="53"/>
+      <c r="A221" s="155" t="s">
+        <v>306</v>
+      </c>
+      <c r="B221" s="105" t="s">
+        <v>299</v>
+      </c>
+      <c r="C221" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D221" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E221" s="105" t="s">
+        <v>310</v>
+      </c>
+      <c r="F221" s="53" t="s">
+        <v>313</v>
+      </c>
       <c r="G221" s="32"/>
-      <c r="H221" s="56"/>
-      <c r="I221" s="44"/>
-      <c r="J221" s="44"/>
+      <c r="H221" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I221" s="54">
+        <v>298</v>
+      </c>
+      <c r="J221" s="44">
+        <v>19.3</v>
+      </c>
       <c r="K221" s="38"/>
-      <c r="L221" s="40"/>
-      <c r="M221" s="40"/>
-      <c r="N221" s="40"/>
+      <c r="L221" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="M221" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N221" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O221" s="44"/>
       <c r="P221" s="44"/>
       <c r="Q221" s="44"/>
@@ -12652,20 +13273,44 @@
       <c r="T221" s="37"/>
     </row>
     <row r="222" spans="1:20" ht="18" customHeight="1">
-      <c r="A222" s="40"/>
-      <c r="B222" s="41"/>
-      <c r="C222" s="30"/>
-      <c r="D222" s="30"/>
-      <c r="E222" s="31"/>
-      <c r="F222" s="53"/>
+      <c r="A222" s="155" t="s">
+        <v>309</v>
+      </c>
+      <c r="B222" s="105" t="s">
+        <v>300</v>
+      </c>
+      <c r="C222" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D222" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E222" s="105" t="s">
+        <v>311</v>
+      </c>
+      <c r="F222" s="53" t="s">
+        <v>313</v>
+      </c>
       <c r="G222" s="32"/>
-      <c r="H222" s="56"/>
-      <c r="I222" s="44"/>
-      <c r="J222" s="44"/>
+      <c r="H222" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I222" s="54">
+        <v>298</v>
+      </c>
+      <c r="J222" s="44">
+        <v>17.399999999999999</v>
+      </c>
       <c r="K222" s="38"/>
-      <c r="L222" s="40"/>
-      <c r="M222" s="40"/>
-      <c r="N222" s="40"/>
+      <c r="L222" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="M222" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N222" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O222" s="44"/>
       <c r="P222" s="44"/>
       <c r="Q222" s="44"/>
@@ -12674,20 +13319,44 @@
       <c r="T222" s="37"/>
     </row>
     <row r="223" spans="1:20" ht="18" customHeight="1">
-      <c r="A223" s="40"/>
-      <c r="B223" s="41"/>
-      <c r="C223" s="30"/>
-      <c r="D223" s="30"/>
-      <c r="E223" s="31"/>
-      <c r="F223" s="53"/>
+      <c r="A223" s="155" t="s">
+        <v>307</v>
+      </c>
+      <c r="B223" s="105" t="s">
+        <v>301</v>
+      </c>
+      <c r="C223" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D223" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E223" s="105" t="s">
+        <v>312</v>
+      </c>
+      <c r="F223" s="53" t="s">
+        <v>313</v>
+      </c>
       <c r="G223" s="32"/>
-      <c r="H223" s="56"/>
-      <c r="I223" s="44"/>
-      <c r="J223" s="44"/>
+      <c r="H223" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I223" s="54">
+        <v>298</v>
+      </c>
+      <c r="J223" s="44">
+        <v>19.399999999999999</v>
+      </c>
       <c r="K223" s="38"/>
-      <c r="L223" s="40"/>
-      <c r="M223" s="40"/>
-      <c r="N223" s="40"/>
+      <c r="L223" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="M223" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N223" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O223" s="44"/>
       <c r="P223" s="44"/>
       <c r="Q223" s="44"/>
@@ -12696,20 +13365,44 @@
       <c r="T223" s="37"/>
     </row>
     <row r="224" spans="1:20" ht="18" customHeight="1">
-      <c r="A224" s="40"/>
-      <c r="B224" s="41"/>
-      <c r="C224" s="30"/>
-      <c r="D224" s="30"/>
-      <c r="E224" s="31"/>
-      <c r="F224" s="53"/>
+      <c r="A224" s="155" t="s">
+        <v>308</v>
+      </c>
+      <c r="B224" s="105" t="s">
+        <v>302</v>
+      </c>
+      <c r="C224" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D224" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E224" s="105" t="s">
+        <v>312</v>
+      </c>
+      <c r="F224" s="53" t="s">
+        <v>313</v>
+      </c>
       <c r="G224" s="32"/>
-      <c r="H224" s="56"/>
-      <c r="I224" s="44"/>
-      <c r="J224" s="44"/>
+      <c r="H224" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I224" s="54">
+        <v>298</v>
+      </c>
+      <c r="J224" s="44">
+        <v>3.7</v>
+      </c>
       <c r="K224" s="38"/>
-      <c r="L224" s="40"/>
-      <c r="M224" s="40"/>
-      <c r="N224" s="40"/>
+      <c r="L224" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="M224" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N224" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O224" s="44"/>
       <c r="P224" s="44"/>
       <c r="Q224" s="44"/>
@@ -12718,20 +13411,42 @@
       <c r="T224" s="37"/>
     </row>
     <row r="225" spans="1:20" ht="18" customHeight="1">
-      <c r="A225" s="40"/>
-      <c r="B225" s="41"/>
-      <c r="C225" s="30"/>
-      <c r="D225" s="30"/>
-      <c r="E225" s="31"/>
-      <c r="F225" s="53"/>
+      <c r="A225" s="154" t="s">
+        <v>282</v>
+      </c>
+      <c r="B225" s="103" t="s">
+        <v>295</v>
+      </c>
+      <c r="C225" s="90" t="s">
+        <v>63</v>
+      </c>
+      <c r="D225" s="90" t="s">
+        <v>131</v>
+      </c>
+      <c r="E225" s="103"/>
+      <c r="F225" s="53" t="s">
+        <v>272</v>
+      </c>
       <c r="G225" s="32"/>
-      <c r="H225" s="56"/>
-      <c r="I225" s="44"/>
-      <c r="J225" s="44"/>
+      <c r="H225" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I225" s="54">
+        <v>298</v>
+      </c>
+      <c r="J225" s="44">
+        <v>60</v>
+      </c>
       <c r="K225" s="38"/>
-      <c r="L225" s="40"/>
-      <c r="M225" s="40"/>
-      <c r="N225" s="40"/>
+      <c r="L225" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="M225" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N225" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O225" s="44"/>
       <c r="P225" s="44"/>
       <c r="Q225" s="44"/>
@@ -12740,20 +13455,44 @@
       <c r="T225" s="37"/>
     </row>
     <row r="226" spans="1:20" ht="18" customHeight="1">
-      <c r="A226" s="40"/>
-      <c r="B226" s="41"/>
-      <c r="C226" s="30"/>
-      <c r="D226" s="30"/>
-      <c r="E226" s="31"/>
-      <c r="F226" s="53"/>
+      <c r="A226" s="155" t="s">
+        <v>303</v>
+      </c>
+      <c r="B226" s="105" t="s">
+        <v>296</v>
+      </c>
+      <c r="C226" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D226" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E226" s="105" t="s">
+        <v>310</v>
+      </c>
+      <c r="F226" s="53" t="s">
+        <v>272</v>
+      </c>
       <c r="G226" s="32"/>
-      <c r="H226" s="56"/>
-      <c r="I226" s="44"/>
-      <c r="J226" s="44"/>
+      <c r="H226" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I226" s="54">
+        <v>298</v>
+      </c>
+      <c r="J226" s="44">
+        <v>60</v>
+      </c>
       <c r="K226" s="38"/>
-      <c r="L226" s="40"/>
-      <c r="M226" s="40"/>
-      <c r="N226" s="40"/>
+      <c r="L226" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="M226" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N226" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O226" s="44"/>
       <c r="P226" s="44"/>
       <c r="Q226" s="44"/>
@@ -12762,20 +13501,44 @@
       <c r="T226" s="37"/>
     </row>
     <row r="227" spans="1:20" ht="18" customHeight="1">
-      <c r="A227" s="40"/>
-      <c r="B227" s="41"/>
-      <c r="C227" s="30"/>
-      <c r="D227" s="30"/>
-      <c r="E227" s="31"/>
-      <c r="F227" s="53"/>
+      <c r="A227" s="155" t="s">
+        <v>304</v>
+      </c>
+      <c r="B227" s="105" t="s">
+        <v>297</v>
+      </c>
+      <c r="C227" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D227" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E227" s="105" t="s">
+        <v>310</v>
+      </c>
+      <c r="F227" s="53" t="s">
+        <v>271</v>
+      </c>
       <c r="G227" s="32"/>
-      <c r="H227" s="56"/>
-      <c r="I227" s="44"/>
-      <c r="J227" s="44"/>
+      <c r="H227" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I227" s="54">
+        <v>298</v>
+      </c>
+      <c r="J227" s="44">
+        <v>45.3</v>
+      </c>
       <c r="K227" s="38"/>
-      <c r="L227" s="40"/>
-      <c r="M227" s="40"/>
-      <c r="N227" s="40"/>
+      <c r="L227" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="M227" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N227" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O227" s="44"/>
       <c r="P227" s="44"/>
       <c r="Q227" s="44"/>
@@ -12784,20 +13547,44 @@
       <c r="T227" s="37"/>
     </row>
     <row r="228" spans="1:20" ht="18" customHeight="1">
-      <c r="A228" s="40"/>
-      <c r="B228" s="41"/>
-      <c r="C228" s="30"/>
-      <c r="D228" s="30"/>
-      <c r="E228" s="31"/>
-      <c r="F228" s="53"/>
+      <c r="A228" s="155" t="s">
+        <v>305</v>
+      </c>
+      <c r="B228" s="105" t="s">
+        <v>298</v>
+      </c>
+      <c r="C228" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D228" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E228" s="105" t="s">
+        <v>310</v>
+      </c>
+      <c r="F228" s="53" t="s">
+        <v>271</v>
+      </c>
       <c r="G228" s="32"/>
-      <c r="H228" s="56"/>
-      <c r="I228" s="44"/>
-      <c r="J228" s="44"/>
+      <c r="H228" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I228" s="54">
+        <v>298</v>
+      </c>
+      <c r="J228" s="44">
+        <v>32.700000000000003</v>
+      </c>
       <c r="K228" s="38"/>
-      <c r="L228" s="40"/>
-      <c r="M228" s="40"/>
-      <c r="N228" s="40"/>
+      <c r="L228" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="M228" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N228" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O228" s="44"/>
       <c r="P228" s="44"/>
       <c r="Q228" s="44"/>
@@ -12806,20 +13593,44 @@
       <c r="T228" s="37"/>
     </row>
     <row r="229" spans="1:20" ht="18" customHeight="1">
-      <c r="A229" s="40"/>
-      <c r="B229" s="41"/>
-      <c r="C229" s="30"/>
-      <c r="D229" s="30"/>
-      <c r="E229" s="31"/>
-      <c r="F229" s="53"/>
+      <c r="A229" s="155" t="s">
+        <v>306</v>
+      </c>
+      <c r="B229" s="105" t="s">
+        <v>299</v>
+      </c>
+      <c r="C229" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D229" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E229" s="105" t="s">
+        <v>310</v>
+      </c>
+      <c r="F229" s="53" t="s">
+        <v>271</v>
+      </c>
       <c r="G229" s="32"/>
-      <c r="H229" s="56"/>
-      <c r="I229" s="44"/>
-      <c r="J229" s="44"/>
+      <c r="H229" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I229" s="54">
+        <v>298</v>
+      </c>
+      <c r="J229" s="44">
+        <v>28.2</v>
+      </c>
       <c r="K229" s="38"/>
-      <c r="L229" s="40"/>
-      <c r="M229" s="40"/>
-      <c r="N229" s="40"/>
+      <c r="L229" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="M229" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N229" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O229" s="44"/>
       <c r="P229" s="44"/>
       <c r="Q229" s="44"/>
@@ -12828,20 +13639,44 @@
       <c r="T229" s="37"/>
     </row>
     <row r="230" spans="1:20" ht="18" customHeight="1">
-      <c r="A230" s="40"/>
-      <c r="B230" s="41"/>
-      <c r="C230" s="30"/>
-      <c r="D230" s="30"/>
-      <c r="E230" s="31"/>
-      <c r="F230" s="53"/>
+      <c r="A230" s="155" t="s">
+        <v>309</v>
+      </c>
+      <c r="B230" s="105" t="s">
+        <v>300</v>
+      </c>
+      <c r="C230" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D230" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E230" s="105" t="s">
+        <v>311</v>
+      </c>
+      <c r="F230" s="53" t="s">
+        <v>271</v>
+      </c>
       <c r="G230" s="32"/>
-      <c r="H230" s="56"/>
-      <c r="I230" s="44"/>
-      <c r="J230" s="44"/>
+      <c r="H230" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I230" s="54">
+        <v>298</v>
+      </c>
+      <c r="J230" s="44">
+        <v>26.7</v>
+      </c>
       <c r="K230" s="38"/>
-      <c r="L230" s="40"/>
-      <c r="M230" s="40"/>
-      <c r="N230" s="40"/>
+      <c r="L230" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="M230" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N230" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O230" s="44"/>
       <c r="P230" s="44"/>
       <c r="Q230" s="44"/>
@@ -12850,20 +13685,44 @@
       <c r="T230" s="37"/>
     </row>
     <row r="231" spans="1:20" ht="18" customHeight="1">
-      <c r="A231" s="40"/>
-      <c r="B231" s="41"/>
-      <c r="C231" s="30"/>
-      <c r="D231" s="30"/>
-      <c r="E231" s="31"/>
-      <c r="F231" s="53"/>
+      <c r="A231" s="155" t="s">
+        <v>307</v>
+      </c>
+      <c r="B231" s="105" t="s">
+        <v>301</v>
+      </c>
+      <c r="C231" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D231" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E231" s="105" t="s">
+        <v>312</v>
+      </c>
+      <c r="F231" s="53" t="s">
+        <v>271</v>
+      </c>
       <c r="G231" s="32"/>
-      <c r="H231" s="56"/>
-      <c r="I231" s="44"/>
-      <c r="J231" s="44"/>
+      <c r="H231" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I231" s="54">
+        <v>298</v>
+      </c>
+      <c r="J231" s="44">
+        <v>27.7</v>
+      </c>
       <c r="K231" s="38"/>
-      <c r="L231" s="40"/>
-      <c r="M231" s="40"/>
-      <c r="N231" s="40"/>
+      <c r="L231" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="M231" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N231" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O231" s="44"/>
       <c r="P231" s="44"/>
       <c r="Q231" s="44"/>
@@ -12872,20 +13731,44 @@
       <c r="T231" s="37"/>
     </row>
     <row r="232" spans="1:20" ht="18" customHeight="1">
-      <c r="A232" s="40"/>
-      <c r="B232" s="41"/>
-      <c r="C232" s="30"/>
-      <c r="D232" s="30"/>
-      <c r="E232" s="31"/>
-      <c r="F232" s="53"/>
+      <c r="A232" s="155" t="s">
+        <v>308</v>
+      </c>
+      <c r="B232" s="105" t="s">
+        <v>302</v>
+      </c>
+      <c r="C232" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D232" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E232" s="105" t="s">
+        <v>312</v>
+      </c>
+      <c r="F232" s="53" t="s">
+        <v>271</v>
+      </c>
       <c r="G232" s="32"/>
-      <c r="H232" s="56"/>
-      <c r="I232" s="44"/>
-      <c r="J232" s="44"/>
+      <c r="H232" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="I232" s="54">
+        <v>298</v>
+      </c>
+      <c r="J232" s="44">
+        <v>10.5</v>
+      </c>
       <c r="K232" s="38"/>
-      <c r="L232" s="40"/>
-      <c r="M232" s="40"/>
-      <c r="N232" s="40"/>
+      <c r="L232" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="M232" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N232" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O232" s="44"/>
       <c r="P232" s="44"/>
       <c r="Q232" s="44"/>
@@ -12894,704 +13777,1544 @@
       <c r="T232" s="37"/>
     </row>
     <row r="233" spans="1:20" ht="18" customHeight="1">
-      <c r="A233" s="40"/>
-      <c r="B233" s="41"/>
-      <c r="C233" s="30"/>
-      <c r="D233" s="30"/>
-      <c r="E233" s="31"/>
-      <c r="F233" s="53"/>
+      <c r="A233" s="154" t="s">
+        <v>282</v>
+      </c>
+      <c r="B233" s="103" t="s">
+        <v>295</v>
+      </c>
+      <c r="C233" s="90" t="s">
+        <v>63</v>
+      </c>
+      <c r="D233" s="90" t="s">
+        <v>131</v>
+      </c>
+      <c r="E233" s="103"/>
+      <c r="F233" s="53" t="s">
+        <v>179</v>
+      </c>
       <c r="G233" s="32"/>
       <c r="H233" s="56"/>
-      <c r="I233" s="44"/>
-      <c r="J233" s="44"/>
+      <c r="I233" s="54">
+        <v>298</v>
+      </c>
+      <c r="J233" s="35">
+        <f t="shared" ref="J233:J248" si="6">P233*9807000</f>
+        <v>1447513200</v>
+      </c>
       <c r="K233" s="38"/>
-      <c r="L233" s="40"/>
-      <c r="M233" s="40"/>
-      <c r="N233" s="40"/>
+      <c r="L233" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M233" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N233" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O233" s="44"/>
-      <c r="P233" s="44"/>
+      <c r="P233" s="44">
+        <v>147.6</v>
+      </c>
       <c r="Q233" s="44"/>
       <c r="R233" s="37"/>
       <c r="S233" s="37"/>
       <c r="T233" s="37"/>
     </row>
     <row r="234" spans="1:20" ht="18" customHeight="1">
-      <c r="A234" s="40"/>
-      <c r="B234" s="41"/>
-      <c r="C234" s="30"/>
-      <c r="D234" s="30"/>
-      <c r="E234" s="31"/>
-      <c r="F234" s="53"/>
+      <c r="A234" s="155" t="s">
+        <v>303</v>
+      </c>
+      <c r="B234" s="105" t="s">
+        <v>296</v>
+      </c>
+      <c r="C234" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D234" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E234" s="105" t="s">
+        <v>310</v>
+      </c>
+      <c r="F234" s="53" t="s">
+        <v>179</v>
+      </c>
       <c r="G234" s="32"/>
       <c r="H234" s="56"/>
-      <c r="I234" s="44"/>
-      <c r="J234" s="44"/>
+      <c r="I234" s="54">
+        <v>298</v>
+      </c>
+      <c r="J234" s="35">
+        <f t="shared" si="6"/>
+        <v>2124196200</v>
+      </c>
       <c r="K234" s="38"/>
-      <c r="L234" s="40"/>
-      <c r="M234" s="40"/>
-      <c r="N234" s="40"/>
+      <c r="L234" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M234" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N234" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O234" s="44"/>
-      <c r="P234" s="44"/>
+      <c r="P234" s="44">
+        <v>216.6</v>
+      </c>
       <c r="Q234" s="44"/>
       <c r="R234" s="37"/>
       <c r="S234" s="37"/>
       <c r="T234" s="37"/>
     </row>
     <row r="235" spans="1:20" ht="18" customHeight="1">
-      <c r="A235" s="40"/>
-      <c r="B235" s="41"/>
-      <c r="C235" s="30"/>
-      <c r="D235" s="30"/>
-      <c r="E235" s="31"/>
-      <c r="F235" s="53"/>
+      <c r="A235" s="155" t="s">
+        <v>304</v>
+      </c>
+      <c r="B235" s="105" t="s">
+        <v>297</v>
+      </c>
+      <c r="C235" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D235" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E235" s="105" t="s">
+        <v>310</v>
+      </c>
+      <c r="F235" s="53" t="s">
+        <v>179</v>
+      </c>
       <c r="G235" s="32"/>
       <c r="H235" s="56"/>
-      <c r="I235" s="44"/>
-      <c r="J235" s="44"/>
+      <c r="I235" s="54">
+        <v>298</v>
+      </c>
+      <c r="J235" s="35">
+        <f t="shared" si="6"/>
+        <v>2653774200</v>
+      </c>
       <c r="K235" s="38"/>
-      <c r="L235" s="40"/>
-      <c r="M235" s="40"/>
-      <c r="N235" s="40"/>
+      <c r="L235" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M235" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N235" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O235" s="44"/>
-      <c r="P235" s="44"/>
+      <c r="P235" s="44">
+        <v>270.60000000000002</v>
+      </c>
       <c r="Q235" s="44"/>
       <c r="R235" s="37"/>
       <c r="S235" s="37"/>
       <c r="T235" s="37"/>
     </row>
     <row r="236" spans="1:20" ht="18" customHeight="1">
-      <c r="A236" s="40"/>
-      <c r="B236" s="41"/>
-      <c r="C236" s="30"/>
-      <c r="D236" s="30"/>
-      <c r="E236" s="31"/>
-      <c r="F236" s="53"/>
+      <c r="A236" s="155" t="s">
+        <v>305</v>
+      </c>
+      <c r="B236" s="105" t="s">
+        <v>298</v>
+      </c>
+      <c r="C236" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D236" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E236" s="105" t="s">
+        <v>310</v>
+      </c>
+      <c r="F236" s="53" t="s">
+        <v>179</v>
+      </c>
       <c r="G236" s="32"/>
       <c r="H236" s="56"/>
-      <c r="I236" s="44"/>
-      <c r="J236" s="44"/>
+      <c r="I236" s="54">
+        <v>298</v>
+      </c>
+      <c r="J236" s="35">
+        <f t="shared" si="6"/>
+        <v>3360858900</v>
+      </c>
       <c r="K236" s="38"/>
-      <c r="L236" s="40"/>
-      <c r="M236" s="40"/>
-      <c r="N236" s="40"/>
+      <c r="L236" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M236" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N236" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O236" s="44"/>
-      <c r="P236" s="44"/>
+      <c r="P236" s="44">
+        <v>342.7</v>
+      </c>
       <c r="Q236" s="44"/>
       <c r="R236" s="37"/>
       <c r="S236" s="37"/>
       <c r="T236" s="37"/>
     </row>
     <row r="237" spans="1:20" ht="18" customHeight="1">
-      <c r="A237" s="40"/>
-      <c r="B237" s="41"/>
-      <c r="C237" s="30"/>
-      <c r="D237" s="30"/>
-      <c r="E237" s="31"/>
-      <c r="F237" s="53"/>
+      <c r="A237" s="155" t="s">
+        <v>306</v>
+      </c>
+      <c r="B237" s="105" t="s">
+        <v>299</v>
+      </c>
+      <c r="C237" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D237" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E237" s="105" t="s">
+        <v>310</v>
+      </c>
+      <c r="F237" s="53" t="s">
+        <v>179</v>
+      </c>
       <c r="G237" s="32"/>
       <c r="H237" s="56"/>
-      <c r="I237" s="44"/>
-      <c r="J237" s="44"/>
+      <c r="I237" s="54">
+        <v>298</v>
+      </c>
+      <c r="J237" s="35">
+        <f t="shared" si="6"/>
+        <v>3859054500</v>
+      </c>
       <c r="K237" s="38"/>
-      <c r="L237" s="40"/>
-      <c r="M237" s="40"/>
-      <c r="N237" s="40"/>
+      <c r="L237" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M237" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N237" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O237" s="44"/>
-      <c r="P237" s="44"/>
+      <c r="P237" s="44">
+        <v>393.5</v>
+      </c>
       <c r="Q237" s="44"/>
       <c r="R237" s="37"/>
       <c r="S237" s="37"/>
       <c r="T237" s="37"/>
     </row>
     <row r="238" spans="1:20" ht="18" customHeight="1">
-      <c r="A238" s="40"/>
-      <c r="B238" s="41"/>
-      <c r="C238" s="30"/>
-      <c r="D238" s="30"/>
-      <c r="E238" s="31"/>
-      <c r="F238" s="53"/>
+      <c r="A238" s="155" t="s">
+        <v>309</v>
+      </c>
+      <c r="B238" s="105" t="s">
+        <v>300</v>
+      </c>
+      <c r="C238" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D238" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E238" s="105" t="s">
+        <v>311</v>
+      </c>
+      <c r="F238" s="53" t="s">
+        <v>179</v>
+      </c>
       <c r="G238" s="32"/>
       <c r="H238" s="56"/>
-      <c r="I238" s="44"/>
-      <c r="J238" s="44"/>
+      <c r="I238" s="54">
+        <v>298</v>
+      </c>
+      <c r="J238" s="35">
+        <f t="shared" si="6"/>
+        <v>4921152600</v>
+      </c>
       <c r="K238" s="38"/>
-      <c r="L238" s="40"/>
-      <c r="M238" s="40"/>
-      <c r="N238" s="40"/>
+      <c r="L238" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M238" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N238" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O238" s="44"/>
-      <c r="P238" s="44"/>
+      <c r="P238" s="44">
+        <v>501.8</v>
+      </c>
       <c r="Q238" s="44"/>
       <c r="R238" s="44"/>
       <c r="S238" s="37"/>
       <c r="T238" s="37"/>
     </row>
     <row r="239" spans="1:20" ht="18" customHeight="1">
-      <c r="A239" s="40"/>
-      <c r="B239" s="41"/>
-      <c r="C239" s="30"/>
-      <c r="D239" s="30"/>
-      <c r="E239" s="31"/>
-      <c r="F239" s="53"/>
+      <c r="A239" s="155" t="s">
+        <v>307</v>
+      </c>
+      <c r="B239" s="105" t="s">
+        <v>301</v>
+      </c>
+      <c r="C239" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D239" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E239" s="105" t="s">
+        <v>312</v>
+      </c>
+      <c r="F239" s="53" t="s">
+        <v>179</v>
+      </c>
       <c r="G239" s="32"/>
       <c r="H239" s="56"/>
-      <c r="I239" s="44"/>
-      <c r="J239" s="44"/>
+      <c r="I239" s="54">
+        <v>298</v>
+      </c>
+      <c r="J239" s="35">
+        <f t="shared" si="6"/>
+        <v>4669112700</v>
+      </c>
       <c r="K239" s="38"/>
-      <c r="L239" s="40"/>
-      <c r="M239" s="40"/>
-      <c r="N239" s="40"/>
+      <c r="L239" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M239" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N239" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O239" s="44"/>
-      <c r="P239" s="44"/>
+      <c r="P239" s="44">
+        <v>476.1</v>
+      </c>
       <c r="Q239" s="44"/>
       <c r="R239" s="44"/>
       <c r="S239" s="37"/>
       <c r="T239" s="37"/>
     </row>
     <row r="240" spans="1:20" ht="18" customHeight="1">
-      <c r="A240" s="40"/>
-      <c r="B240" s="41"/>
-      <c r="C240" s="30"/>
-      <c r="D240" s="30"/>
-      <c r="E240" s="31"/>
-      <c r="F240" s="53"/>
+      <c r="A240" s="155" t="s">
+        <v>308</v>
+      </c>
+      <c r="B240" s="105" t="s">
+        <v>302</v>
+      </c>
+      <c r="C240" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D240" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E240" s="105" t="s">
+        <v>312</v>
+      </c>
+      <c r="F240" s="53" t="s">
+        <v>179</v>
+      </c>
       <c r="G240" s="32"/>
       <c r="H240" s="56"/>
-      <c r="I240" s="44"/>
-      <c r="J240" s="44"/>
+      <c r="I240" s="54">
+        <v>298</v>
+      </c>
+      <c r="J240" s="35">
+        <f t="shared" si="6"/>
+        <v>5147694300</v>
+      </c>
       <c r="K240" s="38"/>
-      <c r="L240" s="40"/>
-      <c r="M240" s="40"/>
-      <c r="N240" s="40"/>
+      <c r="L240" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M240" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N240" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O240" s="44"/>
-      <c r="P240" s="44"/>
+      <c r="P240" s="44">
+        <v>524.9</v>
+      </c>
       <c r="Q240" s="44"/>
       <c r="R240" s="44"/>
       <c r="S240" s="37"/>
       <c r="T240" s="37"/>
     </row>
     <row r="241" spans="1:20" ht="18" customHeight="1">
-      <c r="A241" s="40"/>
-      <c r="B241" s="41"/>
-      <c r="C241" s="30"/>
-      <c r="D241" s="30"/>
-      <c r="E241" s="31"/>
-      <c r="F241" s="53"/>
+      <c r="A241" s="154" t="s">
+        <v>282</v>
+      </c>
+      <c r="B241" s="103" t="s">
+        <v>295</v>
+      </c>
+      <c r="C241" s="90" t="s">
+        <v>63</v>
+      </c>
+      <c r="D241" s="90" t="s">
+        <v>131</v>
+      </c>
+      <c r="E241" s="103"/>
+      <c r="F241" s="53" t="s">
+        <v>315</v>
+      </c>
       <c r="G241" s="32"/>
-      <c r="H241" s="56"/>
-      <c r="I241" s="40"/>
-      <c r="J241" s="40"/>
+      <c r="H241" s="56" t="s">
+        <v>322</v>
+      </c>
+      <c r="I241" s="54">
+        <v>298</v>
+      </c>
+      <c r="J241" s="40">
+        <f>-P241*0.001</f>
+        <v>-0.252</v>
+      </c>
       <c r="K241" s="38"/>
-      <c r="L241" s="40"/>
-      <c r="M241" s="40"/>
-      <c r="N241" s="40"/>
+      <c r="L241" s="40" t="s">
+        <v>318</v>
+      </c>
+      <c r="M241" s="40" t="s">
+        <v>321</v>
+      </c>
+      <c r="N241" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O241" s="44"/>
-      <c r="P241" s="44"/>
+      <c r="P241" s="44">
+        <v>252</v>
+      </c>
       <c r="Q241" s="44"/>
       <c r="R241" s="44"/>
       <c r="S241" s="37"/>
       <c r="T241" s="37"/>
     </row>
     <row r="242" spans="1:20" ht="18" customHeight="1">
-      <c r="A242" s="40"/>
-      <c r="B242" s="41"/>
-      <c r="C242" s="30"/>
-      <c r="D242" s="30"/>
-      <c r="E242" s="31"/>
-      <c r="F242" s="53"/>
+      <c r="A242" s="155" t="s">
+        <v>303</v>
+      </c>
+      <c r="B242" s="105" t="s">
+        <v>296</v>
+      </c>
+      <c r="C242" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D242" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E242" s="105" t="s">
+        <v>310</v>
+      </c>
+      <c r="F242" s="53" t="s">
+        <v>315</v>
+      </c>
       <c r="G242" s="32"/>
-      <c r="H242" s="56"/>
-      <c r="I242" s="40"/>
-      <c r="J242" s="40"/>
+      <c r="H242" s="56" t="s">
+        <v>322</v>
+      </c>
+      <c r="I242" s="54">
+        <v>298</v>
+      </c>
+      <c r="J242" s="40">
+        <f t="shared" ref="J242:J264" si="7">-P242*0.001</f>
+        <v>-0.31900000000000001</v>
+      </c>
       <c r="K242" s="38"/>
-      <c r="L242" s="40"/>
-      <c r="M242" s="40"/>
-      <c r="N242" s="40"/>
+      <c r="L242" s="40" t="s">
+        <v>318</v>
+      </c>
+      <c r="M242" s="40" t="s">
+        <v>321</v>
+      </c>
+      <c r="N242" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O242" s="44"/>
-      <c r="P242" s="44"/>
+      <c r="P242" s="44">
+        <v>319</v>
+      </c>
       <c r="Q242" s="44"/>
       <c r="R242" s="44"/>
       <c r="S242" s="37"/>
       <c r="T242" s="37"/>
     </row>
     <row r="243" spans="1:20" ht="18" customHeight="1">
-      <c r="A243" s="40"/>
-      <c r="B243" s="41"/>
-      <c r="C243" s="30"/>
-      <c r="D243" s="30"/>
-      <c r="E243" s="31"/>
-      <c r="F243" s="53"/>
+      <c r="A243" s="155" t="s">
+        <v>304</v>
+      </c>
+      <c r="B243" s="105" t="s">
+        <v>297</v>
+      </c>
+      <c r="C243" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D243" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E243" s="105" t="s">
+        <v>310</v>
+      </c>
+      <c r="F243" s="53" t="s">
+        <v>315</v>
+      </c>
       <c r="G243" s="32"/>
-      <c r="H243" s="56"/>
-      <c r="I243" s="40"/>
-      <c r="J243" s="40"/>
+      <c r="H243" s="56" t="s">
+        <v>322</v>
+      </c>
+      <c r="I243" s="54">
+        <v>298</v>
+      </c>
+      <c r="J243" s="40">
+        <f t="shared" si="7"/>
+        <v>-0.32300000000000001</v>
+      </c>
       <c r="K243" s="38"/>
-      <c r="L243" s="40"/>
-      <c r="M243" s="40"/>
-      <c r="N243" s="40"/>
+      <c r="L243" s="40" t="s">
+        <v>318</v>
+      </c>
+      <c r="M243" s="40" t="s">
+        <v>321</v>
+      </c>
+      <c r="N243" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O243" s="44"/>
-      <c r="P243" s="44"/>
+      <c r="P243" s="44">
+        <v>323</v>
+      </c>
       <c r="Q243" s="44"/>
       <c r="R243" s="44"/>
       <c r="S243" s="37"/>
       <c r="T243" s="37"/>
     </row>
     <row r="244" spans="1:20" ht="18" customHeight="1">
-      <c r="A244" s="40"/>
-      <c r="B244" s="41"/>
-      <c r="C244" s="30"/>
-      <c r="D244" s="30"/>
-      <c r="E244" s="31"/>
-      <c r="F244" s="53"/>
+      <c r="A244" s="155" t="s">
+        <v>305</v>
+      </c>
+      <c r="B244" s="105" t="s">
+        <v>298</v>
+      </c>
+      <c r="C244" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D244" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E244" s="105" t="s">
+        <v>310</v>
+      </c>
+      <c r="F244" s="53" t="s">
+        <v>315</v>
+      </c>
       <c r="G244" s="32"/>
-      <c r="H244" s="56"/>
-      <c r="I244" s="40"/>
-      <c r="J244" s="40"/>
+      <c r="H244" s="56" t="s">
+        <v>322</v>
+      </c>
+      <c r="I244" s="54">
+        <v>298</v>
+      </c>
+      <c r="J244" s="40">
+        <f t="shared" si="7"/>
+        <v>-0.31</v>
+      </c>
       <c r="K244" s="38"/>
-      <c r="L244" s="40"/>
-      <c r="M244" s="40"/>
-      <c r="N244" s="40"/>
+      <c r="L244" s="40" t="s">
+        <v>318</v>
+      </c>
+      <c r="M244" s="40" t="s">
+        <v>321</v>
+      </c>
+      <c r="N244" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O244" s="44"/>
-      <c r="P244" s="44"/>
+      <c r="P244" s="44">
+        <v>310</v>
+      </c>
       <c r="Q244" s="44"/>
       <c r="R244" s="44"/>
       <c r="S244" s="37"/>
       <c r="T244" s="37"/>
     </row>
     <row r="245" spans="1:20" ht="18" customHeight="1">
-      <c r="A245" s="40"/>
-      <c r="B245" s="41"/>
-      <c r="C245" s="30"/>
-      <c r="D245" s="30"/>
-      <c r="E245" s="31"/>
-      <c r="F245" s="53"/>
+      <c r="A245" s="155" t="s">
+        <v>306</v>
+      </c>
+      <c r="B245" s="105" t="s">
+        <v>299</v>
+      </c>
+      <c r="C245" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D245" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E245" s="105" t="s">
+        <v>310</v>
+      </c>
+      <c r="F245" s="53" t="s">
+        <v>315</v>
+      </c>
       <c r="G245" s="32"/>
-      <c r="H245" s="56"/>
-      <c r="I245" s="40"/>
-      <c r="J245" s="40"/>
+      <c r="H245" s="56" t="s">
+        <v>322</v>
+      </c>
+      <c r="I245" s="54">
+        <v>298</v>
+      </c>
+      <c r="J245" s="40">
+        <f t="shared" si="7"/>
+        <v>-0.28700000000000003</v>
+      </c>
       <c r="K245" s="38"/>
-      <c r="L245" s="40"/>
-      <c r="M245" s="40"/>
-      <c r="N245" s="40"/>
+      <c r="L245" s="40" t="s">
+        <v>318</v>
+      </c>
+      <c r="M245" s="40" t="s">
+        <v>321</v>
+      </c>
+      <c r="N245" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O245" s="44"/>
-      <c r="P245" s="44"/>
+      <c r="P245" s="44">
+        <v>287</v>
+      </c>
       <c r="Q245" s="44"/>
       <c r="R245" s="44"/>
       <c r="S245" s="37"/>
       <c r="T245" s="37"/>
     </row>
     <row r="246" spans="1:20" ht="18" customHeight="1">
-      <c r="A246" s="40"/>
-      <c r="B246" s="41"/>
-      <c r="C246" s="30"/>
-      <c r="D246" s="30"/>
-      <c r="E246" s="31"/>
-      <c r="F246" s="53"/>
+      <c r="A246" s="155" t="s">
+        <v>309</v>
+      </c>
+      <c r="B246" s="105" t="s">
+        <v>300</v>
+      </c>
+      <c r="C246" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D246" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E246" s="105" t="s">
+        <v>311</v>
+      </c>
+      <c r="F246" s="53" t="s">
+        <v>315</v>
+      </c>
       <c r="G246" s="32"/>
-      <c r="H246" s="56"/>
-      <c r="I246" s="40"/>
-      <c r="J246" s="40"/>
+      <c r="H246" s="56" t="s">
+        <v>322</v>
+      </c>
+      <c r="I246" s="54">
+        <v>298</v>
+      </c>
+      <c r="J246" s="40">
+        <f t="shared" si="7"/>
+        <v>-0.33700000000000002</v>
+      </c>
       <c r="K246" s="38"/>
-      <c r="L246" s="40"/>
-      <c r="M246" s="40"/>
-      <c r="N246" s="40"/>
+      <c r="L246" s="40" t="s">
+        <v>318</v>
+      </c>
+      <c r="M246" s="40" t="s">
+        <v>321</v>
+      </c>
+      <c r="N246" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O246" s="44"/>
-      <c r="P246" s="44"/>
+      <c r="P246" s="44">
+        <v>337</v>
+      </c>
       <c r="Q246" s="44"/>
       <c r="R246" s="44"/>
       <c r="S246" s="37"/>
       <c r="T246" s="37"/>
     </row>
     <row r="247" spans="1:20" ht="18" customHeight="1">
-      <c r="A247" s="40"/>
-      <c r="B247" s="41"/>
-      <c r="C247" s="30"/>
-      <c r="D247" s="30"/>
-      <c r="E247" s="31"/>
-      <c r="F247" s="53"/>
+      <c r="A247" s="155" t="s">
+        <v>307</v>
+      </c>
+      <c r="B247" s="105" t="s">
+        <v>301</v>
+      </c>
+      <c r="C247" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D247" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E247" s="105" t="s">
+        <v>312</v>
+      </c>
+      <c r="F247" s="53" t="s">
+        <v>315</v>
+      </c>
       <c r="G247" s="32"/>
-      <c r="H247" s="56"/>
-      <c r="I247" s="40"/>
-      <c r="J247" s="40"/>
+      <c r="H247" s="56" t="s">
+        <v>322</v>
+      </c>
+      <c r="I247" s="54">
+        <v>298</v>
+      </c>
+      <c r="J247" s="40">
+        <f t="shared" si="7"/>
+        <v>-0.29499999999999998</v>
+      </c>
       <c r="K247" s="38"/>
-      <c r="L247" s="40"/>
-      <c r="M247" s="40"/>
-      <c r="N247" s="40"/>
+      <c r="L247" s="40" t="s">
+        <v>318</v>
+      </c>
+      <c r="M247" s="40" t="s">
+        <v>321</v>
+      </c>
+      <c r="N247" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O247" s="44"/>
-      <c r="P247" s="44"/>
+      <c r="P247" s="44">
+        <v>295</v>
+      </c>
       <c r="Q247" s="44"/>
       <c r="R247" s="44"/>
       <c r="S247" s="37"/>
       <c r="T247" s="44"/>
     </row>
     <row r="248" spans="1:20" ht="18" customHeight="1">
-      <c r="A248" s="40"/>
-      <c r="B248" s="41"/>
-      <c r="C248" s="30"/>
-      <c r="D248" s="30"/>
-      <c r="E248" s="31"/>
-      <c r="F248" s="53"/>
+      <c r="A248" s="155" t="s">
+        <v>308</v>
+      </c>
+      <c r="B248" s="105" t="s">
+        <v>302</v>
+      </c>
+      <c r="C248" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D248" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E248" s="105" t="s">
+        <v>312</v>
+      </c>
+      <c r="F248" s="53" t="s">
+        <v>315</v>
+      </c>
       <c r="G248" s="32"/>
-      <c r="H248" s="56"/>
-      <c r="I248" s="40"/>
-      <c r="J248" s="40"/>
+      <c r="H248" s="56" t="s">
+        <v>322</v>
+      </c>
+      <c r="I248" s="54">
+        <v>298</v>
+      </c>
+      <c r="J248" s="40">
+        <f t="shared" si="7"/>
+        <v>-0.35100000000000003</v>
+      </c>
       <c r="K248" s="38"/>
-      <c r="L248" s="40"/>
-      <c r="M248" s="40"/>
-      <c r="N248" s="40"/>
+      <c r="L248" s="40" t="s">
+        <v>318</v>
+      </c>
+      <c r="M248" s="40" t="s">
+        <v>321</v>
+      </c>
+      <c r="N248" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O248" s="44"/>
-      <c r="P248" s="44"/>
+      <c r="P248" s="44">
+        <v>351</v>
+      </c>
       <c r="Q248" s="44"/>
       <c r="R248" s="44"/>
       <c r="S248" s="37"/>
       <c r="T248" s="44"/>
     </row>
     <row r="249" spans="1:20" ht="18" customHeight="1">
-      <c r="A249" s="40"/>
-      <c r="B249" s="41"/>
-      <c r="C249" s="30"/>
-      <c r="D249" s="30"/>
-      <c r="E249" s="31"/>
-      <c r="F249" s="53"/>
+      <c r="A249" s="154" t="s">
+        <v>282</v>
+      </c>
+      <c r="B249" s="103" t="s">
+        <v>295</v>
+      </c>
+      <c r="C249" s="90" t="s">
+        <v>63</v>
+      </c>
+      <c r="D249" s="90" t="s">
+        <v>131</v>
+      </c>
+      <c r="E249" s="103"/>
+      <c r="F249" s="53" t="s">
+        <v>316</v>
+      </c>
       <c r="G249" s="32"/>
-      <c r="H249" s="56"/>
-      <c r="I249" s="57"/>
-      <c r="J249" s="40"/>
+      <c r="H249" s="56" t="s">
+        <v>322</v>
+      </c>
+      <c r="I249" s="54">
+        <v>298</v>
+      </c>
+      <c r="J249" s="40">
+        <f>P249*0.01</f>
+        <v>4.2610000000000002E-2</v>
+      </c>
       <c r="K249" s="38"/>
-      <c r="L249" s="40"/>
-      <c r="M249" s="40"/>
-      <c r="N249" s="40"/>
+      <c r="L249" s="40" t="s">
+        <v>319</v>
+      </c>
+      <c r="M249" s="40" t="s">
+        <v>321</v>
+      </c>
+      <c r="N249" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O249" s="44"/>
-      <c r="P249" s="44"/>
+      <c r="P249" s="44">
+        <v>4.2610000000000001</v>
+      </c>
       <c r="Q249" s="44"/>
       <c r="R249" s="44"/>
       <c r="S249" s="37"/>
       <c r="T249" s="44"/>
     </row>
     <row r="250" spans="1:20" ht="18" customHeight="1">
-      <c r="A250" s="40"/>
-      <c r="B250" s="41"/>
-      <c r="C250" s="30"/>
-      <c r="D250" s="30"/>
-      <c r="E250" s="31"/>
-      <c r="F250" s="53"/>
+      <c r="A250" s="155" t="s">
+        <v>303</v>
+      </c>
+      <c r="B250" s="105" t="s">
+        <v>296</v>
+      </c>
+      <c r="C250" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D250" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E250" s="105" t="s">
+        <v>310</v>
+      </c>
+      <c r="F250" s="53" t="s">
+        <v>316</v>
+      </c>
       <c r="G250" s="32"/>
-      <c r="H250" s="56"/>
-      <c r="I250" s="57"/>
-      <c r="J250" s="40"/>
+      <c r="H250" s="56" t="s">
+        <v>322</v>
+      </c>
+      <c r="I250" s="54">
+        <v>298</v>
+      </c>
+      <c r="J250" s="40">
+        <f t="shared" ref="J250:J264" si="8">P250*0.01</f>
+        <v>4.0960000000000003E-2</v>
+      </c>
       <c r="K250" s="38"/>
-      <c r="L250" s="40"/>
-      <c r="M250" s="40"/>
-      <c r="N250" s="40"/>
+      <c r="L250" s="40" t="s">
+        <v>319</v>
+      </c>
+      <c r="M250" s="40" t="s">
+        <v>321</v>
+      </c>
+      <c r="N250" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O250" s="44"/>
-      <c r="P250" s="44"/>
+      <c r="P250" s="44">
+        <v>4.0960000000000001</v>
+      </c>
       <c r="Q250" s="44"/>
       <c r="R250" s="44"/>
       <c r="S250" s="37"/>
       <c r="T250" s="37"/>
     </row>
     <row r="251" spans="1:20" ht="18" customHeight="1">
-      <c r="A251" s="40"/>
-      <c r="B251" s="41"/>
-      <c r="C251" s="30"/>
-      <c r="D251" s="30"/>
-      <c r="E251" s="31"/>
-      <c r="F251" s="53"/>
+      <c r="A251" s="155" t="s">
+        <v>304</v>
+      </c>
+      <c r="B251" s="105" t="s">
+        <v>297</v>
+      </c>
+      <c r="C251" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D251" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E251" s="105" t="s">
+        <v>310</v>
+      </c>
+      <c r="F251" s="53" t="s">
+        <v>316</v>
+      </c>
       <c r="G251" s="32"/>
-      <c r="H251" s="56"/>
-      <c r="I251" s="57"/>
-      <c r="J251" s="40"/>
+      <c r="H251" s="56" t="s">
+        <v>322</v>
+      </c>
+      <c r="I251" s="54">
+        <v>298</v>
+      </c>
+      <c r="J251" s="40">
+        <f t="shared" si="8"/>
+        <v>3.1789999999999999E-2</v>
+      </c>
       <c r="K251" s="38"/>
-      <c r="L251" s="40"/>
-      <c r="M251" s="40"/>
-      <c r="N251" s="40"/>
+      <c r="L251" s="40" t="s">
+        <v>319</v>
+      </c>
+      <c r="M251" s="40" t="s">
+        <v>321</v>
+      </c>
+      <c r="N251" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O251" s="44"/>
-      <c r="P251" s="44"/>
+      <c r="P251" s="44">
+        <v>3.1789999999999998</v>
+      </c>
       <c r="Q251" s="44"/>
       <c r="R251" s="44"/>
       <c r="S251" s="37"/>
       <c r="T251" s="37"/>
     </row>
     <row r="252" spans="1:20" ht="18" customHeight="1">
-      <c r="A252" s="40"/>
-      <c r="B252" s="41"/>
-      <c r="C252" s="30"/>
-      <c r="D252" s="30"/>
-      <c r="E252" s="31"/>
-      <c r="F252" s="53"/>
+      <c r="A252" s="155" t="s">
+        <v>305</v>
+      </c>
+      <c r="B252" s="105" t="s">
+        <v>298</v>
+      </c>
+      <c r="C252" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D252" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E252" s="105" t="s">
+        <v>310</v>
+      </c>
+      <c r="F252" s="53" t="s">
+        <v>316</v>
+      </c>
       <c r="G252" s="32"/>
-      <c r="H252" s="56"/>
-      <c r="I252" s="57"/>
-      <c r="J252" s="40"/>
+      <c r="H252" s="56" t="s">
+        <v>322</v>
+      </c>
+      <c r="I252" s="54">
+        <v>298</v>
+      </c>
+      <c r="J252" s="40">
+        <f t="shared" si="8"/>
+        <v>3.4970000000000001E-2</v>
+      </c>
       <c r="K252" s="38"/>
-      <c r="L252" s="40"/>
-      <c r="M252" s="40"/>
-      <c r="N252" s="40"/>
+      <c r="L252" s="40" t="s">
+        <v>319</v>
+      </c>
+      <c r="M252" s="40" t="s">
+        <v>321</v>
+      </c>
+      <c r="N252" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O252" s="44"/>
-      <c r="P252" s="44"/>
+      <c r="P252" s="44">
+        <v>3.4969999999999999</v>
+      </c>
       <c r="Q252" s="44"/>
       <c r="R252" s="44"/>
       <c r="S252" s="37"/>
       <c r="T252" s="37"/>
     </row>
     <row r="253" spans="1:20" ht="18" customHeight="1">
-      <c r="A253" s="40"/>
-      <c r="B253" s="41"/>
-      <c r="C253" s="30"/>
-      <c r="D253" s="30"/>
-      <c r="E253" s="31"/>
-      <c r="F253" s="53"/>
+      <c r="A253" s="155" t="s">
+        <v>306</v>
+      </c>
+      <c r="B253" s="105" t="s">
+        <v>299</v>
+      </c>
+      <c r="C253" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D253" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E253" s="105" t="s">
+        <v>310</v>
+      </c>
+      <c r="F253" s="53" t="s">
+        <v>316</v>
+      </c>
       <c r="G253" s="32"/>
-      <c r="H253" s="56"/>
-      <c r="I253" s="57"/>
-      <c r="J253" s="40"/>
+      <c r="H253" s="56" t="s">
+        <v>322</v>
+      </c>
+      <c r="I253" s="54">
+        <v>298</v>
+      </c>
+      <c r="J253" s="40">
+        <f t="shared" si="8"/>
+        <v>3.2809999999999999E-2</v>
+      </c>
       <c r="K253" s="38"/>
-      <c r="L253" s="40"/>
-      <c r="M253" s="40"/>
-      <c r="N253" s="40"/>
+      <c r="L253" s="40" t="s">
+        <v>319</v>
+      </c>
+      <c r="M253" s="40" t="s">
+        <v>321</v>
+      </c>
+      <c r="N253" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O253" s="44"/>
-      <c r="P253" s="44"/>
+      <c r="P253" s="44">
+        <v>3.2810000000000001</v>
+      </c>
       <c r="Q253" s="44"/>
       <c r="R253" s="44"/>
       <c r="S253" s="37"/>
       <c r="T253" s="37"/>
     </row>
     <row r="254" spans="1:20" ht="18" customHeight="1">
-      <c r="A254" s="40"/>
-      <c r="B254" s="41"/>
-      <c r="C254" s="30"/>
-      <c r="D254" s="30"/>
-      <c r="E254" s="31"/>
-      <c r="F254" s="53"/>
+      <c r="A254" s="155" t="s">
+        <v>309</v>
+      </c>
+      <c r="B254" s="105" t="s">
+        <v>300</v>
+      </c>
+      <c r="C254" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D254" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E254" s="105" t="s">
+        <v>311</v>
+      </c>
+      <c r="F254" s="53" t="s">
+        <v>316</v>
+      </c>
       <c r="G254" s="32"/>
-      <c r="H254" s="56"/>
-      <c r="I254" s="57"/>
-      <c r="J254" s="40"/>
+      <c r="H254" s="56" t="s">
+        <v>322</v>
+      </c>
+      <c r="I254" s="54">
+        <v>298</v>
+      </c>
+      <c r="J254" s="40">
+        <f t="shared" si="8"/>
+        <v>4.6429999999999999E-2</v>
+      </c>
       <c r="K254" s="38"/>
-      <c r="L254" s="40"/>
-      <c r="M254" s="40"/>
-      <c r="N254" s="40"/>
+      <c r="L254" s="40" t="s">
+        <v>319</v>
+      </c>
+      <c r="M254" s="40" t="s">
+        <v>321</v>
+      </c>
+      <c r="N254" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O254" s="44"/>
-      <c r="P254" s="44"/>
+      <c r="P254" s="44">
+        <v>4.6429999999999998</v>
+      </c>
       <c r="Q254" s="44"/>
       <c r="R254" s="44"/>
       <c r="S254" s="37"/>
       <c r="T254" s="37"/>
     </row>
     <row r="255" spans="1:20" ht="18" customHeight="1">
-      <c r="A255" s="57"/>
-      <c r="B255" s="41"/>
-      <c r="C255" s="30"/>
-      <c r="D255" s="30"/>
-      <c r="E255" s="31"/>
-      <c r="F255" s="53"/>
+      <c r="A255" s="155" t="s">
+        <v>307</v>
+      </c>
+      <c r="B255" s="105" t="s">
+        <v>301</v>
+      </c>
+      <c r="C255" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D255" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E255" s="105" t="s">
+        <v>312</v>
+      </c>
+      <c r="F255" s="53" t="s">
+        <v>316</v>
+      </c>
       <c r="G255" s="32"/>
-      <c r="H255" s="56"/>
-      <c r="I255" s="57"/>
-      <c r="J255" s="40"/>
+      <c r="H255" s="56" t="s">
+        <v>322</v>
+      </c>
+      <c r="I255" s="54">
+        <v>298</v>
+      </c>
+      <c r="J255" s="40">
+        <f t="shared" si="8"/>
+        <v>5.008E-2</v>
+      </c>
       <c r="K255" s="38"/>
-      <c r="L255" s="40"/>
-      <c r="M255" s="40"/>
-      <c r="N255" s="40"/>
+      <c r="L255" s="40" t="s">
+        <v>319</v>
+      </c>
+      <c r="M255" s="40" t="s">
+        <v>321</v>
+      </c>
+      <c r="N255" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O255" s="44"/>
-      <c r="P255" s="44"/>
+      <c r="P255" s="44">
+        <v>5.008</v>
+      </c>
       <c r="Q255" s="44"/>
       <c r="R255" s="44"/>
       <c r="S255" s="37"/>
       <c r="T255" s="37"/>
     </row>
     <row r="256" spans="1:20" ht="18" customHeight="1">
-      <c r="A256" s="57"/>
-      <c r="B256" s="41"/>
-      <c r="C256" s="30"/>
-      <c r="D256" s="30"/>
-      <c r="E256" s="31"/>
-      <c r="F256" s="53"/>
+      <c r="A256" s="155" t="s">
+        <v>308</v>
+      </c>
+      <c r="B256" s="105" t="s">
+        <v>302</v>
+      </c>
+      <c r="C256" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D256" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E256" s="105" t="s">
+        <v>312</v>
+      </c>
+      <c r="F256" s="53" t="s">
+        <v>316</v>
+      </c>
       <c r="G256" s="32"/>
-      <c r="H256" s="56"/>
-      <c r="I256" s="57"/>
-      <c r="J256" s="40"/>
+      <c r="H256" s="56" t="s">
+        <v>322</v>
+      </c>
+      <c r="I256" s="54">
+        <v>298</v>
+      </c>
+      <c r="J256" s="40">
+        <f t="shared" si="8"/>
+        <v>7.1289999999999992E-2</v>
+      </c>
       <c r="K256" s="38"/>
-      <c r="L256" s="40"/>
-      <c r="M256" s="40"/>
-      <c r="N256" s="40"/>
+      <c r="L256" s="40" t="s">
+        <v>319</v>
+      </c>
+      <c r="M256" s="40" t="s">
+        <v>321</v>
+      </c>
+      <c r="N256" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O256" s="44"/>
-      <c r="P256" s="44"/>
+      <c r="P256" s="44">
+        <v>7.1289999999999996</v>
+      </c>
       <c r="Q256" s="44"/>
       <c r="R256" s="44"/>
       <c r="S256" s="37"/>
       <c r="T256" s="37"/>
     </row>
     <row r="257" spans="1:20" ht="18" customHeight="1">
-      <c r="A257" s="57"/>
-      <c r="B257" s="41"/>
-      <c r="C257" s="30"/>
-      <c r="D257" s="30"/>
-      <c r="E257" s="31"/>
-      <c r="F257" s="53"/>
+      <c r="A257" s="154" t="s">
+        <v>282</v>
+      </c>
+      <c r="B257" s="103" t="s">
+        <v>295</v>
+      </c>
+      <c r="C257" s="90" t="s">
+        <v>63</v>
+      </c>
+      <c r="D257" s="90" t="s">
+        <v>131</v>
+      </c>
+      <c r="E257" s="103"/>
+      <c r="F257" s="53" t="s">
+        <v>317</v>
+      </c>
       <c r="G257" s="32"/>
-      <c r="H257" s="56"/>
-      <c r="I257" s="57"/>
-      <c r="J257" s="40"/>
+      <c r="H257" s="56" t="s">
+        <v>322</v>
+      </c>
+      <c r="I257" s="54">
+        <v>298</v>
+      </c>
+      <c r="J257" s="40">
+        <f>P257*0.001</f>
+        <v>-4.3299999999999998E-2</v>
+      </c>
       <c r="K257" s="38"/>
-      <c r="L257" s="40"/>
-      <c r="M257" s="40"/>
-      <c r="N257" s="40"/>
+      <c r="L257" s="40" t="s">
+        <v>318</v>
+      </c>
+      <c r="M257" s="40" t="s">
+        <v>321</v>
+      </c>
+      <c r="N257" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O257" s="44"/>
-      <c r="P257" s="44"/>
+      <c r="P257" s="44">
+        <v>-43.3</v>
+      </c>
       <c r="Q257" s="44"/>
       <c r="R257" s="44"/>
       <c r="S257" s="37"/>
       <c r="T257" s="37"/>
     </row>
     <row r="258" spans="1:20" ht="18" customHeight="1">
-      <c r="A258" s="57"/>
-      <c r="B258" s="41"/>
-      <c r="C258" s="30"/>
-      <c r="D258" s="30"/>
-      <c r="E258" s="31"/>
-      <c r="F258" s="53"/>
+      <c r="A258" s="155" t="s">
+        <v>303</v>
+      </c>
+      <c r="B258" s="105" t="s">
+        <v>296</v>
+      </c>
+      <c r="C258" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D258" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E258" s="105" t="s">
+        <v>310</v>
+      </c>
+      <c r="F258" s="53" t="s">
+        <v>317</v>
+      </c>
       <c r="G258" s="32"/>
-      <c r="H258" s="56"/>
-      <c r="I258" s="57"/>
-      <c r="J258" s="40"/>
+      <c r="H258" s="56" t="s">
+        <v>322</v>
+      </c>
+      <c r="I258" s="54">
+        <v>298</v>
+      </c>
+      <c r="J258" s="40">
+        <f t="shared" ref="J258:J264" si="9">P258*0.001</f>
+        <v>2.0500000000000001E-2</v>
+      </c>
       <c r="K258" s="38"/>
-      <c r="L258" s="40"/>
-      <c r="M258" s="40"/>
-      <c r="N258" s="40"/>
+      <c r="L258" s="40" t="s">
+        <v>318</v>
+      </c>
+      <c r="M258" s="40" t="s">
+        <v>321</v>
+      </c>
+      <c r="N258" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O258" s="44"/>
-      <c r="P258" s="44"/>
+      <c r="P258" s="44">
+        <v>20.5</v>
+      </c>
       <c r="Q258" s="44"/>
       <c r="R258" s="44"/>
       <c r="S258" s="37"/>
       <c r="T258" s="37"/>
     </row>
     <row r="259" spans="1:20" ht="18" customHeight="1">
-      <c r="A259" s="57"/>
-      <c r="B259" s="41"/>
-      <c r="C259" s="30"/>
-      <c r="D259" s="30"/>
-      <c r="E259" s="31"/>
-      <c r="F259" s="53"/>
+      <c r="A259" s="155" t="s">
+        <v>304</v>
+      </c>
+      <c r="B259" s="105" t="s">
+        <v>297</v>
+      </c>
+      <c r="C259" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D259" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E259" s="105" t="s">
+        <v>310</v>
+      </c>
+      <c r="F259" s="53" t="s">
+        <v>317</v>
+      </c>
       <c r="G259" s="32"/>
-      <c r="H259" s="56"/>
-      <c r="I259" s="57"/>
-      <c r="J259" s="40"/>
+      <c r="H259" s="56" t="s">
+        <v>322</v>
+      </c>
+      <c r="I259" s="54">
+        <v>298</v>
+      </c>
+      <c r="J259" s="40">
+        <f t="shared" si="9"/>
+        <v>7.9200000000000007E-2</v>
+      </c>
       <c r="K259" s="38"/>
-      <c r="L259" s="40"/>
-      <c r="M259" s="40"/>
-      <c r="N259" s="40"/>
+      <c r="L259" s="40" t="s">
+        <v>318</v>
+      </c>
+      <c r="M259" s="40" t="s">
+        <v>321</v>
+      </c>
+      <c r="N259" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O259" s="44"/>
-      <c r="P259" s="44"/>
+      <c r="P259" s="44">
+        <v>79.2</v>
+      </c>
       <c r="Q259" s="44"/>
       <c r="R259" s="44"/>
       <c r="S259" s="37"/>
       <c r="T259" s="37"/>
     </row>
     <row r="260" spans="1:20" ht="18" customHeight="1">
-      <c r="A260" s="57"/>
-      <c r="B260" s="41"/>
-      <c r="C260" s="30"/>
-      <c r="D260" s="30"/>
-      <c r="E260" s="31"/>
-      <c r="F260" s="53"/>
+      <c r="A260" s="155" t="s">
+        <v>305</v>
+      </c>
+      <c r="B260" s="105" t="s">
+        <v>298</v>
+      </c>
+      <c r="C260" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D260" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E260" s="105" t="s">
+        <v>310</v>
+      </c>
+      <c r="F260" s="53" t="s">
+        <v>317</v>
+      </c>
       <c r="G260" s="32"/>
-      <c r="H260" s="56"/>
-      <c r="I260" s="57"/>
-      <c r="J260" s="40"/>
+      <c r="H260" s="56" t="s">
+        <v>322</v>
+      </c>
+      <c r="I260" s="54">
+        <v>298</v>
+      </c>
+      <c r="J260" s="40">
+        <f t="shared" si="9"/>
+        <v>0.13300000000000001</v>
+      </c>
       <c r="K260" s="38"/>
-      <c r="L260" s="40"/>
-      <c r="M260" s="40"/>
-      <c r="N260" s="40"/>
+      <c r="L260" s="40" t="s">
+        <v>318</v>
+      </c>
+      <c r="M260" s="40" t="s">
+        <v>321</v>
+      </c>
+      <c r="N260" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O260" s="44"/>
-      <c r="P260" s="44"/>
+      <c r="P260" s="44">
+        <v>133</v>
+      </c>
       <c r="Q260" s="44"/>
       <c r="R260" s="44"/>
       <c r="S260" s="37"/>
       <c r="T260" s="37"/>
     </row>
     <row r="261" spans="1:20" ht="18" customHeight="1">
-      <c r="A261" s="57"/>
-      <c r="B261" s="41"/>
-      <c r="C261" s="30"/>
-      <c r="D261" s="30"/>
-      <c r="E261" s="31"/>
-      <c r="F261" s="53"/>
+      <c r="A261" s="155" t="s">
+        <v>306</v>
+      </c>
+      <c r="B261" s="105" t="s">
+        <v>299</v>
+      </c>
+      <c r="C261" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D261" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E261" s="105" t="s">
+        <v>310</v>
+      </c>
+      <c r="F261" s="53" t="s">
+        <v>317</v>
+      </c>
       <c r="G261" s="32"/>
-      <c r="H261" s="56"/>
-      <c r="I261" s="57"/>
-      <c r="J261" s="40"/>
+      <c r="H261" s="56" t="s">
+        <v>322</v>
+      </c>
+      <c r="I261" s="54">
+        <v>298</v>
+      </c>
+      <c r="J261" s="40">
+        <f t="shared" si="9"/>
+        <v>0.2</v>
+      </c>
       <c r="K261" s="38"/>
-      <c r="L261" s="40"/>
-      <c r="M261" s="40"/>
-      <c r="N261" s="40"/>
+      <c r="L261" s="40" t="s">
+        <v>318</v>
+      </c>
+      <c r="M261" s="40" t="s">
+        <v>321</v>
+      </c>
+      <c r="N261" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O261" s="44"/>
-      <c r="P261" s="44"/>
+      <c r="P261" s="44">
+        <v>200</v>
+      </c>
       <c r="Q261" s="44"/>
       <c r="R261" s="44"/>
       <c r="S261" s="37"/>
       <c r="T261" s="37"/>
     </row>
     <row r="262" spans="1:20" ht="18" customHeight="1">
-      <c r="A262" s="57"/>
-      <c r="B262" s="41"/>
-      <c r="C262" s="30"/>
-      <c r="D262" s="30"/>
-      <c r="E262" s="31"/>
-      <c r="F262" s="53"/>
+      <c r="A262" s="155" t="s">
+        <v>309</v>
+      </c>
+      <c r="B262" s="105" t="s">
+        <v>300</v>
+      </c>
+      <c r="C262" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D262" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E262" s="105" t="s">
+        <v>311</v>
+      </c>
+      <c r="F262" s="53" t="s">
+        <v>317</v>
+      </c>
       <c r="G262" s="32"/>
-      <c r="H262" s="56"/>
-      <c r="I262" s="57"/>
-      <c r="J262" s="40"/>
+      <c r="H262" s="56" t="s">
+        <v>322</v>
+      </c>
+      <c r="I262" s="54">
+        <v>298</v>
+      </c>
+      <c r="J262" s="40">
+        <f t="shared" si="9"/>
+        <v>0.19600000000000001</v>
+      </c>
       <c r="K262" s="38"/>
-      <c r="L262" s="40"/>
-      <c r="M262" s="40"/>
-      <c r="N262" s="40"/>
+      <c r="L262" s="40" t="s">
+        <v>318</v>
+      </c>
+      <c r="M262" s="40" t="s">
+        <v>321</v>
+      </c>
+      <c r="N262" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O262" s="44"/>
-      <c r="P262" s="44"/>
+      <c r="P262" s="44">
+        <v>196</v>
+      </c>
       <c r="Q262" s="44"/>
       <c r="R262" s="44"/>
       <c r="S262" s="37"/>
       <c r="T262" s="37"/>
     </row>
     <row r="263" spans="1:20" ht="18" customHeight="1">
-      <c r="A263" s="57"/>
-      <c r="B263" s="41"/>
-      <c r="C263" s="30"/>
-      <c r="D263" s="30"/>
-      <c r="E263" s="31"/>
-      <c r="F263" s="53"/>
+      <c r="A263" s="155" t="s">
+        <v>307</v>
+      </c>
+      <c r="B263" s="105" t="s">
+        <v>301</v>
+      </c>
+      <c r="C263" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D263" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E263" s="105" t="s">
+        <v>312</v>
+      </c>
+      <c r="F263" s="53" t="s">
+        <v>317</v>
+      </c>
       <c r="G263" s="32"/>
-      <c r="H263" s="56"/>
-      <c r="I263" s="57"/>
-      <c r="J263" s="40"/>
+      <c r="H263" s="56" t="s">
+        <v>322</v>
+      </c>
+      <c r="I263" s="54">
+        <v>298</v>
+      </c>
+      <c r="J263" s="40">
+        <f t="shared" si="9"/>
+        <v>0.26100000000000001</v>
+      </c>
       <c r="K263" s="38"/>
-      <c r="L263" s="40"/>
-      <c r="M263" s="40"/>
-      <c r="N263" s="40"/>
+      <c r="L263" s="40" t="s">
+        <v>318</v>
+      </c>
+      <c r="M263" s="40" t="s">
+        <v>321</v>
+      </c>
+      <c r="N263" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O263" s="44"/>
-      <c r="P263" s="44"/>
+      <c r="P263" s="44">
+        <v>261</v>
+      </c>
       <c r="Q263" s="44"/>
       <c r="R263" s="44"/>
       <c r="S263" s="37"/>
       <c r="T263" s="37"/>
     </row>
     <row r="264" spans="1:20" ht="18" customHeight="1">
-      <c r="A264" s="57"/>
-      <c r="B264" s="41"/>
-      <c r="C264" s="30"/>
-      <c r="D264" s="30"/>
-      <c r="E264" s="31"/>
-      <c r="F264" s="53"/>
+      <c r="A264" s="155" t="s">
+        <v>308</v>
+      </c>
+      <c r="B264" s="105" t="s">
+        <v>302</v>
+      </c>
+      <c r="C264" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D264" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E264" s="105" t="s">
+        <v>312</v>
+      </c>
+      <c r="F264" s="53" t="s">
+        <v>317</v>
+      </c>
       <c r="G264" s="32"/>
-      <c r="H264" s="56"/>
-      <c r="I264" s="57"/>
-      <c r="J264" s="40"/>
+      <c r="H264" s="56" t="s">
+        <v>322</v>
+      </c>
+      <c r="I264" s="54">
+        <v>298</v>
+      </c>
+      <c r="J264" s="40">
+        <f t="shared" si="9"/>
+        <v>0.247</v>
+      </c>
       <c r="K264" s="38"/>
-      <c r="L264" s="40"/>
-      <c r="M264" s="40"/>
-      <c r="N264" s="40"/>
+      <c r="L264" s="40" t="s">
+        <v>318</v>
+      </c>
+      <c r="M264" s="40" t="s">
+        <v>321</v>
+      </c>
+      <c r="N264" s="30" t="s">
+        <v>323</v>
+      </c>
       <c r="O264" s="44"/>
-      <c r="P264" s="44"/>
+      <c r="P264" s="44">
+        <v>247</v>
+      </c>
       <c r="Q264" s="44"/>
       <c r="R264" s="44"/>
       <c r="S264" s="37"/>

</xml_diff>

<commit_message>
- parsed data from `10.1016/j.msea.2022.143026`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Aug2025.xlsx
+++ b/MiscSmallUploads_Aug2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6FF4F8-B1F5-1B49-8809-A4927400083F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932CE614-ABA5-2A46-9BCF-C752FD90A350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="7580" windowWidth="34560" windowHeight="12760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2389" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2551" uniqueCount="338">
   <si>
     <r>
       <rPr>
@@ -1102,6 +1102,48 @@
   </si>
   <si>
     <t>10.1007/s40195-020-01072-6</t>
+  </si>
+  <si>
+    <t>10.1016/j.msea.2022.143026</t>
+  </si>
+  <si>
+    <t>Fe55Cr15Ni30</t>
+  </si>
+  <si>
+    <t>Fe55Cr15Ni27Nb3</t>
+  </si>
+  <si>
+    <t>Fe55Cr15Ni24Nb6</t>
+  </si>
+  <si>
+    <t>Fe55Cr15Ni21Nb9</t>
+  </si>
+  <si>
+    <t>Fe55Cr15Ni18Nb12</t>
+  </si>
+  <si>
+    <t>Fe55Cr15Ni15Nb15</t>
+  </si>
+  <si>
+    <t>Nb-0</t>
+  </si>
+  <si>
+    <t>Nb-3</t>
+  </si>
+  <si>
+    <t>Nb-6</t>
+  </si>
+  <si>
+    <t>Nb-9</t>
+  </si>
+  <si>
+    <t>Nb-12</t>
+  </si>
+  <si>
+    <t>Nb-15</t>
+  </si>
+  <si>
+    <t>5e-4 strain rate</t>
   </si>
 </sst>
 </file>
@@ -2135,7 +2177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="156">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2454,6 +2496,7 @@
     <xf numFmtId="49" fontId="14" fillId="10" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="10" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="10" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="12" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3616,8 +3659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T960"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A248" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N268" sqref="N268"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A260" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I287" sqref="I287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -13799,7 +13842,7 @@
         <v>298</v>
       </c>
       <c r="J233" s="35">
-        <f t="shared" ref="J233:J248" si="6">P233*9807000</f>
+        <f t="shared" ref="J233:J240" si="6">P233*9807000</f>
         <v>1447513200</v>
       </c>
       <c r="K233" s="38"/>
@@ -14224,7 +14267,7 @@
         <v>298</v>
       </c>
       <c r="J242" s="40">
-        <f t="shared" ref="J242:J264" si="7">-P242*0.001</f>
+        <f t="shared" ref="J242:J248" si="7">-P242*0.001</f>
         <v>-0.31900000000000001</v>
       </c>
       <c r="K242" s="38"/>
@@ -14614,7 +14657,7 @@
         <v>298</v>
       </c>
       <c r="J250" s="40">
-        <f t="shared" ref="J250:J264" si="8">P250*0.01</f>
+        <f t="shared" ref="J250:J256" si="8">P250*0.01</f>
         <v>4.0960000000000003E-2</v>
       </c>
       <c r="K250" s="38"/>
@@ -15321,20 +15364,42 @@
       <c r="T264" s="37"/>
     </row>
     <row r="265" spans="1:20" ht="18" customHeight="1">
-      <c r="A265" s="57"/>
-      <c r="B265" s="41"/>
-      <c r="C265" s="30"/>
-      <c r="D265" s="30"/>
+      <c r="A265" s="57" t="s">
+        <v>331</v>
+      </c>
+      <c r="B265" s="41" t="s">
+        <v>325</v>
+      </c>
+      <c r="C265" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D265" s="30" t="s">
+        <v>64</v>
+      </c>
       <c r="E265" s="31"/>
-      <c r="F265" s="53"/>
+      <c r="F265" s="53" t="s">
+        <v>194</v>
+      </c>
       <c r="G265" s="32"/>
-      <c r="H265" s="56"/>
-      <c r="I265" s="57"/>
-      <c r="J265" s="40"/>
+      <c r="H265" s="56" t="s">
+        <v>337</v>
+      </c>
+      <c r="I265" s="54">
+        <v>298</v>
+      </c>
+      <c r="J265" s="156">
+        <v>317000000</v>
+      </c>
       <c r="K265" s="38"/>
-      <c r="L265" s="40"/>
-      <c r="M265" s="40"/>
-      <c r="N265" s="40"/>
+      <c r="L265" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M265" s="40" t="s">
+        <v>221</v>
+      </c>
+      <c r="N265" s="40" t="s">
+        <v>324</v>
+      </c>
       <c r="O265" s="44"/>
       <c r="P265" s="44"/>
       <c r="Q265" s="44"/>
@@ -15343,20 +15408,42 @@
       <c r="T265" s="37"/>
     </row>
     <row r="266" spans="1:20" ht="18" customHeight="1">
-      <c r="A266" s="57"/>
-      <c r="B266" s="41"/>
-      <c r="C266" s="30"/>
-      <c r="D266" s="30"/>
+      <c r="A266" s="57" t="s">
+        <v>332</v>
+      </c>
+      <c r="B266" s="41" t="s">
+        <v>326</v>
+      </c>
+      <c r="C266" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="D266" s="30" t="s">
+        <v>64</v>
+      </c>
       <c r="E266" s="31"/>
-      <c r="F266" s="53"/>
+      <c r="F266" s="53" t="s">
+        <v>194</v>
+      </c>
       <c r="G266" s="32"/>
-      <c r="H266" s="56"/>
-      <c r="I266" s="57"/>
-      <c r="J266" s="40"/>
+      <c r="H266" s="56" t="s">
+        <v>337</v>
+      </c>
+      <c r="I266" s="54">
+        <v>298</v>
+      </c>
+      <c r="J266" s="156">
+        <v>404000000</v>
+      </c>
       <c r="K266" s="38"/>
-      <c r="L266" s="40"/>
-      <c r="M266" s="40"/>
-      <c r="N266" s="40"/>
+      <c r="L266" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M266" s="40" t="s">
+        <v>221</v>
+      </c>
+      <c r="N266" s="40" t="s">
+        <v>324</v>
+      </c>
       <c r="O266" s="44"/>
       <c r="P266" s="44"/>
       <c r="Q266" s="44"/>
@@ -15365,20 +15452,42 @@
       <c r="T266" s="37"/>
     </row>
     <row r="267" spans="1:20" ht="18" customHeight="1">
-      <c r="A267" s="57"/>
-      <c r="B267" s="41"/>
-      <c r="C267" s="30"/>
-      <c r="D267" s="30"/>
+      <c r="A267" s="57" t="s">
+        <v>333</v>
+      </c>
+      <c r="B267" s="41" t="s">
+        <v>327</v>
+      </c>
+      <c r="C267" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="D267" s="30" t="s">
+        <v>64</v>
+      </c>
       <c r="E267" s="31"/>
-      <c r="F267" s="53"/>
+      <c r="F267" s="53" t="s">
+        <v>194</v>
+      </c>
       <c r="G267" s="32"/>
-      <c r="H267" s="56"/>
-      <c r="I267" s="57"/>
-      <c r="J267" s="40"/>
+      <c r="H267" s="56" t="s">
+        <v>337</v>
+      </c>
+      <c r="I267" s="54">
+        <v>298</v>
+      </c>
+      <c r="J267" s="156">
+        <v>499000000</v>
+      </c>
       <c r="K267" s="38"/>
-      <c r="L267" s="40"/>
-      <c r="M267" s="40"/>
-      <c r="N267" s="40"/>
+      <c r="L267" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M267" s="40" t="s">
+        <v>221</v>
+      </c>
+      <c r="N267" s="40" t="s">
+        <v>324</v>
+      </c>
       <c r="O267" s="44"/>
       <c r="P267" s="44"/>
       <c r="Q267" s="44"/>
@@ -15387,20 +15496,42 @@
       <c r="T267" s="37"/>
     </row>
     <row r="268" spans="1:20" ht="18" customHeight="1">
-      <c r="A268" s="57"/>
-      <c r="B268" s="41"/>
-      <c r="C268" s="30"/>
-      <c r="D268" s="30"/>
+      <c r="A268" s="57" t="s">
+        <v>334</v>
+      </c>
+      <c r="B268" s="41" t="s">
+        <v>328</v>
+      </c>
+      <c r="C268" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="D268" s="30" t="s">
+        <v>64</v>
+      </c>
       <c r="E268" s="31"/>
-      <c r="F268" s="53"/>
+      <c r="F268" s="53" t="s">
+        <v>194</v>
+      </c>
       <c r="G268" s="32"/>
-      <c r="H268" s="56"/>
-      <c r="I268" s="57"/>
-      <c r="J268" s="40"/>
+      <c r="H268" s="56" t="s">
+        <v>337</v>
+      </c>
+      <c r="I268" s="54">
+        <v>298</v>
+      </c>
+      <c r="J268" s="156">
+        <v>749000000</v>
+      </c>
       <c r="K268" s="38"/>
-      <c r="L268" s="40"/>
-      <c r="M268" s="40"/>
-      <c r="N268" s="40"/>
+      <c r="L268" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M268" s="40" t="s">
+        <v>221</v>
+      </c>
+      <c r="N268" s="40" t="s">
+        <v>324</v>
+      </c>
       <c r="O268" s="44"/>
       <c r="P268" s="44"/>
       <c r="Q268" s="44"/>
@@ -15409,20 +15540,42 @@
       <c r="T268" s="37"/>
     </row>
     <row r="269" spans="1:20" ht="18" customHeight="1">
-      <c r="A269" s="57"/>
-      <c r="B269" s="57"/>
-      <c r="C269" s="57"/>
-      <c r="D269" s="57"/>
+      <c r="A269" s="57" t="s">
+        <v>335</v>
+      </c>
+      <c r="B269" s="41" t="s">
+        <v>329</v>
+      </c>
+      <c r="C269" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="D269" s="30" t="s">
+        <v>64</v>
+      </c>
       <c r="E269" s="55"/>
-      <c r="F269" s="57"/>
+      <c r="F269" s="53" t="s">
+        <v>194</v>
+      </c>
       <c r="G269" s="32"/>
-      <c r="H269" s="44"/>
-      <c r="I269" s="38"/>
-      <c r="J269" s="35"/>
+      <c r="H269" s="56" t="s">
+        <v>337</v>
+      </c>
+      <c r="I269" s="54">
+        <v>298</v>
+      </c>
+      <c r="J269" s="35">
+        <v>946000000</v>
+      </c>
       <c r="K269" s="38"/>
-      <c r="L269" s="57"/>
-      <c r="M269" s="57"/>
-      <c r="N269" s="40"/>
+      <c r="L269" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M269" s="40" t="s">
+        <v>221</v>
+      </c>
+      <c r="N269" s="40" t="s">
+        <v>324</v>
+      </c>
       <c r="O269" s="44"/>
       <c r="P269" s="44"/>
       <c r="Q269" s="44"/>
@@ -15431,20 +15584,42 @@
       <c r="T269" s="37"/>
     </row>
     <row r="270" spans="1:20" ht="18" customHeight="1">
-      <c r="A270" s="57"/>
-      <c r="B270" s="57"/>
-      <c r="C270" s="57"/>
-      <c r="D270" s="57"/>
+      <c r="A270" s="57" t="s">
+        <v>336</v>
+      </c>
+      <c r="B270" s="41" t="s">
+        <v>330</v>
+      </c>
+      <c r="C270" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="D270" s="30" t="s">
+        <v>64</v>
+      </c>
       <c r="E270" s="55"/>
-      <c r="F270" s="57"/>
+      <c r="F270" s="53" t="s">
+        <v>194</v>
+      </c>
       <c r="G270" s="32"/>
-      <c r="H270" s="44"/>
-      <c r="I270" s="38"/>
-      <c r="J270" s="35"/>
+      <c r="H270" s="56" t="s">
+        <v>337</v>
+      </c>
+      <c r="I270" s="54">
+        <v>298</v>
+      </c>
+      <c r="J270" s="35">
+        <v>1159000000</v>
+      </c>
       <c r="K270" s="38"/>
-      <c r="L270" s="57"/>
-      <c r="M270" s="57"/>
-      <c r="N270" s="40"/>
+      <c r="L270" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M270" s="40" t="s">
+        <v>221</v>
+      </c>
+      <c r="N270" s="40" t="s">
+        <v>324</v>
+      </c>
       <c r="O270" s="44"/>
       <c r="P270" s="44"/>
       <c r="Q270" s="44"/>
@@ -15453,20 +15628,42 @@
       <c r="T270" s="37"/>
     </row>
     <row r="271" spans="1:20" ht="18" customHeight="1">
-      <c r="A271" s="57"/>
-      <c r="B271" s="57"/>
-      <c r="C271" s="57"/>
-      <c r="D271" s="57"/>
+      <c r="A271" s="57" t="s">
+        <v>331</v>
+      </c>
+      <c r="B271" s="41" t="s">
+        <v>325</v>
+      </c>
+      <c r="C271" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D271" s="30" t="s">
+        <v>64</v>
+      </c>
       <c r="E271" s="55"/>
-      <c r="F271" s="57"/>
+      <c r="F271" s="57" t="s">
+        <v>273</v>
+      </c>
       <c r="G271" s="32"/>
-      <c r="H271" s="44"/>
-      <c r="I271" s="38"/>
-      <c r="J271" s="51"/>
+      <c r="H271" s="56" t="s">
+        <v>337</v>
+      </c>
+      <c r="I271" s="54">
+        <v>298</v>
+      </c>
+      <c r="J271" s="51">
+        <v>900000000</v>
+      </c>
       <c r="K271" s="38"/>
-      <c r="L271" s="57"/>
-      <c r="M271" s="57"/>
-      <c r="N271" s="40"/>
+      <c r="L271" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M271" s="40" t="s">
+        <v>221</v>
+      </c>
+      <c r="N271" s="40" t="s">
+        <v>324</v>
+      </c>
       <c r="O271" s="44"/>
       <c r="P271" s="44"/>
       <c r="Q271" s="44"/>
@@ -15475,20 +15672,42 @@
       <c r="T271" s="37"/>
     </row>
     <row r="272" spans="1:20" ht="18" customHeight="1">
-      <c r="A272" s="57"/>
-      <c r="B272" s="57"/>
-      <c r="C272" s="57"/>
-      <c r="D272" s="57"/>
+      <c r="A272" s="57" t="s">
+        <v>332</v>
+      </c>
+      <c r="B272" s="41" t="s">
+        <v>326</v>
+      </c>
+      <c r="C272" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="D272" s="30" t="s">
+        <v>64</v>
+      </c>
       <c r="E272" s="55"/>
-      <c r="F272" s="57"/>
+      <c r="F272" s="57" t="s">
+        <v>273</v>
+      </c>
       <c r="G272" s="32"/>
-      <c r="H272" s="44"/>
-      <c r="I272" s="38"/>
-      <c r="J272" s="51"/>
+      <c r="H272" s="56" t="s">
+        <v>337</v>
+      </c>
+      <c r="I272" s="54">
+        <v>298</v>
+      </c>
+      <c r="J272" s="51">
+        <v>870000000</v>
+      </c>
       <c r="K272" s="51"/>
-      <c r="L272" s="57"/>
-      <c r="M272" s="57"/>
-      <c r="N272" s="40"/>
+      <c r="L272" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M272" s="40" t="s">
+        <v>221</v>
+      </c>
+      <c r="N272" s="40" t="s">
+        <v>324</v>
+      </c>
       <c r="O272" s="44"/>
       <c r="P272" s="44"/>
       <c r="Q272" s="44"/>
@@ -15497,20 +15716,42 @@
       <c r="T272" s="37"/>
     </row>
     <row r="273" spans="1:20" ht="18" customHeight="1">
-      <c r="A273" s="57"/>
-      <c r="B273" s="57"/>
-      <c r="C273" s="57"/>
-      <c r="D273" s="57"/>
+      <c r="A273" s="57" t="s">
+        <v>333</v>
+      </c>
+      <c r="B273" s="41" t="s">
+        <v>327</v>
+      </c>
+      <c r="C273" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="D273" s="30" t="s">
+        <v>64</v>
+      </c>
       <c r="E273" s="55"/>
-      <c r="F273" s="57"/>
+      <c r="F273" s="57" t="s">
+        <v>274</v>
+      </c>
       <c r="G273" s="32"/>
-      <c r="H273" s="44"/>
-      <c r="I273" s="38"/>
-      <c r="J273" s="51"/>
+      <c r="H273" s="56" t="s">
+        <v>337</v>
+      </c>
+      <c r="I273" s="54">
+        <v>298</v>
+      </c>
+      <c r="J273" s="51">
+        <v>994000000</v>
+      </c>
       <c r="K273" s="51"/>
-      <c r="L273" s="57"/>
-      <c r="M273" s="57"/>
-      <c r="N273" s="40"/>
+      <c r="L273" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M273" s="40" t="s">
+        <v>221</v>
+      </c>
+      <c r="N273" s="40" t="s">
+        <v>324</v>
+      </c>
       <c r="O273" s="44"/>
       <c r="P273" s="44"/>
       <c r="Q273" s="44"/>
@@ -15519,20 +15760,42 @@
       <c r="T273" s="37"/>
     </row>
     <row r="274" spans="1:20" ht="18" customHeight="1">
-      <c r="A274" s="57"/>
-      <c r="B274" s="57"/>
-      <c r="C274" s="57"/>
-      <c r="D274" s="57"/>
+      <c r="A274" s="57" t="s">
+        <v>334</v>
+      </c>
+      <c r="B274" s="41" t="s">
+        <v>328</v>
+      </c>
+      <c r="C274" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="D274" s="30" t="s">
+        <v>64</v>
+      </c>
       <c r="E274" s="55"/>
-      <c r="F274" s="57"/>
+      <c r="F274" s="57" t="s">
+        <v>274</v>
+      </c>
       <c r="G274" s="32"/>
-      <c r="H274" s="44"/>
-      <c r="I274" s="38"/>
-      <c r="J274" s="51"/>
+      <c r="H274" s="56" t="s">
+        <v>337</v>
+      </c>
+      <c r="I274" s="54">
+        <v>298</v>
+      </c>
+      <c r="J274" s="51">
+        <v>1216000000</v>
+      </c>
       <c r="K274" s="38"/>
-      <c r="L274" s="57"/>
-      <c r="M274" s="57"/>
-      <c r="N274" s="40"/>
+      <c r="L274" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M274" s="40" t="s">
+        <v>221</v>
+      </c>
+      <c r="N274" s="40" t="s">
+        <v>324</v>
+      </c>
       <c r="O274" s="44"/>
       <c r="P274" s="44"/>
       <c r="Q274" s="44"/>
@@ -15541,20 +15804,42 @@
       <c r="T274" s="37"/>
     </row>
     <row r="275" spans="1:20" ht="18" customHeight="1">
-      <c r="A275" s="57"/>
-      <c r="B275" s="57"/>
-      <c r="C275" s="57"/>
-      <c r="D275" s="57"/>
+      <c r="A275" s="57" t="s">
+        <v>335</v>
+      </c>
+      <c r="B275" s="41" t="s">
+        <v>329</v>
+      </c>
+      <c r="C275" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="D275" s="30" t="s">
+        <v>64</v>
+      </c>
       <c r="E275" s="55"/>
-      <c r="F275" s="57"/>
+      <c r="F275" s="57" t="s">
+        <v>274</v>
+      </c>
       <c r="G275" s="32"/>
-      <c r="H275" s="44"/>
-      <c r="I275" s="38"/>
-      <c r="J275" s="51"/>
+      <c r="H275" s="56" t="s">
+        <v>337</v>
+      </c>
+      <c r="I275" s="54">
+        <v>298</v>
+      </c>
+      <c r="J275" s="51">
+        <v>1261000000</v>
+      </c>
       <c r="K275" s="38"/>
-      <c r="L275" s="57"/>
-      <c r="M275" s="57"/>
-      <c r="N275" s="40"/>
+      <c r="L275" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M275" s="40" t="s">
+        <v>221</v>
+      </c>
+      <c r="N275" s="40" t="s">
+        <v>324</v>
+      </c>
       <c r="O275" s="44"/>
       <c r="P275" s="44"/>
       <c r="Q275" s="44"/>
@@ -15563,20 +15848,42 @@
       <c r="T275" s="37"/>
     </row>
     <row r="276" spans="1:20" ht="18" customHeight="1">
-      <c r="A276" s="57"/>
-      <c r="B276" s="57"/>
-      <c r="C276" s="57"/>
-      <c r="D276" s="57"/>
+      <c r="A276" s="57" t="s">
+        <v>336</v>
+      </c>
+      <c r="B276" s="41" t="s">
+        <v>330</v>
+      </c>
+      <c r="C276" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="D276" s="30" t="s">
+        <v>64</v>
+      </c>
       <c r="E276" s="55"/>
-      <c r="F276" s="57"/>
+      <c r="F276" s="57" t="s">
+        <v>274</v>
+      </c>
       <c r="G276" s="32"/>
-      <c r="H276" s="44"/>
-      <c r="I276" s="44"/>
-      <c r="J276" s="51"/>
+      <c r="H276" s="56" t="s">
+        <v>337</v>
+      </c>
+      <c r="I276" s="54">
+        <v>298</v>
+      </c>
+      <c r="J276" s="51">
+        <v>1415000000</v>
+      </c>
       <c r="K276" s="44"/>
-      <c r="L276" s="57"/>
-      <c r="M276" s="57"/>
-      <c r="N276" s="40"/>
+      <c r="L276" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M276" s="40" t="s">
+        <v>221</v>
+      </c>
+      <c r="N276" s="40" t="s">
+        <v>324</v>
+      </c>
       <c r="O276" s="92"/>
       <c r="P276" s="44"/>
       <c r="Q276" s="44"/>
@@ -15585,20 +15892,42 @@
       <c r="T276" s="37"/>
     </row>
     <row r="277" spans="1:20" ht="18" customHeight="1">
-      <c r="A277" s="57"/>
-      <c r="B277" s="57"/>
-      <c r="C277" s="57"/>
-      <c r="D277" s="57"/>
+      <c r="A277" s="93" t="s">
+        <v>331</v>
+      </c>
+      <c r="B277" s="103" t="s">
+        <v>325</v>
+      </c>
+      <c r="C277" s="90" t="s">
+        <v>63</v>
+      </c>
+      <c r="D277" s="90" t="s">
+        <v>64</v>
+      </c>
       <c r="E277" s="55"/>
-      <c r="F277" s="57"/>
+      <c r="F277" s="57" t="s">
+        <v>272</v>
+      </c>
       <c r="G277" s="32"/>
-      <c r="H277" s="44"/>
-      <c r="I277" s="44"/>
-      <c r="J277" s="51"/>
+      <c r="H277" s="56" t="s">
+        <v>337</v>
+      </c>
+      <c r="I277" s="54">
+        <v>298</v>
+      </c>
+      <c r="J277" s="51">
+        <v>75</v>
+      </c>
       <c r="K277" s="44"/>
-      <c r="L277" s="57"/>
-      <c r="M277" s="57"/>
-      <c r="N277" s="40"/>
+      <c r="L277" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="M277" s="57" t="s">
+        <v>168</v>
+      </c>
+      <c r="N277" s="40" t="s">
+        <v>324</v>
+      </c>
       <c r="O277" s="44"/>
       <c r="P277" s="44"/>
       <c r="Q277" s="44"/>
@@ -15607,20 +15936,42 @@
       <c r="T277" s="37"/>
     </row>
     <row r="278" spans="1:20" ht="18" customHeight="1">
-      <c r="A278" s="57"/>
-      <c r="B278" s="57"/>
-      <c r="C278" s="57"/>
-      <c r="D278" s="57"/>
+      <c r="A278" s="95" t="s">
+        <v>332</v>
+      </c>
+      <c r="B278" s="105" t="s">
+        <v>326</v>
+      </c>
+      <c r="C278" s="91" t="s">
+        <v>161</v>
+      </c>
+      <c r="D278" s="91" t="s">
+        <v>64</v>
+      </c>
       <c r="E278" s="55"/>
-      <c r="F278" s="57"/>
+      <c r="F278" s="57" t="s">
+        <v>272</v>
+      </c>
       <c r="G278" s="32"/>
-      <c r="H278" s="44"/>
-      <c r="I278" s="44"/>
-      <c r="J278" s="51"/>
+      <c r="H278" s="56" t="s">
+        <v>337</v>
+      </c>
+      <c r="I278" s="54">
+        <v>298</v>
+      </c>
+      <c r="J278" s="51">
+        <v>75</v>
+      </c>
       <c r="K278" s="44"/>
-      <c r="L278" s="57"/>
-      <c r="M278" s="57"/>
-      <c r="N278" s="40"/>
+      <c r="L278" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="M278" s="57" t="s">
+        <v>168</v>
+      </c>
+      <c r="N278" s="40" t="s">
+        <v>324</v>
+      </c>
       <c r="O278" s="44"/>
       <c r="P278" s="44"/>
       <c r="Q278" s="44"/>
@@ -15629,20 +15980,42 @@
       <c r="T278" s="37"/>
     </row>
     <row r="279" spans="1:20" ht="18" customHeight="1">
-      <c r="A279" s="57"/>
-      <c r="B279" s="57"/>
-      <c r="C279" s="57"/>
-      <c r="D279" s="57"/>
+      <c r="A279" s="95" t="s">
+        <v>333</v>
+      </c>
+      <c r="B279" s="105" t="s">
+        <v>327</v>
+      </c>
+      <c r="C279" s="91" t="s">
+        <v>161</v>
+      </c>
+      <c r="D279" s="91" t="s">
+        <v>64</v>
+      </c>
       <c r="E279" s="55"/>
-      <c r="F279" s="57"/>
+      <c r="F279" s="57" t="s">
+        <v>271</v>
+      </c>
       <c r="G279" s="32"/>
-      <c r="H279" s="44"/>
-      <c r="I279" s="44"/>
-      <c r="J279" s="51"/>
+      <c r="H279" s="56" t="s">
+        <v>337</v>
+      </c>
+      <c r="I279" s="54">
+        <v>298</v>
+      </c>
+      <c r="J279" s="44">
+        <v>37.116564417177898</v>
+      </c>
       <c r="K279" s="44"/>
-      <c r="L279" s="57"/>
-      <c r="M279" s="57"/>
-      <c r="N279" s="40"/>
+      <c r="L279" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="M279" s="57" t="s">
+        <v>168</v>
+      </c>
+      <c r="N279" s="40" t="s">
+        <v>324</v>
+      </c>
       <c r="O279" s="44"/>
       <c r="P279" s="44"/>
       <c r="Q279" s="44"/>
@@ -15651,20 +16024,42 @@
       <c r="T279" s="37"/>
     </row>
     <row r="280" spans="1:20" ht="18" customHeight="1">
-      <c r="A280" s="57"/>
-      <c r="B280" s="57"/>
-      <c r="C280" s="57"/>
-      <c r="D280" s="57"/>
+      <c r="A280" s="95" t="s">
+        <v>334</v>
+      </c>
+      <c r="B280" s="105" t="s">
+        <v>328</v>
+      </c>
+      <c r="C280" s="91" t="s">
+        <v>161</v>
+      </c>
+      <c r="D280" s="91" t="s">
+        <v>64</v>
+      </c>
       <c r="E280" s="55"/>
-      <c r="F280" s="57"/>
+      <c r="F280" s="57" t="s">
+        <v>271</v>
+      </c>
       <c r="G280" s="32"/>
-      <c r="H280" s="44"/>
-      <c r="I280" s="44"/>
-      <c r="J280" s="51"/>
+      <c r="H280" s="56" t="s">
+        <v>337</v>
+      </c>
+      <c r="I280" s="54">
+        <v>298</v>
+      </c>
+      <c r="J280" s="44">
+        <v>35.460122699386503</v>
+      </c>
       <c r="K280" s="44"/>
-      <c r="L280" s="57"/>
-      <c r="M280" s="57"/>
-      <c r="N280" s="40"/>
+      <c r="L280" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="M280" s="57" t="s">
+        <v>168</v>
+      </c>
+      <c r="N280" s="40" t="s">
+        <v>324</v>
+      </c>
       <c r="O280" s="44"/>
       <c r="P280" s="44"/>
       <c r="Q280" s="44"/>
@@ -15673,20 +16068,42 @@
       <c r="T280" s="37"/>
     </row>
     <row r="281" spans="1:20" ht="18" customHeight="1">
-      <c r="A281" s="57"/>
-      <c r="B281" s="57"/>
-      <c r="C281" s="57"/>
-      <c r="D281" s="57"/>
+      <c r="A281" s="95" t="s">
+        <v>335</v>
+      </c>
+      <c r="B281" s="105" t="s">
+        <v>329</v>
+      </c>
+      <c r="C281" s="91" t="s">
+        <v>161</v>
+      </c>
+      <c r="D281" s="91" t="s">
+        <v>64</v>
+      </c>
       <c r="E281" s="55"/>
-      <c r="F281" s="57"/>
+      <c r="F281" s="57" t="s">
+        <v>271</v>
+      </c>
       <c r="G281" s="32"/>
-      <c r="H281" s="44"/>
-      <c r="I281" s="38"/>
-      <c r="J281" s="44"/>
+      <c r="H281" s="56" t="s">
+        <v>337</v>
+      </c>
+      <c r="I281" s="54">
+        <v>298</v>
+      </c>
+      <c r="J281" s="44">
+        <v>26.993865030674801</v>
+      </c>
       <c r="K281" s="44"/>
-      <c r="L281" s="57"/>
-      <c r="M281" s="57"/>
-      <c r="N281" s="40"/>
+      <c r="L281" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="M281" s="57" t="s">
+        <v>168</v>
+      </c>
+      <c r="N281" s="40" t="s">
+        <v>324</v>
+      </c>
       <c r="O281" s="44"/>
       <c r="P281" s="44"/>
       <c r="Q281" s="44"/>
@@ -15695,20 +16112,42 @@
       <c r="T281" s="37"/>
     </row>
     <row r="282" spans="1:20" ht="18" customHeight="1">
-      <c r="A282" s="57"/>
-      <c r="B282" s="57"/>
-      <c r="C282" s="57"/>
-      <c r="D282" s="57"/>
+      <c r="A282" s="95" t="s">
+        <v>336</v>
+      </c>
+      <c r="B282" s="105" t="s">
+        <v>330</v>
+      </c>
+      <c r="C282" s="91" t="s">
+        <v>161</v>
+      </c>
+      <c r="D282" s="91" t="s">
+        <v>64</v>
+      </c>
       <c r="E282" s="55"/>
-      <c r="F282" s="57"/>
+      <c r="F282" s="57" t="s">
+        <v>271</v>
+      </c>
       <c r="G282" s="32"/>
-      <c r="H282" s="44"/>
-      <c r="I282" s="38"/>
-      <c r="J282" s="44"/>
+      <c r="H282" s="56" t="s">
+        <v>337</v>
+      </c>
+      <c r="I282" s="54">
+        <v>298</v>
+      </c>
+      <c r="J282" s="44">
+        <v>20.245398773006102</v>
+      </c>
       <c r="K282" s="44"/>
-      <c r="L282" s="57"/>
-      <c r="M282" s="57"/>
-      <c r="N282" s="40"/>
+      <c r="L282" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="M282" s="57" t="s">
+        <v>168</v>
+      </c>
+      <c r="N282" s="40" t="s">
+        <v>324</v>
+      </c>
       <c r="O282" s="44"/>
       <c r="P282" s="44"/>
       <c r="Q282" s="44"/>

</xml_diff>

<commit_message>
- minor fix for missing source qualifier for the last two papers
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Aug2025.xlsx
+++ b/MiscSmallUploads_Aug2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932CE614-ABA5-2A46-9BCF-C752FD90A350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F3F4C8-F602-1E48-ABEA-E5C1522C7B4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="7580" windowWidth="34560" windowHeight="12760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2551" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2633" uniqueCount="338">
   <si>
     <r>
       <rPr>
@@ -2382,57 +2382,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="14" fillId="10" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="14" fillId="10" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="12" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2493,10 +2446,57 @@
     <xf numFmtId="164" fontId="5" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="10" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="12" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3659,8 +3659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T960"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A260" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I287" sqref="I287"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A261" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H284" sqref="H284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -3717,19 +3717,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" s="133" t="s">
+      <c r="D2" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="134"/>
-      <c r="F2" s="137"/>
-      <c r="G2" s="138"/>
-      <c r="H2" s="138"/>
-      <c r="I2" s="139"/>
-      <c r="J2" s="140"/>
-      <c r="K2" s="140"/>
-      <c r="L2" s="138"/>
-      <c r="M2" s="138"/>
-      <c r="N2" s="141"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="124"/>
+      <c r="G2" s="125"/>
+      <c r="H2" s="125"/>
+      <c r="I2" s="126"/>
+      <c r="J2" s="127"/>
+      <c r="K2" s="127"/>
+      <c r="L2" s="125"/>
+      <c r="M2" s="125"/>
+      <c r="N2" s="128"/>
       <c r="O2" s="13"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -3745,17 +3745,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="135"/>
-      <c r="E3" s="136"/>
-      <c r="F3" s="142"/>
-      <c r="G3" s="142"/>
-      <c r="H3" s="142"/>
-      <c r="I3" s="143"/>
-      <c r="J3" s="144"/>
-      <c r="K3" s="144"/>
-      <c r="L3" s="142"/>
-      <c r="M3" s="142"/>
-      <c r="N3" s="145"/>
+      <c r="D3" s="122"/>
+      <c r="E3" s="123"/>
+      <c r="F3" s="129"/>
+      <c r="G3" s="129"/>
+      <c r="H3" s="129"/>
+      <c r="I3" s="130"/>
+      <c r="J3" s="131"/>
+      <c r="K3" s="131"/>
+      <c r="L3" s="129"/>
+      <c r="M3" s="129"/>
+      <c r="N3" s="132"/>
       <c r="O3" s="13"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -3796,43 +3796,43 @@
       <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="146" t="s">
+      <c r="C5" s="133" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="148" t="s">
+      <c r="D5" s="135" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="148" t="s">
+      <c r="E5" s="135" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="148" t="s">
+      <c r="F5" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="148" t="s">
+      <c r="G5" s="135" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="149" t="s">
+      <c r="H5" s="136" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="148" t="s">
+      <c r="I5" s="135" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="148" t="s">
+      <c r="J5" s="135" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="148" t="s">
+      <c r="K5" s="135" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="148" t="s">
+      <c r="L5" s="135" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="148" t="s">
+      <c r="M5" s="135" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="148" t="s">
+      <c r="N5" s="135" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="116" t="s">
+      <c r="O5" s="140" t="s">
         <v>20</v>
       </c>
       <c r="P5" s="25"/>
@@ -3848,19 +3848,19 @@
       <c r="B6" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="147"/>
-      <c r="D6" s="147"/>
-      <c r="E6" s="147"/>
-      <c r="F6" s="147"/>
-      <c r="G6" s="147"/>
-      <c r="H6" s="150"/>
-      <c r="I6" s="151"/>
-      <c r="J6" s="152"/>
-      <c r="K6" s="152"/>
-      <c r="L6" s="147"/>
-      <c r="M6" s="147"/>
-      <c r="N6" s="147"/>
-      <c r="O6" s="117"/>
+      <c r="C6" s="134"/>
+      <c r="D6" s="134"/>
+      <c r="E6" s="134"/>
+      <c r="F6" s="134"/>
+      <c r="G6" s="134"/>
+      <c r="H6" s="137"/>
+      <c r="I6" s="138"/>
+      <c r="J6" s="139"/>
+      <c r="K6" s="139"/>
+      <c r="L6" s="134"/>
+      <c r="M6" s="134"/>
+      <c r="N6" s="134"/>
+      <c r="O6" s="141"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="9"/>
@@ -3910,7 +3910,7 @@
       <c r="N7" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="118"/>
+      <c r="O7" s="142"/>
       <c r="P7" s="64" t="s">
         <v>62</v>
       </c>
@@ -3925,35 +3925,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" thickBot="1">
       <c r="A8" s="59"/>
-      <c r="B8" s="119" t="s">
+      <c r="B8" s="143" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="120"/>
-      <c r="D8" s="120"/>
-      <c r="E8" s="121"/>
-      <c r="F8" s="122" t="s">
+      <c r="C8" s="144"/>
+      <c r="D8" s="144"/>
+      <c r="E8" s="145"/>
+      <c r="F8" s="146" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="123"/>
-      <c r="H8" s="123"/>
-      <c r="I8" s="124"/>
-      <c r="J8" s="125"/>
-      <c r="K8" s="125"/>
-      <c r="L8" s="126"/>
-      <c r="M8" s="127" t="s">
+      <c r="G8" s="147"/>
+      <c r="H8" s="147"/>
+      <c r="I8" s="148"/>
+      <c r="J8" s="149"/>
+      <c r="K8" s="149"/>
+      <c r="L8" s="150"/>
+      <c r="M8" s="151" t="s">
         <v>40</v>
       </c>
-      <c r="N8" s="128"/>
+      <c r="N8" s="152"/>
       <c r="O8" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="P8" s="129" t="s">
+      <c r="P8" s="153" t="s">
         <v>42</v>
       </c>
-      <c r="Q8" s="130"/>
-      <c r="R8" s="131"/>
-      <c r="S8" s="131"/>
-      <c r="T8" s="132"/>
+      <c r="Q8" s="154"/>
+      <c r="R8" s="155"/>
+      <c r="S8" s="155"/>
+      <c r="T8" s="156"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1">
       <c r="A9" s="60" t="s">
@@ -12327,7 +12327,7 @@
       <c r="E200" s="31" t="s">
         <v>311</v>
       </c>
-      <c r="F200" s="153" t="s">
+      <c r="F200" s="116" t="s">
         <v>122</v>
       </c>
       <c r="G200" s="32" t="s">
@@ -12372,7 +12372,9 @@
       <c r="F201" s="52" t="s">
         <v>194</v>
       </c>
-      <c r="G201" s="32"/>
+      <c r="G201" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H201" s="56" t="s">
         <v>195</v>
       </c>
@@ -12418,7 +12420,9 @@
       <c r="F202" s="52" t="s">
         <v>194</v>
       </c>
-      <c r="G202" s="32"/>
+      <c r="G202" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H202" s="56" t="s">
         <v>195</v>
       </c>
@@ -12464,7 +12468,9 @@
       <c r="F203" s="52" t="s">
         <v>194</v>
       </c>
-      <c r="G203" s="32"/>
+      <c r="G203" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H203" s="56" t="s">
         <v>195</v>
       </c>
@@ -12510,7 +12516,9 @@
       <c r="F204" s="52" t="s">
         <v>194</v>
       </c>
-      <c r="G204" s="32"/>
+      <c r="G204" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H204" s="56" t="s">
         <v>195</v>
       </c>
@@ -12556,7 +12564,9 @@
       <c r="F205" s="52" t="s">
         <v>194</v>
       </c>
-      <c r="G205" s="32"/>
+      <c r="G205" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H205" s="56" t="s">
         <v>195</v>
       </c>
@@ -12602,7 +12612,9 @@
       <c r="F206" s="52" t="s">
         <v>194</v>
       </c>
-      <c r="G206" s="32"/>
+      <c r="G206" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H206" s="56" t="s">
         <v>195</v>
       </c>
@@ -12648,7 +12660,9 @@
       <c r="F207" s="52" t="s">
         <v>194</v>
       </c>
-      <c r="G207" s="97"/>
+      <c r="G207" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H207" s="56" t="s">
         <v>195</v>
       </c>
@@ -12694,7 +12708,9 @@
       <c r="F208" s="52" t="s">
         <v>194</v>
       </c>
-      <c r="G208" s="98"/>
+      <c r="G208" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H208" s="56" t="s">
         <v>195</v>
       </c>
@@ -12738,7 +12754,9 @@
       <c r="F209" s="97" t="s">
         <v>273</v>
       </c>
-      <c r="G209" s="98"/>
+      <c r="G209" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H209" s="56" t="s">
         <v>195</v>
       </c>
@@ -12784,7 +12802,9 @@
       <c r="F210" s="97" t="s">
         <v>273</v>
       </c>
-      <c r="G210" s="98"/>
+      <c r="G210" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H210" s="56" t="s">
         <v>195</v>
       </c>
@@ -12830,7 +12850,9 @@
       <c r="F211" s="97" t="s">
         <v>274</v>
       </c>
-      <c r="G211" s="97"/>
+      <c r="G211" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H211" s="56" t="s">
         <v>195</v>
       </c>
@@ -12876,7 +12898,9 @@
       <c r="F212" s="97" t="s">
         <v>274</v>
       </c>
-      <c r="G212" s="98"/>
+      <c r="G212" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H212" s="56" t="s">
         <v>195</v>
       </c>
@@ -12922,7 +12946,9 @@
       <c r="F213" s="97" t="s">
         <v>274</v>
       </c>
-      <c r="G213" s="98"/>
+      <c r="G213" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H213" s="56" t="s">
         <v>195</v>
       </c>
@@ -12968,7 +12994,9 @@
       <c r="F214" s="97" t="s">
         <v>274</v>
       </c>
-      <c r="G214" s="98"/>
+      <c r="G214" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H214" s="56" t="s">
         <v>195</v>
       </c>
@@ -13014,7 +13042,9 @@
       <c r="F215" s="97" t="s">
         <v>274</v>
       </c>
-      <c r="G215" s="98"/>
+      <c r="G215" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H215" s="56" t="s">
         <v>195</v>
       </c>
@@ -13060,7 +13090,9 @@
       <c r="F216" s="97" t="s">
         <v>274</v>
       </c>
-      <c r="G216" s="98"/>
+      <c r="G216" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H216" s="56" t="s">
         <v>195</v>
       </c>
@@ -13088,7 +13120,7 @@
       <c r="T216" s="37"/>
     </row>
     <row r="217" spans="1:20" ht="18" customHeight="1">
-      <c r="A217" s="154" t="s">
+      <c r="A217" s="117" t="s">
         <v>282</v>
       </c>
       <c r="B217" s="103" t="s">
@@ -13104,7 +13136,9 @@
       <c r="F217" s="53" t="s">
         <v>314</v>
       </c>
-      <c r="G217" s="98"/>
+      <c r="G217" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H217" s="56" t="s">
         <v>195</v>
       </c>
@@ -13132,7 +13166,7 @@
       <c r="T217" s="37"/>
     </row>
     <row r="218" spans="1:20" ht="18" customHeight="1">
-      <c r="A218" s="155" t="s">
+      <c r="A218" s="118" t="s">
         <v>303</v>
       </c>
       <c r="B218" s="105" t="s">
@@ -13150,7 +13184,9 @@
       <c r="F218" s="53" t="s">
         <v>314</v>
       </c>
-      <c r="G218" s="98"/>
+      <c r="G218" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H218" s="56" t="s">
         <v>195</v>
       </c>
@@ -13178,7 +13214,7 @@
       <c r="T218" s="37"/>
     </row>
     <row r="219" spans="1:20" ht="18" customHeight="1">
-      <c r="A219" s="155" t="s">
+      <c r="A219" s="118" t="s">
         <v>304</v>
       </c>
       <c r="B219" s="105" t="s">
@@ -13196,7 +13232,9 @@
       <c r="F219" s="53" t="s">
         <v>313</v>
       </c>
-      <c r="G219" s="98"/>
+      <c r="G219" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H219" s="56" t="s">
         <v>195</v>
       </c>
@@ -13224,7 +13262,7 @@
       <c r="T219" s="37"/>
     </row>
     <row r="220" spans="1:20" ht="18" customHeight="1">
-      <c r="A220" s="155" t="s">
+      <c r="A220" s="118" t="s">
         <v>305</v>
       </c>
       <c r="B220" s="105" t="s">
@@ -13242,7 +13280,9 @@
       <c r="F220" s="53" t="s">
         <v>313</v>
       </c>
-      <c r="G220" s="98"/>
+      <c r="G220" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H220" s="56" t="s">
         <v>195</v>
       </c>
@@ -13270,7 +13310,7 @@
       <c r="T220" s="37"/>
     </row>
     <row r="221" spans="1:20" ht="18" customHeight="1">
-      <c r="A221" s="155" t="s">
+      <c r="A221" s="118" t="s">
         <v>306</v>
       </c>
       <c r="B221" s="105" t="s">
@@ -13288,7 +13328,9 @@
       <c r="F221" s="53" t="s">
         <v>313</v>
       </c>
-      <c r="G221" s="32"/>
+      <c r="G221" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H221" s="56" t="s">
         <v>195</v>
       </c>
@@ -13316,7 +13358,7 @@
       <c r="T221" s="37"/>
     </row>
     <row r="222" spans="1:20" ht="18" customHeight="1">
-      <c r="A222" s="155" t="s">
+      <c r="A222" s="118" t="s">
         <v>309</v>
       </c>
       <c r="B222" s="105" t="s">
@@ -13334,7 +13376,9 @@
       <c r="F222" s="53" t="s">
         <v>313</v>
       </c>
-      <c r="G222" s="32"/>
+      <c r="G222" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H222" s="56" t="s">
         <v>195</v>
       </c>
@@ -13362,7 +13406,7 @@
       <c r="T222" s="37"/>
     </row>
     <row r="223" spans="1:20" ht="18" customHeight="1">
-      <c r="A223" s="155" t="s">
+      <c r="A223" s="118" t="s">
         <v>307</v>
       </c>
       <c r="B223" s="105" t="s">
@@ -13380,7 +13424,9 @@
       <c r="F223" s="53" t="s">
         <v>313</v>
       </c>
-      <c r="G223" s="32"/>
+      <c r="G223" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H223" s="56" t="s">
         <v>195</v>
       </c>
@@ -13408,7 +13454,7 @@
       <c r="T223" s="37"/>
     </row>
     <row r="224" spans="1:20" ht="18" customHeight="1">
-      <c r="A224" s="155" t="s">
+      <c r="A224" s="118" t="s">
         <v>308</v>
       </c>
       <c r="B224" s="105" t="s">
@@ -13426,7 +13472,9 @@
       <c r="F224" s="53" t="s">
         <v>313</v>
       </c>
-      <c r="G224" s="32"/>
+      <c r="G224" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H224" s="56" t="s">
         <v>195</v>
       </c>
@@ -13454,7 +13502,7 @@
       <c r="T224" s="37"/>
     </row>
     <row r="225" spans="1:20" ht="18" customHeight="1">
-      <c r="A225" s="154" t="s">
+      <c r="A225" s="117" t="s">
         <v>282</v>
       </c>
       <c r="B225" s="103" t="s">
@@ -13470,7 +13518,9 @@
       <c r="F225" s="53" t="s">
         <v>272</v>
       </c>
-      <c r="G225" s="32"/>
+      <c r="G225" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H225" s="56" t="s">
         <v>195</v>
       </c>
@@ -13498,7 +13548,7 @@
       <c r="T225" s="37"/>
     </row>
     <row r="226" spans="1:20" ht="18" customHeight="1">
-      <c r="A226" s="155" t="s">
+      <c r="A226" s="118" t="s">
         <v>303</v>
       </c>
       <c r="B226" s="105" t="s">
@@ -13516,7 +13566,9 @@
       <c r="F226" s="53" t="s">
         <v>272</v>
       </c>
-      <c r="G226" s="32"/>
+      <c r="G226" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H226" s="56" t="s">
         <v>195</v>
       </c>
@@ -13544,7 +13596,7 @@
       <c r="T226" s="37"/>
     </row>
     <row r="227" spans="1:20" ht="18" customHeight="1">
-      <c r="A227" s="155" t="s">
+      <c r="A227" s="118" t="s">
         <v>304</v>
       </c>
       <c r="B227" s="105" t="s">
@@ -13562,7 +13614,9 @@
       <c r="F227" s="53" t="s">
         <v>271</v>
       </c>
-      <c r="G227" s="32"/>
+      <c r="G227" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H227" s="56" t="s">
         <v>195</v>
       </c>
@@ -13590,7 +13644,7 @@
       <c r="T227" s="37"/>
     </row>
     <row r="228" spans="1:20" ht="18" customHeight="1">
-      <c r="A228" s="155" t="s">
+      <c r="A228" s="118" t="s">
         <v>305</v>
       </c>
       <c r="B228" s="105" t="s">
@@ -13608,7 +13662,9 @@
       <c r="F228" s="53" t="s">
         <v>271</v>
       </c>
-      <c r="G228" s="32"/>
+      <c r="G228" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H228" s="56" t="s">
         <v>195</v>
       </c>
@@ -13636,7 +13692,7 @@
       <c r="T228" s="37"/>
     </row>
     <row r="229" spans="1:20" ht="18" customHeight="1">
-      <c r="A229" s="155" t="s">
+      <c r="A229" s="118" t="s">
         <v>306</v>
       </c>
       <c r="B229" s="105" t="s">
@@ -13654,7 +13710,9 @@
       <c r="F229" s="53" t="s">
         <v>271</v>
       </c>
-      <c r="G229" s="32"/>
+      <c r="G229" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H229" s="56" t="s">
         <v>195</v>
       </c>
@@ -13682,7 +13740,7 @@
       <c r="T229" s="37"/>
     </row>
     <row r="230" spans="1:20" ht="18" customHeight="1">
-      <c r="A230" s="155" t="s">
+      <c r="A230" s="118" t="s">
         <v>309</v>
       </c>
       <c r="B230" s="105" t="s">
@@ -13700,7 +13758,9 @@
       <c r="F230" s="53" t="s">
         <v>271</v>
       </c>
-      <c r="G230" s="32"/>
+      <c r="G230" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H230" s="56" t="s">
         <v>195</v>
       </c>
@@ -13728,7 +13788,7 @@
       <c r="T230" s="37"/>
     </row>
     <row r="231" spans="1:20" ht="18" customHeight="1">
-      <c r="A231" s="155" t="s">
+      <c r="A231" s="118" t="s">
         <v>307</v>
       </c>
       <c r="B231" s="105" t="s">
@@ -13746,7 +13806,9 @@
       <c r="F231" s="53" t="s">
         <v>271</v>
       </c>
-      <c r="G231" s="32"/>
+      <c r="G231" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H231" s="56" t="s">
         <v>195</v>
       </c>
@@ -13774,7 +13836,7 @@
       <c r="T231" s="37"/>
     </row>
     <row r="232" spans="1:20" ht="18" customHeight="1">
-      <c r="A232" s="155" t="s">
+      <c r="A232" s="118" t="s">
         <v>308</v>
       </c>
       <c r="B232" s="105" t="s">
@@ -13792,7 +13854,9 @@
       <c r="F232" s="53" t="s">
         <v>271</v>
       </c>
-      <c r="G232" s="32"/>
+      <c r="G232" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H232" s="56" t="s">
         <v>195</v>
       </c>
@@ -13820,7 +13884,7 @@
       <c r="T232" s="37"/>
     </row>
     <row r="233" spans="1:20" ht="18" customHeight="1">
-      <c r="A233" s="154" t="s">
+      <c r="A233" s="117" t="s">
         <v>282</v>
       </c>
       <c r="B233" s="103" t="s">
@@ -13836,7 +13900,9 @@
       <c r="F233" s="53" t="s">
         <v>179</v>
       </c>
-      <c r="G233" s="32"/>
+      <c r="G233" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H233" s="56"/>
       <c r="I233" s="54">
         <v>298</v>
@@ -13865,7 +13931,7 @@
       <c r="T233" s="37"/>
     </row>
     <row r="234" spans="1:20" ht="18" customHeight="1">
-      <c r="A234" s="155" t="s">
+      <c r="A234" s="118" t="s">
         <v>303</v>
       </c>
       <c r="B234" s="105" t="s">
@@ -13883,7 +13949,9 @@
       <c r="F234" s="53" t="s">
         <v>179</v>
       </c>
-      <c r="G234" s="32"/>
+      <c r="G234" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H234" s="56"/>
       <c r="I234" s="54">
         <v>298</v>
@@ -13912,7 +13980,7 @@
       <c r="T234" s="37"/>
     </row>
     <row r="235" spans="1:20" ht="18" customHeight="1">
-      <c r="A235" s="155" t="s">
+      <c r="A235" s="118" t="s">
         <v>304</v>
       </c>
       <c r="B235" s="105" t="s">
@@ -13930,7 +13998,9 @@
       <c r="F235" s="53" t="s">
         <v>179</v>
       </c>
-      <c r="G235" s="32"/>
+      <c r="G235" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H235" s="56"/>
       <c r="I235" s="54">
         <v>298</v>
@@ -13959,7 +14029,7 @@
       <c r="T235" s="37"/>
     </row>
     <row r="236" spans="1:20" ht="18" customHeight="1">
-      <c r="A236" s="155" t="s">
+      <c r="A236" s="118" t="s">
         <v>305</v>
       </c>
       <c r="B236" s="105" t="s">
@@ -13977,7 +14047,9 @@
       <c r="F236" s="53" t="s">
         <v>179</v>
       </c>
-      <c r="G236" s="32"/>
+      <c r="G236" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H236" s="56"/>
       <c r="I236" s="54">
         <v>298</v>
@@ -14006,7 +14078,7 @@
       <c r="T236" s="37"/>
     </row>
     <row r="237" spans="1:20" ht="18" customHeight="1">
-      <c r="A237" s="155" t="s">
+      <c r="A237" s="118" t="s">
         <v>306</v>
       </c>
       <c r="B237" s="105" t="s">
@@ -14024,7 +14096,9 @@
       <c r="F237" s="53" t="s">
         <v>179</v>
       </c>
-      <c r="G237" s="32"/>
+      <c r="G237" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H237" s="56"/>
       <c r="I237" s="54">
         <v>298</v>
@@ -14053,7 +14127,7 @@
       <c r="T237" s="37"/>
     </row>
     <row r="238" spans="1:20" ht="18" customHeight="1">
-      <c r="A238" s="155" t="s">
+      <c r="A238" s="118" t="s">
         <v>309</v>
       </c>
       <c r="B238" s="105" t="s">
@@ -14071,7 +14145,9 @@
       <c r="F238" s="53" t="s">
         <v>179</v>
       </c>
-      <c r="G238" s="32"/>
+      <c r="G238" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H238" s="56"/>
       <c r="I238" s="54">
         <v>298</v>
@@ -14100,7 +14176,7 @@
       <c r="T238" s="37"/>
     </row>
     <row r="239" spans="1:20" ht="18" customHeight="1">
-      <c r="A239" s="155" t="s">
+      <c r="A239" s="118" t="s">
         <v>307</v>
       </c>
       <c r="B239" s="105" t="s">
@@ -14118,7 +14194,9 @@
       <c r="F239" s="53" t="s">
         <v>179</v>
       </c>
-      <c r="G239" s="32"/>
+      <c r="G239" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H239" s="56"/>
       <c r="I239" s="54">
         <v>298</v>
@@ -14147,7 +14225,7 @@
       <c r="T239" s="37"/>
     </row>
     <row r="240" spans="1:20" ht="18" customHeight="1">
-      <c r="A240" s="155" t="s">
+      <c r="A240" s="118" t="s">
         <v>308</v>
       </c>
       <c r="B240" s="105" t="s">
@@ -14165,7 +14243,9 @@
       <c r="F240" s="53" t="s">
         <v>179</v>
       </c>
-      <c r="G240" s="32"/>
+      <c r="G240" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H240" s="56"/>
       <c r="I240" s="54">
         <v>298</v>
@@ -14194,7 +14274,7 @@
       <c r="T240" s="37"/>
     </row>
     <row r="241" spans="1:20" ht="18" customHeight="1">
-      <c r="A241" s="154" t="s">
+      <c r="A241" s="117" t="s">
         <v>282</v>
       </c>
       <c r="B241" s="103" t="s">
@@ -14210,7 +14290,9 @@
       <c r="F241" s="53" t="s">
         <v>315</v>
       </c>
-      <c r="G241" s="32"/>
+      <c r="G241" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H241" s="56" t="s">
         <v>322</v>
       </c>
@@ -14241,7 +14323,7 @@
       <c r="T241" s="37"/>
     </row>
     <row r="242" spans="1:20" ht="18" customHeight="1">
-      <c r="A242" s="155" t="s">
+      <c r="A242" s="118" t="s">
         <v>303</v>
       </c>
       <c r="B242" s="105" t="s">
@@ -14259,7 +14341,9 @@
       <c r="F242" s="53" t="s">
         <v>315</v>
       </c>
-      <c r="G242" s="32"/>
+      <c r="G242" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H242" s="56" t="s">
         <v>322</v>
       </c>
@@ -14290,7 +14374,7 @@
       <c r="T242" s="37"/>
     </row>
     <row r="243" spans="1:20" ht="18" customHeight="1">
-      <c r="A243" s="155" t="s">
+      <c r="A243" s="118" t="s">
         <v>304</v>
       </c>
       <c r="B243" s="105" t="s">
@@ -14308,7 +14392,9 @@
       <c r="F243" s="53" t="s">
         <v>315</v>
       </c>
-      <c r="G243" s="32"/>
+      <c r="G243" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H243" s="56" t="s">
         <v>322</v>
       </c>
@@ -14339,7 +14425,7 @@
       <c r="T243" s="37"/>
     </row>
     <row r="244" spans="1:20" ht="18" customHeight="1">
-      <c r="A244" s="155" t="s">
+      <c r="A244" s="118" t="s">
         <v>305</v>
       </c>
       <c r="B244" s="105" t="s">
@@ -14357,7 +14443,9 @@
       <c r="F244" s="53" t="s">
         <v>315</v>
       </c>
-      <c r="G244" s="32"/>
+      <c r="G244" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H244" s="56" t="s">
         <v>322</v>
       </c>
@@ -14388,7 +14476,7 @@
       <c r="T244" s="37"/>
     </row>
     <row r="245" spans="1:20" ht="18" customHeight="1">
-      <c r="A245" s="155" t="s">
+      <c r="A245" s="118" t="s">
         <v>306</v>
       </c>
       <c r="B245" s="105" t="s">
@@ -14406,7 +14494,9 @@
       <c r="F245" s="53" t="s">
         <v>315</v>
       </c>
-      <c r="G245" s="32"/>
+      <c r="G245" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H245" s="56" t="s">
         <v>322</v>
       </c>
@@ -14437,7 +14527,7 @@
       <c r="T245" s="37"/>
     </row>
     <row r="246" spans="1:20" ht="18" customHeight="1">
-      <c r="A246" s="155" t="s">
+      <c r="A246" s="118" t="s">
         <v>309</v>
       </c>
       <c r="B246" s="105" t="s">
@@ -14455,7 +14545,9 @@
       <c r="F246" s="53" t="s">
         <v>315</v>
       </c>
-      <c r="G246" s="32"/>
+      <c r="G246" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H246" s="56" t="s">
         <v>322</v>
       </c>
@@ -14486,7 +14578,7 @@
       <c r="T246" s="37"/>
     </row>
     <row r="247" spans="1:20" ht="18" customHeight="1">
-      <c r="A247" s="155" t="s">
+      <c r="A247" s="118" t="s">
         <v>307</v>
       </c>
       <c r="B247" s="105" t="s">
@@ -14504,7 +14596,9 @@
       <c r="F247" s="53" t="s">
         <v>315</v>
       </c>
-      <c r="G247" s="32"/>
+      <c r="G247" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H247" s="56" t="s">
         <v>322</v>
       </c>
@@ -14535,7 +14629,7 @@
       <c r="T247" s="44"/>
     </row>
     <row r="248" spans="1:20" ht="18" customHeight="1">
-      <c r="A248" s="155" t="s">
+      <c r="A248" s="118" t="s">
         <v>308</v>
       </c>
       <c r="B248" s="105" t="s">
@@ -14553,7 +14647,9 @@
       <c r="F248" s="53" t="s">
         <v>315</v>
       </c>
-      <c r="G248" s="32"/>
+      <c r="G248" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H248" s="56" t="s">
         <v>322</v>
       </c>
@@ -14584,7 +14680,7 @@
       <c r="T248" s="44"/>
     </row>
     <row r="249" spans="1:20" ht="18" customHeight="1">
-      <c r="A249" s="154" t="s">
+      <c r="A249" s="117" t="s">
         <v>282</v>
       </c>
       <c r="B249" s="103" t="s">
@@ -14600,7 +14696,9 @@
       <c r="F249" s="53" t="s">
         <v>316</v>
       </c>
-      <c r="G249" s="32"/>
+      <c r="G249" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H249" s="56" t="s">
         <v>322</v>
       </c>
@@ -14631,7 +14729,7 @@
       <c r="T249" s="44"/>
     </row>
     <row r="250" spans="1:20" ht="18" customHeight="1">
-      <c r="A250" s="155" t="s">
+      <c r="A250" s="118" t="s">
         <v>303</v>
       </c>
       <c r="B250" s="105" t="s">
@@ -14649,7 +14747,9 @@
       <c r="F250" s="53" t="s">
         <v>316</v>
       </c>
-      <c r="G250" s="32"/>
+      <c r="G250" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H250" s="56" t="s">
         <v>322</v>
       </c>
@@ -14680,7 +14780,7 @@
       <c r="T250" s="37"/>
     </row>
     <row r="251" spans="1:20" ht="18" customHeight="1">
-      <c r="A251" s="155" t="s">
+      <c r="A251" s="118" t="s">
         <v>304</v>
       </c>
       <c r="B251" s="105" t="s">
@@ -14698,7 +14798,9 @@
       <c r="F251" s="53" t="s">
         <v>316</v>
       </c>
-      <c r="G251" s="32"/>
+      <c r="G251" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H251" s="56" t="s">
         <v>322</v>
       </c>
@@ -14729,7 +14831,7 @@
       <c r="T251" s="37"/>
     </row>
     <row r="252" spans="1:20" ht="18" customHeight="1">
-      <c r="A252" s="155" t="s">
+      <c r="A252" s="118" t="s">
         <v>305</v>
       </c>
       <c r="B252" s="105" t="s">
@@ -14747,7 +14849,9 @@
       <c r="F252" s="53" t="s">
         <v>316</v>
       </c>
-      <c r="G252" s="32"/>
+      <c r="G252" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H252" s="56" t="s">
         <v>322</v>
       </c>
@@ -14778,7 +14882,7 @@
       <c r="T252" s="37"/>
     </row>
     <row r="253" spans="1:20" ht="18" customHeight="1">
-      <c r="A253" s="155" t="s">
+      <c r="A253" s="118" t="s">
         <v>306</v>
       </c>
       <c r="B253" s="105" t="s">
@@ -14796,7 +14900,9 @@
       <c r="F253" s="53" t="s">
         <v>316</v>
       </c>
-      <c r="G253" s="32"/>
+      <c r="G253" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H253" s="56" t="s">
         <v>322</v>
       </c>
@@ -14827,7 +14933,7 @@
       <c r="T253" s="37"/>
     </row>
     <row r="254" spans="1:20" ht="18" customHeight="1">
-      <c r="A254" s="155" t="s">
+      <c r="A254" s="118" t="s">
         <v>309</v>
       </c>
       <c r="B254" s="105" t="s">
@@ -14845,7 +14951,9 @@
       <c r="F254" s="53" t="s">
         <v>316</v>
       </c>
-      <c r="G254" s="32"/>
+      <c r="G254" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H254" s="56" t="s">
         <v>322</v>
       </c>
@@ -14876,7 +14984,7 @@
       <c r="T254" s="37"/>
     </row>
     <row r="255" spans="1:20" ht="18" customHeight="1">
-      <c r="A255" s="155" t="s">
+      <c r="A255" s="118" t="s">
         <v>307</v>
       </c>
       <c r="B255" s="105" t="s">
@@ -14894,7 +15002,9 @@
       <c r="F255" s="53" t="s">
         <v>316</v>
       </c>
-      <c r="G255" s="32"/>
+      <c r="G255" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H255" s="56" t="s">
         <v>322</v>
       </c>
@@ -14925,7 +15035,7 @@
       <c r="T255" s="37"/>
     </row>
     <row r="256" spans="1:20" ht="18" customHeight="1">
-      <c r="A256" s="155" t="s">
+      <c r="A256" s="118" t="s">
         <v>308</v>
       </c>
       <c r="B256" s="105" t="s">
@@ -14943,7 +15053,9 @@
       <c r="F256" s="53" t="s">
         <v>316</v>
       </c>
-      <c r="G256" s="32"/>
+      <c r="G256" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H256" s="56" t="s">
         <v>322</v>
       </c>
@@ -14974,7 +15086,7 @@
       <c r="T256" s="37"/>
     </row>
     <row r="257" spans="1:20" ht="18" customHeight="1">
-      <c r="A257" s="154" t="s">
+      <c r="A257" s="117" t="s">
         <v>282</v>
       </c>
       <c r="B257" s="103" t="s">
@@ -14990,7 +15102,9 @@
       <c r="F257" s="53" t="s">
         <v>317</v>
       </c>
-      <c r="G257" s="32"/>
+      <c r="G257" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H257" s="56" t="s">
         <v>322</v>
       </c>
@@ -15021,7 +15135,7 @@
       <c r="T257" s="37"/>
     </row>
     <row r="258" spans="1:20" ht="18" customHeight="1">
-      <c r="A258" s="155" t="s">
+      <c r="A258" s="118" t="s">
         <v>303</v>
       </c>
       <c r="B258" s="105" t="s">
@@ -15039,7 +15153,9 @@
       <c r="F258" s="53" t="s">
         <v>317</v>
       </c>
-      <c r="G258" s="32"/>
+      <c r="G258" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H258" s="56" t="s">
         <v>322</v>
       </c>
@@ -15070,7 +15186,7 @@
       <c r="T258" s="37"/>
     </row>
     <row r="259" spans="1:20" ht="18" customHeight="1">
-      <c r="A259" s="155" t="s">
+      <c r="A259" s="118" t="s">
         <v>304</v>
       </c>
       <c r="B259" s="105" t="s">
@@ -15088,7 +15204,9 @@
       <c r="F259" s="53" t="s">
         <v>317</v>
       </c>
-      <c r="G259" s="32"/>
+      <c r="G259" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H259" s="56" t="s">
         <v>322</v>
       </c>
@@ -15119,7 +15237,7 @@
       <c r="T259" s="37"/>
     </row>
     <row r="260" spans="1:20" ht="18" customHeight="1">
-      <c r="A260" s="155" t="s">
+      <c r="A260" s="118" t="s">
         <v>305</v>
       </c>
       <c r="B260" s="105" t="s">
@@ -15137,7 +15255,9 @@
       <c r="F260" s="53" t="s">
         <v>317</v>
       </c>
-      <c r="G260" s="32"/>
+      <c r="G260" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H260" s="56" t="s">
         <v>322</v>
       </c>
@@ -15168,7 +15288,7 @@
       <c r="T260" s="37"/>
     </row>
     <row r="261" spans="1:20" ht="18" customHeight="1">
-      <c r="A261" s="155" t="s">
+      <c r="A261" s="118" t="s">
         <v>306</v>
       </c>
       <c r="B261" s="105" t="s">
@@ -15186,7 +15306,9 @@
       <c r="F261" s="53" t="s">
         <v>317</v>
       </c>
-      <c r="G261" s="32"/>
+      <c r="G261" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H261" s="56" t="s">
         <v>322</v>
       </c>
@@ -15217,7 +15339,7 @@
       <c r="T261" s="37"/>
     </row>
     <row r="262" spans="1:20" ht="18" customHeight="1">
-      <c r="A262" s="155" t="s">
+      <c r="A262" s="118" t="s">
         <v>309</v>
       </c>
       <c r="B262" s="105" t="s">
@@ -15235,7 +15357,9 @@
       <c r="F262" s="53" t="s">
         <v>317</v>
       </c>
-      <c r="G262" s="32"/>
+      <c r="G262" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H262" s="56" t="s">
         <v>322</v>
       </c>
@@ -15266,7 +15390,7 @@
       <c r="T262" s="37"/>
     </row>
     <row r="263" spans="1:20" ht="18" customHeight="1">
-      <c r="A263" s="155" t="s">
+      <c r="A263" s="118" t="s">
         <v>307</v>
       </c>
       <c r="B263" s="105" t="s">
@@ -15284,7 +15408,9 @@
       <c r="F263" s="53" t="s">
         <v>317</v>
       </c>
-      <c r="G263" s="32"/>
+      <c r="G263" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H263" s="56" t="s">
         <v>322</v>
       </c>
@@ -15315,7 +15441,7 @@
       <c r="T263" s="37"/>
     </row>
     <row r="264" spans="1:20" ht="18" customHeight="1">
-      <c r="A264" s="155" t="s">
+      <c r="A264" s="118" t="s">
         <v>308</v>
       </c>
       <c r="B264" s="105" t="s">
@@ -15333,7 +15459,9 @@
       <c r="F264" s="53" t="s">
         <v>317</v>
       </c>
-      <c r="G264" s="32"/>
+      <c r="G264" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H264" s="56" t="s">
         <v>322</v>
       </c>
@@ -15380,14 +15508,16 @@
       <c r="F265" s="53" t="s">
         <v>194</v>
       </c>
-      <c r="G265" s="32"/>
+      <c r="G265" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H265" s="56" t="s">
         <v>337</v>
       </c>
       <c r="I265" s="54">
         <v>298</v>
       </c>
-      <c r="J265" s="156">
+      <c r="J265" s="119">
         <v>317000000</v>
       </c>
       <c r="K265" s="38"/>
@@ -15424,14 +15554,16 @@
       <c r="F266" s="53" t="s">
         <v>194</v>
       </c>
-      <c r="G266" s="32"/>
+      <c r="G266" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H266" s="56" t="s">
         <v>337</v>
       </c>
       <c r="I266" s="54">
         <v>298</v>
       </c>
-      <c r="J266" s="156">
+      <c r="J266" s="119">
         <v>404000000</v>
       </c>
       <c r="K266" s="38"/>
@@ -15468,14 +15600,16 @@
       <c r="F267" s="53" t="s">
         <v>194</v>
       </c>
-      <c r="G267" s="32"/>
+      <c r="G267" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H267" s="56" t="s">
         <v>337</v>
       </c>
       <c r="I267" s="54">
         <v>298</v>
       </c>
-      <c r="J267" s="156">
+      <c r="J267" s="119">
         <v>499000000</v>
       </c>
       <c r="K267" s="38"/>
@@ -15512,14 +15646,16 @@
       <c r="F268" s="53" t="s">
         <v>194</v>
       </c>
-      <c r="G268" s="32"/>
+      <c r="G268" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H268" s="56" t="s">
         <v>337</v>
       </c>
       <c r="I268" s="54">
         <v>298</v>
       </c>
-      <c r="J268" s="156">
+      <c r="J268" s="119">
         <v>749000000</v>
       </c>
       <c r="K268" s="38"/>
@@ -15556,7 +15692,9 @@
       <c r="F269" s="53" t="s">
         <v>194</v>
       </c>
-      <c r="G269" s="32"/>
+      <c r="G269" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H269" s="56" t="s">
         <v>337</v>
       </c>
@@ -15600,7 +15738,9 @@
       <c r="F270" s="53" t="s">
         <v>194</v>
       </c>
-      <c r="G270" s="32"/>
+      <c r="G270" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H270" s="56" t="s">
         <v>337</v>
       </c>
@@ -15644,7 +15784,9 @@
       <c r="F271" s="57" t="s">
         <v>273</v>
       </c>
-      <c r="G271" s="32"/>
+      <c r="G271" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H271" s="56" t="s">
         <v>337</v>
       </c>
@@ -15688,7 +15830,9 @@
       <c r="F272" s="57" t="s">
         <v>273</v>
       </c>
-      <c r="G272" s="32"/>
+      <c r="G272" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H272" s="56" t="s">
         <v>337</v>
       </c>
@@ -15732,7 +15876,9 @@
       <c r="F273" s="57" t="s">
         <v>274</v>
       </c>
-      <c r="G273" s="32"/>
+      <c r="G273" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H273" s="56" t="s">
         <v>337</v>
       </c>
@@ -15776,7 +15922,9 @@
       <c r="F274" s="57" t="s">
         <v>274</v>
       </c>
-      <c r="G274" s="32"/>
+      <c r="G274" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H274" s="56" t="s">
         <v>337</v>
       </c>
@@ -15820,7 +15968,9 @@
       <c r="F275" s="57" t="s">
         <v>274</v>
       </c>
-      <c r="G275" s="32"/>
+      <c r="G275" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H275" s="56" t="s">
         <v>337</v>
       </c>
@@ -15864,7 +16014,9 @@
       <c r="F276" s="57" t="s">
         <v>274</v>
       </c>
-      <c r="G276" s="32"/>
+      <c r="G276" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H276" s="56" t="s">
         <v>337</v>
       </c>
@@ -15908,7 +16060,9 @@
       <c r="F277" s="57" t="s">
         <v>272</v>
       </c>
-      <c r="G277" s="32"/>
+      <c r="G277" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H277" s="56" t="s">
         <v>337</v>
       </c>
@@ -15952,7 +16106,9 @@
       <c r="F278" s="57" t="s">
         <v>272</v>
       </c>
-      <c r="G278" s="32"/>
+      <c r="G278" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H278" s="56" t="s">
         <v>337</v>
       </c>
@@ -15996,7 +16152,9 @@
       <c r="F279" s="57" t="s">
         <v>271</v>
       </c>
-      <c r="G279" s="32"/>
+      <c r="G279" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H279" s="56" t="s">
         <v>337</v>
       </c>
@@ -16040,7 +16198,9 @@
       <c r="F280" s="57" t="s">
         <v>271</v>
       </c>
-      <c r="G280" s="32"/>
+      <c r="G280" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H280" s="56" t="s">
         <v>337</v>
       </c>
@@ -16084,7 +16244,9 @@
       <c r="F281" s="57" t="s">
         <v>271</v>
       </c>
-      <c r="G281" s="32"/>
+      <c r="G281" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H281" s="56" t="s">
         <v>337</v>
       </c>
@@ -16128,7 +16290,9 @@
       <c r="F282" s="57" t="s">
         <v>271</v>
       </c>
-      <c r="G282" s="32"/>
+      <c r="G282" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H282" s="56" t="s">
         <v>337</v>
       </c>
@@ -30930,6 +31094,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -30944,11 +31113,6 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
- parsed data from `10.1038/s41586-022-04914-8`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Aug2025.xlsx
+++ b/MiscSmallUploads_Aug2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F3F4C8-F602-1E48-ABEA-E5C1522C7B4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABDE725F-CE89-E848-A825-E11B249682FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="7580" windowWidth="34560" windowHeight="12760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2633" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2750" uniqueCount="347">
   <si>
     <r>
       <rPr>
@@ -1144,6 +1144,33 @@
   </si>
   <si>
     <t>5e-4 strain rate</t>
+  </si>
+  <si>
+    <t>AlCoCrFeNi2.1</t>
+  </si>
+  <si>
+    <t>LPBF of prealloyed gas-atomized powder onto preheated steel plate in Ar using 400W laser and optimized deposition strategy</t>
+  </si>
+  <si>
+    <t>LPBF+A+WQ</t>
+  </si>
+  <si>
+    <t>LPBF of prealloyed gas-atomized powder onto preheated steel plate in Ar using 400W laser and optimized deposition strategy; annealed at 873K for 5h in Ar</t>
+  </si>
+  <si>
+    <t>L12+B2</t>
+  </si>
+  <si>
+    <t>LPBF of prealloyed gas-atomized powder onto preheated steel plate in Ar using 400W laser and optimized deposition strategy; annealed at 1073K for 1h in Ar</t>
+  </si>
+  <si>
+    <t>2e-4 strain rate</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>10.1038/s41586-022-04914-8</t>
   </si>
 </sst>
 </file>
@@ -2386,6 +2413,57 @@
     <xf numFmtId="0" fontId="15" fillId="10" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="10" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="12" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2445,57 +2523,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3659,8 +3686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T960"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A261" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H284" sqref="H284"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A283" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F305" sqref="F305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -3717,19 +3744,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" s="120" t="s">
+      <c r="D2" s="137" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="121"/>
-      <c r="F2" s="124"/>
-      <c r="G2" s="125"/>
-      <c r="H2" s="125"/>
-      <c r="I2" s="126"/>
-      <c r="J2" s="127"/>
-      <c r="K2" s="127"/>
-      <c r="L2" s="125"/>
-      <c r="M2" s="125"/>
-      <c r="N2" s="128"/>
+      <c r="E2" s="138"/>
+      <c r="F2" s="141"/>
+      <c r="G2" s="142"/>
+      <c r="H2" s="142"/>
+      <c r="I2" s="143"/>
+      <c r="J2" s="144"/>
+      <c r="K2" s="144"/>
+      <c r="L2" s="142"/>
+      <c r="M2" s="142"/>
+      <c r="N2" s="145"/>
       <c r="O2" s="13"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -3745,17 +3772,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="122"/>
-      <c r="E3" s="123"/>
-      <c r="F3" s="129"/>
-      <c r="G3" s="129"/>
-      <c r="H3" s="129"/>
-      <c r="I3" s="130"/>
-      <c r="J3" s="131"/>
-      <c r="K3" s="131"/>
-      <c r="L3" s="129"/>
-      <c r="M3" s="129"/>
-      <c r="N3" s="132"/>
+      <c r="D3" s="139"/>
+      <c r="E3" s="140"/>
+      <c r="F3" s="146"/>
+      <c r="G3" s="146"/>
+      <c r="H3" s="146"/>
+      <c r="I3" s="147"/>
+      <c r="J3" s="148"/>
+      <c r="K3" s="148"/>
+      <c r="L3" s="146"/>
+      <c r="M3" s="146"/>
+      <c r="N3" s="149"/>
       <c r="O3" s="13"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -3796,43 +3823,43 @@
       <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="133" t="s">
+      <c r="C5" s="150" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="135" t="s">
+      <c r="D5" s="152" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="135" t="s">
+      <c r="E5" s="152" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="135" t="s">
+      <c r="F5" s="152" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="135" t="s">
+      <c r="G5" s="152" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="136" t="s">
+      <c r="H5" s="153" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="135" t="s">
+      <c r="I5" s="152" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="135" t="s">
+      <c r="J5" s="152" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="135" t="s">
+      <c r="K5" s="152" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="135" t="s">
+      <c r="L5" s="152" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="135" t="s">
+      <c r="M5" s="152" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="135" t="s">
+      <c r="N5" s="152" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="140" t="s">
+      <c r="O5" s="120" t="s">
         <v>20</v>
       </c>
       <c r="P5" s="25"/>
@@ -3848,19 +3875,19 @@
       <c r="B6" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="134"/>
-      <c r="D6" s="134"/>
-      <c r="E6" s="134"/>
-      <c r="F6" s="134"/>
-      <c r="G6" s="134"/>
-      <c r="H6" s="137"/>
-      <c r="I6" s="138"/>
-      <c r="J6" s="139"/>
-      <c r="K6" s="139"/>
-      <c r="L6" s="134"/>
-      <c r="M6" s="134"/>
-      <c r="N6" s="134"/>
-      <c r="O6" s="141"/>
+      <c r="C6" s="151"/>
+      <c r="D6" s="151"/>
+      <c r="E6" s="151"/>
+      <c r="F6" s="151"/>
+      <c r="G6" s="151"/>
+      <c r="H6" s="154"/>
+      <c r="I6" s="155"/>
+      <c r="J6" s="156"/>
+      <c r="K6" s="156"/>
+      <c r="L6" s="151"/>
+      <c r="M6" s="151"/>
+      <c r="N6" s="151"/>
+      <c r="O6" s="121"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="9"/>
@@ -3910,7 +3937,7 @@
       <c r="N7" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="142"/>
+      <c r="O7" s="122"/>
       <c r="P7" s="64" t="s">
         <v>62</v>
       </c>
@@ -3925,35 +3952,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" thickBot="1">
       <c r="A8" s="59"/>
-      <c r="B8" s="143" t="s">
+      <c r="B8" s="123" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="144"/>
-      <c r="D8" s="144"/>
-      <c r="E8" s="145"/>
-      <c r="F8" s="146" t="s">
+      <c r="C8" s="124"/>
+      <c r="D8" s="124"/>
+      <c r="E8" s="125"/>
+      <c r="F8" s="126" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="147"/>
-      <c r="H8" s="147"/>
-      <c r="I8" s="148"/>
-      <c r="J8" s="149"/>
-      <c r="K8" s="149"/>
-      <c r="L8" s="150"/>
-      <c r="M8" s="151" t="s">
+      <c r="G8" s="127"/>
+      <c r="H8" s="127"/>
+      <c r="I8" s="128"/>
+      <c r="J8" s="129"/>
+      <c r="K8" s="129"/>
+      <c r="L8" s="130"/>
+      <c r="M8" s="131" t="s">
         <v>40</v>
       </c>
-      <c r="N8" s="152"/>
+      <c r="N8" s="132"/>
       <c r="O8" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="P8" s="153" t="s">
+      <c r="P8" s="133" t="s">
         <v>42</v>
       </c>
-      <c r="Q8" s="154"/>
-      <c r="R8" s="155"/>
-      <c r="S8" s="155"/>
-      <c r="T8" s="156"/>
+      <c r="Q8" s="134"/>
+      <c r="R8" s="135"/>
+      <c r="S8" s="135"/>
+      <c r="T8" s="136"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1">
       <c r="A9" s="60" t="s">
@@ -16321,19 +16348,43 @@
     </row>
     <row r="283" spans="1:20" ht="18" customHeight="1">
       <c r="A283" s="57"/>
-      <c r="B283" s="57"/>
-      <c r="C283" s="57"/>
-      <c r="D283" s="57"/>
-      <c r="E283" s="55"/>
-      <c r="F283" s="57"/>
-      <c r="G283" s="32"/>
-      <c r="H283" s="44"/>
-      <c r="I283" s="38"/>
-      <c r="J283" s="44"/>
-      <c r="K283" s="48"/>
-      <c r="L283" s="57"/>
-      <c r="M283" s="57"/>
-      <c r="N283" s="40"/>
+      <c r="B283" s="57" t="s">
+        <v>338</v>
+      </c>
+      <c r="C283" s="57" t="s">
+        <v>342</v>
+      </c>
+      <c r="D283" s="57" t="s">
+        <v>64</v>
+      </c>
+      <c r="E283" s="57"/>
+      <c r="F283" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="G283" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H283" s="57" t="s">
+        <v>344</v>
+      </c>
+      <c r="I283" s="54">
+        <v>298</v>
+      </c>
+      <c r="J283" s="58">
+        <v>510000000</v>
+      </c>
+      <c r="K283" s="48">
+        <v>15000000</v>
+      </c>
+      <c r="L283" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="M283" s="57" t="s">
+        <v>345</v>
+      </c>
+      <c r="N283" s="40" t="s">
+        <v>346</v>
+      </c>
       <c r="O283" s="44"/>
       <c r="P283" s="44"/>
       <c r="Q283" s="44"/>
@@ -16343,19 +16394,45 @@
     </row>
     <row r="284" spans="1:20" ht="18" customHeight="1">
       <c r="A284" s="57"/>
-      <c r="B284" s="57"/>
-      <c r="C284" s="57"/>
-      <c r="D284" s="57"/>
-      <c r="E284" s="55"/>
-      <c r="F284" s="57"/>
-      <c r="G284" s="32"/>
-      <c r="H284" s="44"/>
-      <c r="I284" s="38"/>
-      <c r="J284" s="44"/>
-      <c r="K284" s="58"/>
-      <c r="L284" s="57"/>
-      <c r="M284" s="57"/>
-      <c r="N284" s="40"/>
+      <c r="B284" s="57" t="s">
+        <v>338</v>
+      </c>
+      <c r="C284" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="D284" s="57" t="s">
+        <v>246</v>
+      </c>
+      <c r="E284" s="57" t="s">
+        <v>339</v>
+      </c>
+      <c r="F284" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="G284" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H284" s="57" t="s">
+        <v>344</v>
+      </c>
+      <c r="I284" s="54">
+        <v>298</v>
+      </c>
+      <c r="J284" s="58">
+        <v>1333000000</v>
+      </c>
+      <c r="K284" s="58">
+        <v>38000000</v>
+      </c>
+      <c r="L284" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="M284" s="57" t="s">
+        <v>345</v>
+      </c>
+      <c r="N284" s="40" t="s">
+        <v>346</v>
+      </c>
       <c r="O284" s="44"/>
       <c r="P284" s="44"/>
       <c r="Q284" s="44"/>
@@ -16365,19 +16442,43 @@
     </row>
     <row r="285" spans="1:20" ht="18" customHeight="1">
       <c r="A285" s="57"/>
-      <c r="B285" s="57"/>
-      <c r="C285" s="57"/>
-      <c r="D285" s="57"/>
-      <c r="E285" s="55"/>
-      <c r="F285" s="57"/>
-      <c r="G285" s="32"/>
-      <c r="H285" s="44"/>
-      <c r="I285" s="38"/>
-      <c r="J285" s="44"/>
+      <c r="B285" s="57" t="s">
+        <v>338</v>
+      </c>
+      <c r="C285" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="D285" s="57" t="s">
+        <v>340</v>
+      </c>
+      <c r="E285" s="57" t="s">
+        <v>341</v>
+      </c>
+      <c r="F285" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="G285" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H285" s="57" t="s">
+        <v>344</v>
+      </c>
+      <c r="I285" s="54">
+        <v>298</v>
+      </c>
+      <c r="J285" s="58">
+        <v>1615000000</v>
+      </c>
       <c r="K285" s="58"/>
-      <c r="L285" s="57"/>
-      <c r="M285" s="57"/>
-      <c r="N285" s="40"/>
+      <c r="L285" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="M285" s="57" t="s">
+        <v>345</v>
+      </c>
+      <c r="N285" s="40" t="s">
+        <v>346</v>
+      </c>
       <c r="O285" s="44"/>
       <c r="P285" s="44"/>
       <c r="Q285" s="44"/>
@@ -16387,19 +16488,43 @@
     </row>
     <row r="286" spans="1:20" ht="18" customHeight="1">
       <c r="A286" s="57"/>
-      <c r="B286" s="57"/>
-      <c r="C286" s="57"/>
-      <c r="D286" s="57"/>
-      <c r="E286" s="55"/>
-      <c r="F286" s="57"/>
-      <c r="G286" s="32"/>
-      <c r="H286" s="44"/>
-      <c r="I286" s="38"/>
-      <c r="J286" s="44"/>
+      <c r="B286" s="57" t="s">
+        <v>338</v>
+      </c>
+      <c r="C286" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="D286" s="57" t="s">
+        <v>340</v>
+      </c>
+      <c r="E286" s="57" t="s">
+        <v>343</v>
+      </c>
+      <c r="F286" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="G286" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H286" s="57" t="s">
+        <v>344</v>
+      </c>
+      <c r="I286" s="54">
+        <v>298</v>
+      </c>
+      <c r="J286" s="58">
+        <v>1003000000</v>
+      </c>
       <c r="K286" s="44"/>
-      <c r="L286" s="57"/>
-      <c r="M286" s="57"/>
-      <c r="N286" s="40"/>
+      <c r="L286" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="M286" s="57" t="s">
+        <v>345</v>
+      </c>
+      <c r="N286" s="40" t="s">
+        <v>346</v>
+      </c>
       <c r="O286" s="44"/>
       <c r="P286" s="44"/>
       <c r="Q286" s="44"/>
@@ -16409,19 +16534,41 @@
     </row>
     <row r="287" spans="1:20" ht="18" customHeight="1">
       <c r="A287" s="57"/>
-      <c r="B287" s="57"/>
-      <c r="C287" s="57"/>
-      <c r="D287" s="57"/>
-      <c r="E287" s="55"/>
-      <c r="F287" s="57"/>
-      <c r="G287" s="32"/>
-      <c r="H287" s="44"/>
-      <c r="I287" s="38"/>
-      <c r="J287" s="44"/>
+      <c r="B287" s="57" t="s">
+        <v>338</v>
+      </c>
+      <c r="C287" s="57" t="s">
+        <v>342</v>
+      </c>
+      <c r="D287" s="57" t="s">
+        <v>64</v>
+      </c>
+      <c r="E287" s="57"/>
+      <c r="F287" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="G287" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H287" s="57" t="s">
+        <v>344</v>
+      </c>
+      <c r="I287" s="54">
+        <v>298</v>
+      </c>
+      <c r="J287" s="58">
+        <v>1198000000</v>
+      </c>
       <c r="K287" s="44"/>
-      <c r="L287" s="57"/>
-      <c r="M287" s="57"/>
-      <c r="N287" s="40"/>
+      <c r="L287" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="M287" s="57" t="s">
+        <v>345</v>
+      </c>
+      <c r="N287" s="40" t="s">
+        <v>346</v>
+      </c>
       <c r="O287" s="44"/>
       <c r="P287" s="44"/>
       <c r="Q287" s="44"/>
@@ -16431,19 +16578,45 @@
     </row>
     <row r="288" spans="1:20" ht="18" customHeight="1">
       <c r="A288" s="57"/>
-      <c r="B288" s="57"/>
-      <c r="C288" s="57"/>
-      <c r="D288" s="57"/>
-      <c r="E288" s="55"/>
-      <c r="F288" s="57"/>
-      <c r="G288" s="32"/>
-      <c r="H288" s="44"/>
-      <c r="I288" s="38"/>
-      <c r="J288" s="44"/>
-      <c r="K288" s="44"/>
-      <c r="L288" s="57"/>
-      <c r="M288" s="57"/>
-      <c r="N288" s="40"/>
+      <c r="B288" s="57" t="s">
+        <v>338</v>
+      </c>
+      <c r="C288" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="D288" s="57" t="s">
+        <v>246</v>
+      </c>
+      <c r="E288" s="57" t="s">
+        <v>339</v>
+      </c>
+      <c r="F288" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="G288" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H288" s="57" t="s">
+        <v>344</v>
+      </c>
+      <c r="I288" s="54">
+        <v>298</v>
+      </c>
+      <c r="J288" s="58">
+        <v>1640000000</v>
+      </c>
+      <c r="K288" s="58">
+        <v>38000000</v>
+      </c>
+      <c r="L288" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="M288" s="57" t="s">
+        <v>345</v>
+      </c>
+      <c r="N288" s="40" t="s">
+        <v>346</v>
+      </c>
       <c r="O288" s="44"/>
       <c r="P288" s="44"/>
       <c r="Q288" s="44"/>
@@ -16453,19 +16626,43 @@
     </row>
     <row r="289" spans="1:20" ht="18" customHeight="1">
       <c r="A289" s="57"/>
-      <c r="B289" s="57"/>
-      <c r="C289" s="57"/>
-      <c r="D289" s="57"/>
-      <c r="E289" s="55"/>
-      <c r="F289" s="57"/>
-      <c r="G289" s="32"/>
-      <c r="H289" s="44"/>
-      <c r="I289" s="38"/>
-      <c r="J289" s="44"/>
+      <c r="B289" s="57" t="s">
+        <v>338</v>
+      </c>
+      <c r="C289" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="D289" s="57" t="s">
+        <v>340</v>
+      </c>
+      <c r="E289" s="57" t="s">
+        <v>341</v>
+      </c>
+      <c r="F289" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="G289" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H289" s="57" t="s">
+        <v>344</v>
+      </c>
+      <c r="I289" s="54">
+        <v>298</v>
+      </c>
+      <c r="J289" s="58">
+        <v>1907000000</v>
+      </c>
       <c r="K289" s="44"/>
-      <c r="L289" s="57"/>
-      <c r="M289" s="57"/>
-      <c r="N289" s="40"/>
+      <c r="L289" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="M289" s="57" t="s">
+        <v>345</v>
+      </c>
+      <c r="N289" s="40" t="s">
+        <v>346</v>
+      </c>
       <c r="O289" s="44"/>
       <c r="P289" s="44"/>
       <c r="Q289" s="44"/>
@@ -16475,19 +16672,43 @@
     </row>
     <row r="290" spans="1:20" ht="18" customHeight="1">
       <c r="A290" s="57"/>
-      <c r="B290" s="57"/>
-      <c r="C290" s="57"/>
-      <c r="D290" s="57"/>
-      <c r="E290" s="55"/>
-      <c r="F290" s="57"/>
-      <c r="G290" s="32"/>
-      <c r="H290" s="57"/>
-      <c r="I290" s="38"/>
-      <c r="J290" s="51"/>
+      <c r="B290" s="57" t="s">
+        <v>338</v>
+      </c>
+      <c r="C290" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="D290" s="57" t="s">
+        <v>340</v>
+      </c>
+      <c r="E290" s="57" t="s">
+        <v>343</v>
+      </c>
+      <c r="F290" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="G290" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H290" s="57" t="s">
+        <v>344</v>
+      </c>
+      <c r="I290" s="54">
+        <v>298</v>
+      </c>
+      <c r="J290" s="51">
+        <v>1286000000</v>
+      </c>
       <c r="K290" s="44"/>
-      <c r="L290" s="57"/>
-      <c r="M290" s="57"/>
-      <c r="N290" s="40"/>
+      <c r="L290" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="M290" s="57" t="s">
+        <v>345</v>
+      </c>
+      <c r="N290" s="40" t="s">
+        <v>346</v>
+      </c>
       <c r="O290" s="44"/>
       <c r="P290" s="44"/>
       <c r="Q290" s="44"/>
@@ -16497,19 +16718,41 @@
     </row>
     <row r="291" spans="1:20" ht="18" customHeight="1">
       <c r="A291" s="57"/>
-      <c r="B291" s="57"/>
-      <c r="C291" s="57"/>
-      <c r="D291" s="57"/>
-      <c r="E291" s="55"/>
-      <c r="F291" s="57"/>
-      <c r="G291" s="32"/>
-      <c r="H291" s="57"/>
-      <c r="I291" s="38"/>
-      <c r="J291" s="51"/>
+      <c r="B291" s="57" t="s">
+        <v>338</v>
+      </c>
+      <c r="C291" s="57" t="s">
+        <v>342</v>
+      </c>
+      <c r="D291" s="57" t="s">
+        <v>64</v>
+      </c>
+      <c r="E291" s="57"/>
+      <c r="F291" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="G291" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H291" s="57" t="s">
+        <v>344</v>
+      </c>
+      <c r="I291" s="54">
+        <v>298</v>
+      </c>
+      <c r="J291" s="44">
+        <v>13.4384858044164</v>
+      </c>
       <c r="K291" s="44"/>
-      <c r="L291" s="57"/>
-      <c r="M291" s="57"/>
-      <c r="N291" s="40"/>
+      <c r="L291" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="M291" s="57" t="s">
+        <v>345</v>
+      </c>
+      <c r="N291" s="40" t="s">
+        <v>346</v>
+      </c>
       <c r="O291" s="44"/>
       <c r="P291" s="44"/>
       <c r="Q291" s="44"/>
@@ -16519,19 +16762,43 @@
     </row>
     <row r="292" spans="1:20" ht="18" customHeight="1">
       <c r="A292" s="57"/>
-      <c r="B292" s="57"/>
-      <c r="C292" s="57"/>
-      <c r="D292" s="57"/>
-      <c r="E292" s="55"/>
-      <c r="F292" s="57"/>
-      <c r="G292" s="32"/>
-      <c r="H292" s="57"/>
-      <c r="I292" s="38"/>
-      <c r="J292" s="51"/>
+      <c r="B292" s="57" t="s">
+        <v>338</v>
+      </c>
+      <c r="C292" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="D292" s="57" t="s">
+        <v>246</v>
+      </c>
+      <c r="E292" s="57" t="s">
+        <v>339</v>
+      </c>
+      <c r="F292" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="G292" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H292" s="57" t="s">
+        <v>344</v>
+      </c>
+      <c r="I292" s="54">
+        <v>298</v>
+      </c>
+      <c r="J292" s="44">
+        <v>15.7308096740273</v>
+      </c>
       <c r="K292" s="44"/>
-      <c r="L292" s="57"/>
-      <c r="M292" s="57"/>
-      <c r="N292" s="40"/>
+      <c r="L292" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="M292" s="57" t="s">
+        <v>345</v>
+      </c>
+      <c r="N292" s="40" t="s">
+        <v>346</v>
+      </c>
       <c r="O292" s="44"/>
       <c r="P292" s="44"/>
       <c r="Q292" s="44"/>
@@ -16541,19 +16808,43 @@
     </row>
     <row r="293" spans="1:20" ht="18" customHeight="1">
       <c r="A293" s="57"/>
-      <c r="B293" s="57"/>
-      <c r="C293" s="57"/>
-      <c r="D293" s="57"/>
-      <c r="E293" s="55"/>
-      <c r="F293" s="57"/>
-      <c r="G293" s="32"/>
-      <c r="H293" s="57"/>
-      <c r="I293" s="38"/>
-      <c r="J293" s="51"/>
+      <c r="B293" s="57" t="s">
+        <v>338</v>
+      </c>
+      <c r="C293" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="D293" s="57" t="s">
+        <v>340</v>
+      </c>
+      <c r="E293" s="57" t="s">
+        <v>341</v>
+      </c>
+      <c r="F293" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="G293" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H293" s="57" t="s">
+        <v>344</v>
+      </c>
+      <c r="I293" s="54">
+        <v>298</v>
+      </c>
+      <c r="J293" s="44">
+        <v>7.4868559411146096</v>
+      </c>
       <c r="K293" s="44"/>
-      <c r="L293" s="57"/>
-      <c r="M293" s="57"/>
-      <c r="N293" s="40"/>
+      <c r="L293" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="M293" s="57" t="s">
+        <v>345</v>
+      </c>
+      <c r="N293" s="40" t="s">
+        <v>346</v>
+      </c>
       <c r="O293" s="44"/>
       <c r="P293" s="44"/>
       <c r="Q293" s="44"/>
@@ -16563,19 +16854,43 @@
     </row>
     <row r="294" spans="1:20" ht="18" customHeight="1">
       <c r="A294" s="57"/>
-      <c r="B294" s="57"/>
-      <c r="C294" s="57"/>
-      <c r="D294" s="57"/>
-      <c r="E294" s="55"/>
-      <c r="F294" s="57"/>
-      <c r="G294" s="32"/>
-      <c r="H294" s="57"/>
-      <c r="I294" s="38"/>
-      <c r="J294" s="51"/>
+      <c r="B294" s="57" t="s">
+        <v>338</v>
+      </c>
+      <c r="C294" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="D294" s="57" t="s">
+        <v>340</v>
+      </c>
+      <c r="E294" s="57" t="s">
+        <v>343</v>
+      </c>
+      <c r="F294" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="G294" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H294" s="57" t="s">
+        <v>344</v>
+      </c>
+      <c r="I294" s="54">
+        <v>298</v>
+      </c>
+      <c r="J294" s="44">
+        <v>23.806519453207098</v>
+      </c>
       <c r="K294" s="44"/>
-      <c r="L294" s="57"/>
-      <c r="M294" s="57"/>
-      <c r="N294" s="40"/>
+      <c r="L294" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="M294" s="57" t="s">
+        <v>345</v>
+      </c>
+      <c r="N294" s="40" t="s">
+        <v>346</v>
+      </c>
       <c r="O294" s="44"/>
       <c r="P294" s="44"/>
       <c r="Q294" s="44"/>
@@ -31094,11 +31409,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -31113,6 +31423,11 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
- parsed data from `10.1016/j.msea.2025.149028`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Aug2025.xlsx
+++ b/MiscSmallUploads_Aug2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABDE725F-CE89-E848-A825-E11B249682FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9547974-0791-8647-8FFB-C2F2E03D2C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7580" windowWidth="34560" windowHeight="12760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-300" yWindow="8580" windowWidth="34560" windowHeight="12760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2750" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3100" uniqueCount="364">
   <si>
     <r>
       <rPr>
@@ -1171,6 +1171,57 @@
   </si>
   <si>
     <t>10.1038/s41586-022-04914-8</t>
+  </si>
+  <si>
+    <t>10.1016/j.msea.2025.149028</t>
+  </si>
+  <si>
+    <t>Ti50Zr30Nb20</t>
+  </si>
+  <si>
+    <t>Ti50Zr30 Nb17.5 Al2.5</t>
+  </si>
+  <si>
+    <t>Ti50Zr30 Nb15 Al5</t>
+  </si>
+  <si>
+    <t>Ti50Zr30 Nb12.5 Al7.5</t>
+  </si>
+  <si>
+    <t>Ti50Zr30 Nb10 Al10</t>
+  </si>
+  <si>
+    <t>AAM+CR+RX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cold rolled to 80% reduction and annealed at 973K for 1h in vacuum to recrystalize </t>
+  </si>
+  <si>
+    <t>F4b</t>
+  </si>
+  <si>
+    <t>P9</t>
+  </si>
+  <si>
+    <t>F15a</t>
+  </si>
+  <si>
+    <t>F13</t>
+  </si>
+  <si>
+    <t>F15b</t>
+  </si>
+  <si>
+    <t>160-atom supercells GGA-PBE in VASP</t>
+  </si>
+  <si>
+    <t>B/G ratio</t>
+  </si>
+  <si>
+    <t>poissons ratio</t>
+  </si>
+  <si>
+    <t>TS4</t>
   </si>
 </sst>
 </file>
@@ -2204,7 +2255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2396,9 +2447,7 @@
     <xf numFmtId="49" fontId="14" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="14" fillId="10" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3686,8 +3735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T960"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A283" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F305" sqref="F305"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A315" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N338" sqref="N338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -3744,19 +3793,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" s="137" t="s">
+      <c r="D2" s="135" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="138"/>
-      <c r="F2" s="141"/>
-      <c r="G2" s="142"/>
-      <c r="H2" s="142"/>
-      <c r="I2" s="143"/>
-      <c r="J2" s="144"/>
-      <c r="K2" s="144"/>
-      <c r="L2" s="142"/>
-      <c r="M2" s="142"/>
-      <c r="N2" s="145"/>
+      <c r="E2" s="136"/>
+      <c r="F2" s="139"/>
+      <c r="G2" s="140"/>
+      <c r="H2" s="140"/>
+      <c r="I2" s="141"/>
+      <c r="J2" s="142"/>
+      <c r="K2" s="142"/>
+      <c r="L2" s="140"/>
+      <c r="M2" s="140"/>
+      <c r="N2" s="143"/>
       <c r="O2" s="13"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -3772,17 +3821,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="139"/>
-      <c r="E3" s="140"/>
-      <c r="F3" s="146"/>
-      <c r="G3" s="146"/>
-      <c r="H3" s="146"/>
-      <c r="I3" s="147"/>
-      <c r="J3" s="148"/>
-      <c r="K3" s="148"/>
-      <c r="L3" s="146"/>
-      <c r="M3" s="146"/>
-      <c r="N3" s="149"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="138"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="144"/>
+      <c r="H3" s="144"/>
+      <c r="I3" s="145"/>
+      <c r="J3" s="146"/>
+      <c r="K3" s="146"/>
+      <c r="L3" s="144"/>
+      <c r="M3" s="144"/>
+      <c r="N3" s="147"/>
       <c r="O3" s="13"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -3823,43 +3872,43 @@
       <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="150" t="s">
+      <c r="C5" s="148" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="152" t="s">
+      <c r="D5" s="150" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="152" t="s">
+      <c r="E5" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="152" t="s">
+      <c r="F5" s="150" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="152" t="s">
+      <c r="G5" s="150" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="153" t="s">
+      <c r="H5" s="151" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="152" t="s">
+      <c r="I5" s="150" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="152" t="s">
+      <c r="J5" s="150" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="152" t="s">
+      <c r="K5" s="150" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="152" t="s">
+      <c r="L5" s="150" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="152" t="s">
+      <c r="M5" s="150" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="152" t="s">
+      <c r="N5" s="150" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="120" t="s">
+      <c r="O5" s="118" t="s">
         <v>20</v>
       </c>
       <c r="P5" s="25"/>
@@ -3875,19 +3924,19 @@
       <c r="B6" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="151"/>
-      <c r="D6" s="151"/>
-      <c r="E6" s="151"/>
-      <c r="F6" s="151"/>
-      <c r="G6" s="151"/>
-      <c r="H6" s="154"/>
-      <c r="I6" s="155"/>
-      <c r="J6" s="156"/>
-      <c r="K6" s="156"/>
-      <c r="L6" s="151"/>
-      <c r="M6" s="151"/>
-      <c r="N6" s="151"/>
-      <c r="O6" s="121"/>
+      <c r="C6" s="149"/>
+      <c r="D6" s="149"/>
+      <c r="E6" s="149"/>
+      <c r="F6" s="149"/>
+      <c r="G6" s="149"/>
+      <c r="H6" s="152"/>
+      <c r="I6" s="153"/>
+      <c r="J6" s="154"/>
+      <c r="K6" s="154"/>
+      <c r="L6" s="149"/>
+      <c r="M6" s="149"/>
+      <c r="N6" s="149"/>
+      <c r="O6" s="119"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="9"/>
@@ -3937,7 +3986,7 @@
       <c r="N7" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="122"/>
+      <c r="O7" s="120"/>
       <c r="P7" s="64" t="s">
         <v>62</v>
       </c>
@@ -3952,35 +4001,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" thickBot="1">
       <c r="A8" s="59"/>
-      <c r="B8" s="123" t="s">
+      <c r="B8" s="121" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="124"/>
-      <c r="D8" s="124"/>
-      <c r="E8" s="125"/>
-      <c r="F8" s="126" t="s">
+      <c r="C8" s="122"/>
+      <c r="D8" s="122"/>
+      <c r="E8" s="123"/>
+      <c r="F8" s="124" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="127"/>
-      <c r="H8" s="127"/>
-      <c r="I8" s="128"/>
-      <c r="J8" s="129"/>
-      <c r="K8" s="129"/>
-      <c r="L8" s="130"/>
-      <c r="M8" s="131" t="s">
+      <c r="G8" s="125"/>
+      <c r="H8" s="125"/>
+      <c r="I8" s="126"/>
+      <c r="J8" s="127"/>
+      <c r="K8" s="127"/>
+      <c r="L8" s="128"/>
+      <c r="M8" s="129" t="s">
         <v>40</v>
       </c>
-      <c r="N8" s="132"/>
+      <c r="N8" s="130"/>
       <c r="O8" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="P8" s="133" t="s">
+      <c r="P8" s="131" t="s">
         <v>42</v>
       </c>
-      <c r="Q8" s="134"/>
-      <c r="R8" s="135"/>
-      <c r="S8" s="135"/>
-      <c r="T8" s="136"/>
+      <c r="Q8" s="132"/>
+      <c r="R8" s="133"/>
+      <c r="S8" s="133"/>
+      <c r="T8" s="134"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1">
       <c r="A9" s="60" t="s">
@@ -5157,7 +5206,7 @@
       <c r="T38" s="37"/>
     </row>
     <row r="39" spans="1:20" ht="18.75" customHeight="1">
-      <c r="A39" s="110" t="s">
+      <c r="A39" s="108" t="s">
         <v>99</v>
       </c>
       <c r="B39" s="103" t="s">
@@ -5203,7 +5252,7 @@
       <c r="T39" s="37"/>
     </row>
     <row r="40" spans="1:20" ht="18.75" customHeight="1">
-      <c r="A40" s="111" t="s">
+      <c r="A40" s="109" t="s">
         <v>105</v>
       </c>
       <c r="B40" s="105" t="s">
@@ -5295,7 +5344,7 @@
       <c r="T41" s="37"/>
     </row>
     <row r="42" spans="1:20" ht="18.75" customHeight="1">
-      <c r="A42" s="110" t="s">
+      <c r="A42" s="108" t="s">
         <v>107</v>
       </c>
       <c r="B42" s="105" t="s">
@@ -5341,7 +5390,7 @@
       <c r="T42" s="37"/>
     </row>
     <row r="43" spans="1:20" ht="18" customHeight="1">
-      <c r="A43" s="111" t="s">
+      <c r="A43" s="109" t="s">
         <v>108</v>
       </c>
       <c r="B43" s="105" t="s">
@@ -5387,7 +5436,7 @@
       <c r="T43" s="37"/>
     </row>
     <row r="44" spans="1:20" ht="18" customHeight="1">
-      <c r="A44" s="111" t="s">
+      <c r="A44" s="109" t="s">
         <v>109</v>
       </c>
       <c r="B44" s="105" t="s">
@@ -7685,7 +7734,7 @@
       <c r="T97" s="37"/>
     </row>
     <row r="98" spans="1:20" ht="18" customHeight="1">
-      <c r="A98" s="110" t="s">
+      <c r="A98" s="108" t="s">
         <v>187</v>
       </c>
       <c r="B98" s="103" t="s">
@@ -7731,7 +7780,7 @@
       <c r="T98" s="37"/>
     </row>
     <row r="99" spans="1:20" ht="18" customHeight="1">
-      <c r="A99" s="111" t="s">
+      <c r="A99" s="109" t="s">
         <v>188</v>
       </c>
       <c r="B99" s="105" t="s">
@@ -7777,7 +7826,7 @@
       <c r="T99" s="37"/>
     </row>
     <row r="100" spans="1:20" ht="18" customHeight="1">
-      <c r="A100" s="111" t="s">
+      <c r="A100" s="109" t="s">
         <v>189</v>
       </c>
       <c r="B100" s="105" t="s">
@@ -7823,7 +7872,7 @@
       <c r="T100" s="37"/>
     </row>
     <row r="101" spans="1:20" ht="18" customHeight="1">
-      <c r="A101" s="111" t="s">
+      <c r="A101" s="109" t="s">
         <v>190</v>
       </c>
       <c r="B101" s="105" t="s">
@@ -7869,7 +7918,7 @@
       <c r="T101" s="37"/>
     </row>
     <row r="102" spans="1:20" ht="18" customHeight="1">
-      <c r="A102" s="110" t="s">
+      <c r="A102" s="108" t="s">
         <v>187</v>
       </c>
       <c r="B102" s="103" t="s">
@@ -7915,7 +7964,7 @@
       <c r="T102" s="37"/>
     </row>
     <row r="103" spans="1:20" ht="18" customHeight="1">
-      <c r="A103" s="111" t="s">
+      <c r="A103" s="109" t="s">
         <v>188</v>
       </c>
       <c r="B103" s="105" t="s">
@@ -7961,7 +8010,7 @@
       <c r="T103" s="37"/>
     </row>
     <row r="104" spans="1:20" ht="18" customHeight="1">
-      <c r="A104" s="111" t="s">
+      <c r="A104" s="109" t="s">
         <v>189</v>
       </c>
       <c r="B104" s="105" t="s">
@@ -8007,7 +8056,7 @@
       <c r="T104" s="37"/>
     </row>
     <row r="105" spans="1:20" ht="18" customHeight="1">
-      <c r="A105" s="111" t="s">
+      <c r="A105" s="109" t="s">
         <v>190</v>
       </c>
       <c r="B105" s="105" t="s">
@@ -8053,7 +8102,7 @@
       <c r="T105" s="37"/>
     </row>
     <row r="106" spans="1:20" ht="18" customHeight="1">
-      <c r="A106" s="110" t="s">
+      <c r="A106" s="108" t="s">
         <v>187</v>
       </c>
       <c r="B106" s="103" t="s">
@@ -8099,7 +8148,7 @@
       <c r="T106" s="37"/>
     </row>
     <row r="107" spans="1:20" ht="18" customHeight="1">
-      <c r="A107" s="111" t="s">
+      <c r="A107" s="109" t="s">
         <v>188</v>
       </c>
       <c r="B107" s="105" t="s">
@@ -8145,7 +8194,7 @@
       <c r="T107" s="37"/>
     </row>
     <row r="108" spans="1:20" ht="18" customHeight="1">
-      <c r="A108" s="111" t="s">
+      <c r="A108" s="109" t="s">
         <v>189</v>
       </c>
       <c r="B108" s="105" t="s">
@@ -8191,7 +8240,7 @@
       <c r="T108" s="37"/>
     </row>
     <row r="109" spans="1:20" ht="18" customHeight="1">
-      <c r="A109" s="111" t="s">
+      <c r="A109" s="109" t="s">
         <v>190</v>
       </c>
       <c r="B109" s="105" t="s">
@@ -8237,7 +8286,7 @@
       <c r="T109" s="37"/>
     </row>
     <row r="110" spans="1:20" ht="18" customHeight="1">
-      <c r="A110" s="110" t="s">
+      <c r="A110" s="108" t="s">
         <v>187</v>
       </c>
       <c r="B110" s="103" t="s">
@@ -8283,7 +8332,7 @@
       <c r="T110" s="37"/>
     </row>
     <row r="111" spans="1:20" ht="18" customHeight="1">
-      <c r="A111" s="111" t="s">
+      <c r="A111" s="109" t="s">
         <v>188</v>
       </c>
       <c r="B111" s="105" t="s">
@@ -8329,7 +8378,7 @@
       <c r="T111" s="37"/>
     </row>
     <row r="112" spans="1:20" ht="18" customHeight="1">
-      <c r="A112" s="111" t="s">
+      <c r="A112" s="109" t="s">
         <v>189</v>
       </c>
       <c r="B112" s="105" t="s">
@@ -8375,7 +8424,7 @@
       <c r="T112" s="37"/>
     </row>
     <row r="113" spans="1:20" ht="18" customHeight="1">
-      <c r="A113" s="111" t="s">
+      <c r="A113" s="109" t="s">
         <v>190</v>
       </c>
       <c r="B113" s="105" t="s">
@@ -8421,7 +8470,7 @@
       <c r="T113" s="37"/>
     </row>
     <row r="114" spans="1:20" ht="18" customHeight="1">
-      <c r="A114" s="111" t="s">
+      <c r="A114" s="109" t="s">
         <v>188</v>
       </c>
       <c r="B114" s="105" t="s">
@@ -8467,7 +8516,7 @@
       <c r="T114" s="37"/>
     </row>
     <row r="115" spans="1:20" ht="18" customHeight="1">
-      <c r="A115" s="111" t="s">
+      <c r="A115" s="109" t="s">
         <v>189</v>
       </c>
       <c r="B115" s="105" t="s">
@@ -8513,7 +8562,7 @@
       <c r="T115" s="37"/>
     </row>
     <row r="116" spans="1:20" ht="18" customHeight="1">
-      <c r="A116" s="111" t="s">
+      <c r="A116" s="109" t="s">
         <v>190</v>
       </c>
       <c r="B116" s="105" t="s">
@@ -11067,7 +11116,7 @@
       <c r="T173" s="37"/>
     </row>
     <row r="174" spans="1:20" ht="18" customHeight="1">
-      <c r="A174" s="112" t="s">
+      <c r="A174" s="110" t="s">
         <v>266</v>
       </c>
       <c r="B174" s="103" t="s">
@@ -11091,7 +11140,7 @@
       <c r="H174" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="I174" s="113">
+      <c r="I174" s="111">
         <v>298</v>
       </c>
       <c r="J174" s="48">
@@ -11115,7 +11164,7 @@
       <c r="T174" s="37"/>
     </row>
     <row r="175" spans="1:20" ht="18" customHeight="1">
-      <c r="A175" s="114" t="s">
+      <c r="A175" s="112" t="s">
         <v>267</v>
       </c>
       <c r="B175" s="105" t="s">
@@ -11139,7 +11188,7 @@
       <c r="H175" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="I175" s="115">
+      <c r="I175" s="113">
         <v>298</v>
       </c>
       <c r="J175" s="48">
@@ -11163,7 +11212,7 @@
       <c r="T175" s="37"/>
     </row>
     <row r="176" spans="1:20" ht="18" customHeight="1">
-      <c r="A176" s="114" t="s">
+      <c r="A176" s="112" t="s">
         <v>268</v>
       </c>
       <c r="B176" s="105" t="s">
@@ -11187,7 +11236,7 @@
       <c r="H176" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="I176" s="115">
+      <c r="I176" s="113">
         <v>298</v>
       </c>
       <c r="J176" s="48">
@@ -11211,7 +11260,7 @@
       <c r="T176" s="37"/>
     </row>
     <row r="177" spans="1:20" ht="18" customHeight="1">
-      <c r="A177" s="114" t="s">
+      <c r="A177" s="112" t="s">
         <v>269</v>
       </c>
       <c r="B177" s="105" t="s">
@@ -11235,7 +11284,7 @@
       <c r="H177" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="I177" s="115">
+      <c r="I177" s="113">
         <v>298</v>
       </c>
       <c r="J177" s="35">
@@ -11259,7 +11308,7 @@
       <c r="T177" s="37"/>
     </row>
     <row r="178" spans="1:20" ht="18" customHeight="1">
-      <c r="A178" s="112" t="s">
+      <c r="A178" s="110" t="s">
         <v>266</v>
       </c>
       <c r="B178" s="103" t="s">
@@ -11283,7 +11332,7 @@
       <c r="H178" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="I178" s="113">
+      <c r="I178" s="111">
         <v>298</v>
       </c>
       <c r="J178" s="35">
@@ -11307,7 +11356,7 @@
       <c r="T178" s="37"/>
     </row>
     <row r="179" spans="1:20" ht="18" customHeight="1">
-      <c r="A179" s="114" t="s">
+      <c r="A179" s="112" t="s">
         <v>267</v>
       </c>
       <c r="B179" s="105" t="s">
@@ -11331,7 +11380,7 @@
       <c r="H179" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="I179" s="115">
+      <c r="I179" s="113">
         <v>298</v>
       </c>
       <c r="J179" s="35">
@@ -11355,7 +11404,7 @@
       <c r="T179" s="37"/>
     </row>
     <row r="180" spans="1:20" ht="18" customHeight="1">
-      <c r="A180" s="114" t="s">
+      <c r="A180" s="112" t="s">
         <v>268</v>
       </c>
       <c r="B180" s="105" t="s">
@@ -11379,7 +11428,7 @@
       <c r="H180" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="I180" s="115">
+      <c r="I180" s="113">
         <v>298</v>
       </c>
       <c r="J180" s="35">
@@ -11403,7 +11452,7 @@
       <c r="T180" s="37"/>
     </row>
     <row r="181" spans="1:20" ht="18" customHeight="1">
-      <c r="A181" s="114" t="s">
+      <c r="A181" s="112" t="s">
         <v>269</v>
       </c>
       <c r="B181" s="105" t="s">
@@ -11427,7 +11476,7 @@
       <c r="H181" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="I181" s="115">
+      <c r="I181" s="113">
         <v>298</v>
       </c>
       <c r="J181" s="35">
@@ -11635,7 +11684,7 @@
       <c r="T185" s="37"/>
     </row>
     <row r="186" spans="1:20" ht="18" customHeight="1">
-      <c r="A186" s="112" t="s">
+      <c r="A186" s="110" t="s">
         <v>266</v>
       </c>
       <c r="B186" s="103" t="s">
@@ -11681,7 +11730,7 @@
       <c r="T186" s="37"/>
     </row>
     <row r="187" spans="1:20" ht="18" customHeight="1">
-      <c r="A187" s="114" t="s">
+      <c r="A187" s="112" t="s">
         <v>267</v>
       </c>
       <c r="B187" s="105" t="s">
@@ -11727,7 +11776,7 @@
       <c r="T187" s="37"/>
     </row>
     <row r="188" spans="1:20" ht="18" customHeight="1">
-      <c r="A188" s="114" t="s">
+      <c r="A188" s="112" t="s">
         <v>268</v>
       </c>
       <c r="B188" s="105" t="s">
@@ -11773,7 +11822,7 @@
       <c r="T188" s="37"/>
     </row>
     <row r="189" spans="1:20" ht="18" customHeight="1">
-      <c r="A189" s="114" t="s">
+      <c r="A189" s="112" t="s">
         <v>269</v>
       </c>
       <c r="B189" s="105" t="s">
@@ -11819,7 +11868,7 @@
       <c r="T189" s="37"/>
     </row>
     <row r="190" spans="1:20" ht="18" customHeight="1">
-      <c r="A190" s="112" t="s">
+      <c r="A190" s="110" t="s">
         <v>266</v>
       </c>
       <c r="B190" s="103" t="s">
@@ -11865,7 +11914,7 @@
       <c r="T190" s="37"/>
     </row>
     <row r="191" spans="1:20" ht="18" customHeight="1">
-      <c r="A191" s="114" t="s">
+      <c r="A191" s="112" t="s">
         <v>267</v>
       </c>
       <c r="B191" s="105" t="s">
@@ -11911,7 +11960,7 @@
       <c r="T191" s="37"/>
     </row>
     <row r="192" spans="1:20" ht="18" customHeight="1">
-      <c r="A192" s="114" t="s">
+      <c r="A192" s="112" t="s">
         <v>268</v>
       </c>
       <c r="B192" s="105" t="s">
@@ -11957,7 +12006,7 @@
       <c r="T192" s="37"/>
     </row>
     <row r="193" spans="1:20" ht="18" customHeight="1">
-      <c r="A193" s="114" t="s">
+      <c r="A193" s="112" t="s">
         <v>269</v>
       </c>
       <c r="B193" s="105" t="s">
@@ -12354,7 +12403,7 @@
       <c r="E200" s="31" t="s">
         <v>311</v>
       </c>
-      <c r="F200" s="116" t="s">
+      <c r="F200" s="114" t="s">
         <v>122</v>
       </c>
       <c r="G200" s="32" t="s">
@@ -13147,7 +13196,7 @@
       <c r="T216" s="37"/>
     </row>
     <row r="217" spans="1:20" ht="18" customHeight="1">
-      <c r="A217" s="117" t="s">
+      <c r="A217" s="115" t="s">
         <v>282</v>
       </c>
       <c r="B217" s="103" t="s">
@@ -13193,7 +13242,7 @@
       <c r="T217" s="37"/>
     </row>
     <row r="218" spans="1:20" ht="18" customHeight="1">
-      <c r="A218" s="118" t="s">
+      <c r="A218" s="116" t="s">
         <v>303</v>
       </c>
       <c r="B218" s="105" t="s">
@@ -13241,7 +13290,7 @@
       <c r="T218" s="37"/>
     </row>
     <row r="219" spans="1:20" ht="18" customHeight="1">
-      <c r="A219" s="118" t="s">
+      <c r="A219" s="116" t="s">
         <v>304</v>
       </c>
       <c r="B219" s="105" t="s">
@@ -13289,7 +13338,7 @@
       <c r="T219" s="37"/>
     </row>
     <row r="220" spans="1:20" ht="18" customHeight="1">
-      <c r="A220" s="118" t="s">
+      <c r="A220" s="116" t="s">
         <v>305</v>
       </c>
       <c r="B220" s="105" t="s">
@@ -13337,7 +13386,7 @@
       <c r="T220" s="37"/>
     </row>
     <row r="221" spans="1:20" ht="18" customHeight="1">
-      <c r="A221" s="118" t="s">
+      <c r="A221" s="116" t="s">
         <v>306</v>
       </c>
       <c r="B221" s="105" t="s">
@@ -13385,7 +13434,7 @@
       <c r="T221" s="37"/>
     </row>
     <row r="222" spans="1:20" ht="18" customHeight="1">
-      <c r="A222" s="118" t="s">
+      <c r="A222" s="116" t="s">
         <v>309</v>
       </c>
       <c r="B222" s="105" t="s">
@@ -13433,7 +13482,7 @@
       <c r="T222" s="37"/>
     </row>
     <row r="223" spans="1:20" ht="18" customHeight="1">
-      <c r="A223" s="118" t="s">
+      <c r="A223" s="116" t="s">
         <v>307</v>
       </c>
       <c r="B223" s="105" t="s">
@@ -13481,7 +13530,7 @@
       <c r="T223" s="37"/>
     </row>
     <row r="224" spans="1:20" ht="18" customHeight="1">
-      <c r="A224" s="118" t="s">
+      <c r="A224" s="116" t="s">
         <v>308</v>
       </c>
       <c r="B224" s="105" t="s">
@@ -13529,7 +13578,7 @@
       <c r="T224" s="37"/>
     </row>
     <row r="225" spans="1:20" ht="18" customHeight="1">
-      <c r="A225" s="117" t="s">
+      <c r="A225" s="115" t="s">
         <v>282</v>
       </c>
       <c r="B225" s="103" t="s">
@@ -13575,7 +13624,7 @@
       <c r="T225" s="37"/>
     </row>
     <row r="226" spans="1:20" ht="18" customHeight="1">
-      <c r="A226" s="118" t="s">
+      <c r="A226" s="116" t="s">
         <v>303</v>
       </c>
       <c r="B226" s="105" t="s">
@@ -13623,7 +13672,7 @@
       <c r="T226" s="37"/>
     </row>
     <row r="227" spans="1:20" ht="18" customHeight="1">
-      <c r="A227" s="118" t="s">
+      <c r="A227" s="116" t="s">
         <v>304</v>
       </c>
       <c r="B227" s="105" t="s">
@@ -13671,7 +13720,7 @@
       <c r="T227" s="37"/>
     </row>
     <row r="228" spans="1:20" ht="18" customHeight="1">
-      <c r="A228" s="118" t="s">
+      <c r="A228" s="116" t="s">
         <v>305</v>
       </c>
       <c r="B228" s="105" t="s">
@@ -13719,7 +13768,7 @@
       <c r="T228" s="37"/>
     </row>
     <row r="229" spans="1:20" ht="18" customHeight="1">
-      <c r="A229" s="118" t="s">
+      <c r="A229" s="116" t="s">
         <v>306</v>
       </c>
       <c r="B229" s="105" t="s">
@@ -13767,7 +13816,7 @@
       <c r="T229" s="37"/>
     </row>
     <row r="230" spans="1:20" ht="18" customHeight="1">
-      <c r="A230" s="118" t="s">
+      <c r="A230" s="116" t="s">
         <v>309</v>
       </c>
       <c r="B230" s="105" t="s">
@@ -13815,7 +13864,7 @@
       <c r="T230" s="37"/>
     </row>
     <row r="231" spans="1:20" ht="18" customHeight="1">
-      <c r="A231" s="118" t="s">
+      <c r="A231" s="116" t="s">
         <v>307</v>
       </c>
       <c r="B231" s="105" t="s">
@@ -13863,7 +13912,7 @@
       <c r="T231" s="37"/>
     </row>
     <row r="232" spans="1:20" ht="18" customHeight="1">
-      <c r="A232" s="118" t="s">
+      <c r="A232" s="116" t="s">
         <v>308</v>
       </c>
       <c r="B232" s="105" t="s">
@@ -13911,7 +13960,7 @@
       <c r="T232" s="37"/>
     </row>
     <row r="233" spans="1:20" ht="18" customHeight="1">
-      <c r="A233" s="117" t="s">
+      <c r="A233" s="115" t="s">
         <v>282</v>
       </c>
       <c r="B233" s="103" t="s">
@@ -13958,7 +14007,7 @@
       <c r="T233" s="37"/>
     </row>
     <row r="234" spans="1:20" ht="18" customHeight="1">
-      <c r="A234" s="118" t="s">
+      <c r="A234" s="116" t="s">
         <v>303</v>
       </c>
       <c r="B234" s="105" t="s">
@@ -14007,7 +14056,7 @@
       <c r="T234" s="37"/>
     </row>
     <row r="235" spans="1:20" ht="18" customHeight="1">
-      <c r="A235" s="118" t="s">
+      <c r="A235" s="116" t="s">
         <v>304</v>
       </c>
       <c r="B235" s="105" t="s">
@@ -14056,7 +14105,7 @@
       <c r="T235" s="37"/>
     </row>
     <row r="236" spans="1:20" ht="18" customHeight="1">
-      <c r="A236" s="118" t="s">
+      <c r="A236" s="116" t="s">
         <v>305</v>
       </c>
       <c r="B236" s="105" t="s">
@@ -14105,7 +14154,7 @@
       <c r="T236" s="37"/>
     </row>
     <row r="237" spans="1:20" ht="18" customHeight="1">
-      <c r="A237" s="118" t="s">
+      <c r="A237" s="116" t="s">
         <v>306</v>
       </c>
       <c r="B237" s="105" t="s">
@@ -14154,7 +14203,7 @@
       <c r="T237" s="37"/>
     </row>
     <row r="238" spans="1:20" ht="18" customHeight="1">
-      <c r="A238" s="118" t="s">
+      <c r="A238" s="116" t="s">
         <v>309</v>
       </c>
       <c r="B238" s="105" t="s">
@@ -14203,7 +14252,7 @@
       <c r="T238" s="37"/>
     </row>
     <row r="239" spans="1:20" ht="18" customHeight="1">
-      <c r="A239" s="118" t="s">
+      <c r="A239" s="116" t="s">
         <v>307</v>
       </c>
       <c r="B239" s="105" t="s">
@@ -14252,7 +14301,7 @@
       <c r="T239" s="37"/>
     </row>
     <row r="240" spans="1:20" ht="18" customHeight="1">
-      <c r="A240" s="118" t="s">
+      <c r="A240" s="116" t="s">
         <v>308</v>
       </c>
       <c r="B240" s="105" t="s">
@@ -14301,7 +14350,7 @@
       <c r="T240" s="37"/>
     </row>
     <row r="241" spans="1:20" ht="18" customHeight="1">
-      <c r="A241" s="117" t="s">
+      <c r="A241" s="115" t="s">
         <v>282</v>
       </c>
       <c r="B241" s="103" t="s">
@@ -14350,7 +14399,7 @@
       <c r="T241" s="37"/>
     </row>
     <row r="242" spans="1:20" ht="18" customHeight="1">
-      <c r="A242" s="118" t="s">
+      <c r="A242" s="116" t="s">
         <v>303</v>
       </c>
       <c r="B242" s="105" t="s">
@@ -14401,7 +14450,7 @@
       <c r="T242" s="37"/>
     </row>
     <row r="243" spans="1:20" ht="18" customHeight="1">
-      <c r="A243" s="118" t="s">
+      <c r="A243" s="116" t="s">
         <v>304</v>
       </c>
       <c r="B243" s="105" t="s">
@@ -14452,7 +14501,7 @@
       <c r="T243" s="37"/>
     </row>
     <row r="244" spans="1:20" ht="18" customHeight="1">
-      <c r="A244" s="118" t="s">
+      <c r="A244" s="116" t="s">
         <v>305</v>
       </c>
       <c r="B244" s="105" t="s">
@@ -14503,7 +14552,7 @@
       <c r="T244" s="37"/>
     </row>
     <row r="245" spans="1:20" ht="18" customHeight="1">
-      <c r="A245" s="118" t="s">
+      <c r="A245" s="116" t="s">
         <v>306</v>
       </c>
       <c r="B245" s="105" t="s">
@@ -14554,7 +14603,7 @@
       <c r="T245" s="37"/>
     </row>
     <row r="246" spans="1:20" ht="18" customHeight="1">
-      <c r="A246" s="118" t="s">
+      <c r="A246" s="116" t="s">
         <v>309</v>
       </c>
       <c r="B246" s="105" t="s">
@@ -14605,7 +14654,7 @@
       <c r="T246" s="37"/>
     </row>
     <row r="247" spans="1:20" ht="18" customHeight="1">
-      <c r="A247" s="118" t="s">
+      <c r="A247" s="116" t="s">
         <v>307</v>
       </c>
       <c r="B247" s="105" t="s">
@@ -14656,7 +14705,7 @@
       <c r="T247" s="44"/>
     </row>
     <row r="248" spans="1:20" ht="18" customHeight="1">
-      <c r="A248" s="118" t="s">
+      <c r="A248" s="116" t="s">
         <v>308</v>
       </c>
       <c r="B248" s="105" t="s">
@@ -14707,7 +14756,7 @@
       <c r="T248" s="44"/>
     </row>
     <row r="249" spans="1:20" ht="18" customHeight="1">
-      <c r="A249" s="117" t="s">
+      <c r="A249" s="115" t="s">
         <v>282</v>
       </c>
       <c r="B249" s="103" t="s">
@@ -14756,7 +14805,7 @@
       <c r="T249" s="44"/>
     </row>
     <row r="250" spans="1:20" ht="18" customHeight="1">
-      <c r="A250" s="118" t="s">
+      <c r="A250" s="116" t="s">
         <v>303</v>
       </c>
       <c r="B250" s="105" t="s">
@@ -14807,7 +14856,7 @@
       <c r="T250" s="37"/>
     </row>
     <row r="251" spans="1:20" ht="18" customHeight="1">
-      <c r="A251" s="118" t="s">
+      <c r="A251" s="116" t="s">
         <v>304</v>
       </c>
       <c r="B251" s="105" t="s">
@@ -14858,7 +14907,7 @@
       <c r="T251" s="37"/>
     </row>
     <row r="252" spans="1:20" ht="18" customHeight="1">
-      <c r="A252" s="118" t="s">
+      <c r="A252" s="116" t="s">
         <v>305</v>
       </c>
       <c r="B252" s="105" t="s">
@@ -14909,7 +14958,7 @@
       <c r="T252" s="37"/>
     </row>
     <row r="253" spans="1:20" ht="18" customHeight="1">
-      <c r="A253" s="118" t="s">
+      <c r="A253" s="116" t="s">
         <v>306</v>
       </c>
       <c r="B253" s="105" t="s">
@@ -14960,7 +15009,7 @@
       <c r="T253" s="37"/>
     </row>
     <row r="254" spans="1:20" ht="18" customHeight="1">
-      <c r="A254" s="118" t="s">
+      <c r="A254" s="116" t="s">
         <v>309</v>
       </c>
       <c r="B254" s="105" t="s">
@@ -15011,7 +15060,7 @@
       <c r="T254" s="37"/>
     </row>
     <row r="255" spans="1:20" ht="18" customHeight="1">
-      <c r="A255" s="118" t="s">
+      <c r="A255" s="116" t="s">
         <v>307</v>
       </c>
       <c r="B255" s="105" t="s">
@@ -15062,7 +15111,7 @@
       <c r="T255" s="37"/>
     </row>
     <row r="256" spans="1:20" ht="18" customHeight="1">
-      <c r="A256" s="118" t="s">
+      <c r="A256" s="116" t="s">
         <v>308</v>
       </c>
       <c r="B256" s="105" t="s">
@@ -15113,7 +15162,7 @@
       <c r="T256" s="37"/>
     </row>
     <row r="257" spans="1:20" ht="18" customHeight="1">
-      <c r="A257" s="117" t="s">
+      <c r="A257" s="115" t="s">
         <v>282</v>
       </c>
       <c r="B257" s="103" t="s">
@@ -15162,7 +15211,7 @@
       <c r="T257" s="37"/>
     </row>
     <row r="258" spans="1:20" ht="18" customHeight="1">
-      <c r="A258" s="118" t="s">
+      <c r="A258" s="116" t="s">
         <v>303</v>
       </c>
       <c r="B258" s="105" t="s">
@@ -15213,7 +15262,7 @@
       <c r="T258" s="37"/>
     </row>
     <row r="259" spans="1:20" ht="18" customHeight="1">
-      <c r="A259" s="118" t="s">
+      <c r="A259" s="116" t="s">
         <v>304</v>
       </c>
       <c r="B259" s="105" t="s">
@@ -15264,7 +15313,7 @@
       <c r="T259" s="37"/>
     </row>
     <row r="260" spans="1:20" ht="18" customHeight="1">
-      <c r="A260" s="118" t="s">
+      <c r="A260" s="116" t="s">
         <v>305</v>
       </c>
       <c r="B260" s="105" t="s">
@@ -15315,7 +15364,7 @@
       <c r="T260" s="37"/>
     </row>
     <row r="261" spans="1:20" ht="18" customHeight="1">
-      <c r="A261" s="118" t="s">
+      <c r="A261" s="116" t="s">
         <v>306</v>
       </c>
       <c r="B261" s="105" t="s">
@@ -15366,7 +15415,7 @@
       <c r="T261" s="37"/>
     </row>
     <row r="262" spans="1:20" ht="18" customHeight="1">
-      <c r="A262" s="118" t="s">
+      <c r="A262" s="116" t="s">
         <v>309</v>
       </c>
       <c r="B262" s="105" t="s">
@@ -15417,7 +15466,7 @@
       <c r="T262" s="37"/>
     </row>
     <row r="263" spans="1:20" ht="18" customHeight="1">
-      <c r="A263" s="118" t="s">
+      <c r="A263" s="116" t="s">
         <v>307</v>
       </c>
       <c r="B263" s="105" t="s">
@@ -15468,7 +15517,7 @@
       <c r="T263" s="37"/>
     </row>
     <row r="264" spans="1:20" ht="18" customHeight="1">
-      <c r="A264" s="118" t="s">
+      <c r="A264" s="116" t="s">
         <v>308</v>
       </c>
       <c r="B264" s="105" t="s">
@@ -15544,7 +15593,7 @@
       <c r="I265" s="54">
         <v>298</v>
       </c>
-      <c r="J265" s="119">
+      <c r="J265" s="117">
         <v>317000000</v>
       </c>
       <c r="K265" s="38"/>
@@ -15590,7 +15639,7 @@
       <c r="I266" s="54">
         <v>298</v>
       </c>
-      <c r="J266" s="119">
+      <c r="J266" s="117">
         <v>404000000</v>
       </c>
       <c r="K266" s="38"/>
@@ -15636,7 +15685,7 @@
       <c r="I267" s="54">
         <v>298</v>
       </c>
-      <c r="J267" s="119">
+      <c r="J267" s="117">
         <v>499000000</v>
       </c>
       <c r="K267" s="38"/>
@@ -15682,7 +15731,7 @@
       <c r="I268" s="54">
         <v>298</v>
       </c>
-      <c r="J268" s="119">
+      <c r="J268" s="117">
         <v>749000000</v>
       </c>
       <c r="K268" s="38"/>
@@ -16900,19 +16949,39 @@
     </row>
     <row r="295" spans="1:20" ht="18" customHeight="1">
       <c r="A295" s="57"/>
-      <c r="B295" s="57"/>
-      <c r="C295" s="57"/>
-      <c r="D295" s="57"/>
+      <c r="B295" s="57" t="s">
+        <v>348</v>
+      </c>
+      <c r="C295" s="57" t="s">
+        <v>160</v>
+      </c>
+      <c r="D295" s="57" t="s">
+        <v>64</v>
+      </c>
       <c r="E295" s="55"/>
-      <c r="F295" s="57"/>
-      <c r="G295" s="32"/>
+      <c r="F295" s="57" t="s">
+        <v>260</v>
+      </c>
+      <c r="G295" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H295" s="57"/>
-      <c r="I295" s="38"/>
-      <c r="J295" s="58"/>
+      <c r="I295" s="38">
+        <v>298</v>
+      </c>
+      <c r="J295" s="44">
+        <v>6036.4025695931396</v>
+      </c>
       <c r="K295" s="44"/>
-      <c r="L295" s="57"/>
-      <c r="M295" s="57"/>
-      <c r="N295" s="40"/>
+      <c r="L295" s="57" t="s">
+        <v>261</v>
+      </c>
+      <c r="M295" s="57" t="s">
+        <v>355</v>
+      </c>
+      <c r="N295" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O295" s="44"/>
       <c r="P295" s="44"/>
       <c r="Q295" s="44"/>
@@ -16922,19 +16991,39 @@
     </row>
     <row r="296" spans="1:20" ht="18" customHeight="1">
       <c r="A296" s="57"/>
-      <c r="B296" s="57"/>
-      <c r="C296" s="57"/>
-      <c r="D296" s="57"/>
+      <c r="B296" s="57" t="s">
+        <v>349</v>
+      </c>
+      <c r="C296" s="57" t="s">
+        <v>160</v>
+      </c>
+      <c r="D296" s="57" t="s">
+        <v>64</v>
+      </c>
       <c r="E296" s="55"/>
-      <c r="F296" s="57"/>
-      <c r="G296" s="32"/>
-      <c r="H296" s="44"/>
-      <c r="I296" s="38"/>
-      <c r="J296" s="35"/>
+      <c r="F296" s="57" t="s">
+        <v>260</v>
+      </c>
+      <c r="G296" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H296" s="57"/>
+      <c r="I296" s="38">
+        <v>298</v>
+      </c>
+      <c r="J296" s="44">
+        <v>5842.3982869378997</v>
+      </c>
       <c r="K296" s="44"/>
-      <c r="L296" s="57"/>
-      <c r="M296" s="57"/>
-      <c r="N296" s="40"/>
+      <c r="L296" s="57" t="s">
+        <v>261</v>
+      </c>
+      <c r="M296" s="57" t="s">
+        <v>355</v>
+      </c>
+      <c r="N296" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O296" s="44"/>
       <c r="P296" s="44"/>
       <c r="Q296" s="44"/>
@@ -16944,19 +17033,39 @@
     </row>
     <row r="297" spans="1:20" ht="18" customHeight="1">
       <c r="A297" s="57"/>
-      <c r="B297" s="57"/>
-      <c r="C297" s="57"/>
-      <c r="D297" s="57"/>
+      <c r="B297" s="57" t="s">
+        <v>350</v>
+      </c>
+      <c r="C297" s="57" t="s">
+        <v>160</v>
+      </c>
+      <c r="D297" s="57" t="s">
+        <v>64</v>
+      </c>
       <c r="E297" s="55"/>
-      <c r="F297" s="57"/>
-      <c r="G297" s="32"/>
-      <c r="H297" s="44"/>
-      <c r="I297" s="38"/>
-      <c r="J297" s="35"/>
+      <c r="F297" s="57" t="s">
+        <v>260</v>
+      </c>
+      <c r="G297" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H297" s="57"/>
+      <c r="I297" s="38">
+        <v>298</v>
+      </c>
+      <c r="J297" s="44">
+        <v>5749.8929336188403</v>
+      </c>
       <c r="K297" s="44"/>
-      <c r="L297" s="57"/>
-      <c r="M297" s="57"/>
-      <c r="N297" s="40"/>
+      <c r="L297" s="57" t="s">
+        <v>261</v>
+      </c>
+      <c r="M297" s="57" t="s">
+        <v>355</v>
+      </c>
+      <c r="N297" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O297" s="44"/>
       <c r="P297" s="44"/>
       <c r="Q297" s="44"/>
@@ -16966,19 +17075,39 @@
     </row>
     <row r="298" spans="1:20" ht="18" customHeight="1">
       <c r="A298" s="57"/>
-      <c r="B298" s="57"/>
-      <c r="C298" s="57"/>
-      <c r="D298" s="57"/>
+      <c r="B298" s="57" t="s">
+        <v>351</v>
+      </c>
+      <c r="C298" s="57" t="s">
+        <v>160</v>
+      </c>
+      <c r="D298" s="57" t="s">
+        <v>64</v>
+      </c>
       <c r="E298" s="55"/>
-      <c r="F298" s="57"/>
-      <c r="G298" s="32"/>
-      <c r="H298" s="44"/>
-      <c r="I298" s="38"/>
-      <c r="J298" s="35"/>
+      <c r="F298" s="57" t="s">
+        <v>260</v>
+      </c>
+      <c r="G298" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H298" s="57"/>
+      <c r="I298" s="38">
+        <v>298</v>
+      </c>
+      <c r="J298" s="44">
+        <v>5595.7173447537398</v>
+      </c>
       <c r="K298" s="44"/>
-      <c r="L298" s="57"/>
-      <c r="M298" s="57"/>
-      <c r="N298" s="40"/>
+      <c r="L298" s="57" t="s">
+        <v>261</v>
+      </c>
+      <c r="M298" s="57" t="s">
+        <v>355</v>
+      </c>
+      <c r="N298" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O298" s="44"/>
       <c r="P298" s="44"/>
       <c r="Q298" s="44"/>
@@ -16988,19 +17117,39 @@
     </row>
     <row r="299" spans="1:20" ht="18" customHeight="1">
       <c r="A299" s="57"/>
-      <c r="B299" s="57"/>
-      <c r="C299" s="57"/>
-      <c r="D299" s="57"/>
+      <c r="B299" s="57" t="s">
+        <v>352</v>
+      </c>
+      <c r="C299" s="57" t="s">
+        <v>160</v>
+      </c>
+      <c r="D299" s="57" t="s">
+        <v>64</v>
+      </c>
       <c r="E299" s="55"/>
-      <c r="F299" s="57"/>
-      <c r="G299" s="32"/>
-      <c r="H299" s="44"/>
-      <c r="I299" s="38"/>
-      <c r="J299" s="35"/>
+      <c r="F299" s="57" t="s">
+        <v>260</v>
+      </c>
+      <c r="G299" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H299" s="57"/>
+      <c r="I299" s="38">
+        <v>298</v>
+      </c>
+      <c r="J299" s="44">
+        <v>5495.5032119914304</v>
+      </c>
       <c r="K299" s="44"/>
-      <c r="L299" s="57"/>
-      <c r="M299" s="57"/>
-      <c r="N299" s="40"/>
+      <c r="L299" s="57" t="s">
+        <v>261</v>
+      </c>
+      <c r="M299" s="57" t="s">
+        <v>355</v>
+      </c>
+      <c r="N299" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O299" s="44"/>
       <c r="P299" s="44"/>
       <c r="Q299" s="44"/>
@@ -17010,19 +17159,43 @@
     </row>
     <row r="300" spans="1:20" ht="18" customHeight="1">
       <c r="A300" s="57"/>
-      <c r="B300" s="57"/>
-      <c r="C300" s="57"/>
-      <c r="D300" s="57"/>
-      <c r="E300" s="55"/>
-      <c r="F300" s="57"/>
-      <c r="G300" s="32"/>
-      <c r="H300" s="57"/>
-      <c r="I300" s="38"/>
-      <c r="J300" s="58"/>
+      <c r="B300" s="57" t="s">
+        <v>348</v>
+      </c>
+      <c r="C300" s="57" t="s">
+        <v>160</v>
+      </c>
+      <c r="D300" s="57" t="s">
+        <v>353</v>
+      </c>
+      <c r="E300" s="55" t="s">
+        <v>354</v>
+      </c>
+      <c r="F300" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="G300" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H300" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="I300" s="38">
+        <v>298</v>
+      </c>
+      <c r="J300" s="58">
+        <v>537000000</v>
+      </c>
       <c r="K300" s="44"/>
-      <c r="L300" s="57"/>
-      <c r="M300" s="57"/>
-      <c r="N300" s="40"/>
+      <c r="L300" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="M300" s="57" t="s">
+        <v>357</v>
+      </c>
+      <c r="N300" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O300" s="44"/>
       <c r="P300" s="44"/>
       <c r="Q300" s="44"/>
@@ -17032,19 +17205,43 @@
     </row>
     <row r="301" spans="1:20" ht="18" customHeight="1">
       <c r="A301" s="57"/>
-      <c r="B301" s="57"/>
-      <c r="C301" s="57"/>
-      <c r="D301" s="57"/>
-      <c r="E301" s="55"/>
-      <c r="F301" s="57"/>
-      <c r="G301" s="32"/>
-      <c r="H301" s="57"/>
-      <c r="I301" s="38"/>
-      <c r="J301" s="58"/>
+      <c r="B301" s="57" t="s">
+        <v>349</v>
+      </c>
+      <c r="C301" s="57" t="s">
+        <v>160</v>
+      </c>
+      <c r="D301" s="57" t="s">
+        <v>353</v>
+      </c>
+      <c r="E301" s="55" t="s">
+        <v>354</v>
+      </c>
+      <c r="F301" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="G301" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H301" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="I301" s="38">
+        <v>298</v>
+      </c>
+      <c r="J301" s="58">
+        <v>619000000</v>
+      </c>
       <c r="K301" s="44"/>
-      <c r="L301" s="57"/>
-      <c r="M301" s="57"/>
-      <c r="N301" s="40"/>
+      <c r="L301" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="M301" s="57" t="s">
+        <v>357</v>
+      </c>
+      <c r="N301" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O301" s="44"/>
       <c r="P301" s="44"/>
       <c r="Q301" s="44"/>
@@ -17054,19 +17251,43 @@
     </row>
     <row r="302" spans="1:20" ht="18" customHeight="1">
       <c r="A302" s="57"/>
-      <c r="B302" s="57"/>
-      <c r="C302" s="57"/>
-      <c r="D302" s="57"/>
-      <c r="E302" s="55"/>
-      <c r="F302" s="57"/>
-      <c r="G302" s="32"/>
-      <c r="H302" s="57"/>
-      <c r="I302" s="38"/>
-      <c r="J302" s="58"/>
+      <c r="B302" s="57" t="s">
+        <v>350</v>
+      </c>
+      <c r="C302" s="57" t="s">
+        <v>160</v>
+      </c>
+      <c r="D302" s="57" t="s">
+        <v>353</v>
+      </c>
+      <c r="E302" s="55" t="s">
+        <v>354</v>
+      </c>
+      <c r="F302" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="G302" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H302" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="I302" s="38">
+        <v>298</v>
+      </c>
+      <c r="J302" s="58">
+        <v>655000000</v>
+      </c>
       <c r="K302" s="44"/>
-      <c r="L302" s="57"/>
-      <c r="M302" s="57"/>
-      <c r="N302" s="40"/>
+      <c r="L302" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="M302" s="57" t="s">
+        <v>357</v>
+      </c>
+      <c r="N302" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O302" s="44"/>
       <c r="P302" s="44"/>
       <c r="Q302" s="44"/>
@@ -17076,19 +17297,43 @@
     </row>
     <row r="303" spans="1:20" ht="18" customHeight="1">
       <c r="A303" s="93"/>
-      <c r="B303" s="94"/>
-      <c r="C303" s="94"/>
-      <c r="D303" s="94"/>
-      <c r="E303" s="106"/>
-      <c r="F303" s="94"/>
-      <c r="G303" s="97"/>
-      <c r="H303" s="57"/>
-      <c r="I303" s="107"/>
-      <c r="J303" s="58"/>
+      <c r="B303" s="57" t="s">
+        <v>351</v>
+      </c>
+      <c r="C303" s="57" t="s">
+        <v>160</v>
+      </c>
+      <c r="D303" s="57" t="s">
+        <v>353</v>
+      </c>
+      <c r="E303" s="55" t="s">
+        <v>354</v>
+      </c>
+      <c r="F303" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="G303" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H303" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="I303" s="38">
+        <v>298</v>
+      </c>
+      <c r="J303" s="58">
+        <v>724000000</v>
+      </c>
       <c r="K303" s="44"/>
-      <c r="L303" s="57"/>
-      <c r="M303" s="57"/>
-      <c r="N303" s="40"/>
+      <c r="L303" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="M303" s="57" t="s">
+        <v>357</v>
+      </c>
+      <c r="N303" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O303" s="44"/>
       <c r="P303" s="44"/>
       <c r="Q303" s="44"/>
@@ -17098,19 +17343,43 @@
     </row>
     <row r="304" spans="1:20" ht="18" customHeight="1">
       <c r="A304" s="95"/>
-      <c r="B304" s="96"/>
-      <c r="C304" s="96"/>
-      <c r="D304" s="96"/>
-      <c r="E304" s="108"/>
-      <c r="F304" s="94"/>
-      <c r="G304" s="98"/>
-      <c r="H304" s="57"/>
-      <c r="I304" s="109"/>
-      <c r="J304" s="58"/>
+      <c r="B304" s="57" t="s">
+        <v>352</v>
+      </c>
+      <c r="C304" s="57" t="s">
+        <v>160</v>
+      </c>
+      <c r="D304" s="57" t="s">
+        <v>353</v>
+      </c>
+      <c r="E304" s="55" t="s">
+        <v>354</v>
+      </c>
+      <c r="F304" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="G304" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H304" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="I304" s="38">
+        <v>298</v>
+      </c>
+      <c r="J304" s="58">
+        <v>820000000</v>
+      </c>
       <c r="K304" s="44"/>
-      <c r="L304" s="57"/>
-      <c r="M304" s="57"/>
-      <c r="N304" s="40"/>
+      <c r="L304" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="M304" s="57" t="s">
+        <v>357</v>
+      </c>
+      <c r="N304" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O304" s="44"/>
       <c r="P304" s="44"/>
       <c r="Q304" s="44"/>
@@ -17120,19 +17389,43 @@
     </row>
     <row r="305" spans="1:20" ht="18" customHeight="1">
       <c r="A305" s="95"/>
-      <c r="B305" s="96"/>
-      <c r="C305" s="96"/>
-      <c r="D305" s="96"/>
-      <c r="E305" s="108"/>
-      <c r="F305" s="94"/>
-      <c r="G305" s="98"/>
-      <c r="H305" s="57"/>
-      <c r="I305" s="109"/>
-      <c r="J305" s="58"/>
+      <c r="B305" s="57" t="s">
+        <v>348</v>
+      </c>
+      <c r="C305" s="57" t="s">
+        <v>160</v>
+      </c>
+      <c r="D305" s="57" t="s">
+        <v>353</v>
+      </c>
+      <c r="E305" s="55" t="s">
+        <v>354</v>
+      </c>
+      <c r="F305" s="94" t="s">
+        <v>70</v>
+      </c>
+      <c r="G305" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H305" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="I305" s="38">
+        <v>298</v>
+      </c>
+      <c r="J305" s="58">
+        <v>627000000</v>
+      </c>
       <c r="K305" s="44"/>
-      <c r="L305" s="57"/>
-      <c r="M305" s="57"/>
-      <c r="N305" s="40"/>
+      <c r="L305" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="M305" s="57" t="s">
+        <v>358</v>
+      </c>
+      <c r="N305" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O305" s="44"/>
       <c r="P305" s="44"/>
       <c r="Q305" s="44"/>
@@ -17142,19 +17435,43 @@
     </row>
     <row r="306" spans="1:20" ht="18" customHeight="1">
       <c r="A306" s="93"/>
-      <c r="B306" s="94"/>
-      <c r="C306" s="94"/>
-      <c r="D306" s="94"/>
-      <c r="E306" s="106"/>
-      <c r="F306" s="94"/>
-      <c r="G306" s="97"/>
-      <c r="H306" s="57"/>
-      <c r="I306" s="107"/>
-      <c r="J306" s="44"/>
+      <c r="B306" s="57" t="s">
+        <v>349</v>
+      </c>
+      <c r="C306" s="57" t="s">
+        <v>160</v>
+      </c>
+      <c r="D306" s="57" t="s">
+        <v>353</v>
+      </c>
+      <c r="E306" s="55" t="s">
+        <v>354</v>
+      </c>
+      <c r="F306" s="94" t="s">
+        <v>70</v>
+      </c>
+      <c r="G306" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H306" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="I306" s="38">
+        <v>298</v>
+      </c>
+      <c r="J306" s="58">
+        <v>658000000</v>
+      </c>
       <c r="K306" s="44"/>
-      <c r="L306" s="57"/>
-      <c r="M306" s="57"/>
-      <c r="N306" s="40"/>
+      <c r="L306" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="M306" s="57" t="s">
+        <v>358</v>
+      </c>
+      <c r="N306" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O306" s="44"/>
       <c r="P306" s="44"/>
       <c r="Q306" s="44"/>
@@ -17164,19 +17481,43 @@
     </row>
     <row r="307" spans="1:20" ht="18" customHeight="1">
       <c r="A307" s="95"/>
-      <c r="B307" s="96"/>
-      <c r="C307" s="96"/>
-      <c r="D307" s="96"/>
-      <c r="E307" s="108"/>
-      <c r="F307" s="94"/>
-      <c r="G307" s="98"/>
-      <c r="H307" s="57"/>
-      <c r="I307" s="109"/>
-      <c r="J307" s="44"/>
+      <c r="B307" s="57" t="s">
+        <v>350</v>
+      </c>
+      <c r="C307" s="57" t="s">
+        <v>160</v>
+      </c>
+      <c r="D307" s="57" t="s">
+        <v>353</v>
+      </c>
+      <c r="E307" s="55" t="s">
+        <v>354</v>
+      </c>
+      <c r="F307" s="94" t="s">
+        <v>70</v>
+      </c>
+      <c r="G307" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H307" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="I307" s="38">
+        <v>298</v>
+      </c>
+      <c r="J307" s="58">
+        <v>737000000</v>
+      </c>
       <c r="K307" s="44"/>
-      <c r="L307" s="57"/>
-      <c r="M307" s="57"/>
-      <c r="N307" s="40"/>
+      <c r="L307" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="M307" s="57" t="s">
+        <v>358</v>
+      </c>
+      <c r="N307" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O307" s="44"/>
       <c r="P307" s="44"/>
       <c r="Q307" s="44"/>
@@ -17186,19 +17527,43 @@
     </row>
     <row r="308" spans="1:20" ht="18" customHeight="1">
       <c r="A308" s="95"/>
-      <c r="B308" s="96"/>
-      <c r="C308" s="96"/>
-      <c r="D308" s="96"/>
-      <c r="E308" s="108"/>
-      <c r="F308" s="94"/>
-      <c r="G308" s="98"/>
-      <c r="H308" s="57"/>
-      <c r="I308" s="109"/>
-      <c r="J308" s="44"/>
+      <c r="B308" s="57" t="s">
+        <v>351</v>
+      </c>
+      <c r="C308" s="57" t="s">
+        <v>160</v>
+      </c>
+      <c r="D308" s="57" t="s">
+        <v>353</v>
+      </c>
+      <c r="E308" s="55" t="s">
+        <v>354</v>
+      </c>
+      <c r="F308" s="94" t="s">
+        <v>70</v>
+      </c>
+      <c r="G308" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H308" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="I308" s="38">
+        <v>298</v>
+      </c>
+      <c r="J308" s="58">
+        <v>761000000</v>
+      </c>
       <c r="K308" s="44"/>
-      <c r="L308" s="57"/>
-      <c r="M308" s="57"/>
-      <c r="N308" s="40"/>
+      <c r="L308" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="M308" s="57" t="s">
+        <v>358</v>
+      </c>
+      <c r="N308" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O308" s="44"/>
       <c r="P308" s="44"/>
       <c r="Q308" s="44"/>
@@ -17208,19 +17573,43 @@
     </row>
     <row r="309" spans="1:20" ht="18" customHeight="1">
       <c r="A309" s="57"/>
-      <c r="B309" s="57"/>
-      <c r="C309" s="57"/>
-      <c r="D309" s="57"/>
-      <c r="E309" s="55"/>
-      <c r="F309" s="57"/>
-      <c r="G309" s="32"/>
-      <c r="H309" s="44"/>
-      <c r="I309" s="38"/>
-      <c r="J309" s="44"/>
+      <c r="B309" s="57" t="s">
+        <v>352</v>
+      </c>
+      <c r="C309" s="57" t="s">
+        <v>160</v>
+      </c>
+      <c r="D309" s="57" t="s">
+        <v>353</v>
+      </c>
+      <c r="E309" s="55" t="s">
+        <v>354</v>
+      </c>
+      <c r="F309" s="94" t="s">
+        <v>70</v>
+      </c>
+      <c r="G309" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H309" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="I309" s="38">
+        <v>298</v>
+      </c>
+      <c r="J309" s="58">
+        <v>810000000</v>
+      </c>
       <c r="K309" s="44"/>
-      <c r="L309" s="57"/>
-      <c r="M309" s="57"/>
-      <c r="N309" s="40"/>
+      <c r="L309" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="M309" s="57" t="s">
+        <v>358</v>
+      </c>
+      <c r="N309" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O309" s="44"/>
       <c r="P309" s="44"/>
       <c r="Q309" s="44"/>
@@ -17230,19 +17619,43 @@
     </row>
     <row r="310" spans="1:20" ht="18" customHeight="1">
       <c r="A310" s="57"/>
-      <c r="B310" s="57"/>
-      <c r="C310" s="57"/>
-      <c r="D310" s="57"/>
-      <c r="E310" s="55"/>
-      <c r="F310" s="57"/>
-      <c r="G310" s="32"/>
-      <c r="H310" s="44"/>
-      <c r="I310" s="38"/>
-      <c r="J310" s="44"/>
+      <c r="B310" s="93" t="s">
+        <v>348</v>
+      </c>
+      <c r="C310" s="94" t="s">
+        <v>160</v>
+      </c>
+      <c r="D310" s="94" t="s">
+        <v>353</v>
+      </c>
+      <c r="E310" s="106" t="s">
+        <v>354</v>
+      </c>
+      <c r="F310" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="G310" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H310" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="I310" s="38">
+        <v>298</v>
+      </c>
+      <c r="J310" s="44">
+        <v>20.5</v>
+      </c>
       <c r="K310" s="44"/>
-      <c r="L310" s="57"/>
-      <c r="M310" s="57"/>
-      <c r="N310" s="40"/>
+      <c r="L310" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="M310" s="57" t="s">
+        <v>356</v>
+      </c>
+      <c r="N310" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O310" s="44"/>
       <c r="P310" s="44"/>
       <c r="Q310" s="44"/>
@@ -17252,19 +17665,43 @@
     </row>
     <row r="311" spans="1:20" ht="18" customHeight="1">
       <c r="A311" s="57"/>
-      <c r="B311" s="57"/>
-      <c r="C311" s="57"/>
-      <c r="D311" s="57"/>
-      <c r="E311" s="55"/>
-      <c r="F311" s="57"/>
-      <c r="G311" s="32"/>
-      <c r="H311" s="44"/>
-      <c r="I311" s="38"/>
-      <c r="J311" s="44"/>
+      <c r="B311" s="95" t="s">
+        <v>349</v>
+      </c>
+      <c r="C311" s="96" t="s">
+        <v>160</v>
+      </c>
+      <c r="D311" s="96" t="s">
+        <v>353</v>
+      </c>
+      <c r="E311" s="107" t="s">
+        <v>354</v>
+      </c>
+      <c r="F311" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="G311" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H311" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="I311" s="38">
+        <v>298</v>
+      </c>
+      <c r="J311" s="44">
+        <v>22</v>
+      </c>
       <c r="K311" s="44"/>
-      <c r="L311" s="57"/>
-      <c r="M311" s="57"/>
-      <c r="N311" s="40"/>
+      <c r="L311" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="M311" s="57" t="s">
+        <v>356</v>
+      </c>
+      <c r="N311" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O311" s="44"/>
       <c r="P311" s="44"/>
       <c r="Q311" s="44"/>
@@ -17274,19 +17711,43 @@
     </row>
     <row r="312" spans="1:20" ht="18" customHeight="1">
       <c r="A312" s="57"/>
-      <c r="B312" s="57"/>
-      <c r="C312" s="57"/>
-      <c r="D312" s="57"/>
-      <c r="E312" s="55"/>
-      <c r="F312" s="57"/>
-      <c r="G312" s="32"/>
-      <c r="H312" s="44"/>
-      <c r="I312" s="38"/>
-      <c r="J312" s="44"/>
+      <c r="B312" s="95" t="s">
+        <v>350</v>
+      </c>
+      <c r="C312" s="96" t="s">
+        <v>160</v>
+      </c>
+      <c r="D312" s="96" t="s">
+        <v>353</v>
+      </c>
+      <c r="E312" s="107" t="s">
+        <v>354</v>
+      </c>
+      <c r="F312" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="G312" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H312" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="I312" s="38">
+        <v>298</v>
+      </c>
+      <c r="J312" s="44">
+        <v>17</v>
+      </c>
       <c r="K312" s="44"/>
-      <c r="L312" s="57"/>
-      <c r="M312" s="57"/>
-      <c r="N312" s="40"/>
+      <c r="L312" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="M312" s="57" t="s">
+        <v>356</v>
+      </c>
+      <c r="N312" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O312" s="44"/>
       <c r="P312" s="44"/>
       <c r="Q312" s="44"/>
@@ -17296,19 +17757,43 @@
     </row>
     <row r="313" spans="1:20" ht="18" customHeight="1">
       <c r="A313" s="57"/>
-      <c r="B313" s="57"/>
-      <c r="C313" s="57"/>
-      <c r="D313" s="57"/>
-      <c r="E313" s="55"/>
-      <c r="F313" s="57"/>
-      <c r="G313" s="32"/>
-      <c r="H313" s="44"/>
-      <c r="I313" s="38"/>
-      <c r="J313" s="44"/>
+      <c r="B313" s="95" t="s">
+        <v>351</v>
+      </c>
+      <c r="C313" s="96" t="s">
+        <v>160</v>
+      </c>
+      <c r="D313" s="96" t="s">
+        <v>353</v>
+      </c>
+      <c r="E313" s="107" t="s">
+        <v>354</v>
+      </c>
+      <c r="F313" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="G313" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H313" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="I313" s="38">
+        <v>298</v>
+      </c>
+      <c r="J313" s="44">
+        <v>15.5</v>
+      </c>
       <c r="K313" s="44"/>
-      <c r="L313" s="57"/>
-      <c r="M313" s="57"/>
-      <c r="N313" s="40"/>
+      <c r="L313" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="M313" s="57" t="s">
+        <v>356</v>
+      </c>
+      <c r="N313" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O313" s="44"/>
       <c r="P313" s="44"/>
       <c r="Q313" s="44"/>
@@ -17318,19 +17803,43 @@
     </row>
     <row r="314" spans="1:20" ht="18" customHeight="1">
       <c r="A314" s="57"/>
-      <c r="B314" s="57"/>
-      <c r="C314" s="57"/>
-      <c r="D314" s="57"/>
-      <c r="E314" s="55"/>
-      <c r="F314" s="57"/>
-      <c r="G314" s="32"/>
-      <c r="H314" s="44"/>
-      <c r="I314" s="38"/>
-      <c r="J314" s="44"/>
+      <c r="B314" s="95" t="s">
+        <v>352</v>
+      </c>
+      <c r="C314" s="96" t="s">
+        <v>160</v>
+      </c>
+      <c r="D314" s="96" t="s">
+        <v>353</v>
+      </c>
+      <c r="E314" s="107" t="s">
+        <v>354</v>
+      </c>
+      <c r="F314" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="G314" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H314" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="I314" s="38">
+        <v>298</v>
+      </c>
+      <c r="J314" s="44">
+        <v>14</v>
+      </c>
       <c r="K314" s="44"/>
-      <c r="L314" s="57"/>
-      <c r="M314" s="57"/>
-      <c r="N314" s="40"/>
+      <c r="L314" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="M314" s="57" t="s">
+        <v>356</v>
+      </c>
+      <c r="N314" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O314" s="44"/>
       <c r="P314" s="44"/>
       <c r="Q314" s="44"/>
@@ -17340,129 +17849,306 @@
     </row>
     <row r="315" spans="1:20" ht="18" customHeight="1">
       <c r="A315" s="57"/>
-      <c r="B315" s="57"/>
-      <c r="C315" s="57"/>
-      <c r="D315" s="57"/>
-      <c r="E315" s="55"/>
-      <c r="F315" s="57"/>
-      <c r="G315" s="32"/>
-      <c r="H315" s="44"/>
-      <c r="I315" s="38"/>
-      <c r="J315" s="44"/>
-      <c r="K315" s="44"/>
-      <c r="L315" s="57"/>
-      <c r="M315" s="57"/>
-      <c r="N315" s="40"/>
+      <c r="B315" s="93" t="s">
+        <v>348</v>
+      </c>
+      <c r="C315" s="94" t="s">
+        <v>160</v>
+      </c>
+      <c r="D315" s="94" t="s">
+        <v>353</v>
+      </c>
+      <c r="E315" s="106" t="s">
+        <v>354</v>
+      </c>
+      <c r="F315" s="57" t="s">
+        <v>179</v>
+      </c>
+      <c r="G315" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H315" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="I315" s="38">
+        <v>298</v>
+      </c>
+      <c r="J315" s="35">
+        <f t="shared" ref="J315:K319" si="10">P315*9807000</f>
+        <v>2132002027.7481291</v>
+      </c>
+      <c r="K315" s="35">
+        <f>(Q315-Q314)*9807000</f>
+        <v>2171250960.5122676</v>
+      </c>
+      <c r="L315" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="M315" s="57" t="s">
+        <v>359</v>
+      </c>
+      <c r="N315" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O315" s="44"/>
-      <c r="P315" s="44"/>
-      <c r="Q315" s="44"/>
+      <c r="P315" s="44">
+        <v>217.395944503735</v>
+      </c>
+      <c r="Q315" s="44">
+        <v>221.39807897545299</v>
+      </c>
       <c r="R315" s="44"/>
       <c r="S315" s="37"/>
       <c r="T315" s="37"/>
     </row>
     <row r="316" spans="1:20" ht="18" customHeight="1">
       <c r="A316" s="57"/>
-      <c r="B316" s="57"/>
-      <c r="C316" s="57"/>
-      <c r="D316" s="57"/>
-      <c r="E316" s="55"/>
-      <c r="F316" s="57"/>
-      <c r="G316" s="32"/>
-      <c r="H316" s="44"/>
-      <c r="I316" s="38"/>
-      <c r="J316" s="44"/>
-      <c r="K316" s="44"/>
-      <c r="L316" s="57"/>
-      <c r="M316" s="57"/>
-      <c r="N316" s="40"/>
+      <c r="B316" s="95" t="s">
+        <v>349</v>
+      </c>
+      <c r="C316" s="96" t="s">
+        <v>160</v>
+      </c>
+      <c r="D316" s="96" t="s">
+        <v>353</v>
+      </c>
+      <c r="E316" s="107" t="s">
+        <v>354</v>
+      </c>
+      <c r="F316" s="57" t="s">
+        <v>179</v>
+      </c>
+      <c r="G316" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H316" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="I316" s="38">
+        <v>298</v>
+      </c>
+      <c r="J316" s="35">
+        <f t="shared" si="10"/>
+        <v>2228816061.8996763</v>
+      </c>
+      <c r="K316" s="35">
+        <f t="shared" ref="K316:K319" si="11">(Q316-Q315)*9807000</f>
+        <v>94197438.63394022</v>
+      </c>
+      <c r="L316" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="M316" s="57" t="s">
+        <v>359</v>
+      </c>
+      <c r="N316" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O316" s="44"/>
-      <c r="P316" s="44"/>
-      <c r="Q316" s="44"/>
+      <c r="P316" s="44">
+        <v>227.26787620063999</v>
+      </c>
+      <c r="Q316" s="44">
+        <v>231.00320170757701</v>
+      </c>
       <c r="R316" s="44"/>
       <c r="S316" s="37"/>
       <c r="T316" s="37"/>
     </row>
     <row r="317" spans="1:20" ht="18" customHeight="1">
       <c r="A317" s="57"/>
-      <c r="B317" s="57"/>
-      <c r="C317" s="57"/>
-      <c r="D317" s="57"/>
-      <c r="E317" s="55"/>
-      <c r="F317" s="57"/>
-      <c r="G317" s="32"/>
-      <c r="H317" s="44"/>
-      <c r="I317" s="38"/>
-      <c r="J317" s="44"/>
-      <c r="K317" s="44"/>
-      <c r="L317" s="57"/>
-      <c r="M317" s="57"/>
-      <c r="N317" s="40"/>
+      <c r="B317" s="95" t="s">
+        <v>350</v>
+      </c>
+      <c r="C317" s="96" t="s">
+        <v>160</v>
+      </c>
+      <c r="D317" s="96" t="s">
+        <v>353</v>
+      </c>
+      <c r="E317" s="107" t="s">
+        <v>354</v>
+      </c>
+      <c r="F317" s="57" t="s">
+        <v>179</v>
+      </c>
+      <c r="G317" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H317" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="I317" s="38">
+        <v>298</v>
+      </c>
+      <c r="J317" s="35">
+        <f t="shared" si="10"/>
+        <v>2532341141.9423647</v>
+      </c>
+      <c r="K317" s="35">
+        <f t="shared" si="11"/>
+        <v>334924226.2540049</v>
+      </c>
+      <c r="L317" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="M317" s="57" t="s">
+        <v>359</v>
+      </c>
+      <c r="N317" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O317" s="44"/>
-      <c r="P317" s="44"/>
-      <c r="Q317" s="44"/>
+      <c r="P317" s="44">
+        <v>258.217716115261</v>
+      </c>
+      <c r="Q317" s="44">
+        <v>265.15474919957302</v>
+      </c>
       <c r="R317" s="44"/>
       <c r="S317" s="37"/>
       <c r="T317" s="37"/>
     </row>
     <row r="318" spans="1:20" ht="18" customHeight="1">
       <c r="A318" s="57"/>
-      <c r="B318" s="57"/>
-      <c r="C318" s="57"/>
-      <c r="D318" s="57"/>
-      <c r="E318" s="55"/>
-      <c r="F318" s="57"/>
-      <c r="G318" s="32"/>
-      <c r="H318" s="44"/>
-      <c r="I318" s="38"/>
-      <c r="J318" s="44"/>
-      <c r="K318" s="44"/>
-      <c r="L318" s="57"/>
-      <c r="M318" s="57"/>
-      <c r="N318" s="40"/>
+      <c r="B318" s="95" t="s">
+        <v>351</v>
+      </c>
+      <c r="C318" s="96" t="s">
+        <v>160</v>
+      </c>
+      <c r="D318" s="96" t="s">
+        <v>353</v>
+      </c>
+      <c r="E318" s="107" t="s">
+        <v>354</v>
+      </c>
+      <c r="F318" s="57" t="s">
+        <v>179</v>
+      </c>
+      <c r="G318" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H318" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="I318" s="38">
+        <v>298</v>
+      </c>
+      <c r="J318" s="35">
+        <f t="shared" si="10"/>
+        <v>2757368356.4567761</v>
+      </c>
+      <c r="K318" s="35">
+        <f t="shared" si="11"/>
+        <v>209327641.408748</v>
+      </c>
+      <c r="L318" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="M318" s="57" t="s">
+        <v>359</v>
+      </c>
+      <c r="N318" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O318" s="44"/>
-      <c r="P318" s="44"/>
-      <c r="Q318" s="44"/>
+      <c r="P318" s="44">
+        <v>281.16328708644602</v>
+      </c>
+      <c r="Q318" s="44">
+        <v>286.49946638207001</v>
+      </c>
       <c r="R318" s="44"/>
       <c r="S318" s="37"/>
       <c r="T318" s="37"/>
     </row>
     <row r="319" spans="1:20" ht="18" customHeight="1">
       <c r="A319" s="57"/>
-      <c r="B319" s="57"/>
-      <c r="C319" s="57"/>
-      <c r="D319" s="57"/>
-      <c r="E319" s="57"/>
-      <c r="F319" s="57"/>
-      <c r="G319" s="32"/>
-      <c r="H319" s="44"/>
-      <c r="I319" s="44"/>
-      <c r="J319" s="44"/>
-      <c r="K319" s="44"/>
-      <c r="L319" s="57"/>
-      <c r="M319" s="57"/>
-      <c r="N319" s="57"/>
+      <c r="B319" s="95" t="s">
+        <v>352</v>
+      </c>
+      <c r="C319" s="96" t="s">
+        <v>160</v>
+      </c>
+      <c r="D319" s="96" t="s">
+        <v>353</v>
+      </c>
+      <c r="E319" s="107" t="s">
+        <v>354</v>
+      </c>
+      <c r="F319" s="57" t="s">
+        <v>179</v>
+      </c>
+      <c r="G319" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H319" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="I319" s="38">
+        <v>298</v>
+      </c>
+      <c r="J319" s="35">
+        <f t="shared" si="10"/>
+        <v>2940530042.6894317</v>
+      </c>
+      <c r="K319" s="35">
+        <f t="shared" si="11"/>
+        <v>240726787.62006438</v>
+      </c>
+      <c r="L319" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="M319" s="57" t="s">
+        <v>359</v>
+      </c>
+      <c r="N319" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O319" s="44"/>
-      <c r="P319" s="44"/>
-      <c r="Q319" s="44"/>
+      <c r="P319" s="44">
+        <v>299.83991462113102</v>
+      </c>
+      <c r="Q319" s="44">
+        <v>311.04589114194198</v>
+      </c>
       <c r="R319" s="44"/>
       <c r="S319" s="37"/>
       <c r="T319" s="37"/>
     </row>
     <row r="320" spans="1:20" ht="18" customHeight="1">
       <c r="A320" s="57"/>
-      <c r="B320" s="57"/>
-      <c r="C320" s="57"/>
+      <c r="B320" s="93" t="s">
+        <v>348</v>
+      </c>
+      <c r="C320" s="94" t="s">
+        <v>160</v>
+      </c>
       <c r="D320" s="57"/>
-      <c r="E320" s="57"/>
-      <c r="F320" s="57"/>
-      <c r="G320" s="32"/>
+      <c r="E320" s="57" t="s">
+        <v>360</v>
+      </c>
+      <c r="F320" s="57" t="s">
+        <v>361</v>
+      </c>
+      <c r="G320" s="32" t="s">
+        <v>144</v>
+      </c>
       <c r="H320" s="57"/>
       <c r="I320" s="44"/>
-      <c r="J320" s="44"/>
+      <c r="J320" s="44">
+        <f>105/23</f>
+        <v>4.5652173913043477</v>
+      </c>
       <c r="K320" s="44"/>
       <c r="L320" s="57"/>
-      <c r="M320" s="57"/>
-      <c r="N320" s="57"/>
+      <c r="M320" s="57" t="s">
+        <v>363</v>
+      </c>
+      <c r="N320" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O320" s="44"/>
       <c r="P320" s="44"/>
       <c r="Q320" s="44"/>
@@ -17472,19 +18158,36 @@
     </row>
     <row r="321" spans="1:20" ht="18" customHeight="1">
       <c r="A321" s="57"/>
-      <c r="B321" s="57"/>
-      <c r="C321" s="57"/>
+      <c r="B321" s="95" t="s">
+        <v>349</v>
+      </c>
+      <c r="C321" s="96" t="s">
+        <v>160</v>
+      </c>
       <c r="D321" s="57"/>
-      <c r="E321" s="57"/>
-      <c r="F321" s="57"/>
-      <c r="G321" s="32"/>
+      <c r="E321" s="57" t="s">
+        <v>360</v>
+      </c>
+      <c r="F321" s="57" t="s">
+        <v>361</v>
+      </c>
+      <c r="G321" s="32" t="s">
+        <v>144</v>
+      </c>
       <c r="H321" s="57"/>
       <c r="I321" s="44"/>
-      <c r="J321" s="44"/>
+      <c r="J321" s="44">
+        <f t="shared" ref="J321:J324" si="12">105/23</f>
+        <v>4.5652173913043477</v>
+      </c>
       <c r="K321" s="48"/>
       <c r="L321" s="57"/>
-      <c r="M321" s="57"/>
-      <c r="N321" s="57"/>
+      <c r="M321" s="57" t="s">
+        <v>363</v>
+      </c>
+      <c r="N321" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O321" s="44"/>
       <c r="P321" s="44"/>
       <c r="Q321" s="44"/>
@@ -17494,19 +18197,36 @@
     </row>
     <row r="322" spans="1:20" ht="18" customHeight="1">
       <c r="A322" s="57"/>
-      <c r="B322" s="57"/>
-      <c r="C322" s="57"/>
+      <c r="B322" s="95" t="s">
+        <v>350</v>
+      </c>
+      <c r="C322" s="96" t="s">
+        <v>160</v>
+      </c>
       <c r="D322" s="57"/>
-      <c r="E322" s="57"/>
-      <c r="F322" s="57"/>
-      <c r="G322" s="32"/>
+      <c r="E322" s="57" t="s">
+        <v>360</v>
+      </c>
+      <c r="F322" s="57" t="s">
+        <v>361</v>
+      </c>
+      <c r="G322" s="32" t="s">
+        <v>144</v>
+      </c>
       <c r="H322" s="57"/>
       <c r="I322" s="44"/>
-      <c r="J322" s="44"/>
+      <c r="J322" s="44">
+        <f>105/21</f>
+        <v>5</v>
+      </c>
       <c r="K322" s="48"/>
       <c r="L322" s="57"/>
-      <c r="M322" s="57"/>
-      <c r="N322" s="57"/>
+      <c r="M322" s="57" t="s">
+        <v>363</v>
+      </c>
+      <c r="N322" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O322" s="44"/>
       <c r="P322" s="44"/>
       <c r="Q322" s="44"/>
@@ -17516,19 +18236,36 @@
     </row>
     <row r="323" spans="1:20" ht="18" customHeight="1">
       <c r="A323" s="57"/>
-      <c r="B323" s="57"/>
-      <c r="C323" s="57"/>
+      <c r="B323" s="95" t="s">
+        <v>351</v>
+      </c>
+      <c r="C323" s="96" t="s">
+        <v>160</v>
+      </c>
       <c r="D323" s="57"/>
-      <c r="E323" s="57"/>
-      <c r="F323" s="57"/>
-      <c r="G323" s="32"/>
+      <c r="E323" s="57" t="s">
+        <v>360</v>
+      </c>
+      <c r="F323" s="57" t="s">
+        <v>361</v>
+      </c>
+      <c r="G323" s="32" t="s">
+        <v>144</v>
+      </c>
       <c r="H323" s="44"/>
       <c r="I323" s="44"/>
-      <c r="J323" s="44"/>
+      <c r="J323" s="44">
+        <f>103/22</f>
+        <v>4.6818181818181817</v>
+      </c>
       <c r="K323" s="48"/>
       <c r="L323" s="57"/>
-      <c r="M323" s="57"/>
-      <c r="N323" s="57"/>
+      <c r="M323" s="57" t="s">
+        <v>363</v>
+      </c>
+      <c r="N323" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O323" s="44"/>
       <c r="P323" s="44"/>
       <c r="Q323" s="44"/>
@@ -17538,19 +18275,36 @@
     </row>
     <row r="324" spans="1:20" ht="18" customHeight="1">
       <c r="A324" s="57"/>
-      <c r="B324" s="57"/>
-      <c r="C324" s="57"/>
+      <c r="B324" s="95" t="s">
+        <v>352</v>
+      </c>
+      <c r="C324" s="96" t="s">
+        <v>160</v>
+      </c>
       <c r="D324" s="57"/>
-      <c r="E324" s="57"/>
-      <c r="F324" s="57"/>
-      <c r="G324" s="32"/>
+      <c r="E324" s="57" t="s">
+        <v>360</v>
+      </c>
+      <c r="F324" s="57" t="s">
+        <v>361</v>
+      </c>
+      <c r="G324" s="32" t="s">
+        <v>144</v>
+      </c>
       <c r="H324" s="44"/>
       <c r="I324" s="44"/>
-      <c r="J324" s="44"/>
+      <c r="J324" s="44">
+        <f>103/24</f>
+        <v>4.291666666666667</v>
+      </c>
       <c r="K324" s="48"/>
       <c r="L324" s="57"/>
-      <c r="M324" s="57"/>
-      <c r="N324" s="57"/>
+      <c r="M324" s="57" t="s">
+        <v>363</v>
+      </c>
+      <c r="N324" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O324" s="44"/>
       <c r="P324" s="44"/>
       <c r="Q324" s="44"/>
@@ -17560,19 +18314,37 @@
     </row>
     <row r="325" spans="1:20" ht="18" customHeight="1">
       <c r="A325" s="57"/>
-      <c r="B325" s="57"/>
-      <c r="C325" s="57"/>
+      <c r="B325" s="93" t="s">
+        <v>348</v>
+      </c>
+      <c r="C325" s="94" t="s">
+        <v>160</v>
+      </c>
       <c r="D325" s="57"/>
-      <c r="E325" s="57"/>
-      <c r="F325" s="57"/>
-      <c r="G325" s="32"/>
+      <c r="E325" s="57" t="s">
+        <v>360</v>
+      </c>
+      <c r="F325" s="57" t="s">
+        <v>242</v>
+      </c>
+      <c r="G325" s="32" t="s">
+        <v>144</v>
+      </c>
       <c r="H325" s="44"/>
       <c r="I325" s="44"/>
-      <c r="J325" s="44"/>
+      <c r="J325" s="58">
+        <v>64000000000</v>
+      </c>
       <c r="K325" s="48"/>
-      <c r="L325" s="57"/>
-      <c r="M325" s="57"/>
-      <c r="N325" s="57"/>
+      <c r="L325" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="M325" s="57" t="s">
+        <v>363</v>
+      </c>
+      <c r="N325" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O325" s="44"/>
       <c r="P325" s="44"/>
       <c r="Q325" s="44"/>
@@ -17582,19 +18354,37 @@
     </row>
     <row r="326" spans="1:20" ht="18" customHeight="1">
       <c r="A326" s="57"/>
-      <c r="B326" s="57"/>
-      <c r="C326" s="57"/>
+      <c r="B326" s="95" t="s">
+        <v>349</v>
+      </c>
+      <c r="C326" s="96" t="s">
+        <v>160</v>
+      </c>
       <c r="D326" s="57"/>
-      <c r="E326" s="57"/>
-      <c r="F326" s="57"/>
-      <c r="G326" s="32"/>
+      <c r="E326" s="57" t="s">
+        <v>360</v>
+      </c>
+      <c r="F326" s="57" t="s">
+        <v>242</v>
+      </c>
+      <c r="G326" s="32" t="s">
+        <v>144</v>
+      </c>
       <c r="H326" s="44"/>
       <c r="I326" s="44"/>
-      <c r="J326" s="44"/>
+      <c r="J326" s="58">
+        <v>63000000000</v>
+      </c>
       <c r="K326" s="48"/>
-      <c r="L326" s="57"/>
-      <c r="M326" s="57"/>
-      <c r="N326" s="57"/>
+      <c r="L326" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="M326" s="57" t="s">
+        <v>363</v>
+      </c>
+      <c r="N326" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O326" s="44"/>
       <c r="P326" s="44"/>
       <c r="Q326" s="44"/>
@@ -17604,19 +18394,37 @@
     </row>
     <row r="327" spans="1:20" ht="18" customHeight="1">
       <c r="A327" s="57"/>
-      <c r="B327" s="57"/>
-      <c r="C327" s="57"/>
+      <c r="B327" s="95" t="s">
+        <v>350</v>
+      </c>
+      <c r="C327" s="96" t="s">
+        <v>160</v>
+      </c>
       <c r="D327" s="57"/>
-      <c r="E327" s="57"/>
-      <c r="F327" s="57"/>
-      <c r="G327" s="32"/>
+      <c r="E327" s="57" t="s">
+        <v>360</v>
+      </c>
+      <c r="F327" s="57" t="s">
+        <v>242</v>
+      </c>
+      <c r="G327" s="32" t="s">
+        <v>144</v>
+      </c>
       <c r="H327" s="44"/>
       <c r="I327" s="44"/>
-      <c r="J327" s="44"/>
+      <c r="J327" s="58">
+        <v>59000000000</v>
+      </c>
       <c r="K327" s="48"/>
-      <c r="L327" s="57"/>
-      <c r="M327" s="57"/>
-      <c r="N327" s="57"/>
+      <c r="L327" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="M327" s="57" t="s">
+        <v>363</v>
+      </c>
+      <c r="N327" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O327" s="44"/>
       <c r="P327" s="44"/>
       <c r="Q327" s="44"/>
@@ -17626,19 +18434,37 @@
     </row>
     <row r="328" spans="1:20" ht="18" customHeight="1">
       <c r="A328" s="57"/>
-      <c r="B328" s="57"/>
-      <c r="C328" s="57"/>
+      <c r="B328" s="95" t="s">
+        <v>351</v>
+      </c>
+      <c r="C328" s="96" t="s">
+        <v>160</v>
+      </c>
       <c r="D328" s="57"/>
-      <c r="E328" s="57"/>
-      <c r="F328" s="57"/>
-      <c r="G328" s="32"/>
+      <c r="E328" s="57" t="s">
+        <v>360</v>
+      </c>
+      <c r="F328" s="57" t="s">
+        <v>242</v>
+      </c>
+      <c r="G328" s="32" t="s">
+        <v>144</v>
+      </c>
       <c r="H328" s="44"/>
       <c r="I328" s="44"/>
-      <c r="J328" s="44"/>
+      <c r="J328" s="58">
+        <v>60000000</v>
+      </c>
       <c r="K328" s="48"/>
-      <c r="L328" s="57"/>
-      <c r="M328" s="57"/>
-      <c r="N328" s="57"/>
+      <c r="L328" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="M328" s="57" t="s">
+        <v>363</v>
+      </c>
+      <c r="N328" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O328" s="44"/>
       <c r="P328" s="44"/>
       <c r="Q328" s="44"/>
@@ -17648,19 +18474,37 @@
     </row>
     <row r="329" spans="1:20" ht="18" customHeight="1">
       <c r="A329" s="57"/>
-      <c r="B329" s="57"/>
-      <c r="C329" s="57"/>
+      <c r="B329" s="95" t="s">
+        <v>352</v>
+      </c>
+      <c r="C329" s="96" t="s">
+        <v>160</v>
+      </c>
       <c r="D329" s="57"/>
-      <c r="E329" s="57"/>
-      <c r="F329" s="57"/>
-      <c r="G329" s="32"/>
+      <c r="E329" s="57" t="s">
+        <v>360</v>
+      </c>
+      <c r="F329" s="57" t="s">
+        <v>242</v>
+      </c>
+      <c r="G329" s="32" t="s">
+        <v>144</v>
+      </c>
       <c r="H329" s="44"/>
       <c r="I329" s="44"/>
-      <c r="J329" s="44"/>
+      <c r="J329" s="58">
+        <v>68000000000</v>
+      </c>
       <c r="K329" s="48"/>
-      <c r="L329" s="57"/>
-      <c r="M329" s="57"/>
-      <c r="N329" s="57"/>
+      <c r="L329" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="M329" s="57" t="s">
+        <v>363</v>
+      </c>
+      <c r="N329" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O329" s="44"/>
       <c r="P329" s="44"/>
       <c r="Q329" s="44"/>
@@ -17670,19 +18514,35 @@
     </row>
     <row r="330" spans="1:20" ht="18" customHeight="1">
       <c r="A330" s="57"/>
-      <c r="B330" s="57"/>
-      <c r="C330" s="57"/>
-      <c r="D330" s="57"/>
-      <c r="E330" s="57"/>
-      <c r="F330" s="57"/>
-      <c r="G330" s="32"/>
+      <c r="B330" s="93" t="s">
+        <v>348</v>
+      </c>
+      <c r="C330" s="94" t="s">
+        <v>160</v>
+      </c>
+      <c r="D330" s="94"/>
+      <c r="E330" s="94" t="s">
+        <v>360</v>
+      </c>
+      <c r="F330" s="94" t="s">
+        <v>362</v>
+      </c>
+      <c r="G330" s="97" t="s">
+        <v>144</v>
+      </c>
       <c r="H330" s="44"/>
       <c r="I330" s="44"/>
-      <c r="J330" s="44"/>
+      <c r="J330" s="44">
+        <v>0.39900000000000002</v>
+      </c>
       <c r="K330" s="48"/>
       <c r="L330" s="57"/>
-      <c r="M330" s="57"/>
-      <c r="N330" s="57"/>
+      <c r="M330" s="57" t="s">
+        <v>363</v>
+      </c>
+      <c r="N330" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O330" s="44"/>
       <c r="P330" s="44"/>
       <c r="Q330" s="44"/>
@@ -17692,19 +18552,35 @@
     </row>
     <row r="331" spans="1:20" ht="18" customHeight="1">
       <c r="A331" s="57"/>
-      <c r="B331" s="57"/>
-      <c r="C331" s="57"/>
-      <c r="D331" s="57"/>
-      <c r="E331" s="57"/>
-      <c r="F331" s="57"/>
-      <c r="G331" s="32"/>
+      <c r="B331" s="95" t="s">
+        <v>349</v>
+      </c>
+      <c r="C331" s="96" t="s">
+        <v>160</v>
+      </c>
+      <c r="D331" s="96"/>
+      <c r="E331" s="96" t="s">
+        <v>360</v>
+      </c>
+      <c r="F331" s="94" t="s">
+        <v>362</v>
+      </c>
+      <c r="G331" s="98" t="s">
+        <v>144</v>
+      </c>
       <c r="H331" s="44"/>
       <c r="I331" s="44"/>
-      <c r="J331" s="44"/>
+      <c r="J331" s="44">
+        <v>0.39900000000000002</v>
+      </c>
       <c r="K331" s="48"/>
       <c r="L331" s="57"/>
-      <c r="M331" s="57"/>
-      <c r="N331" s="57"/>
+      <c r="M331" s="57" t="s">
+        <v>363</v>
+      </c>
+      <c r="N331" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O331" s="44"/>
       <c r="P331" s="44"/>
       <c r="Q331" s="44"/>
@@ -17714,19 +18590,35 @@
     </row>
     <row r="332" spans="1:20" ht="18" customHeight="1">
       <c r="A332" s="57"/>
-      <c r="B332" s="57"/>
-      <c r="C332" s="57"/>
-      <c r="D332" s="57"/>
-      <c r="E332" s="57"/>
-      <c r="F332" s="57"/>
-      <c r="G332" s="32"/>
+      <c r="B332" s="95" t="s">
+        <v>350</v>
+      </c>
+      <c r="C332" s="96" t="s">
+        <v>160</v>
+      </c>
+      <c r="D332" s="96"/>
+      <c r="E332" s="96" t="s">
+        <v>360</v>
+      </c>
+      <c r="F332" s="94" t="s">
+        <v>362</v>
+      </c>
+      <c r="G332" s="98" t="s">
+        <v>144</v>
+      </c>
       <c r="H332" s="44"/>
       <c r="I332" s="44"/>
-      <c r="J332" s="44"/>
+      <c r="J332" s="44">
+        <v>0.40600000000000003</v>
+      </c>
       <c r="K332" s="48"/>
       <c r="L332" s="57"/>
-      <c r="M332" s="57"/>
-      <c r="N332" s="57"/>
+      <c r="M332" s="57" t="s">
+        <v>363</v>
+      </c>
+      <c r="N332" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O332" s="44"/>
       <c r="P332" s="44"/>
       <c r="Q332" s="44"/>
@@ -17736,19 +18628,35 @@
     </row>
     <row r="333" spans="1:20" ht="18" customHeight="1">
       <c r="A333" s="57"/>
-      <c r="B333" s="57"/>
-      <c r="C333" s="57"/>
-      <c r="D333" s="57"/>
-      <c r="E333" s="57"/>
-      <c r="F333" s="57"/>
-      <c r="G333" s="32"/>
+      <c r="B333" s="95" t="s">
+        <v>351</v>
+      </c>
+      <c r="C333" s="96" t="s">
+        <v>160</v>
+      </c>
+      <c r="D333" s="96"/>
+      <c r="E333" s="96" t="s">
+        <v>360</v>
+      </c>
+      <c r="F333" s="94" t="s">
+        <v>362</v>
+      </c>
+      <c r="G333" s="98" t="s">
+        <v>144</v>
+      </c>
       <c r="H333" s="44"/>
       <c r="I333" s="44"/>
-      <c r="J333" s="44"/>
+      <c r="J333" s="44">
+        <v>0.40300000000000002</v>
+      </c>
       <c r="K333" s="48"/>
       <c r="L333" s="57"/>
-      <c r="M333" s="57"/>
-      <c r="N333" s="57"/>
+      <c r="M333" s="57" t="s">
+        <v>363</v>
+      </c>
+      <c r="N333" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O333" s="44"/>
       <c r="P333" s="44"/>
       <c r="Q333" s="44"/>
@@ -17758,19 +18666,35 @@
     </row>
     <row r="334" spans="1:20" ht="18" customHeight="1">
       <c r="A334" s="57"/>
-      <c r="B334" s="57"/>
-      <c r="C334" s="57"/>
-      <c r="D334" s="57"/>
-      <c r="E334" s="57"/>
-      <c r="F334" s="57"/>
-      <c r="G334" s="32"/>
+      <c r="B334" s="95" t="s">
+        <v>352</v>
+      </c>
+      <c r="C334" s="96" t="s">
+        <v>160</v>
+      </c>
+      <c r="D334" s="96"/>
+      <c r="E334" s="96" t="s">
+        <v>360</v>
+      </c>
+      <c r="F334" s="94" t="s">
+        <v>362</v>
+      </c>
+      <c r="G334" s="98" t="s">
+        <v>144</v>
+      </c>
       <c r="H334" s="44"/>
       <c r="I334" s="44"/>
-      <c r="J334" s="44"/>
+      <c r="J334" s="44">
+        <v>0.38900000000000001</v>
+      </c>
       <c r="K334" s="48"/>
       <c r="L334" s="57"/>
-      <c r="M334" s="57"/>
-      <c r="N334" s="57"/>
+      <c r="M334" s="57" t="s">
+        <v>363</v>
+      </c>
+      <c r="N334" s="40" t="s">
+        <v>347</v>
+      </c>
       <c r="O334" s="44"/>
       <c r="P334" s="44"/>
       <c r="Q334" s="44"/>

</xml_diff>